<commit_message>
diameter measured by max side length of cell
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -875,7 +875,7 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <v>-2.446304268323845</v>
+        <v>-2.446861267673397</v>
       </c>
       <c r="G21">
         <v>-0.02512155297761431</v>
@@ -898,7 +898,7 @@
         <v>6</v>
       </c>
       <c r="F22">
-        <v>-2.46253614305795</v>
+        <v>-2.4627908385039</v>
       </c>
       <c r="G22">
         <v>-0.02885137346255817</v>
@@ -921,7 +921,7 @@
         <v>7</v>
       </c>
       <c r="F23">
-        <v>-2.478211018442502</v>
+        <v>-2.478913794385451</v>
       </c>
       <c r="G23">
         <v>-0.03202419459794914</v>
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>-2.493885893827055</v>
+        <v>-2.494479750917451</v>
       </c>
       <c r="G24">
         <v>-0.03519701573334055</v>
@@ -990,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="F26">
-        <v>-2.525260539905271</v>
+        <v>-2.525316179332341</v>
       </c>
       <c r="G26">
         <v>-0.04156755331323514</v>
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.538590468069642</v>
+        <v>-2.53895801383046</v>
       </c>
       <c r="G27">
         <v>-0.0423954272284448</v>
@@ -1036,7 +1036,7 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <v>-2.553458082449747</v>
+        <v>-2.554191710881758</v>
       </c>
       <c r="G28">
         <v>-0.04476098735938883</v>
@@ -1059,7 +1059,7 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <v>-2.567878685464839</v>
+        <v>-2.569627523964137</v>
       </c>
       <c r="G29">
         <v>-0.04667953612532028</v>
@@ -1082,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <v>-2.583576884697776</v>
+        <v>-2.585565746260133</v>
       </c>
       <c r="G30">
         <v>-0.04987568110909657</v>
@@ -1105,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="F31">
-        <v>-2.598345208117325</v>
+        <v>-2.600317647995041</v>
       </c>
       <c r="G31">
         <v>-0.05214195027948443</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.611577197799168</v>
+        <v>-2.613829166823519</v>
       </c>
       <c r="G32">
         <v>-0.05287188571216661</v>
@@ -1220,7 +1220,7 @@
         <v>20</v>
       </c>
       <c r="F36">
-        <v>-2.668985900200962</v>
+        <v>-2.670054148115264</v>
       </c>
       <c r="G36">
         <v>-0.0602723711173172</v>
@@ -1243,7 +1243,7 @@
         <v>21</v>
       </c>
       <c r="F37">
-        <v>-2.681542021430008</v>
+        <v>-2.685274916457318</v>
       </c>
       <c r="G37">
         <v>-0.06032643809720217</v>
@@ -1266,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="F38">
-        <v>-2.696067335419448</v>
+        <v>-2.69653929818537</v>
       </c>
       <c r="G38">
         <v>-0.06234969783748068</v>
@@ -1289,7 +1289,7 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.709700069816162</v>
+        <v>-2.709784141431431</v>
       </c>
       <c r="G39">
         <v>-0.06348037798503348</v>
@@ -1335,7 +1335,7 @@
         <v>25</v>
       </c>
       <c r="F41">
-        <v>-2.733344320569291</v>
+        <v>-2.736116639561843</v>
       </c>
       <c r="G41">
         <v>-0.06212052023984116</v>
@@ -1358,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.748818213047949</v>
+        <v>-2.748976580326271</v>
       </c>
       <c r="G42">
         <v>-0.0650923584693377</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.760564593402365</v>
+        <v>-2.76294278232252</v>
       </c>
       <c r="G43">
         <v>-0.06433668457459296</v>
@@ -1427,7 +1427,7 @@
         <v>29</v>
       </c>
       <c r="F45">
-        <v>-2.785077927831195</v>
+        <v>-2.785099086349504</v>
       </c>
       <c r="G45">
         <v>-0.06384591050510124</v>
@@ -1473,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="F47">
-        <v>-2.80967412575646</v>
+        <v>-2.811376040333823</v>
       </c>
       <c r="G47">
         <v>-0.06343799993204424</v>
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.819172190093838</v>
+        <v>-2.823106893876452</v>
       </c>
       <c r="G48">
         <v>-0.06043401002026194</v>
@@ -1519,7 +1519,7 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.832091904518389</v>
+        <v>-2.834657214447406</v>
       </c>
       <c r="G49">
         <v>-0.06085167019565196</v>
@@ -1542,7 +1542,7 @@
         <v>34</v>
       </c>
       <c r="F50">
-        <v>-2.842829667956442</v>
+        <v>-2.846430012960594</v>
       </c>
       <c r="G50">
         <v>-0.059087379384544</v>
@@ -1565,7 +1565,7 @@
         <v>35</v>
       </c>
       <c r="F51">
-        <v>-2.855560284179206</v>
+        <v>-2.85564213899431</v>
       </c>
       <c r="G51">
         <v>-0.05931594135814644</v>
@@ -1588,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.865491920547252</v>
+        <v>-2.867386159347139</v>
       </c>
       <c r="G52">
         <v>-0.05674552347703155</v>
@@ -1611,7 +1611,7 @@
         <v>37</v>
       </c>
       <c r="F53">
-        <v>-2.879423677346405</v>
+        <v>-2.879576437505818</v>
       </c>
       <c r="G53">
         <v>-0.05817522602702407</v>
@@ -1634,7 +1634,7 @@
         <v>38</v>
       </c>
       <c r="F54">
-        <v>-2.888770734849971</v>
+        <v>-2.890334064759451</v>
       </c>
       <c r="G54">
         <v>-0.0550202292814288</v>
@@ -1657,7 +1657,7 @@
         <v>39</v>
       </c>
       <c r="F55">
-        <v>-2.899237423357019</v>
+        <v>-2.900336666771084</v>
       </c>
       <c r="G55">
         <v>-0.05298486353931542</v>
@@ -1680,7 +1680,7 @@
         <v>40</v>
       </c>
       <c r="F56">
-        <v>-2.909972766684932</v>
+        <v>-2.911006771982149</v>
       </c>
       <c r="G56">
         <v>-0.05121815261806784</v>
@@ -1703,7 +1703,7 @@
         <v>41</v>
       </c>
       <c r="F57">
-        <v>-2.92083108279133</v>
+        <v>-2.921642634576131</v>
       </c>
       <c r="G57">
         <v>-0.04957441447530531</v>
@@ -1726,7 +1726,7 @@
         <v>42</v>
       </c>
       <c r="F58">
-        <v>-2.928951667764456</v>
+        <v>-2.933242809114328</v>
       </c>
       <c r="G58">
         <v>-0.04519294519926986</v>
@@ -1772,7 +1772,7 @@
         <v>44</v>
       </c>
       <c r="F60">
-        <v>-2.950672759085879</v>
+        <v>-2.951162173853596</v>
       </c>
       <c r="G60">
         <v>-0.04190992802237153</v>
@@ -1795,7 +1795,7 @@
         <v>45</v>
       </c>
       <c r="F61">
-        <v>-2.960234706538099</v>
+        <v>-2.961108249322427</v>
       </c>
       <c r="G61">
         <v>-0.03896982122542986</v>
@@ -1818,7 +1818,7 @@
         <v>46</v>
       </c>
       <c r="F62">
-        <v>-2.969090452937647</v>
+        <v>-2.970910478976625</v>
       </c>
       <c r="G62">
         <v>-0.03532351337581685</v>
@@ -1933,7 +1933,7 @@
         <v>51</v>
       </c>
       <c r="F67">
-        <v>-3.014979193855097</v>
+        <v>-3.015708890824793</v>
       </c>
       <c r="G67">
         <v>-0.01870198304746321</v>
@@ -2117,7 +2117,7 @@
         <v>3</v>
       </c>
       <c r="F75">
-        <v>-2.549224937741412</v>
+        <v>-2.549645888452907</v>
       </c>
       <c r="G75">
         <v>-0.007008898470076019</v>
@@ -2163,7 +2163,7 @@
         <v>5</v>
       </c>
       <c r="F77">
-        <v>-2.5637771600514</v>
+        <v>-2.563803711582159</v>
       </c>
       <c r="G77">
         <v>-0.01153748281947742</v>
@@ -2186,7 +2186,7 @@
         <v>6</v>
       </c>
       <c r="F78">
-        <v>-2.569999045564249</v>
+        <v>-2.571117660587071</v>
       </c>
       <c r="G78">
         <v>-0.01274754935203282</v>
@@ -2209,7 +2209,7 @@
         <v>7</v>
       </c>
       <c r="F79">
-        <v>-2.577362399903862</v>
+        <v>-2.577635415776877</v>
       </c>
       <c r="G79">
         <v>-0.01509908471135235</v>
@@ -2255,7 +2255,7 @@
         <v>9</v>
       </c>
       <c r="F81">
-        <v>-2.590286788925643</v>
+        <v>-2.590773153387083</v>
       </c>
       <c r="G81">
         <v>-0.01799983577254682</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <v>-2.596921012188377</v>
+        <v>-2.597828327361313</v>
       </c>
       <c r="G82">
         <v>-0.01962224005498747</v>
@@ -2301,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="F83">
-        <v>-2.603836864285735</v>
+        <v>-2.604111928897288</v>
       </c>
       <c r="G83">
         <v>-0.02152627317205269</v>
@@ -2347,7 +2347,7 @@
         <v>13</v>
       </c>
       <c r="F85">
-        <v>-2.616601622821598</v>
+        <v>-2.617483820161325</v>
       </c>
       <c r="G85">
         <v>-0.02426739374732811</v>
@@ -2370,7 +2370,7 @@
         <v>14</v>
       </c>
       <c r="F86">
-        <v>-2.623574878174282</v>
+        <v>-2.624373120727923</v>
       </c>
       <c r="G86">
         <v>-0.02622883011971888</v>
@@ -2393,7 +2393,7 @@
         <v>15</v>
       </c>
       <c r="F87">
-        <v>-2.628896286900178</v>
+        <v>-2.631046206209842</v>
       </c>
       <c r="G87">
         <v>-0.02653841986532246</v>
@@ -2416,7 +2416,7 @@
         <v>16</v>
       </c>
       <c r="F88">
-        <v>-2.635523635771994</v>
+        <v>-2.636997266693653</v>
       </c>
       <c r="G88">
         <v>-0.02815394975684438</v>
@@ -2462,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="F90">
-        <v>-2.648235865203298</v>
+        <v>-2.649704467294752</v>
       </c>
       <c r="G90">
         <v>-0.03084254122756214</v>
@@ -2485,7 +2485,7 @@
         <v>19</v>
       </c>
       <c r="F91">
-        <v>-2.655797334095641</v>
+        <v>-2.655845450918066</v>
       </c>
       <c r="G91">
         <v>-0.03339219113961223</v>
@@ -2531,7 +2531,7 @@
         <v>21</v>
       </c>
       <c r="F93">
-        <v>-2.667866499708578</v>
+        <v>-2.667934753083544</v>
       </c>
       <c r="G93">
         <v>-0.03543771879196145</v>
@@ -2554,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="F94">
-        <v>-2.673498241737283</v>
+        <v>-2.675394893960385</v>
       </c>
       <c r="G94">
         <v>-0.0360576418403733</v>
@@ -2600,7 +2600,7 @@
         <v>24</v>
       </c>
       <c r="F96">
-        <v>-2.686040775161607</v>
+        <v>-2.686328935085805</v>
       </c>
       <c r="G96">
         <v>-0.03857653730411048</v>
@@ -2646,7 +2646,7 @@
         <v>26</v>
       </c>
       <c r="F98">
-        <v>-2.698305024946408</v>
+        <v>-2.699644622221615</v>
       </c>
       <c r="G98">
         <v>-0.0408171491283249</v>
@@ -2692,7 +2692,7 @@
         <v>28</v>
       </c>
       <c r="F100">
-        <v>-2.710950673726911</v>
+        <v>-2.711903960902909</v>
       </c>
       <c r="G100">
         <v>-0.04343915994824155</v>
@@ -2738,7 +2738,7 @@
         <v>30</v>
       </c>
       <c r="F102">
-        <v>-2.721497920690854</v>
+        <v>-2.723197531789195</v>
       </c>
       <c r="G102">
         <v>-0.04396276895159845</v>
@@ -2784,7 +2784,7 @@
         <v>32</v>
       </c>
       <c r="F104">
-        <v>-2.733932912056694</v>
+        <v>-2.734841896097155</v>
       </c>
       <c r="G104">
         <v>-0.04637412235685168</v>
@@ -2807,7 +2807,7 @@
         <v>33</v>
       </c>
       <c r="F105">
-        <v>-2.74074374035155</v>
+        <v>-2.74198346745841</v>
       </c>
       <c r="G105">
         <v>-0.04817313167141402</v>
@@ -2830,7 +2830,7 @@
         <v>34</v>
       </c>
       <c r="F106">
-        <v>-2.745921500807752</v>
+        <v>-2.746910308154112</v>
       </c>
       <c r="G106">
         <v>-0.04833907314732233</v>
@@ -2876,7 +2876,7 @@
         <v>36</v>
       </c>
       <c r="F108">
-        <v>-2.756320066351996</v>
+        <v>-2.759191329649788</v>
       </c>
       <c r="G108">
         <v>-0.04871400073098031</v>
@@ -2922,7 +2922,7 @@
         <v>38</v>
       </c>
       <c r="F110">
-        <v>-2.769300310672788</v>
+        <v>-2.76991277035548</v>
       </c>
       <c r="G110">
         <v>-0.05167060709118543</v>
@@ -2945,7 +2945,7 @@
         <v>39</v>
       </c>
       <c r="F111">
-        <v>-2.775732453128144</v>
+        <v>-2.776495217187342</v>
       </c>
       <c r="G111">
         <v>-0.05309093056624747</v>
@@ -2968,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.78006918453531</v>
+        <v>-2.78084232724349</v>
       </c>
       <c r="G112">
         <v>-0.05241584299312052</v>
@@ -2991,7 +2991,7 @@
         <v>41</v>
       </c>
       <c r="F113">
-        <v>-2.787191709803604</v>
+        <v>-2.787430658876814</v>
       </c>
       <c r="G113">
         <v>-0.05452654928112111</v>
@@ -3014,7 +3014,7 @@
         <v>42</v>
       </c>
       <c r="F114">
-        <v>-2.79276475675031</v>
+        <v>-2.794003889466307</v>
       </c>
       <c r="G114">
         <v>-0.05508777724753333</v>
@@ -3060,7 +3060,7 @@
         <v>44</v>
       </c>
       <c r="F116">
-        <v>-2.803294722142879</v>
+        <v>-2.804297164510983</v>
       </c>
       <c r="G116">
         <v>-0.05559410467951587</v>
@@ -3083,7 +3083,7 @@
         <v>45</v>
       </c>
       <c r="F117">
-        <v>-2.809265290124293</v>
+        <v>-2.810352855206683</v>
       </c>
       <c r="G117">
         <v>-0.05655285368063656</v>
@@ -3106,7 +3106,7 @@
         <v>46</v>
       </c>
       <c r="F118">
-        <v>-2.815866402883023</v>
+        <v>-2.816805008523441</v>
       </c>
       <c r="G118">
         <v>-0.05814214745907353</v>
@@ -3129,7 +3129,7 @@
         <v>47</v>
       </c>
       <c r="F119">
-        <v>-2.821410850528963</v>
+        <v>-2.822089121331726</v>
       </c>
       <c r="G119">
         <v>-0.05867477612472016</v>
@@ -3152,7 +3152,7 @@
         <v>48</v>
       </c>
       <c r="F120">
-        <v>-2.826110441402161</v>
+        <v>-2.827518631445594</v>
       </c>
       <c r="G120">
         <v>-0.05836254801762486</v>
@@ -3175,7 +3175,7 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.831580676878582</v>
+        <v>-2.83211018396532</v>
       </c>
       <c r="G121">
         <v>-0.05882096451375207</v>
@@ -3198,7 +3198,7 @@
         <v>50</v>
       </c>
       <c r="F122">
-        <v>-2.837593736688727</v>
+        <v>-2.838690763344899</v>
       </c>
       <c r="G122">
         <v>-0.05982220534360372</v>
@@ -3221,7 +3221,7 @@
         <v>51</v>
       </c>
       <c r="F123">
-        <v>-2.841307756770089</v>
+        <v>-2.843982736750677</v>
       </c>
       <c r="G123">
         <v>-0.05852440644467238</v>
@@ -3244,7 +3244,7 @@
         <v>52</v>
       </c>
       <c r="F124">
-        <v>-2.847542369914219</v>
+        <v>-2.849826490038113</v>
       </c>
       <c r="G124">
         <v>-0.05974720060850958</v>
@@ -3267,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.853243622516836</v>
+        <v>-2.854583052712755</v>
       </c>
       <c r="G125">
         <v>-0.06043663423083312</v>
@@ -3290,7 +3290,7 @@
         <v>54</v>
       </c>
       <c r="F126">
-        <v>-2.858316968898654</v>
+        <v>-2.859132449250283</v>
       </c>
       <c r="G126">
         <v>-0.06049816163235744</v>
@@ -3313,7 +3313,7 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.863991218875005</v>
+        <v>-2.86719983493051</v>
       </c>
       <c r="G127">
         <v>-0.06116059262841467</v>
@@ -3336,7 +3336,7 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.867840744315324</v>
+        <v>-2.870362107343745</v>
       </c>
       <c r="G128">
         <v>-0.05999829908844112</v>
@@ -3359,7 +3359,7 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.874475503637542</v>
+        <v>-2.875876582211734</v>
       </c>
       <c r="G129">
         <v>-0.06162123943036568</v>
@@ -3382,7 +3382,7 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.880222122645228</v>
+        <v>-2.882435439562722</v>
       </c>
       <c r="G130">
         <v>-0.06235603945775781</v>
@@ -3405,7 +3405,7 @@
         <v>59</v>
       </c>
       <c r="F131">
-        <v>-2.884636024186367</v>
+        <v>-2.889240698585287</v>
       </c>
       <c r="G131">
         <v>-0.06175812201860365</v>
@@ -3428,7 +3428,7 @@
         <v>60</v>
       </c>
       <c r="F132">
-        <v>-2.891619868154029</v>
+        <v>-2.893465846059668</v>
       </c>
       <c r="G132">
         <v>-0.06373014700597257</v>
@@ -3451,7 +3451,7 @@
         <v>61</v>
       </c>
       <c r="F133">
-        <v>-2.897922019928143</v>
+        <v>-2.898599839698962</v>
       </c>
       <c r="G133">
         <v>-0.06502047979979309</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.902333539835631</v>
+        <v>-2.902784262781478</v>
       </c>
       <c r="G134">
         <v>-0.06442018072698819</v>
@@ -3497,7 +3497,7 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.907844510210378</v>
+        <v>-2.911344959368382</v>
       </c>
       <c r="G135">
         <v>-0.06491933212144141</v>
@@ -3520,7 +3520,7 @@
         <v>64</v>
       </c>
       <c r="F136">
-        <v>-2.913667479428813</v>
+        <v>-2.915119194748633</v>
       </c>
       <c r="G136">
         <v>-0.06573048235958368</v>
@@ -3543,7 +3543,7 @@
         <v>65</v>
       </c>
       <c r="F137">
-        <v>-2.917004532781728</v>
+        <v>-2.918736041320013</v>
       </c>
       <c r="G137">
         <v>-0.06405571673220445</v>
@@ -3612,7 +3612,7 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.933548912838784</v>
+        <v>-2.934396255636049</v>
       </c>
       <c r="G140">
         <v>-0.06556463984838112</v>
@@ -3635,7 +3635,7 @@
         <v>69</v>
       </c>
       <c r="F141">
-        <v>-2.938839401051222</v>
+        <v>-2.939035433085397</v>
       </c>
       <c r="G141">
         <v>-0.06584330908052571</v>
@@ -3658,7 +3658,7 @@
         <v>70</v>
       </c>
       <c r="F142">
-        <v>-2.942698001904313</v>
+        <v>-2.944116527247888</v>
       </c>
       <c r="G142">
         <v>-0.06469009095332323</v>
@@ -3704,7 +3704,7 @@
         <v>72</v>
       </c>
       <c r="F144">
-        <v>-2.953897011367544</v>
+        <v>-2.955285717616995</v>
       </c>
       <c r="G144">
         <v>-0.06586546245596736</v>
@@ -3750,7 +3750,7 @@
         <v>74</v>
       </c>
       <c r="F146">
-        <v>-2.96326163966478</v>
+        <v>-2.964646617165207</v>
       </c>
       <c r="G146">
         <v>-0.06520645279261617</v>
@@ -3796,7 +3796,7 @@
         <v>76</v>
       </c>
       <c r="F148">
-        <v>-2.972745849725552</v>
+        <v>-2.974853673529919</v>
       </c>
       <c r="G148">
         <v>-0.06466702489280229</v>
@@ -3819,7 +3819,7 @@
         <v>77</v>
       </c>
       <c r="F149">
-        <v>-2.97823401895261</v>
+        <v>-2.981286530873104</v>
       </c>
       <c r="G149">
         <v>-0.06514337513956647</v>
@@ -3888,7 +3888,7 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.992714826305125</v>
+        <v>-2.994525855714862</v>
       </c>
       <c r="G152">
         <v>-0.06458872555120188</v>
@@ -3911,7 +3911,7 @@
         <v>81</v>
       </c>
       <c r="F153">
-        <v>-2.997842388432455</v>
+        <v>-2.999357774161187</v>
       </c>
       <c r="G153">
         <v>-0.06470446869823787</v>
@@ -3934,7 +3934,7 @@
         <v>82</v>
       </c>
       <c r="F154">
-        <v>-3.001375241236655</v>
+        <v>-3.004439759900296</v>
       </c>
       <c r="G154">
         <v>-0.06322550252214532</v>
@@ -3957,7 +3957,7 @@
         <v>83</v>
       </c>
       <c r="F155">
-        <v>-3.005680536519928</v>
+        <v>-3.008119125448723</v>
       </c>
       <c r="G155">
         <v>-0.06251897882512414</v>
@@ -3980,7 +3980,7 @@
         <v>84</v>
       </c>
       <c r="F156">
-        <v>-3.012397622028552</v>
+        <v>-3.014982823420358</v>
       </c>
       <c r="G156">
         <v>-0.06422424535345517</v>
@@ -4003,7 +4003,7 @@
         <v>85</v>
       </c>
       <c r="F157">
-        <v>-3.015088459887066</v>
+        <v>-3.018098786361477</v>
       </c>
       <c r="G157">
         <v>-0.06190326423167614</v>
@@ -4026,7 +4026,7 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.024430774396691</v>
+        <v>-3.024750886846435</v>
       </c>
       <c r="G158">
         <v>-0.0662337597610072</v>
@@ -4072,7 +4072,7 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.030204798416815</v>
+        <v>-3.032698724719683</v>
       </c>
       <c r="G160">
         <v>-0.06198414582054457</v>
@@ -4210,7 +4210,7 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.058879328375883</v>
+        <v>-3.060136029088066</v>
       </c>
       <c r="G166">
         <v>-0.06058776189785309</v>
@@ -4233,7 +4233,7 @@
         <v>95</v>
       </c>
       <c r="F167">
-        <v>-3.064271464506121</v>
+        <v>-3.064968187189892</v>
       </c>
       <c r="G167">
         <v>-0.06096807904779766</v>
@@ -4256,7 +4256,7 @@
         <v>96</v>
       </c>
       <c r="F168">
-        <v>-3.067918572873439</v>
+        <v>-3.068273021974731</v>
       </c>
       <c r="G168">
         <v>-0.05960336843482184</v>
@@ -4279,7 +4279,7 @@
         <v>97</v>
       </c>
       <c r="F169">
-        <v>-3.072240581556022</v>
+        <v>-3.073370432202983</v>
       </c>
       <c r="G169">
         <v>-0.05891355813711219</v>
@@ -4302,7 +4302,7 @@
         <v>98</v>
       </c>
       <c r="F170">
-        <v>-3.075643345068223</v>
+        <v>-3.079332351276757</v>
       </c>
       <c r="G170">
         <v>-0.05730450266901987</v>
@@ -4325,7 +4325,7 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.082047268529166</v>
+        <v>-3.082461602294905</v>
       </c>
       <c r="G171">
         <v>-0.05869660714966918</v>
@@ -4348,7 +4348,7 @@
         <v>100</v>
       </c>
       <c r="F172">
-        <v>-3.086916267589751</v>
+        <v>-3.08766604047963</v>
       </c>
       <c r="G172">
         <v>-0.05855378722996052</v>
@@ -4371,7 +4371,7 @@
         <v>101</v>
       </c>
       <c r="F173">
-        <v>-3.089683423169322</v>
+        <v>-3.091946288182141</v>
       </c>
       <c r="G173">
         <v>-0.05630912382923858</v>
@@ -4394,7 +4394,7 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.094398059802805</v>
+        <v>-3.096716494882646</v>
       </c>
       <c r="G174">
         <v>-0.0560119414824285</v>
@@ -4417,7 +4417,7 @@
         <v>103</v>
       </c>
       <c r="F175">
-        <v>-3.099818499860421</v>
+        <v>-3.100456974546988</v>
       </c>
       <c r="G175">
         <v>-0.05642056255975092</v>
@@ -4463,7 +4463,7 @@
         <v>105</v>
       </c>
       <c r="F177">
-        <v>-3.107882906223762</v>
+        <v>-3.109829449511393</v>
       </c>
       <c r="G177">
         <v>-0.05446133096250516</v>
@@ -4532,7 +4532,7 @@
         <v>108</v>
       </c>
       <c r="F180">
-        <v>-3.120931822700043</v>
+        <v>-3.12212140043591</v>
       </c>
       <c r="G180">
         <v>-0.05247479049790593</v>
@@ -4555,7 +4555,7 @@
         <v>109</v>
       </c>
       <c r="F181">
-        <v>-3.125022710449717</v>
+        <v>-3.126639158692338</v>
       </c>
       <c r="G181">
         <v>-0.05155385926728662</v>
@@ -4578,7 +4578,7 @@
         <v>110</v>
       </c>
       <c r="F182">
-        <v>-3.129899714547076</v>
+        <v>-3.131122799614015</v>
       </c>
       <c r="G182">
         <v>-0.0514190443843523</v>
@@ -4601,7 +4601,7 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.133819209030275</v>
+        <v>-3.134310979988831</v>
       </c>
       <c r="G183">
         <v>-0.05032671988725779</v>
@@ -4647,7 +4647,7 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.141042832182841</v>
+        <v>-3.142932424913802</v>
       </c>
       <c r="G185">
         <v>-0.0475267050792374</v>
@@ -4670,7 +4670,7 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.146917215892854</v>
+        <v>-3.147222261639312</v>
       </c>
       <c r="G186">
         <v>-0.0483892698089563</v>
@@ -4693,7 +4693,7 @@
         <v>115</v>
       </c>
       <c r="F187">
-        <v>-3.149832541278458</v>
+        <v>-3.151378322013548</v>
       </c>
       <c r="G187">
         <v>-0.04629277621426797</v>
@@ -4716,7 +4716,7 @@
         <v>116</v>
       </c>
       <c r="F188">
-        <v>-3.153322777952597</v>
+        <v>-3.154395216013283</v>
       </c>
       <c r="G188">
         <v>-0.04477119390811302</v>
@@ -4739,7 +4739,7 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.157952357319359</v>
+        <v>-3.158639559257619</v>
       </c>
       <c r="G189">
         <v>-0.04438895429458223</v>
@@ -4762,7 +4762,7 @@
         <v>118</v>
       </c>
       <c r="F190">
-        <v>-3.163527839286385</v>
+        <v>-3.164086877749303</v>
       </c>
       <c r="G190">
         <v>-0.04495261728131517</v>
@@ -4785,7 +4785,7 @@
         <v>119</v>
       </c>
       <c r="F191">
-        <v>-3.16593475033183</v>
+        <v>-3.167963602154305</v>
       </c>
       <c r="G191">
         <v>-0.04234770934646692</v>
@@ -4831,7 +4831,7 @@
         <v>121</v>
       </c>
       <c r="F193">
-        <v>-3.173323994311076</v>
+        <v>-3.175214119743011</v>
       </c>
       <c r="G193">
         <v>-0.03971331536512507</v>
@@ -4854,7 +4854,7 @@
         <v>122</v>
       </c>
       <c r="F194">
-        <v>-3.179033949545417</v>
+        <v>-3.180288055942324</v>
       </c>
       <c r="G194">
         <v>-0.0404114516191727</v>
@@ -4877,7 +4877,7 @@
         <v>123</v>
       </c>
       <c r="F195">
-        <v>-3.181235170653781</v>
+        <v>-3.181987514978506</v>
       </c>
       <c r="G195">
         <v>-0.03760085374724426</v>
@@ -4923,7 +4923,7 @@
         <v>125</v>
       </c>
       <c r="F197">
-        <v>-3.189153390356859</v>
+        <v>-3.191851091102457</v>
       </c>
       <c r="G197">
         <v>-0.03549543548973461</v>
@@ -4969,7 +4969,7 @@
         <v>127</v>
       </c>
       <c r="F199">
-        <v>-3.198262141282629</v>
+        <v>-3.198916613499793</v>
       </c>
       <c r="G199">
         <v>-0.03458054845491842</v>
@@ -4992,7 +4992,7 @@
         <v>128</v>
       </c>
       <c r="F200">
-        <v>-3.19896655967908</v>
+        <v>-3.20322597192534</v>
       </c>
       <c r="G200">
         <v>-0.03027314787107582</v>
@@ -5015,7 +5015,7 @@
         <v>129</v>
       </c>
       <c r="F201">
-        <v>-3.204527935021595</v>
+        <v>-3.206463821361251</v>
       </c>
       <c r="G201">
         <v>-0.03082270423329841</v>
@@ -5038,7 +5038,7 @@
         <v>130</v>
       </c>
       <c r="F202">
-        <v>-3.208813934302035</v>
+        <v>-3.210279052586828</v>
       </c>
       <c r="G202">
         <v>-0.03009688453344472</v>
@@ -5061,7 +5061,7 @@
         <v>131</v>
       </c>
       <c r="F203">
-        <v>-3.212285544250408</v>
+        <v>-3.213212167664172</v>
       </c>
       <c r="G203">
         <v>-0.02855667550152441</v>
@@ -5084,7 +5084,7 @@
         <v>132</v>
       </c>
       <c r="F204">
-        <v>-3.214812568386761</v>
+        <v>-3.217115825779265</v>
       </c>
       <c r="G204">
         <v>-0.02607188065758331</v>
@@ -5107,7 +5107,7 @@
         <v>133</v>
       </c>
       <c r="F205">
-        <v>-3.218946197856297</v>
+        <v>-3.219624270538844</v>
       </c>
       <c r="G205">
         <v>-0.02519369114682696</v>
@@ -5130,7 +5130,7 @@
         <v>134</v>
       </c>
       <c r="F206">
-        <v>-3.223489318231697</v>
+        <v>-3.224000609868446</v>
       </c>
       <c r="G206">
         <v>-0.02472499254193353</v>
@@ -5153,7 +5153,7 @@
         <v>135</v>
       </c>
       <c r="F207">
-        <v>-3.227235288687158</v>
+        <v>-3.22798087891676</v>
       </c>
       <c r="G207">
         <v>-0.023459144017101</v>
@@ -5176,7 +5176,7 @@
         <v>136</v>
       </c>
       <c r="F208">
-        <v>-3.229980787708872</v>
+        <v>-3.230680608947998</v>
       </c>
       <c r="G208">
         <v>-0.02119282405852102</v>
@@ -5199,7 +5199,7 @@
         <v>137</v>
       </c>
       <c r="F209">
-        <v>-3.233540659175669</v>
+        <v>-3.23379488012825</v>
       </c>
       <c r="G209">
         <v>-0.01974087654502524</v>
@@ -5222,7 +5222,7 @@
         <v>138</v>
       </c>
       <c r="F210">
-        <v>-3.236276755681332</v>
+        <v>-3.238177520384522</v>
       </c>
       <c r="G210">
         <v>-0.01746515407039462</v>
@@ -5268,7 +5268,7 @@
         <v>140</v>
       </c>
       <c r="F212">
-        <v>-3.242882560820803</v>
+        <v>-3.24328493202876</v>
       </c>
       <c r="G212">
         <v>-0.01404732124927888</v>
@@ -5291,7 +5291,7 @@
         <v>141</v>
       </c>
       <c r="F213">
-        <v>-3.246250141058008</v>
+        <v>-3.246757671067543</v>
       </c>
       <c r="G213">
         <v>-0.01240308250619089</v>
@@ -5337,7 +5337,7 @@
         <v>143</v>
       </c>
       <c r="F215">
-        <v>-3.251970241513355</v>
+        <v>-3.252477771522887</v>
       </c>
       <c r="G215">
         <v>-0.008099545000950795</v>
@@ -5475,7 +5475,7 @@
         <v>30</v>
       </c>
       <c r="F221">
-        <v>-2.72188797946074</v>
+        <v>-2.722098622839157</v>
       </c>
       <c r="G221">
         <v>-0.02598157408172064</v>
@@ -5498,7 +5498,7 @@
         <v>61</v>
       </c>
       <c r="F222">
-        <v>-2.817235903591573</v>
+        <v>-2.818414889382493</v>
       </c>
       <c r="G222">
         <v>-0.04465284086214671</v>
@@ -5521,7 +5521,7 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.905938355931358</v>
+        <v>-2.906581417191302</v>
       </c>
       <c r="G223">
         <v>-0.05667863585152433</v>
@@ -5544,7 +5544,7 @@
         <v>123</v>
       </c>
       <c r="F224">
-        <v>-2.988016705096978</v>
+        <v>-2.990162523613378</v>
       </c>
       <c r="G224">
         <v>-0.06208032766673743</v>
@@ -5567,7 +5567,7 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.067792577576289</v>
+        <v>-3.068132663677019</v>
       </c>
       <c r="G225">
         <v>-0.0651795427956412</v>
@@ -5590,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.141053867807812</v>
+        <v>-3.142806209668382</v>
       </c>
       <c r="G226">
         <v>-0.06176417567675752</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.274998678623595</v>
+        <v>-3.275748615166611</v>
       </c>
       <c r="G228">
         <v>-0.04235567179172572</v>
@@ -5659,7 +5659,7 @@
         <v>278</v>
       </c>
       <c r="F229">
-        <v>-3.33406656798564</v>
+        <v>-3.334782959800346</v>
       </c>
       <c r="G229">
         <v>-0.02474690380336431</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.786240178245846</v>
+        <v>-2.78687455409906</v>
       </c>
       <c r="G232">
         <v>-0.02627093675704639</v>
@@ -5751,7 +5751,7 @@
         <v>112</v>
       </c>
       <c r="F233">
-        <v>-2.881980806095768</v>
+        <v>-2.883379759432807</v>
       </c>
       <c r="G233">
         <v>-0.04396603691345913</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.972463421737286</v>
+        <v>-2.972662389406547</v>
       </c>
       <c r="G234">
         <v>-0.05640312486146803</v>
@@ -5797,7 +5797,7 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.055414113540615</v>
+        <v>-3.055648623971288</v>
       </c>
       <c r="G235">
         <v>-0.06130828897128859</v>
@@ -5820,7 +5820,7 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.135647754395753</v>
+        <v>-3.136442855885208</v>
       </c>
       <c r="G236">
         <v>-0.06349640213291674</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.280823422108233</v>
+        <v>-3.282719771767355</v>
       </c>
       <c r="G238">
         <v>-0.05258101445837926</v>
@@ -5889,7 +5889,7 @@
         <v>448</v>
       </c>
       <c r="F239">
-        <v>-3.346739977860398</v>
+        <v>-3.347663222189207</v>
       </c>
       <c r="G239">
         <v>-0.04045204251703594</v>
@@ -5912,7 +5912,7 @@
         <v>504</v>
       </c>
       <c r="F240">
-        <v>-3.408870648171125</v>
+        <v>-3.409099268613306</v>
       </c>
       <c r="G240">
         <v>-0.02453718513425368</v>
@@ -5981,7 +5981,7 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.828522224254397</v>
+        <v>-2.828563068146172</v>
       </c>
       <c r="G243">
         <v>-0.02581220560998343</v>
@@ -6004,7 +6004,7 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.925695904575883</v>
+        <v>-2.926043781772897</v>
       </c>
       <c r="G244">
         <v>-0.04384498982082752</v>
@@ -6027,7 +6027,7 @@
         <v>276</v>
       </c>
       <c r="F245">
-        <v>-3.016805601316094</v>
+        <v>-3.017401623633949</v>
       </c>
       <c r="G245">
         <v>-0.05581379045039592</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.101371483891614</v>
+        <v>-3.102163394301011</v>
       </c>
       <c r="G246">
         <v>-0.06037854978363622</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.258741124426968</v>
+        <v>-3.259546611615602</v>
       </c>
       <c r="G248">
         <v>-0.05946639809770504</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.331481683878906</v>
+        <v>-3.332450252831135</v>
       </c>
       <c r="G249">
         <v>-0.05220583430736225</v>
@@ -6165,7 +6165,7 @@
         <v>830</v>
       </c>
       <c r="F251">
-        <v>-3.461041550919604</v>
+        <v>-3.461293727546931</v>
       </c>
       <c r="G251">
         <v>-0.02348390912677606</v>
@@ -6257,7 +6257,7 @@
         <v>283</v>
       </c>
       <c r="F255">
-        <v>-2.958435354675863</v>
+        <v>-2.958811360264598</v>
       </c>
       <c r="G255">
         <v>-0.04380213962222745</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.135450143171877</v>
+        <v>-3.136058546667661</v>
       </c>
       <c r="G257">
         <v>-0.06024136341956599</v>
@@ -6326,7 +6326,7 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.216850879325006</v>
+        <v>-3.216996919513611</v>
       </c>
       <c r="G258">
         <v>-0.06163801963448479</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.294588426271033</v>
+        <v>-3.295131676644201</v>
       </c>
       <c r="G259">
         <v>-0.05880408182004593</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.366917683253881</v>
+        <v>-3.367635510717266</v>
       </c>
       <c r="G260">
         <v>-0.05112925886468378</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.436046704171573</v>
+        <v>-3.436345395248071</v>
       </c>
       <c r="G261">
         <v>-0.03968679502190919</v>
@@ -6418,7 +6418,7 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.499310195153469</v>
+        <v>-3.499322169800306</v>
       </c>
       <c r="G262">
         <v>-0.02294620606559572</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.8824079705537</v>
+        <v>-2.882575362766908</v>
       </c>
       <c r="G265">
         <v>-0.02438565895318945</v>
@@ -6510,7 +6510,7 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.9816884750399</v>
+        <v>-2.981894842247037</v>
       </c>
       <c r="G266">
         <v>-0.04258180329186079</v>
@@ -6556,7 +6556,7 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.160650036082037</v>
+        <v>-3.161237017899919</v>
       </c>
       <c r="G268">
         <v>-0.05976825743771474</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.242949548602908</v>
+        <v>-3.243194088622016</v>
       </c>
       <c r="G269">
         <v>-0.0609834098110571</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.463885609761365</v>
+        <v>-3.464103345814953</v>
       </c>
       <c r="G272">
         <v>-0.0390600039257023</v>
@@ -6671,7 +6671,7 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.528067804416733</v>
+        <v>-3.528366437609532</v>
       </c>
       <c r="G273">
         <v>-0.02215783843354158</v>
@@ -6740,7 +6740,7 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.901025683762118</v>
+        <v>-2.901443699658546</v>
       </c>
       <c r="G276">
         <v>-0.02410492755691784</v>
@@ -6763,7 +6763,7 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.00073265942732</v>
+        <v>-3.001056707528472</v>
       </c>
       <c r="G277">
         <v>-0.04228245081358217</v>
@@ -6809,7 +6809,7 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.181168162799583</v>
+        <v>-3.18129682226542</v>
       </c>
       <c r="G279">
         <v>-0.05965904936877275</v>
@@ -6832,7 +6832,7 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.263082956944234</v>
+        <v>-3.26372487840872</v>
       </c>
       <c r="G280">
         <v>-0.06004439110488713</v>
@@ -6855,7 +6855,7 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.342363472746117</v>
+        <v>-3.342391231771877</v>
       </c>
       <c r="G281">
         <v>-0.05779545449823376</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.486157443187338</v>
+        <v>-3.486506876446435</v>
       </c>
       <c r="G283">
         <v>-0.03853052012238201</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.551411858235559</v>
+        <v>-3.551496875574995</v>
       </c>
       <c r="G284">
         <v>-0.02225548276206646</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.916445277232262</v>
+        <v>-2.916601379362112</v>
       </c>
       <c r="G287">
         <v>-0.02403030586568988</v>
@@ -7016,7 +7016,7 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.016194391084935</v>
+        <v>-3.01657384583281</v>
       </c>
       <c r="G288">
         <v>-0.04186728267844808</v>
@@ -7039,7 +7039,7 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.10969448151351</v>
+        <v>-3.110365763700011</v>
       </c>
       <c r="G289">
         <v>-0.05345523606710678</v>
@@ -7062,7 +7062,7 @@
         <v>1548</v>
       </c>
       <c r="F290">
-        <v>-3.197493471595882</v>
+        <v>-3.197963346160399</v>
       </c>
       <c r="G290">
         <v>-0.05934208910956373</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.279966517216308</v>
+        <v>-3.280198966464786</v>
       </c>
       <c r="G291">
         <v>-0.05990299769007379</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.434290084454982</v>
+        <v>-3.434300611327811</v>
       </c>
       <c r="G293">
         <v>-0.05040229084891523</v>
@@ -7154,7 +7154,7 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.504411677685154</v>
+        <v>-3.504718570703486</v>
       </c>
       <c r="G294">
         <v>-0.03861174703917247</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.569542136939481</v>
+        <v>-3.569797998343901</v>
       </c>
       <c r="G295">
         <v>-0.02183006925358355</v>
@@ -7246,7 +7246,7 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.928826953921778</v>
+        <v>-2.929232203878962</v>
       </c>
       <c r="G298">
         <v>-0.02385052765782003</v>
@@ -7269,7 +7269,7 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.028342930380532</v>
+        <v>-3.02910818475723</v>
       </c>
       <c r="G299">
         <v>-0.04112516752593587</v>
@@ -7315,7 +7315,7 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.211175649134936</v>
+        <v>-3.211572943585542</v>
       </c>
       <c r="G301">
         <v>-0.0593133207041987</v>
@@ -7361,7 +7361,7 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.373807306458421</v>
+        <v>-3.374121614949914</v>
       </c>
       <c r="G303">
         <v>-0.0574623048464058</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.448879198339359</v>
+        <v>-3.449271828226094</v>
       </c>
       <c r="G304">
         <v>-0.05013096774184156</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.519432275689927</v>
+        <v>-3.519497223934051</v>
       </c>
       <c r="G305">
         <v>-0.03844270850177123</v>
@@ -7430,7 +7430,7 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.585033637052112</v>
+        <v>-3.58512853509191</v>
       </c>
       <c r="G306">
         <v>-0.02180273327331667</v>
@@ -7499,7 +7499,7 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.939073013976924</v>
+        <v>-2.939136172932044</v>
       </c>
       <c r="G309">
         <v>-0.02354941484064899</v>
@@ -7522,7 +7522,7 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.039578180127189</v>
+        <v>-3.039818930885545</v>
       </c>
       <c r="G310">
         <v>-0.04140220600042799</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.134056202250301</v>
+        <v>-3.134240025413718</v>
       </c>
       <c r="G311">
         <v>-0.05335442644850641</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.305782416135067</v>
+        <v>-3.306134144065003</v>
       </c>
       <c r="G313">
         <v>-0.0599024636677512</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.385773183774699</v>
+        <v>-3.38586528075065</v>
       </c>
       <c r="G314">
         <v>-0.05724085631689713</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.461253346192799</v>
+        <v>-3.461515714368445</v>
       </c>
       <c r="G315">
         <v>-0.05019521705996333</v>
@@ -7683,7 +7683,7 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.597905549539582</v>
+        <v>-3.597989908329401</v>
       </c>
       <c r="G317">
         <v>-0.02166924374122592</v>
@@ -7752,7 +7752,7 @@
         <v>821</v>
       </c>
       <c r="F320">
-        <v>-2.947931330222333</v>
+        <v>-2.947997040156169</v>
       </c>
       <c r="G320">
         <v>-0.02342755294048926</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.232414962326071</v>
+        <v>-3.232551248063721</v>
       </c>
       <c r="G323">
         <v>-0.05939024509142476</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.315598012982561</v>
+        <v>-3.315976955209198</v>
       </c>
       <c r="G324">
         <v>-0.05969937581233586</v>
@@ -7867,7 +7867,7 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.396107665954268</v>
+        <v>-3.396505072566357</v>
       </c>
       <c r="G325">
         <v>-0.0573351088484626</v>
@@ -7890,7 +7890,7 @@
         <v>5751</v>
       </c>
       <c r="F326">
-        <v>-3.471575137648325</v>
+        <v>-3.47172504092641</v>
       </c>
       <c r="G326">
         <v>-0.05002948046087663</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.542603563540434</v>
+        <v>-3.542637137548372</v>
       </c>
       <c r="G327">
         <v>-0.03818398641740572</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.608906806605201</v>
+        <v>-3.608970444137059</v>
       </c>
       <c r="G328">
         <v>-0.02161330954659391</v>
@@ -8097,7 +8097,7 @@
         <v>5089</v>
       </c>
       <c r="F335">
-        <v>-3.324413414814976</v>
+        <v>-3.324804893999144</v>
       </c>
       <c r="G335">
         <v>-0.05988781128979959</v>
@@ -8120,7 +8120,7 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.404646635731754</v>
+        <v>-3.404755423289157</v>
       </c>
       <c r="G336">
         <v>-0.05704993979205852</v>
@@ -8143,7 +8143,7 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.480763961510984</v>
+        <v>-3.480911486080865</v>
       </c>
       <c r="G337">
         <v>-0.05009617315676917</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.551903238519709</v>
+        <v>-3.55204219625536</v>
       </c>
       <c r="G338">
         <v>-0.03816435775097549</v>

</xml_diff>

<commit_message>
percent of new structs found now saved in log file
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -898,7 +898,7 @@
         <v>6</v>
       </c>
       <c r="F22">
-        <v>-2.4627908385039</v>
+        <v>-2.463904837203004</v>
       </c>
       <c r="G22">
         <v>-0.02885137346255817</v>
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.53895801383046</v>
+        <v>-2.540382347402585</v>
       </c>
       <c r="G27">
         <v>-0.0423954272284448</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.613829166823519</v>
+        <v>-2.614139480402818</v>
       </c>
       <c r="G32">
         <v>-0.05287188571216661</v>
@@ -1174,7 +1174,7 @@
         <v>18</v>
       </c>
       <c r="F34">
-        <v>-2.641199472048642</v>
+        <v>-2.643324220252976</v>
       </c>
       <c r="G34">
         <v>-0.05749005146331854</v>
@@ -1197,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.655807189944601</v>
+        <v>-2.657188743433353</v>
       </c>
       <c r="G35">
         <v>-0.05959571511011652</v>
@@ -1266,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="F38">
-        <v>-2.69653929818537</v>
+        <v>-2.697258812392174</v>
       </c>
       <c r="G38">
         <v>-0.06234969783748068</v>
@@ -1289,7 +1289,7 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.710683899603793</v>
+        <v>-2.711655230095728</v>
       </c>
       <c r="G39">
         <v>-0.06348037798503348</v>
@@ -1358,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.749415135778646</v>
+        <v>-2.750299688142324</v>
       </c>
       <c r="G42">
         <v>-0.0650923584693377</v>
@@ -1404,7 +1404,7 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <v>-2.774548624088178</v>
+        <v>-2.775300402212856</v>
       </c>
       <c r="G44">
         <v>-0.06581866101124545</v>
@@ -1427,7 +1427,7 @@
         <v>29</v>
       </c>
       <c r="F45">
-        <v>-2.785751985373821</v>
+        <v>-2.786881539942656</v>
       </c>
       <c r="G45">
         <v>-0.06384591050510124</v>
@@ -1473,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="F47">
-        <v>-2.811376040333823</v>
+        <v>-2.812206426156286</v>
       </c>
       <c r="G47">
         <v>-0.06343799993204424</v>
@@ -1565,7 +1565,7 @@
         <v>35</v>
       </c>
       <c r="F51">
-        <v>-2.856266485231876</v>
+        <v>-2.856435862089547</v>
       </c>
       <c r="G51">
         <v>-0.05931594135814644</v>
@@ -1588,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.867386159347139</v>
+        <v>-2.868787814752423</v>
       </c>
       <c r="G52">
         <v>-0.05674552347703155</v>
@@ -1634,7 +1634,7 @@
         <v>38</v>
       </c>
       <c r="F54">
-        <v>-2.890334064759451</v>
+        <v>-2.890424833919337</v>
       </c>
       <c r="G54">
         <v>-0.0550202292814288</v>
@@ -1657,7 +1657,7 @@
         <v>39</v>
       </c>
       <c r="F55">
-        <v>-2.900336666771084</v>
+        <v>-2.900370909388167</v>
       </c>
       <c r="G55">
         <v>-0.05298486353931542</v>
@@ -1703,7 +1703,7 @@
         <v>41</v>
       </c>
       <c r="F57">
-        <v>-2.921642634576131</v>
+        <v>-2.921764399235781</v>
       </c>
       <c r="G57">
         <v>-0.04957441447530531</v>
@@ -1749,7 +1749,7 @@
         <v>43</v>
       </c>
       <c r="F59">
-        <v>-2.942233486983726</v>
+        <v>-2.943188884583158</v>
       </c>
       <c r="G59">
         <v>-0.04509916738505093</v>
@@ -1795,7 +1795,7 @@
         <v>45</v>
       </c>
       <c r="F61">
-        <v>-2.961108249322427</v>
+        <v>-2.961950796606992</v>
       </c>
       <c r="G61">
         <v>-0.03896982122542986</v>
@@ -1841,7 +1841,7 @@
         <v>47</v>
       </c>
       <c r="F63">
-        <v>-2.979726315531626</v>
+        <v>-2.979870161346258</v>
       </c>
       <c r="G63">
         <v>-0.03345732172063559</v>
@@ -1864,7 +1864,7 @@
         <v>48</v>
       </c>
       <c r="F64">
-        <v>-2.988685997901261</v>
+        <v>-2.988829843715893</v>
       </c>
       <c r="G64">
         <v>-0.02991494984110976</v>
@@ -2140,7 +2140,7 @@
         <v>4</v>
       </c>
       <c r="F76">
-        <v>-2.556713373115562</v>
+        <v>-2.557134323827057</v>
       </c>
       <c r="G76">
         <v>-0.009360433829395998</v>
@@ -2163,7 +2163,7 @@
         <v>5</v>
       </c>
       <c r="F77">
-        <v>-2.563803711582159</v>
+        <v>-2.564076727455176</v>
       </c>
       <c r="G77">
         <v>-0.01153748281947742</v>
@@ -2232,7 +2232,7 @@
         <v>8</v>
       </c>
       <c r="F80">
-        <v>-2.58427825200122</v>
+        <v>-2.584551267874236</v>
       </c>
       <c r="G80">
         <v>-0.01700311782841757</v>
@@ -2301,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="F83">
-        <v>-2.604111928897288</v>
+        <v>-2.604331841708785</v>
       </c>
       <c r="G83">
         <v>-0.02152627317205269</v>
@@ -2324,7 +2324,7 @@
         <v>12</v>
       </c>
       <c r="F84">
-        <v>-2.610693049098502</v>
+        <v>-2.611300796867662</v>
       </c>
       <c r="G84">
         <v>-0.02337063900452652</v>
@@ -2508,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.662106198650099</v>
+        <v>-2.662789002538529</v>
       </c>
       <c r="G92">
         <v>-0.03468923671377633</v>
@@ -2531,7 +2531,7 @@
         <v>21</v>
       </c>
       <c r="F93">
-        <v>-2.667934753083544</v>
+        <v>-2.669005091855501</v>
       </c>
       <c r="G93">
         <v>-0.03543771879196145</v>
@@ -2623,7 +2623,7 @@
         <v>25</v>
       </c>
       <c r="F97">
-        <v>-2.69220356973723</v>
+        <v>-2.693188897878067</v>
       </c>
       <c r="G97">
         <v>-0.03972751289944121</v>
@@ -2715,7 +2715,7 @@
         <v>29</v>
       </c>
       <c r="F101">
-        <v>-2.717532696594788</v>
+        <v>-2.717548943531261</v>
       </c>
       <c r="G101">
         <v>-0.04500936383582488</v>
@@ -2784,7 +2784,7 @@
         <v>32</v>
       </c>
       <c r="F104">
-        <v>-2.735100812081686</v>
+        <v>-2.736701257101549</v>
       </c>
       <c r="G104">
         <v>-0.04637412235685168</v>
@@ -2830,7 +2830,7 @@
         <v>34</v>
       </c>
       <c r="F106">
-        <v>-2.746910308154112</v>
+        <v>-2.747110504249598</v>
       </c>
       <c r="G106">
         <v>-0.04833907314732233</v>
@@ -2876,7 +2876,7 @@
         <v>36</v>
       </c>
       <c r="F108">
-        <v>-2.759262525365628</v>
+        <v>-2.759519326444865</v>
       </c>
       <c r="G108">
         <v>-0.04871400073098031</v>
@@ -2922,7 +2922,7 @@
         <v>38</v>
       </c>
       <c r="F110">
-        <v>-2.76991277035548</v>
+        <v>-2.771649862580533</v>
       </c>
       <c r="G110">
         <v>-0.05167060709118543</v>
@@ -2968,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.781677343524233</v>
+        <v>-2.781948030029919</v>
       </c>
       <c r="G112">
         <v>-0.05241584299312052</v>
@@ -2991,7 +2991,7 @@
         <v>41</v>
       </c>
       <c r="F113">
-        <v>-2.787430658876814</v>
+        <v>-2.787805151659301</v>
       </c>
       <c r="G113">
         <v>-0.05452654928112111</v>
@@ -3083,7 +3083,7 @@
         <v>45</v>
       </c>
       <c r="F117">
-        <v>-2.810352855206683</v>
+        <v>-2.810860559334021</v>
       </c>
       <c r="G117">
         <v>-0.05655285368063656</v>
@@ -3175,7 +3175,7 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.832513052163756</v>
+        <v>-2.833379174433034</v>
       </c>
       <c r="G121">
         <v>-0.05882096451375207</v>
@@ -3198,7 +3198,7 @@
         <v>50</v>
       </c>
       <c r="F122">
-        <v>-2.838690763344899</v>
+        <v>-2.839545365365931</v>
       </c>
       <c r="G122">
         <v>-0.05982220534360372</v>
@@ -3244,7 +3244,7 @@
         <v>52</v>
       </c>
       <c r="F124">
-        <v>-2.850170930628872</v>
+        <v>-2.850408432227866</v>
       </c>
       <c r="G124">
         <v>-0.05974720060850958</v>
@@ -3267,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.854583052712755</v>
+        <v>-2.856011638706397</v>
       </c>
       <c r="G125">
         <v>-0.06043663423083312</v>
@@ -3290,7 +3290,7 @@
         <v>54</v>
       </c>
       <c r="F126">
-        <v>-2.859374356073122</v>
+        <v>-2.860488375992292</v>
       </c>
       <c r="G126">
         <v>-0.06049816163235744</v>
@@ -3336,7 +3336,7 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.871376122770107</v>
+        <v>-2.871999603441503</v>
       </c>
       <c r="G128">
         <v>-0.05999829908844112</v>
@@ -3359,7 +3359,7 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.875876582211734</v>
+        <v>-2.875894050472358</v>
       </c>
       <c r="G129">
         <v>-0.06162123943036568</v>
@@ -3382,7 +3382,7 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.882435439562722</v>
+        <v>-2.883556126790109</v>
       </c>
       <c r="G130">
         <v>-0.06235603945775781</v>
@@ -3428,7 +3428,7 @@
         <v>60</v>
       </c>
       <c r="F132">
-        <v>-2.893465846059668</v>
+        <v>-2.894064959300075</v>
       </c>
       <c r="G132">
         <v>-0.06373014700597257</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.903598049718333</v>
+        <v>-2.904413795603185</v>
       </c>
       <c r="G134">
         <v>-0.06442018072698819</v>
@@ -3566,7 +3566,7 @@
         <v>66</v>
       </c>
       <c r="F138">
-        <v>-2.923117999470372</v>
+        <v>-2.923909127918091</v>
       </c>
       <c r="G138">
         <v>-0.06515736444055586</v>
@@ -3589,7 +3589,7 @@
         <v>67</v>
       </c>
       <c r="F139">
-        <v>-2.929616807956883</v>
+        <v>-2.930059097336152</v>
       </c>
       <c r="G139">
         <v>-0.06664435394677382</v>
@@ -3612,7 +3612,7 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.934441609892988</v>
+        <v>-2.934977873033891</v>
       </c>
       <c r="G140">
         <v>-0.06556463984838112</v>
@@ -3635,7 +3635,7 @@
         <v>69</v>
       </c>
       <c r="F141">
-        <v>-2.939035433085397</v>
+        <v>-2.939697872182133</v>
       </c>
       <c r="G141">
         <v>-0.06584330908052571</v>
@@ -3658,7 +3658,7 @@
         <v>70</v>
       </c>
       <c r="F142">
-        <v>-2.944116527247888</v>
+        <v>-2.945372154202433</v>
       </c>
       <c r="G142">
         <v>-0.06469009095332323</v>
@@ -3681,7 +3681,7 @@
         <v>71</v>
       </c>
       <c r="F143">
-        <v>-2.949894790418023</v>
+        <v>-2.951136943588652</v>
       </c>
       <c r="G143">
         <v>-0.06612790255270729</v>
@@ -3727,7 +3727,7 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.959620722459045</v>
+        <v>-2.961054334598898</v>
       </c>
       <c r="G145">
         <v>-0.06657735456717484</v>
@@ -3773,7 +3773,7 @@
         <v>75</v>
       </c>
       <c r="F147">
-        <v>-2.969364114603599</v>
+        <v>-2.971534776698191</v>
       </c>
       <c r="G147">
         <v>-0.06629710875114192</v>
@@ -3865,7 +3865,7 @@
         <v>79</v>
       </c>
       <c r="F151">
-        <v>-2.990108125292879</v>
+        <v>-2.990202064445956</v>
       </c>
       <c r="G151">
         <v>-0.06699384351924897</v>
@@ -3888,7 +3888,7 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.994525855714862</v>
+        <v>-2.995295187321518</v>
       </c>
       <c r="G152">
         <v>-0.06458872555120188</v>
@@ -4049,7 +4049,7 @@
         <v>87</v>
       </c>
       <c r="F159">
-        <v>-3.027769272482463</v>
+        <v>-3.02911740148376</v>
       </c>
       <c r="G159">
         <v>-0.06403073811491899</v>
@@ -4072,7 +4072,7 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.032698724719683</v>
+        <v>-3.033385928604418</v>
       </c>
       <c r="G160">
         <v>-0.06198414582054457</v>
@@ -4118,7 +4118,7 @@
         <v>90</v>
       </c>
       <c r="F162">
-        <v>-3.042442065689875</v>
+        <v>-3.042571263506562</v>
       </c>
       <c r="G162">
         <v>-0.06419777513301805</v>
@@ -4210,7 +4210,7 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.060136029088066</v>
+        <v>-3.061107026443836</v>
       </c>
       <c r="G166">
         <v>-0.06058776189785309</v>
@@ -4256,7 +4256,7 @@
         <v>96</v>
       </c>
       <c r="F168">
-        <v>-3.069853123541955</v>
+        <v>-3.070260695053905</v>
       </c>
       <c r="G168">
         <v>-0.05960336843482184</v>
@@ -4302,7 +4302,7 @@
         <v>98</v>
       </c>
       <c r="F170">
-        <v>-3.079332351276757</v>
+        <v>-3.079427557755675</v>
       </c>
       <c r="G170">
         <v>-0.05730450266901987</v>
@@ -4394,7 +4394,7 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.096716494882646</v>
+        <v>-3.097555938576017</v>
       </c>
       <c r="G174">
         <v>-0.0560119414824285</v>
@@ -4417,7 +4417,7 @@
         <v>103</v>
       </c>
       <c r="F175">
-        <v>-3.100456974546988</v>
+        <v>-3.101988758274533</v>
       </c>
       <c r="G175">
         <v>-0.05642056255975092</v>
@@ -4440,7 +4440,7 @@
         <v>104</v>
       </c>
       <c r="F176">
-        <v>-3.105758701614341</v>
+        <v>-3.105976057964619</v>
       </c>
       <c r="G176">
         <v>-0.05617350751213446</v>
@@ -4463,7 +4463,7 @@
         <v>105</v>
       </c>
       <c r="F177">
-        <v>-3.109829449511393</v>
+        <v>-3.110294937476311</v>
       </c>
       <c r="G177">
         <v>-0.05446133096250516</v>
@@ -4624,7 +4624,7 @@
         <v>112</v>
       </c>
       <c r="F184">
-        <v>-3.137545223679478</v>
+        <v>-3.138849008417895</v>
       </c>
       <c r="G184">
         <v>-0.04904091555616807</v>
@@ -4670,7 +4670,7 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.147407045610624</v>
+        <v>-3.147765094018068</v>
       </c>
       <c r="G186">
         <v>-0.0483892698089563</v>
@@ -4716,7 +4716,7 @@
         <v>116</v>
       </c>
       <c r="F188">
-        <v>-3.154623250111502</v>
+        <v>-3.156794968015595</v>
       </c>
       <c r="G188">
         <v>-0.04477119390811302</v>
@@ -4739,7 +4739,7 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.158639559257619</v>
+        <v>-3.15946046327876</v>
       </c>
       <c r="G189">
         <v>-0.04438895429458223</v>
@@ -4808,7 +4808,7 @@
         <v>120</v>
       </c>
       <c r="F192">
-        <v>-3.170925723724702</v>
+        <v>-3.171162479734372</v>
       </c>
       <c r="G192">
         <v>-0.04134060640137954</v>
@@ -4831,7 +4831,7 @@
         <v>121</v>
       </c>
       <c r="F193">
-        <v>-3.175385397417834</v>
+        <v>-3.175882201545098</v>
       </c>
       <c r="G193">
         <v>-0.03971331536512507</v>
@@ -4900,7 +4900,7 @@
         <v>124</v>
       </c>
       <c r="F196">
-        <v>-3.187991298525615</v>
+        <v>-3.188068828917364</v>
       </c>
       <c r="G196">
         <v>-0.03934516263878435</v>
@@ -5038,7 +5038,7 @@
         <v>130</v>
       </c>
       <c r="F202">
-        <v>-3.210279052586828</v>
+        <v>-3.210756083297581</v>
       </c>
       <c r="G202">
         <v>-0.03009688453344472</v>
@@ -5084,7 +5084,7 @@
         <v>132</v>
       </c>
       <c r="F204">
-        <v>-3.217115825779265</v>
+        <v>-3.217614299192846</v>
       </c>
       <c r="G204">
         <v>-0.02607188065758331</v>
@@ -5107,7 +5107,7 @@
         <v>133</v>
       </c>
       <c r="F205">
-        <v>-3.220190075502073</v>
+        <v>-3.220276872121658</v>
       </c>
       <c r="G205">
         <v>-0.02519369114682696</v>
@@ -5176,7 +5176,7 @@
         <v>136</v>
       </c>
       <c r="F208">
-        <v>-3.23071157380949</v>
+        <v>-3.230903865039085</v>
       </c>
       <c r="G208">
         <v>-0.02119282405852102</v>
@@ -5199,7 +5199,7 @@
         <v>137</v>
       </c>
       <c r="F209">
-        <v>-3.23379488012825</v>
+        <v>-3.234302410137784</v>
       </c>
       <c r="G209">
         <v>-0.01974087654502524</v>
@@ -5521,7 +5521,7 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.906657628442232</v>
+        <v>-2.90684110929937</v>
       </c>
       <c r="G223">
         <v>-0.05667863585152433</v>
@@ -5613,7 +5613,7 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.211629008317785</v>
+        <v>-3.212303752390315</v>
       </c>
       <c r="G227">
         <v>-0.05535611381859917</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.275748615166611</v>
+        <v>-3.275901294844515</v>
       </c>
       <c r="G228">
         <v>-0.04235567179172572</v>
@@ -5751,7 +5751,7 @@
         <v>112</v>
       </c>
       <c r="F233">
-        <v>-2.883379759432807</v>
+        <v>-2.883672456550075</v>
       </c>
       <c r="G233">
         <v>-0.04396603691345913</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.972687485694784</v>
+        <v>-2.972777551450976</v>
       </c>
       <c r="G234">
         <v>-0.05640312486146803</v>
@@ -5797,7 +5797,7 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.05591625522073</v>
+        <v>-3.056110884215312</v>
       </c>
       <c r="G235">
         <v>-0.06130828897128859</v>
@@ -5912,7 +5912,7 @@
         <v>504</v>
       </c>
       <c r="F240">
-        <v>-3.409099268613306</v>
+        <v>-3.409462033509221</v>
       </c>
       <c r="G240">
         <v>-0.02453718513425368</v>
@@ -6004,7 +6004,7 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.926043781772897</v>
+        <v>-2.926082642094345</v>
       </c>
       <c r="G244">
         <v>-0.04384498982082752</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.102335121024724</v>
+        <v>-3.102819258940653</v>
       </c>
       <c r="G246">
         <v>-0.06037854978363622</v>
@@ -6073,7 +6073,7 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.182367434013215</v>
+        <v>-3.182508651189247</v>
       </c>
       <c r="G247">
         <v>-0.06223360379459431</v>
@@ -6280,7 +6280,7 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.050125677164596</v>
+        <v>-3.050313708814578</v>
       </c>
       <c r="G256">
         <v>-0.05548838217275165</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.136058546667661</v>
+        <v>-3.136084028574278</v>
       </c>
       <c r="G257">
         <v>-0.06024136341956599</v>
@@ -6326,7 +6326,7 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.216996919513611</v>
+        <v>-3.217061700669015</v>
       </c>
       <c r="G258">
         <v>-0.06163801963448479</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.367767743048307</v>
+        <v>-3.367829167640465</v>
       </c>
       <c r="G260">
         <v>-0.05112925886468378</v>
@@ -6418,7 +6418,7 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.499322169800306</v>
+        <v>-3.499487504523403</v>
       </c>
       <c r="G262">
         <v>-0.02294620606559572</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.882635743137529</v>
+        <v>-2.88277732051883</v>
       </c>
       <c r="G265">
         <v>-0.02438565895318945</v>
@@ -6510,7 +6510,7 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.981936053892435</v>
+        <v>-2.982121530089364</v>
       </c>
       <c r="G266">
         <v>-0.04258180329186079</v>
@@ -6556,7 +6556,7 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.16134681880191</v>
+        <v>-3.161598411330683</v>
       </c>
       <c r="G268">
         <v>-0.05976825743771474</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.321485500414305</v>
+        <v>-3.321642388029861</v>
       </c>
       <c r="G270">
         <v>-0.05843500147492464</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.464164638740598</v>
+        <v>-3.464209229948666</v>
       </c>
       <c r="G272">
         <v>-0.0390600039257023</v>
@@ -6671,7 +6671,7 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.528366437609532</v>
+        <v>-3.528467235584596</v>
       </c>
       <c r="G273">
         <v>-0.02215783843354158</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.094629145141583</v>
+        <v>-3.094833691468409</v>
       </c>
       <c r="G278">
         <v>-0.05464948411930903</v>
@@ -6878,7 +6878,7 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.4169923626565</v>
+        <v>-3.417413941893833</v>
       </c>
       <c r="G282">
         <v>-0.05089489200008046</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.486506876446435</v>
+        <v>-3.486686237316042</v>
       </c>
       <c r="G283">
         <v>-0.03853052012238201</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.551496875574995</v>
+        <v>-3.551564040973521</v>
       </c>
       <c r="G284">
         <v>-0.02225548276206646</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.35976200214916</v>
+        <v>-3.359822163206362</v>
       </c>
       <c r="G292">
         <v>-0.05778634558300988</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.434487631317682</v>
+        <v>-3.434533603304953</v>
       </c>
       <c r="G293">
         <v>-0.05040229084891523</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.569797998343901</v>
+        <v>-3.569824402480835</v>
       </c>
       <c r="G295">
         <v>-0.02183006925358355</v>
@@ -7292,7 +7292,7 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.122968483482378</v>
+        <v>-3.123229776992641</v>
       </c>
       <c r="G300">
         <v>-0.05326578981867036</v>
@@ -7338,7 +7338,7 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.294342261947778</v>
+        <v>-3.294469968025844</v>
       </c>
       <c r="G302">
         <v>-0.06023859692640099</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.449271828226094</v>
+        <v>-3.4494885664904</v>
       </c>
       <c r="G304">
         <v>-0.05013096774184156</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.519497223934051</v>
+        <v>-3.519557576645006</v>
       </c>
       <c r="G305">
         <v>-0.03844270850177123</v>
@@ -7430,7 +7430,7 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.58512853509191</v>
+        <v>-3.585195908341226</v>
       </c>
       <c r="G306">
         <v>-0.02180273327331667</v>
@@ -7683,7 +7683,7 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.597989908329401</v>
+        <v>-3.598024360885891</v>
       </c>
       <c r="G317">
         <v>-0.02166924374122592</v>
@@ -7775,7 +7775,7 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.048431521149749</v>
+        <v>-3.048629946401157</v>
       </c>
       <c r="G321">
         <v>-0.04105382393232659</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.315976955209198</v>
+        <v>-3.316060725688103</v>
       </c>
       <c r="G324">
         <v>-0.05969937581233586</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.542637137548372</v>
+        <v>-3.542779945524092</v>
       </c>
       <c r="G327">
         <v>-0.03818398641740572</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.609021567958673</v>
+        <v>-3.609115289175988</v>
       </c>
       <c r="G328">
         <v>-0.02161330954659391</v>
@@ -8051,7 +8051,7 @@
         <v>3053</v>
       </c>
       <c r="F333">
-        <v>-3.151394079108226</v>
+        <v>-3.151668405989521</v>
       </c>
       <c r="G333">
         <v>-0.05301066041208702</v>
@@ -8074,7 +8074,7 @@
         <v>4071</v>
       </c>
       <c r="F334">
-        <v>-3.240815787879667</v>
+        <v>-3.240857744400971</v>
       </c>
       <c r="G334">
         <v>-0.05933993847991159</v>
@@ -8189,7 +8189,7 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.618470140010812</v>
+        <v>-3.6184838224893</v>
       </c>
       <c r="G339">
         <v>-0.0216601668275595</v>

</xml_diff>

<commit_message>
successfully ran GA with new C dll
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>n_atoms</t>
+    <t>num_atoms</t>
   </si>
   <si>
     <t>diameter</t>
@@ -438,10 +438,10 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>-1.98466167250952</v>
+        <v>-1.984661672509521</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>-1.77635683940025e-15</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>-2.042228299641554</v>
+        <v>-2.042228299641555</v>
       </c>
       <c r="G3">
-        <v>-0.01306052443690486</v>
+        <v>-0.01306052443690664</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -484,10 +484,10 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>-2.099794926773587</v>
+        <v>-2.099794926773589</v>
       </c>
       <c r="G4">
-        <v>-0.02612104887380973</v>
+        <v>-0.02612104887381195</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -507,10 +507,10 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>-2.15736155390562</v>
+        <v>-2.157361553905622</v>
       </c>
       <c r="G5">
-        <v>-0.03918157331071437</v>
+        <v>-0.03918157331071614</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -530,10 +530,10 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>-2.214928181037653</v>
+        <v>-2.214928181037654</v>
       </c>
       <c r="G6">
-        <v>-0.05224209774761834</v>
+        <v>-0.05224209774761879</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -553,10 +553,10 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>-2.262929532377207</v>
+        <v>-2.262929532377208</v>
       </c>
       <c r="G7">
-        <v>-0.05573734639204364</v>
+        <v>-0.05573734639204408</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -576,10 +576,10 @@
         <v>6</v>
       </c>
       <c r="F8">
-        <v>-2.310930883716761</v>
+        <v>-2.310930883716762</v>
       </c>
       <c r="G8">
-        <v>-0.05923259503646916</v>
+        <v>-0.0592325950364696</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -602,7 +602,7 @@
         <v>-2.358932235056315</v>
       </c>
       <c r="G9">
-        <v>-0.06272784368089379</v>
+        <v>-0.06272784368089335</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -622,10 +622,10 @@
         <v>8</v>
       </c>
       <c r="F10">
-        <v>-2.406933586395869</v>
+        <v>-2.406933586395867</v>
       </c>
       <c r="G10">
-        <v>-0.06622309232531876</v>
+        <v>-0.06622309232531742</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -645,10 +645,10 @@
         <v>9</v>
       </c>
       <c r="F11">
-        <v>-2.445369661942943</v>
+        <v>-2.445369661942942</v>
       </c>
       <c r="G11">
-        <v>-0.06015306517726438</v>
+        <v>-0.06015306517726304</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -668,10 +668,10 @@
         <v>10</v>
       </c>
       <c r="F12">
-        <v>-2.483805737490017</v>
+        <v>-2.483805737490016</v>
       </c>
       <c r="G12">
-        <v>-0.05408303802920922</v>
+        <v>-0.05408303802920789</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -691,10 +691,10 @@
         <v>11</v>
       </c>
       <c r="F13">
-        <v>-2.522241813037091</v>
+        <v>-2.522241813037089</v>
       </c>
       <c r="G13">
-        <v>-0.04801301088115484</v>
+        <v>-0.04801301088115306</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -714,10 +714,10 @@
         <v>12</v>
       </c>
       <c r="F14">
-        <v>-2.560677888584165</v>
+        <v>-2.560677888584162</v>
       </c>
       <c r="G14">
-        <v>-0.0419429837331004</v>
+        <v>-0.04194298373309729</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -737,10 +737,10 @@
         <v>13</v>
       </c>
       <c r="F15">
-        <v>-2.563241007546194</v>
+        <v>-2.563241007546191</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>3.108624468950438e-15</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -760,10 +760,10 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>-2.358672444100427</v>
+        <v>-2.358672444100425</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1.332267629550188e-15</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -783,10 +783,10 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>-2.378686989554972</v>
+        <v>-2.378686989554971</v>
       </c>
       <c r="G17">
-        <v>-0.007512491205384553</v>
+        <v>-0.007512491205383665</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -806,10 +806,10 @@
         <v>2</v>
       </c>
       <c r="F18">
-        <v>-2.395730559084578</v>
+        <v>-2.395730559084579</v>
       </c>
       <c r="G18">
-        <v>-0.01205400648582966</v>
+        <v>-0.0120540064858301</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -829,10 +829,10 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <v>-2.412774128614184</v>
+        <v>-2.412774128614186</v>
       </c>
       <c r="G19">
-        <v>-0.01659552176627521</v>
+        <v>-0.01659552176627699</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -852,10 +852,10 @@
         <v>4</v>
       </c>
       <c r="F20">
-        <v>-2.429817698143791</v>
+        <v>-2.429817698143792</v>
       </c>
       <c r="G20">
-        <v>-0.02113703704672121</v>
+        <v>-0.02113703704672254</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -875,10 +875,10 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <v>-2.446861267673397</v>
+        <v>-2.4468612676734</v>
       </c>
       <c r="G21">
-        <v>-0.02512155297761431</v>
+        <v>-0.02567855232716854</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -898,10 +898,10 @@
         <v>6</v>
       </c>
       <c r="F22">
-        <v>-2.463904837203004</v>
+        <v>-2.463904837203005</v>
       </c>
       <c r="G22">
-        <v>-0.02885137346255817</v>
+        <v>-0.03022006760761364</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -921,10 +921,10 @@
         <v>7</v>
       </c>
       <c r="F23">
-        <v>-2.479022713238004</v>
+        <v>-2.479579712587558</v>
       </c>
       <c r="G23">
-        <v>-0.03202419459794914</v>
+        <v>-0.03339288874300506</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -944,10 +944,10 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>-2.495145669119555</v>
+        <v>-2.493858972800308</v>
       </c>
       <c r="G24">
-        <v>-0.03519701573334055</v>
+        <v>-0.03517009470659405</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -967,10 +967,10 @@
         <v>9</v>
       </c>
       <c r="F25">
-        <v>-2.510619128483641</v>
+        <v>-2.510619128483644</v>
       </c>
       <c r="G25">
-        <v>-0.03942819614076609</v>
+        <v>-0.0394281961407692</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -990,10 +990,10 @@
         <v>10</v>
       </c>
       <c r="F26">
-        <v>-2.525482309072692</v>
+        <v>-2.524150472668484</v>
       </c>
       <c r="G26">
-        <v>-0.04156755331323514</v>
+        <v>-0.04045748607644772</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1013,10 +1013,10 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.540382347402585</v>
+        <v>-2.539769708625962</v>
       </c>
       <c r="G27">
-        <v>-0.0423954272284448</v>
+        <v>-0.0435746677847646</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1036,10 +1036,10 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <v>-2.554661607615335</v>
+        <v>-2.554857629083865</v>
       </c>
       <c r="G28">
-        <v>-0.04476098735938883</v>
+        <v>-0.04616053399350739</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1059,10 +1059,10 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <v>-2.569627523964137</v>
+        <v>-2.569904932558636</v>
       </c>
       <c r="G29">
-        <v>-0.04667953612532028</v>
+        <v>-0.04870578321911712</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1082,10 +1082,10 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <v>-2.585565746260133</v>
+        <v>-2.584899828058029</v>
       </c>
       <c r="G30">
-        <v>-0.04987568110909657</v>
+        <v>-0.0511986244693492</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1105,10 +1105,10 @@
         <v>15</v>
       </c>
       <c r="F31">
-        <v>-2.600317647995041</v>
+        <v>-2.598833969446377</v>
       </c>
       <c r="G31">
-        <v>-0.05214195027948443</v>
+        <v>-0.0526307116085365</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1128,10 +1128,10 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.614139480402818</v>
+        <v>-2.613138687596258</v>
       </c>
       <c r="G32">
-        <v>-0.05287188571216661</v>
+        <v>-0.05443337550925675</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1151,10 +1151,10 @@
         <v>17</v>
       </c>
       <c r="F33">
-        <v>-2.628257174331095</v>
+        <v>-2.627856346714079</v>
       </c>
       <c r="G33">
-        <v>-0.05704980799493198</v>
+        <v>-0.05664898037791666</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1174,10 +1174,10 @@
         <v>18</v>
       </c>
       <c r="F34">
-        <v>-2.643324220252976</v>
+        <v>-2.64176358061228</v>
       </c>
       <c r="G34">
-        <v>-0.05749005146331854</v>
+        <v>-0.0580541600269564</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1197,10 +1197,10 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.657188743433353</v>
+        <v>-2.653950584619783</v>
       </c>
       <c r="G35">
-        <v>-0.05959571511011652</v>
+        <v>-0.05773910978529906</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1220,10 +1220,10 @@
         <v>20</v>
       </c>
       <c r="F36">
-        <v>-2.670054148115264</v>
+        <v>-2.669002863219898</v>
       </c>
       <c r="G36">
-        <v>-0.0602723711173172</v>
+        <v>-0.06028933413625248</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1243,10 +1243,10 @@
         <v>21</v>
       </c>
       <c r="F37">
-        <v>-2.685274916457318</v>
+        <v>-2.683249197154117</v>
       </c>
       <c r="G37">
-        <v>-0.06032643809720217</v>
+        <v>-0.06203361382131134</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1266,10 +1266,10 @@
         <v>22</v>
       </c>
       <c r="F38">
-        <v>-2.697351542072284</v>
+        <v>-2.694493225735216</v>
       </c>
       <c r="G38">
-        <v>-0.06234969783748068</v>
+        <v>-0.06077558815324902</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1289,10 +1289,10 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.711655230095728</v>
+        <v>-2.71015530207535</v>
       </c>
       <c r="G39">
-        <v>-0.06348037798503348</v>
+        <v>-0.06393561024422234</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1312,10 +1312,10 @@
         <v>24</v>
       </c>
       <c r="F40">
-        <v>-2.724005709872746</v>
+        <v>-2.722128270175237</v>
       </c>
       <c r="G40">
-        <v>-0.06528396379245738</v>
+        <v>-0.06340652409494751</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1335,10 +1335,10 @@
         <v>25</v>
       </c>
       <c r="F41">
-        <v>-2.737050818343691</v>
+        <v>-2.737295759091805</v>
       </c>
       <c r="G41">
-        <v>-0.06212052023984116</v>
+        <v>-0.06607195876235483</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1358,10 +1358,10 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.750299688142324</v>
+        <v>-2.747363109888908</v>
       </c>
       <c r="G42">
-        <v>-0.0650923584693377</v>
+        <v>-0.06363725531029729</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1381,10 +1381,10 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.76294278232252</v>
+        <v>-2.758883633066294</v>
       </c>
       <c r="G43">
-        <v>-0.06433668457459296</v>
+        <v>-0.06265572423852195</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1404,10 +1404,10 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <v>-2.775391171372742</v>
+        <v>-2.774019239367364</v>
       </c>
       <c r="G44">
-        <v>-0.06581866101124545</v>
+        <v>-0.06528927629043091</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1427,10 +1427,10 @@
         <v>29</v>
       </c>
       <c r="F45">
-        <v>-2.786881539942656</v>
+        <v>-2.784287451853277</v>
       </c>
       <c r="G45">
-        <v>-0.06384591050510124</v>
+        <v>-0.06305543452718299</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1450,10 +1450,10 @@
         <v>30</v>
       </c>
       <c r="F46">
-        <v>-2.799854473493411</v>
+        <v>-2.797872776822711</v>
       </c>
       <c r="G46">
-        <v>-0.06612040191815649</v>
+        <v>-0.06413870524745602</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1473,10 +1473,10 @@
         <v>31</v>
       </c>
       <c r="F47">
-        <v>-2.812206426156286</v>
+        <v>-2.810294422838588</v>
       </c>
       <c r="G47">
-        <v>-0.06343799993204424</v>
+        <v>-0.06405829701417254</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1496,10 +1496,10 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.824041215669002</v>
+        <v>-2.821803828216897</v>
       </c>
       <c r="G48">
-        <v>-0.06043401002026194</v>
+        <v>-0.06306564814332039</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1519,10 +1519,10 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.834657214447406</v>
+        <v>-2.8355716968542</v>
       </c>
       <c r="G49">
-        <v>-0.06085167019565196</v>
+        <v>-0.06433146253146271</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1542,10 +1542,10 @@
         <v>34</v>
       </c>
       <c r="F50">
-        <v>-2.846430012960594</v>
+        <v>-2.844859183468374</v>
       </c>
       <c r="G50">
-        <v>-0.059087379384544</v>
+        <v>-0.06111689489647565</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1565,10 +1565,10 @@
         <v>35</v>
       </c>
       <c r="F51">
-        <v>-2.856435862089547</v>
+        <v>-2.857482028848871</v>
       </c>
       <c r="G51">
-        <v>-0.05931594135814644</v>
+        <v>-0.06123768602781177</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1588,10 +1588,10 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.869031344071724</v>
+        <v>-2.865582547235674</v>
       </c>
       <c r="G52">
-        <v>-0.05674552347703155</v>
+        <v>-0.05683615016545374</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1611,10 +1611,10 @@
         <v>37</v>
       </c>
       <c r="F53">
-        <v>-2.879576437505818</v>
+        <v>-2.87884674053612</v>
       </c>
       <c r="G53">
-        <v>-0.05817522602702407</v>
+        <v>-0.0575982892167386</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1634,10 +1634,10 @@
         <v>38</v>
       </c>
       <c r="F54">
-        <v>-2.890424833919337</v>
+        <v>-2.889316676160492</v>
       </c>
       <c r="G54">
-        <v>-0.0550202292814288</v>
+        <v>-0.05556617059195057</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1657,10 +1657,10 @@
         <v>39</v>
       </c>
       <c r="F55">
-        <v>-2.90042743593097</v>
+        <v>-2.898804332361363</v>
       </c>
       <c r="G55">
-        <v>-0.05298486353931542</v>
+        <v>-0.05255177254366028</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1680,10 +1680,10 @@
         <v>40</v>
       </c>
       <c r="F56">
-        <v>-2.911006771982149</v>
+        <v>-2.910902836012063</v>
       </c>
       <c r="G56">
-        <v>-0.05121815261806784</v>
+        <v>-0.0521482219451993</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1703,10 +1703,10 @@
         <v>41</v>
       </c>
       <c r="F57">
-        <v>-2.921764399235781</v>
+        <v>-2.920921851951215</v>
       </c>
       <c r="G57">
-        <v>-0.04957441447530531</v>
+        <v>-0.04966518363519057</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1726,10 +1726,10 @@
         <v>42</v>
       </c>
       <c r="F58">
-        <v>-2.933242809114328</v>
+        <v>-2.931077214122262</v>
       </c>
       <c r="G58">
-        <v>-0.04519294519926986</v>
+        <v>-0.04731849155707635</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1749,10 +1749,10 @@
         <v>43</v>
       </c>
       <c r="F59">
-        <v>-2.943188884583158</v>
+        <v>-2.939732790935115</v>
       </c>
       <c r="G59">
-        <v>-0.04509916738505093</v>
+        <v>-0.04347201412076784</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1772,10 +1772,10 @@
         <v>44</v>
       </c>
       <c r="F60">
-        <v>-2.952004721138161</v>
+        <v>-2.951314934013007</v>
       </c>
       <c r="G60">
-        <v>-0.04190992802237153</v>
+        <v>-0.04255210294949902</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1795,10 +1795,10 @@
         <v>45</v>
       </c>
       <c r="F61">
-        <v>-2.961950796606992</v>
+        <v>-2.959472181713357</v>
       </c>
       <c r="G61">
-        <v>-0.03896982122542986</v>
+        <v>-0.03820729640068848</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1818,10 +1818,10 @@
         <v>46</v>
       </c>
       <c r="F62">
-        <v>-2.970910478976625</v>
+        <v>-2.970036936192295</v>
       </c>
       <c r="G62">
-        <v>-0.03532351337581685</v>
+        <v>-0.03626999663046548</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1841,10 +1841,10 @@
         <v>47</v>
       </c>
       <c r="F63">
-        <v>-2.979870161346258</v>
+        <v>-2.979726315531624</v>
       </c>
       <c r="G63">
-        <v>-0.03345732172063559</v>
+        <v>-0.03345732172063337</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1864,10 +1864,10 @@
         <v>48</v>
       </c>
       <c r="F64">
-        <v>-2.988829843715893</v>
+        <v>-2.988829843715886</v>
       </c>
       <c r="G64">
-        <v>-0.02991494984110976</v>
+        <v>-0.03005879565573477</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1887,10 +1887,10 @@
         <v>49</v>
       </c>
       <c r="F65">
-        <v>-2.997789526085527</v>
+        <v>-2.99778952608552</v>
       </c>
       <c r="G65">
-        <v>-0.02651642377621433</v>
+        <v>-0.02651642377620722</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1910,10 +1910,10 @@
         <v>50</v>
       </c>
       <c r="F66">
-        <v>-3.00674920845516</v>
+        <v>-3.006749208455155</v>
       </c>
       <c r="G66">
-        <v>-0.02297405189668672</v>
+        <v>-0.02297405189668139</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1933,10 +1933,10 @@
         <v>51</v>
       </c>
       <c r="F67">
-        <v>-3.015708890824793</v>
+        <v>-3.015708890824789</v>
       </c>
       <c r="G67">
-        <v>-0.01870198304746321</v>
+        <v>-0.0194316800171547</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -1956,10 +1956,10 @@
         <v>52</v>
       </c>
       <c r="F68">
-        <v>-3.023353025069665</v>
+        <v>-3.02335302506966</v>
       </c>
       <c r="G68">
-        <v>-0.01457376001287003</v>
+        <v>-0.0145737600128647</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -1979,10 +1979,10 @@
         <v>53</v>
       </c>
       <c r="F69">
-        <v>-3.030997159314536</v>
+        <v>-3.030997159314529</v>
       </c>
       <c r="G69">
-        <v>-0.009715840008580459</v>
+        <v>-0.009715840008573354</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2002,10 +2002,10 @@
         <v>54</v>
       </c>
       <c r="F70">
-        <v>-3.038641293559408</v>
+        <v>-3.038641293559397</v>
       </c>
       <c r="G70">
-        <v>-0.004857920004290452</v>
+        <v>-0.004857920004280238</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2025,10 +2025,10 @@
         <v>55</v>
       </c>
       <c r="F71">
-        <v>-3.046285427804278</v>
+        <v>-3.046285427804264</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1.4210854715202e-14</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2048,10 +2048,10 @@
         <v>0</v>
       </c>
       <c r="F72">
-        <v>-2.527180582330456</v>
+        <v>-2.527180582330468</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>-1.199040866595169e-14</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2071,10 +2071,10 @@
         <v>1</v>
       </c>
       <c r="F73">
-        <v>-2.534669017704607</v>
+        <v>-2.534669017704617</v>
       </c>
       <c r="G73">
-        <v>-0.002476616393857878</v>
+        <v>-0.002476616393867204</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2094,10 +2094,10 @@
         <v>2</v>
       </c>
       <c r="F74">
-        <v>-2.542157453078758</v>
+        <v>-2.542157453078766</v>
       </c>
       <c r="G74">
-        <v>-0.004953232787715312</v>
+        <v>-0.004953232787723749</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2117,10 +2117,10 @@
         <v>3</v>
       </c>
       <c r="F75">
-        <v>-2.549645888452907</v>
+        <v>-2.549645888452914</v>
       </c>
       <c r="G75">
-        <v>-0.007008898470076019</v>
+        <v>-0.007429849181578074</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2140,10 +2140,10 @@
         <v>4</v>
       </c>
       <c r="F76">
-        <v>-2.557134323827057</v>
+        <v>-2.55658829208103</v>
       </c>
       <c r="G76">
-        <v>-0.009360433829395998</v>
+        <v>-0.009360433829400439</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2163,10 +2163,10 @@
         <v>5</v>
       </c>
       <c r="F77">
-        <v>-2.564076727455176</v>
+        <v>-2.5639287926167</v>
       </c>
       <c r="G77">
-        <v>-0.01153748281947742</v>
+        <v>-0.01168911538477779</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2186,10 +2186,10 @@
         <v>6</v>
       </c>
       <c r="F78">
-        <v>-2.571117660587071</v>
+        <v>-2.570446547806509</v>
       </c>
       <c r="G78">
-        <v>-0.01274754935203282</v>
+        <v>-0.01319505159429335</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2209,10 +2209,10 @@
         <v>7</v>
       </c>
       <c r="F79">
-        <v>-2.577787048342173</v>
+        <v>-2.577089384030851</v>
       </c>
       <c r="G79">
-        <v>-0.01509908471135235</v>
+        <v>-0.01482606883834148</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2232,10 +2232,10 @@
         <v>8</v>
       </c>
       <c r="F80">
-        <v>-2.584551267874236</v>
+        <v>-2.584008933855023</v>
       </c>
       <c r="G80">
-        <v>-0.01700311782841757</v>
+        <v>-0.01673379968222033</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2255,10 +2255,10 @@
         <v>9</v>
       </c>
       <c r="F81">
-        <v>-2.591220655629338</v>
+        <v>-2.591033858571673</v>
       </c>
       <c r="G81">
-        <v>-0.01799983577254682</v>
+        <v>-0.01874690541857671</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <v>-2.597828327361313</v>
+        <v>-2.597680392522835</v>
       </c>
       <c r="G82">
-        <v>-0.01962224005498747</v>
+        <v>-0.02038162038944558</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2301,10 +2301,10 @@
         <v>11</v>
       </c>
       <c r="F83">
-        <v>-2.604331841708785</v>
+        <v>-2.603101429675862</v>
       </c>
       <c r="G83">
-        <v>-0.02152627317205269</v>
+        <v>-0.02079083856217956</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2324,10 +2324,10 @@
         <v>12</v>
       </c>
       <c r="F84">
-        <v>-2.611300796867662</v>
+        <v>-2.611293929490623</v>
       </c>
       <c r="G84">
-        <v>-0.02337063900452652</v>
+        <v>-0.02397151939664788</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2347,10 +2347,10 @@
         <v>13</v>
       </c>
       <c r="F85">
-        <v>-2.617483820161325</v>
+        <v>-2.616944014812231</v>
       </c>
       <c r="G85">
-        <v>-0.02426739374732811</v>
+        <v>-0.02460978573796169</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2370,10 +2370,10 @@
         <v>14</v>
       </c>
       <c r="F86">
-        <v>-2.624373120727923</v>
+        <v>-2.624459339543276</v>
       </c>
       <c r="G86">
-        <v>-0.02622883011971888</v>
+        <v>-0.02711329148871311</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2393,10 +2393,10 @@
         <v>15</v>
       </c>
       <c r="F87">
-        <v>-2.631046206209842</v>
+        <v>-2.630132587503912</v>
       </c>
       <c r="G87">
-        <v>-0.02653841986532246</v>
+        <v>-0.02777472046905638</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2416,10 +2416,10 @@
         <v>16</v>
       </c>
       <c r="F88">
-        <v>-2.637234144738298</v>
+        <v>-2.637997222799576</v>
       </c>
       <c r="G88">
-        <v>-0.02815394975684438</v>
+        <v>-0.03062753678442665</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2439,10 +2439,10 @@
         <v>17</v>
       </c>
       <c r="F89">
-        <v>-2.643221538771175</v>
+        <v>-2.642477829025828</v>
       </c>
       <c r="G89">
-        <v>-0.03084003377573286</v>
+        <v>-0.03009632403038554</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2462,10 +2462,10 @@
         <v>18</v>
       </c>
       <c r="F90">
-        <v>-2.649704467294752</v>
+        <v>-2.648787341112458</v>
       </c>
       <c r="G90">
-        <v>-0.03084254122756214</v>
+        <v>-0.03139401713672241</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2485,10 +2485,10 @@
         <v>19</v>
       </c>
       <c r="F91">
-        <v>-2.656160506461429</v>
+        <v>-2.655749325284129</v>
       </c>
       <c r="G91">
-        <v>-0.03339219113961223</v>
+        <v>-0.03334418232809933</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2508,10 +2508,10 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.662789002538529</v>
+        <v>-2.660921109052133</v>
       </c>
       <c r="G92">
-        <v>-0.03468923671377633</v>
+        <v>-0.0335041471158104</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2531,10 +2531,10 @@
         <v>21</v>
       </c>
       <c r="F93">
-        <v>-2.669005091855501</v>
+        <v>-2.669294398769136</v>
       </c>
       <c r="G93">
-        <v>-0.03543771879196145</v>
+        <v>-0.03686561785251952</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2554,10 +2554,10 @@
         <v>22</v>
       </c>
       <c r="F94">
-        <v>-2.675394893960385</v>
+        <v>-2.67331428252893</v>
       </c>
       <c r="G94">
-        <v>-0.0360576418403733</v>
+        <v>-0.03587368263202073</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2577,10 +2577,10 @@
         <v>23</v>
       </c>
       <c r="F95">
-        <v>-2.681354208786683</v>
+        <v>-2.67997798810731</v>
       </c>
       <c r="G95">
-        <v>-0.03890178990948012</v>
+        <v>-0.03752556923010752</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2600,10 +2600,10 @@
         <v>24</v>
       </c>
       <c r="F96">
-        <v>-2.687254967819745</v>
+        <v>-2.685016028083973</v>
       </c>
       <c r="G96">
-        <v>-0.03857653730411048</v>
+        <v>-0.03755179022647681</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2623,10 +2623,10 @@
         <v>25</v>
       </c>
       <c r="F97">
-        <v>-2.693188897878067</v>
+        <v>-2.691823863905655</v>
       </c>
       <c r="G97">
-        <v>-0.03972751289944121</v>
+        <v>-0.03934780706786567</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2646,10 +2646,10 @@
         <v>26</v>
       </c>
       <c r="F98">
-        <v>-2.699644622221615</v>
+        <v>-2.698560453394495</v>
       </c>
       <c r="G98">
-        <v>-0.0408171491283249</v>
+        <v>-0.04107257757641181</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2669,10 +2669,10 @@
         <v>27</v>
       </c>
       <c r="F99">
-        <v>-2.705775128168424</v>
+        <v>-2.704267371005806</v>
       </c>
       <c r="G99">
-        <v>-0.04304768158578343</v>
+        <v>-0.04176767620742927</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2692,10 +2692,10 @@
         <v>28</v>
       </c>
       <c r="F100">
-        <v>-2.711903960902909</v>
+        <v>-2.710825702497996</v>
       </c>
       <c r="G100">
-        <v>-0.04343915994824155</v>
+        <v>-0.04331418871932691</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2715,10 +2715,10 @@
         <v>29</v>
       </c>
       <c r="F101">
-        <v>-2.718773631676454</v>
+        <v>-2.71682066018195</v>
       </c>
       <c r="G101">
-        <v>-0.04500936383582488</v>
+        <v>-0.0442973274229872</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -2738,10 +2738,10 @@
         <v>30</v>
       </c>
       <c r="F102">
-        <v>-2.72493751895977</v>
+        <v>-2.722207010508159</v>
       </c>
       <c r="G102">
-        <v>-0.04396276895159845</v>
+        <v>-0.04467185876890278</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2761,10 +2761,10 @@
         <v>31</v>
       </c>
       <c r="F103">
-        <v>-2.729802333998807</v>
+        <v>-2.728385957994885</v>
       </c>
       <c r="G103">
-        <v>-0.04694913523662292</v>
+        <v>-0.04583898727533553</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -2784,10 +2784,10 @@
         <v>32</v>
       </c>
       <c r="F104">
-        <v>-2.736701257101549</v>
+        <v>-2.735955382133135</v>
       </c>
       <c r="G104">
-        <v>-0.04637412235685168</v>
+        <v>-0.04839659243329231</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2807,10 +2807,10 @@
         <v>33</v>
       </c>
       <c r="F105">
-        <v>-2.74198346745841</v>
+        <v>-2.740878194225086</v>
       </c>
       <c r="G105">
-        <v>-0.04817313167141402</v>
+        <v>-0.04830758554495018</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2830,10 +2830,10 @@
         <v>34</v>
       </c>
       <c r="F106">
-        <v>-2.747110504249598</v>
+        <v>-2.747956031091275</v>
       </c>
       <c r="G106">
-        <v>-0.04833907314732233</v>
+        <v>-0.05037360343084574</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -2853,10 +2853,10 @@
         <v>35</v>
       </c>
       <c r="F107">
-        <v>-2.753384446826677</v>
+        <v>-2.752216965129325</v>
       </c>
       <c r="G107">
-        <v>-0.05027076247147755</v>
+        <v>-0.04962271848860245</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2876,10 +2876,10 @@
         <v>36</v>
       </c>
       <c r="F108">
-        <v>-2.759519326444865</v>
+        <v>-2.758853954117912</v>
       </c>
       <c r="G108">
-        <v>-0.04871400073098031</v>
+        <v>-0.05124788849689588</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2899,10 +2899,10 @@
         <v>37</v>
       </c>
       <c r="F109">
-        <v>-2.765066096136249</v>
+        <v>-2.764290973934087</v>
       </c>
       <c r="G109">
-        <v>-0.0515892749948017</v>
+        <v>-0.05167308933277748</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2922,10 +2922,10 @@
         <v>38</v>
       </c>
       <c r="F110">
-        <v>-2.771649862580533</v>
+        <v>-2.770715044108685</v>
       </c>
       <c r="G110">
-        <v>-0.05167060709118543</v>
+        <v>-0.05308534052708236</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2945,10 +2945,10 @@
         <v>39</v>
       </c>
       <c r="F111">
-        <v>-2.776876816848366</v>
+        <v>-2.775735340132129</v>
       </c>
       <c r="G111">
-        <v>-0.05309093056624747</v>
+        <v>-0.05309381757023268</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -2968,10 +2968,10 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.781948030029919</v>
+        <v>-2.781446435258457</v>
       </c>
       <c r="G112">
-        <v>-0.05241584299312052</v>
+        <v>-0.05379309371626739</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2991,10 +2991,10 @@
         <v>41</v>
       </c>
       <c r="F113">
-        <v>-2.787805151659301</v>
+        <v>-2.789263077304626</v>
       </c>
       <c r="G113">
-        <v>-0.05452654928112111</v>
+        <v>-0.0565979167821431</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3014,10 +3014,10 @@
         <v>42</v>
       </c>
       <c r="F114">
-        <v>-2.794003889466307</v>
+        <v>-2.792910574129658</v>
       </c>
       <c r="G114">
-        <v>-0.05508777724753333</v>
+        <v>-0.05523359462688138</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3037,10 +3037,10 @@
         <v>43</v>
       </c>
       <c r="F115">
-        <v>-2.798339032542215</v>
+        <v>-2.799321249247869</v>
       </c>
       <c r="G115">
-        <v>-0.05551541338758215</v>
+        <v>-0.05663245076479884</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3060,10 +3060,10 @@
         <v>44</v>
       </c>
       <c r="F116">
-        <v>-2.804297164510983</v>
+        <v>-2.80228001301945</v>
       </c>
       <c r="G116">
-        <v>-0.05559410467951587</v>
+        <v>-0.05457939555608693</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3083,10 +3083,10 @@
         <v>45</v>
       </c>
       <c r="F117">
-        <v>-2.810860559334021</v>
+        <v>-2.810043878293136</v>
       </c>
       <c r="G117">
-        <v>-0.05655285368063656</v>
+        <v>-0.05733144184947991</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3106,10 +3106,10 @@
         <v>46</v>
       </c>
       <c r="F118">
-        <v>-2.816805008523441</v>
+        <v>-2.81608535868666</v>
       </c>
       <c r="G118">
-        <v>-0.05814214745907353</v>
+        <v>-0.05836110326271005</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3129,10 +3129,10 @@
         <v>47</v>
       </c>
       <c r="F119">
-        <v>-2.822089121331726</v>
+        <v>-2.820995416089896</v>
       </c>
       <c r="G119">
-        <v>-0.05867477612472016</v>
+        <v>-0.05825934168565339</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3152,10 +3152,10 @@
         <v>48</v>
       </c>
       <c r="F120">
-        <v>-2.827787230302178</v>
+        <v>-2.826867593709021</v>
       </c>
       <c r="G120">
-        <v>-0.05836254801762486</v>
+        <v>-0.0591197003244841</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3175,10 +3175,10 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.833379174433034</v>
+        <v>-2.832875603008955</v>
       </c>
       <c r="G121">
-        <v>-0.05882096451375207</v>
+        <v>-0.06011589064412548</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3198,10 +3198,10 @@
         <v>50</v>
       </c>
       <c r="F122">
-        <v>-2.839545365365931</v>
+        <v>-2.839047481591393</v>
       </c>
       <c r="G122">
-        <v>-0.05982220534360372</v>
+        <v>-0.06127595024627008</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3221,10 +3221,10 @@
         <v>51</v>
       </c>
       <c r="F123">
-        <v>-2.844560816080724</v>
+        <v>-2.843896086242533</v>
       </c>
       <c r="G123">
-        <v>-0.05852440644467238</v>
+        <v>-0.06111273591711663</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3244,10 +3244,10 @@
         <v>52</v>
       </c>
       <c r="F124">
-        <v>-2.850408432227866</v>
+        <v>-2.850292849638052</v>
       </c>
       <c r="G124">
-        <v>-0.05974720060850958</v>
+        <v>-0.06249768033234204</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3267,10 +3267,10 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.856011638706397</v>
+        <v>-2.854854374240741</v>
       </c>
       <c r="G125">
-        <v>-0.06043663423083312</v>
+        <v>-0.06204738595473791</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3290,10 +3290,10 @@
         <v>54</v>
       </c>
       <c r="F126">
-        <v>-2.860488375992292</v>
+        <v>-2.85877391362527</v>
       </c>
       <c r="G126">
-        <v>-0.06049816163235744</v>
+        <v>-0.06095510635897328</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3313,10 +3313,10 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.86719983493051</v>
+        <v>-2.866402312210238</v>
       </c>
       <c r="G127">
-        <v>-0.06116059262841467</v>
+        <v>-0.06357168596364748</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3336,10 +3336,10 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.871999603441503</v>
+        <v>-2.869206086060882</v>
       </c>
       <c r="G128">
-        <v>-0.05999829908844112</v>
+        <v>-0.06136364083399903</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3359,10 +3359,10 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.876581793692501</v>
+        <v>-2.876316768237813</v>
       </c>
       <c r="G129">
-        <v>-0.06162123943036568</v>
+        <v>-0.06346250403063602</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3382,10 +3382,10 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.883556126790109</v>
+        <v>-2.880750425093523</v>
       </c>
       <c r="G130">
-        <v>-0.06235603945775781</v>
+        <v>-0.06288434190605274</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3405,10 +3405,10 @@
         <v>59</v>
       </c>
       <c r="F131">
-        <v>-2.889240698585287</v>
+        <v>-2.885727239966789</v>
       </c>
       <c r="G131">
-        <v>-0.06175812201860365</v>
+        <v>-0.06284933779902624</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3428,10 +3428,10 @@
         <v>60</v>
       </c>
       <c r="F132">
-        <v>-2.894064959300075</v>
+        <v>-2.893634382373857</v>
       </c>
       <c r="G132">
-        <v>-0.06373014700597257</v>
+        <v>-0.06574466122580058</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3451,10 +3451,10 @@
         <v>61</v>
       </c>
       <c r="F133">
-        <v>-2.898599839698962</v>
+        <v>-2.896937220151821</v>
       </c>
       <c r="G133">
-        <v>-0.06502047979979309</v>
+        <v>-0.06403568002347071</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3474,10 +3474,10 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.904413795603185</v>
+        <v>-2.902502460634975</v>
       </c>
       <c r="G134">
-        <v>-0.06442018072698819</v>
+        <v>-0.06458910152633202</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3497,10 +3497,10 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.911344959368382</v>
+        <v>-2.908689990128642</v>
       </c>
       <c r="G135">
-        <v>-0.06491933212144141</v>
+        <v>-0.06576481203970608</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3520,10 +3520,10 @@
         <v>64</v>
       </c>
       <c r="F136">
-        <v>-2.915119194748633</v>
+        <v>-2.91593551636215</v>
       </c>
       <c r="G136">
-        <v>-0.06573048235958368</v>
+        <v>-0.06799851929292</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -3543,10 +3543,10 @@
         <v>65</v>
       </c>
       <c r="F137">
-        <v>-2.918736041320013</v>
+        <v>-2.920091898552963</v>
       </c>
       <c r="G137">
-        <v>-0.06405571673220445</v>
+        <v>-0.06714308250343981</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -3566,10 +3566,10 @@
         <v>66</v>
       </c>
       <c r="F138">
-        <v>-2.923909127918091</v>
+        <v>-2.922411691118897</v>
       </c>
       <c r="G138">
-        <v>-0.06515736444055586</v>
+        <v>-0.06445105608908031</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -3589,10 +3589,10 @@
         <v>67</v>
       </c>
       <c r="F139">
-        <v>-2.930059097336152</v>
+        <v>-2.929005421487068</v>
       </c>
       <c r="G139">
-        <v>-0.06664435394677382</v>
+        <v>-0.06603296747695842</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -3612,10 +3612,10 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.934977873033891</v>
+        <v>-2.935901568346875</v>
       </c>
       <c r="G140">
-        <v>-0.06556463984838112</v>
+        <v>-0.06791729535647217</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -3635,10 +3635,10 @@
         <v>69</v>
       </c>
       <c r="F141">
-        <v>-2.939697872182133</v>
+        <v>-2.940935050703278</v>
       </c>
       <c r="G141">
-        <v>-0.06584330908052571</v>
+        <v>-0.0679389587325816</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -3658,10 +3658,10 @@
         <v>70</v>
       </c>
       <c r="F142">
-        <v>-2.945372154202433</v>
+        <v>-2.945738389721404</v>
       </c>
       <c r="G142">
-        <v>-0.06469009095332323</v>
+        <v>-0.06773047877041449</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -3681,10 +3681,10 @@
         <v>71</v>
       </c>
       <c r="F143">
-        <v>-2.951136943588652</v>
+        <v>-2.950407938665473</v>
       </c>
       <c r="G143">
-        <v>-0.06612790255270729</v>
+        <v>-0.06738820873418949</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -3704,10 +3704,10 @@
         <v>72</v>
       </c>
       <c r="F144">
-        <v>-2.955285717616995</v>
+        <v>-2.956999208266978</v>
       </c>
       <c r="G144">
-        <v>-0.06586546245596736</v>
+        <v>-0.06896765935540161</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -3727,10 +3727,10 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.962414663771074</v>
+        <v>-2.960524556538067</v>
       </c>
       <c r="G145">
-        <v>-0.06657735456717484</v>
+        <v>-0.06748118864619723</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -3750,10 +3750,10 @@
         <v>74</v>
       </c>
       <c r="F146">
-        <v>-2.965197642837644</v>
+        <v>-2.964460550580648</v>
       </c>
       <c r="G146">
-        <v>-0.06520645279261617</v>
+        <v>-0.06640536370848471</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -3773,10 +3773,10 @@
         <v>75</v>
       </c>
       <c r="F147">
-        <v>-2.971534776698191</v>
+        <v>-2.966466238585252</v>
       </c>
       <c r="G147">
-        <v>-0.06629710875114192</v>
+        <v>-0.06339923273279569</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -3796,10 +3796,10 @@
         <v>76</v>
       </c>
       <c r="F148">
-        <v>-2.974853673529919</v>
+        <v>-2.976876368968091</v>
       </c>
       <c r="G148">
-        <v>-0.06466702489280229</v>
+        <v>-0.06879754413534145</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -3819,10 +3819,10 @@
         <v>77</v>
       </c>
       <c r="F149">
-        <v>-2.981286530873104</v>
+        <v>-2.980597831757254</v>
       </c>
       <c r="G149">
-        <v>-0.06514337513956647</v>
+        <v>-0.06750718794421084</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -3842,10 +3842,10 @@
         <v>78</v>
       </c>
       <c r="F150">
-        <v>-2.986803463028139</v>
+        <v>-2.985380094830802</v>
       </c>
       <c r="G150">
-        <v>-0.06555015090333249</v>
+        <v>-0.06727763203746573</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -3865,10 +3865,10 @@
         <v>79</v>
       </c>
       <c r="F151">
-        <v>-2.990202064445956</v>
+        <v>-2.987676672715433</v>
       </c>
       <c r="G151">
-        <v>-0.06699384351924897</v>
+        <v>-0.06456239094180272</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -3888,10 +3888,10 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.995295187321518</v>
+        <v>-2.995858882499368</v>
       </c>
       <c r="G152">
-        <v>-0.06458872555120188</v>
+        <v>-0.06773278174544517</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -3911,10 +3911,10 @@
         <v>81</v>
       </c>
       <c r="F153">
-        <v>-3.000671357133846</v>
+        <v>-2.997925337577441</v>
       </c>
       <c r="G153">
-        <v>-0.06470446869823787</v>
+        <v>-0.06478741784322395</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -3934,10 +3934,10 @@
         <v>82</v>
       </c>
       <c r="F154">
-        <v>-3.004439759900296</v>
+        <v>-3.004719453832646</v>
       </c>
       <c r="G154">
-        <v>-0.06322550252214532</v>
+        <v>-0.0665697151181357</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -3957,10 +3957,10 @@
         <v>83</v>
       </c>
       <c r="F155">
-        <v>-3.008493482935768</v>
+        <v>-3.009934275880199</v>
       </c>
       <c r="G155">
-        <v>-0.06251897882512414</v>
+        <v>-0.0667727181853961</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -3980,10 +3980,10 @@
         <v>84</v>
       </c>
       <c r="F156">
-        <v>-3.014982823420358</v>
+        <v>-3.014200406633095</v>
       </c>
       <c r="G156">
-        <v>-0.06422424535345517</v>
+        <v>-0.06602702995799836</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -4003,10 +4003,10 @@
         <v>85</v>
       </c>
       <c r="F157">
-        <v>-3.019969961958234</v>
+        <v>-3.020874140688279</v>
       </c>
       <c r="G157">
-        <v>-0.06190326423167614</v>
+        <v>-0.06768894503288925</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -4026,10 +4026,10 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.024750886846435</v>
+        <v>-3.023778383444115</v>
       </c>
       <c r="G158">
-        <v>-0.0662337597610072</v>
+        <v>-0.06558136880843191</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -4049,10 +4049,10 @@
         <v>87</v>
       </c>
       <c r="F159">
-        <v>-3.02911740148376</v>
+        <v>-3.029083706150644</v>
       </c>
       <c r="G159">
-        <v>-0.06403073811491899</v>
+        <v>-0.06587487253466695</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -4072,10 +4072,10 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.033660843265621</v>
+        <v>-3.033822331398909</v>
       </c>
       <c r="G160">
-        <v>-0.06198414582054457</v>
+        <v>-0.06560167880263923</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -4095,10 +4095,10 @@
         <v>89</v>
       </c>
       <c r="F161">
-        <v>-3.038200124556521</v>
+        <v>-3.038560383490193</v>
       </c>
       <c r="G161">
-        <v>-0.06496765297995788</v>
+        <v>-0.06532791191362941</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -4118,10 +4118,10 @@
         <v>90</v>
       </c>
       <c r="F162">
-        <v>-3.042571263506562</v>
+        <v>-3.042358212216969</v>
       </c>
       <c r="G162">
-        <v>-0.06419777513301805</v>
+        <v>-0.06411392166011232</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -4141,10 +4141,10 @@
         <v>91</v>
       </c>
       <c r="F163">
-        <v>-3.047599013147726</v>
+        <v>-3.047308026418245</v>
       </c>
       <c r="G163">
-        <v>-0.06434290361057582</v>
+        <v>-0.06405191688109535</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -4164,10 +4164,10 @@
         <v>92</v>
       </c>
       <c r="F164">
-        <v>-3.052435820176851</v>
+        <v>-3.053446742499242</v>
       </c>
       <c r="G164">
-        <v>-0.06416789165940784</v>
+        <v>-0.06517881398179826</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -4187,10 +4187,10 @@
         <v>93</v>
       </c>
       <c r="F165">
-        <v>-3.057535082165673</v>
+        <v>-3.056034511921426</v>
       </c>
       <c r="G165">
-        <v>-0.06425533466793676</v>
+        <v>-0.06275476442368888</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -4210,10 +4210,10 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.061107026443836</v>
+        <v>-3.062104677424069</v>
       </c>
       <c r="G166">
-        <v>-0.06058776189785309</v>
+        <v>-0.06381311094603859</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -4233,10 +4233,10 @@
         <v>95</v>
       </c>
       <c r="F167">
-        <v>-3.066777616093671</v>
+        <v>-3.066147671850681</v>
       </c>
       <c r="G167">
-        <v>-0.06096807904779766</v>
+        <v>-0.06284428639235717</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -4256,10 +4256,10 @@
         <v>96</v>
       </c>
       <c r="F168">
-        <v>-3.070260695053905</v>
+        <v>-3.070393536808382</v>
       </c>
       <c r="G168">
-        <v>-0.05960336843482184</v>
+        <v>-0.06207833236976512</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -4279,10 +4279,10 @@
         <v>97</v>
       </c>
       <c r="F169">
-        <v>-3.074646259304478</v>
+        <v>-3.073694227466299</v>
       </c>
       <c r="G169">
-        <v>-0.05891355813711219</v>
+        <v>-0.06036720404738916</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -4302,10 +4302,10 @@
         <v>98</v>
       </c>
       <c r="F170">
-        <v>-3.079427557755675</v>
+        <v>-3.079984830751882</v>
       </c>
       <c r="G170">
-        <v>-0.05730450266901987</v>
+        <v>-0.06164598835267909</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -4325,10 +4325,10 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.083420816631987</v>
+        <v>-3.083040039174117</v>
       </c>
       <c r="G171">
-        <v>-0.05869660714966918</v>
+        <v>-0.05968937779462025</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -4348,10 +4348,10 @@
         <v>100</v>
       </c>
       <c r="F172">
-        <v>-3.088971018400142</v>
+        <v>-3.089939289968849</v>
       </c>
       <c r="G172">
-        <v>-0.05855378722996052</v>
+        <v>-0.06157680960905887</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -4371,10 +4371,10 @@
         <v>101</v>
       </c>
       <c r="F173">
-        <v>-3.091946288182141</v>
+        <v>-3.093976687304298</v>
       </c>
       <c r="G173">
-        <v>-0.05630912382923858</v>
+        <v>-0.0606023879642148</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -4394,10 +4394,10 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.097555938576017</v>
+        <v>-3.095696542563779</v>
       </c>
       <c r="G174">
-        <v>-0.0560119414824285</v>
+        <v>-0.05731042424340216</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -4417,10 +4417,10 @@
         <v>103</v>
       </c>
       <c r="F175">
-        <v>-3.101988758274533</v>
+        <v>-3.102921715754679</v>
       </c>
       <c r="G175">
-        <v>-0.05642056255975092</v>
+        <v>-0.0595237784540088</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -4440,10 +4440,10 @@
         <v>104</v>
       </c>
       <c r="F176">
-        <v>-3.105976057964619</v>
+        <v>-3.105425129691536</v>
       </c>
       <c r="G176">
-        <v>-0.05617350751213446</v>
+        <v>-0.05701537341057217</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -4463,10 +4463,10 @@
         <v>105</v>
       </c>
       <c r="F177">
-        <v>-3.110294937476311</v>
+        <v>-3.109079491314813</v>
       </c>
       <c r="G177">
-        <v>-0.05446133096250516</v>
+        <v>-0.05565791605355563</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -4486,10 +4486,10 @@
         <v>106</v>
       </c>
       <c r="F178">
-        <v>-3.114789793084493</v>
+        <v>-3.114031005796952</v>
       </c>
       <c r="G178">
-        <v>-0.05635639884294241</v>
+        <v>-0.05559761155540122</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -4509,10 +4509,10 @@
         <v>107</v>
       </c>
       <c r="F179">
-        <v>-3.118551081606937</v>
+        <v>-3.119383826962398</v>
       </c>
       <c r="G179">
-        <v>-0.05399819652519644</v>
+        <v>-0.05593861374055409</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -4532,10 +4532,10 @@
         <v>108</v>
       </c>
       <c r="F180">
-        <v>-3.12212140043591</v>
+        <v>-3.124273964997457</v>
       </c>
       <c r="G180">
-        <v>-0.05247479049790593</v>
+        <v>-0.05581693279531974</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -4555,10 +4555,10 @@
         <v>109</v>
       </c>
       <c r="F181">
-        <v>-3.126639158692338</v>
+        <v>-3.125869403569847</v>
       </c>
       <c r="G181">
-        <v>-0.05155385926728662</v>
+        <v>-0.05240055238741648</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -4578,10 +4578,10 @@
         <v>110</v>
       </c>
       <c r="F182">
-        <v>-3.131122799614015</v>
+        <v>-3.130518399658781</v>
       </c>
       <c r="G182">
-        <v>-0.0514190443843523</v>
+        <v>-0.05203772949605678</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -4601,10 +4601,10 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.134984378277463</v>
+        <v>-3.134782904058981</v>
       </c>
       <c r="G183">
-        <v>-0.05032671988725779</v>
+        <v>-0.05129041491596353</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -4624,10 +4624,10 @@
         <v>112</v>
       </c>
       <c r="F184">
-        <v>-3.138849008417895</v>
+        <v>-3.14087100199626</v>
       </c>
       <c r="G184">
-        <v>-0.04904091555616807</v>
+        <v>-0.05236669387295001</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -4647,10 +4647,10 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.143162086087445</v>
+        <v>-3.141966245646907</v>
       </c>
       <c r="G185">
-        <v>-0.0475267050792374</v>
+        <v>-0.04845011854330328</v>
       </c>
     </row>
     <row r="186" spans="1:7">
@@ -4670,10 +4670,10 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.147765094018068</v>
+        <v>-3.147779738725947</v>
       </c>
       <c r="G186">
-        <v>-0.0483892698089563</v>
+        <v>-0.04925179264205015</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -4693,10 +4693,10 @@
         <v>115</v>
       </c>
       <c r="F187">
-        <v>-3.151378322013548</v>
+        <v>-3.150898939419395</v>
       </c>
       <c r="G187">
-        <v>-0.04629277621426797</v>
+        <v>-0.04735917435520443</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -4716,10 +4716,10 @@
         <v>116</v>
       </c>
       <c r="F188">
-        <v>-3.156794968015595</v>
+        <v>-3.155012747948987</v>
       </c>
       <c r="G188">
-        <v>-0.04477119390811302</v>
+        <v>-0.04646116390450361</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -4739,10 +4739,10 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.15946046327876</v>
+        <v>-3.159550649159591</v>
       </c>
       <c r="G189">
-        <v>-0.04438895429458223</v>
+        <v>-0.04598724613481375</v>
       </c>
     </row>
     <row r="190" spans="1:7">
@@ -4762,10 +4762,10 @@
         <v>118</v>
       </c>
       <c r="F190">
-        <v>-3.164086877749303</v>
+        <v>-3.163724832661905</v>
       </c>
       <c r="G190">
-        <v>-0.04495261728131517</v>
+        <v>-0.0451496106568342</v>
       </c>
     </row>
     <row r="191" spans="1:7">
@@ -4785,10 +4785,10 @@
         <v>119</v>
       </c>
       <c r="F191">
-        <v>-3.167963602154305</v>
+        <v>-3.168246459210928</v>
       </c>
       <c r="G191">
-        <v>-0.04234770934646692</v>
+        <v>-0.0446594182255643</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -4808,10 +4808,10 @@
         <v>120</v>
       </c>
       <c r="F192">
-        <v>-3.171162479734372</v>
+        <v>-3.173435111890394</v>
       </c>
       <c r="G192">
-        <v>-0.04134060640137954</v>
+        <v>-0.044836251924737</v>
       </c>
     </row>
     <row r="193" spans="1:7">
@@ -4831,10 +4831,10 @@
         <v>121</v>
       </c>
       <c r="F193">
-        <v>-3.175882201545098</v>
+        <v>-3.176173472008438</v>
       </c>
       <c r="G193">
-        <v>-0.03971331536512507</v>
+        <v>-0.04256279306248706</v>
       </c>
     </row>
     <row r="194" spans="1:7">
@@ -4854,10 +4854,10 @@
         <v>122</v>
       </c>
       <c r="F194">
-        <v>-3.180288055942324</v>
+        <v>-3.177434961695387</v>
       </c>
       <c r="G194">
-        <v>-0.0404114516191727</v>
+        <v>-0.03881246376914294</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -4877,10 +4877,10 @@
         <v>123</v>
       </c>
       <c r="F195">
-        <v>-3.183638411539827</v>
+        <v>-3.183580108248109</v>
       </c>
       <c r="G195">
-        <v>-0.03760085374724426</v>
+        <v>-0.03994579134157211</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -4900,10 +4900,10 @@
         <v>124</v>
       </c>
       <c r="F196">
-        <v>-3.188068828917364</v>
+        <v>-3.188058576347226</v>
       </c>
       <c r="G196">
-        <v>-0.03934516263878435</v>
+        <v>-0.03941244046039544</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -4923,10 +4923,10 @@
         <v>125</v>
       </c>
       <c r="F197">
-        <v>-3.191851091102457</v>
+        <v>-3.189936585305512</v>
       </c>
       <c r="G197">
-        <v>-0.03549543548973461</v>
+        <v>-0.03627863043838803</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -4946,10 +4946,10 @@
         <v>126</v>
       </c>
       <c r="F198">
-        <v>-3.196607353778104</v>
+        <v>-3.196010794281656</v>
       </c>
       <c r="G198">
-        <v>-0.03793757993068719</v>
+        <v>-0.03734102043423909</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -4969,10 +4969,10 @@
         <v>127</v>
       </c>
       <c r="F199">
-        <v>-3.198916613499793</v>
+        <v>-3.198319782422274</v>
       </c>
       <c r="G199">
-        <v>-0.03458054845491842</v>
+        <v>-0.03463818959456333</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -4992,10 +4992,10 @@
         <v>128</v>
       </c>
       <c r="F200">
-        <v>-3.20322597192534</v>
+        <v>-3.202470218677251</v>
       </c>
       <c r="G200">
-        <v>-0.03027314787107582</v>
+        <v>-0.03377680686924722</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -5015,10 +5015,10 @@
         <v>129</v>
       </c>
       <c r="F201">
-        <v>-3.206463821361251</v>
+        <v>-3.207967688723123</v>
       </c>
       <c r="G201">
-        <v>-0.03082270423329841</v>
+        <v>-0.03426245793482557</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -5038,10 +5038,10 @@
         <v>130</v>
       </c>
       <c r="F202">
-        <v>-3.210756083297581</v>
+        <v>-3.209080613784895</v>
       </c>
       <c r="G202">
-        <v>-0.03009688453344472</v>
+        <v>-0.03036356401630436</v>
       </c>
     </row>
     <row r="203" spans="1:7">
@@ -5061,10 +5061,10 @@
         <v>131</v>
       </c>
       <c r="F203">
-        <v>-3.213292892307595</v>
+        <v>-3.214049241656778</v>
       </c>
       <c r="G203">
-        <v>-0.02855667550152441</v>
+        <v>-0.03032037290789391</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -5084,10 +5084,10 @@
         <v>132</v>
       </c>
       <c r="F204">
-        <v>-3.217614299192846</v>
+        <v>-3.216143145267341</v>
       </c>
       <c r="G204">
-        <v>-0.02607188065758331</v>
+        <v>-0.02740245753816334</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -5107,10 +5107,10 @@
         <v>133</v>
       </c>
       <c r="F205">
-        <v>-3.220276872121658</v>
+        <v>-3.221752686988122</v>
       </c>
       <c r="G205">
-        <v>-0.02519369114682696</v>
+        <v>-0.02800018027865142</v>
       </c>
     </row>
     <row r="206" spans="1:7">
@@ -5130,10 +5130,10 @@
         <v>134</v>
       </c>
       <c r="F206">
-        <v>-3.225109570643657</v>
+        <v>-3.222721375028642</v>
       </c>
       <c r="G206">
-        <v>-0.02472499254193353</v>
+        <v>-0.02395704933887857</v>
       </c>
     </row>
     <row r="207" spans="1:7">
@@ -5153,10 +5153,10 @@
         <v>135</v>
       </c>
       <c r="F207">
-        <v>-3.22798087891676</v>
+        <v>-3.226849402050685</v>
       </c>
       <c r="G207">
-        <v>-0.023459144017101</v>
+        <v>-0.02307325738062735</v>
       </c>
     </row>
     <row r="208" spans="1:7">
@@ -5176,10 +5176,10 @@
         <v>136</v>
       </c>
       <c r="F208">
-        <v>-3.230903865039085</v>
+        <v>-3.231949889919643</v>
       </c>
       <c r="G208">
-        <v>-0.02119282405852102</v>
+        <v>-0.02316192626929275</v>
       </c>
     </row>
     <row r="209" spans="1:7">
@@ -5199,10 +5199,10 @@
         <v>137</v>
       </c>
       <c r="F209">
-        <v>-3.234302410137784</v>
+        <v>-3.234302410137776</v>
       </c>
       <c r="G209">
-        <v>-0.01974087654502524</v>
+        <v>-0.02050262750713219</v>
       </c>
     </row>
     <row r="210" spans="1:7">
@@ -5222,10 +5222,10 @@
         <v>138</v>
       </c>
       <c r="F210">
-        <v>-3.238177520384522</v>
+        <v>-3.237669990374982</v>
       </c>
       <c r="G210">
-        <v>-0.01746515407039462</v>
+        <v>-0.01885838876404511</v>
       </c>
     </row>
     <row r="211" spans="1:7">
@@ -5245,10 +5245,10 @@
         <v>139</v>
       </c>
       <c r="F211">
-        <v>-3.240530040602663</v>
+        <v>-3.240022510593126</v>
       </c>
       <c r="G211">
-        <v>-0.01670662001143261</v>
+        <v>-0.01619909000189521</v>
       </c>
     </row>
     <row r="212" spans="1:7">
@@ -5268,10 +5268,10 @@
         <v>140</v>
       </c>
       <c r="F212">
-        <v>-3.243390090830336</v>
+        <v>-3.243390090830335</v>
       </c>
       <c r="G212">
-        <v>-0.01404732124927888</v>
+        <v>-0.01455485125881051</v>
       </c>
     </row>
     <row r="213" spans="1:7">
@@ -5291,10 +5291,10 @@
         <v>141</v>
       </c>
       <c r="F213">
-        <v>-3.246757671067543</v>
+        <v>-3.246757671067538</v>
       </c>
       <c r="G213">
-        <v>-0.01240308250619089</v>
+        <v>-0.0129106125157203</v>
       </c>
     </row>
     <row r="214" spans="1:7">
@@ -5314,10 +5314,10 @@
         <v>142</v>
       </c>
       <c r="F214">
-        <v>-3.249617721295215</v>
+        <v>-3.249617721295208</v>
       </c>
       <c r="G214">
-        <v>-0.01075884376310425</v>
+        <v>-0.01075884376309759</v>
       </c>
     </row>
     <row r="215" spans="1:7">
@@ -5337,10 +5337,10 @@
         <v>143</v>
       </c>
       <c r="F215">
-        <v>-3.252477771522887</v>
+        <v>-3.252477771522878</v>
       </c>
       <c r="G215">
-        <v>-0.008099545000950795</v>
+        <v>-0.008607075010473988</v>
       </c>
     </row>
     <row r="216" spans="1:7">
@@ -5360,10 +5360,10 @@
         <v>144</v>
       </c>
       <c r="F216">
-        <v>-3.25533782175056</v>
+        <v>-3.255337821750548</v>
       </c>
       <c r="G216">
-        <v>-0.006455306257863259</v>
+        <v>-0.006455306257851269</v>
       </c>
     </row>
     <row r="217" spans="1:7">
@@ -5383,10 +5383,10 @@
         <v>145</v>
       </c>
       <c r="F217">
-        <v>-3.258197871978234</v>
+        <v>-3.258197871978218</v>
       </c>
       <c r="G217">
-        <v>-0.004303537505242767</v>
+        <v>-0.004303537505227224</v>
       </c>
     </row>
     <row r="218" spans="1:7">
@@ -5406,10 +5406,10 @@
         <v>146</v>
       </c>
       <c r="F218">
-        <v>-3.261057922205906</v>
+        <v>-3.261057922205887</v>
       </c>
       <c r="G218">
-        <v>-0.002151768752621828</v>
+        <v>-0.002151768752603176</v>
       </c>
     </row>
     <row r="219" spans="1:7">
@@ -5429,10 +5429,10 @@
         <v>147</v>
       </c>
       <c r="F219">
-        <v>-3.263917972433577</v>
+        <v>-3.263917972433557</v>
       </c>
       <c r="G219">
-        <v>0</v>
+        <v>2.087219286295294e-14</v>
       </c>
     </row>
     <row r="220" spans="1:7">
@@ -5452,10 +5452,10 @@
         <v>0</v>
       </c>
       <c r="F220">
-        <v>-2.621703188588303</v>
+        <v>-2.621703188588206</v>
       </c>
       <c r="G220">
-        <v>0</v>
+        <v>9.769962616701378e-14</v>
       </c>
     </row>
     <row r="221" spans="1:7">
@@ -5475,10 +5475,10 @@
         <v>30</v>
       </c>
       <c r="F221">
-        <v>-2.722330616005841</v>
+        <v>-2.721372130328087</v>
       </c>
       <c r="G221">
-        <v>-0.02598157408172064</v>
+        <v>-0.02546572494906751</v>
       </c>
     </row>
     <row r="222" spans="1:7">
@@ -5498,10 +5498,10 @@
         <v>61</v>
       </c>
       <c r="F222">
-        <v>-2.818414889382493</v>
+        <v>-2.817925695426455</v>
       </c>
       <c r="G222">
-        <v>-0.04465284086214671</v>
+        <v>-0.04534263269702832</v>
       </c>
     </row>
     <row r="223" spans="1:7">
@@ -5521,10 +5521,10 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.90684110929937</v>
+        <v>-2.908422681011093</v>
       </c>
       <c r="G223">
-        <v>-0.05667863585152433</v>
+        <v>-0.05916296093125939</v>
       </c>
     </row>
     <row r="224" spans="1:7">
@@ -5544,10 +5544,10 @@
         <v>123</v>
       </c>
       <c r="F224">
-        <v>-2.990162523613378</v>
+        <v>-2.991786745210991</v>
       </c>
       <c r="G224">
-        <v>-0.06208032766673743</v>
+        <v>-0.06585036778075026</v>
       </c>
     </row>
     <row r="225" spans="1:7">
@@ -5567,10 +5567,10 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.06903949676441</v>
+        <v>-3.069679093338019</v>
       </c>
       <c r="G225">
-        <v>-0.0651795427956412</v>
+        <v>-0.06706605855737169</v>
       </c>
     </row>
     <row r="226" spans="1:7">
@@ -5590,10 +5590,10 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.142806209668382</v>
+        <v>-3.144550909475877</v>
       </c>
       <c r="G226">
-        <v>-0.06176417567675752</v>
+        <v>-0.06526121734482282</v>
       </c>
     </row>
     <row r="227" spans="1:7">
@@ -5613,10 +5613,10 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.212303752390315</v>
+        <v>-3.213922992188545</v>
       </c>
       <c r="G227">
-        <v>-0.05535611381859917</v>
+        <v>-0.05795664270708345</v>
       </c>
     </row>
     <row r="228" spans="1:7">
@@ -5636,10 +5636,10 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.275901294844515</v>
+        <v>-3.277980858521302</v>
       </c>
       <c r="G228">
-        <v>-0.04235567179172572</v>
+        <v>-0.04533785168943294</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -5659,10 +5659,10 @@
         <v>278</v>
       </c>
       <c r="F229">
-        <v>-3.334848039901463</v>
+        <v>-3.334986834440572</v>
       </c>
       <c r="G229">
-        <v>-0.02474690380336431</v>
+        <v>-0.0256671702582969</v>
       </c>
     </row>
     <row r="230" spans="1:7">
@@ -5682,10 +5682,10 @@
         <v>309</v>
       </c>
       <c r="F230">
-        <v>-3.385996321532683</v>
+        <v>-3.38599632153265</v>
       </c>
       <c r="G230">
-        <v>0</v>
+        <v>3.241851231905457e-14</v>
       </c>
     </row>
     <row r="231" spans="1:7">
@@ -5705,10 +5705,10 @@
         <v>0</v>
       </c>
       <c r="F231">
-        <v>-2.681923713795291</v>
+        <v>-2.681923713795318</v>
       </c>
       <c r="G231">
-        <v>0</v>
+        <v>-2.708944180085382e-14</v>
       </c>
     </row>
     <row r="232" spans="1:7">
@@ -5728,10 +5728,10 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.786960842615138</v>
+        <v>-2.786019717367762</v>
       </c>
       <c r="G232">
-        <v>-0.02627093675704639</v>
+        <v>-0.0260504758789617</v>
       </c>
     </row>
     <row r="233" spans="1:7">
@@ -5751,10 +5751,10 @@
         <v>112</v>
       </c>
       <c r="F233">
-        <v>-2.883672456550075</v>
+        <v>-2.88281455592801</v>
       </c>
       <c r="G233">
-        <v>-0.04396603691345913</v>
+        <v>-0.04479978674570084</v>
       </c>
     </row>
     <row r="234" spans="1:7">
@@ -5774,10 +5774,10 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.972777551450976</v>
+        <v>-2.974334596308505</v>
       </c>
       <c r="G234">
-        <v>-0.05640312486146803</v>
+        <v>-0.05827429943268769</v>
       </c>
     </row>
     <row r="235" spans="1:7">
@@ -5797,10 +5797,10 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.056110884215312</v>
+        <v>-3.05992860600994</v>
       </c>
       <c r="G235">
-        <v>-0.06130828897128859</v>
+        <v>-0.06582278144061338</v>
       </c>
     </row>
     <row r="236" spans="1:7">
@@ -5820,10 +5820,10 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.136442855885208</v>
+        <v>-3.141646965559532</v>
       </c>
       <c r="G236">
-        <v>-0.06349640213291674</v>
+        <v>-0.06949561329669662</v>
       </c>
     </row>
     <row r="237" spans="1:7">
@@ -5843,10 +5843,10 @@
         <v>336</v>
       </c>
       <c r="F237">
-        <v>-3.211682891594476</v>
+        <v>-3.216149655374434</v>
       </c>
       <c r="G237">
-        <v>-0.06148601163813172</v>
+        <v>-0.06595277541808997</v>
       </c>
     </row>
     <row r="238" spans="1:7">
@@ -5866,10 +5866,10 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.282719771767355</v>
+        <v>-3.28633820608926</v>
       </c>
       <c r="G238">
-        <v>-0.05258101445837926</v>
+        <v>-0.05809579843940671</v>
       </c>
     </row>
     <row r="239" spans="1:7">
@@ -5889,10 +5889,10 @@
         <v>448</v>
       </c>
       <c r="F239">
-        <v>-3.348413697751413</v>
+        <v>-3.351195610319622</v>
       </c>
       <c r="G239">
-        <v>-0.04045204251703594</v>
+        <v>-0.04490767497625925</v>
       </c>
     </row>
     <row r="240" spans="1:7">
@@ -5912,10 +5912,10 @@
         <v>504</v>
       </c>
       <c r="F240">
-        <v>-3.409462033509221</v>
+        <v>-3.411836790186109</v>
       </c>
       <c r="G240">
-        <v>-0.02453718513425368</v>
+        <v>-0.0275033271492377</v>
       </c>
     </row>
     <row r="241" spans="1:7">
@@ -5935,10 +5935,10 @@
         <v>561</v>
       </c>
       <c r="F241">
-        <v>-3.463772660867764</v>
+        <v>-3.463772660868219</v>
       </c>
       <c r="G241">
-        <v>0</v>
+        <v>-4.547473508864641e-13</v>
       </c>
     </row>
     <row r="242" spans="1:7">
@@ -5958,10 +5958,10 @@
         <v>0</v>
       </c>
       <c r="F242">
-        <v>-2.723569122533771</v>
+        <v>-2.723569122533946</v>
       </c>
       <c r="G242">
-        <v>0</v>
+        <v>-1.749711486809247e-13</v>
       </c>
     </row>
     <row r="243" spans="1:7">
@@ -5981,10 +5981,10 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.829053807146745</v>
+        <v>-2.82912645721084</v>
       </c>
       <c r="G243">
-        <v>-0.02581220560998343</v>
+        <v>-0.02641643856642695</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -6004,10 +6004,10 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.92615519608042</v>
+        <v>-2.927573942591553</v>
       </c>
       <c r="G244">
-        <v>-0.04384498982082752</v>
+        <v>-0.04572302783649684</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -6027,10 +6027,10 @@
         <v>276</v>
       </c>
       <c r="F245">
-        <v>-3.017401623633949</v>
+        <v>-3.020058596200119</v>
       </c>
       <c r="G245">
-        <v>-0.05581379045039592</v>
+        <v>-0.05906678533442067</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -6050,10 +6050,10 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.102819258940653</v>
+        <v>-3.107249243503461</v>
       </c>
       <c r="G246">
-        <v>-0.06037854978363622</v>
+        <v>-0.06625630939548288</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -6073,10 +6073,10 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.182508651189247</v>
+        <v>-3.188380491166494</v>
       </c>
       <c r="G247">
-        <v>-0.06223360379459431</v>
+        <v>-0.06824666094787357</v>
       </c>
     </row>
     <row r="248" spans="1:7">
@@ -6096,10 +6096,10 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.259663348519579</v>
+        <v>-3.264882577851401</v>
       </c>
       <c r="G248">
-        <v>-0.05946639809770504</v>
+        <v>-0.06560785152213766</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -6119,10 +6119,10 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.332450252831135</v>
+        <v>-3.337443151648606</v>
       </c>
       <c r="G249">
-        <v>-0.05220583430736225</v>
+        <v>-0.05816730207706311</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -6142,10 +6142,10 @@
         <v>738</v>
       </c>
       <c r="F250">
-        <v>-3.399368132892079</v>
+        <v>-3.403459083100889</v>
       </c>
       <c r="G250">
-        <v>-0.04095138720989344</v>
+        <v>-0.04504233741870345</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -6165,10 +6165,10 @@
         <v>830</v>
       </c>
       <c r="F251">
-        <v>-3.461293727546931</v>
+        <v>-3.463723656752894</v>
       </c>
       <c r="G251">
-        <v>-0.02348390912677606</v>
+        <v>-0.02616601496006538</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -6188,10 +6188,10 @@
         <v>923</v>
       </c>
       <c r="F252">
-        <v>-3.517558765035108</v>
+        <v>-3.517558765035645</v>
       </c>
       <c r="G252">
-        <v>0</v>
+        <v>-5.364597654988756e-13</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -6211,10 +6211,10 @@
         <v>0</v>
       </c>
       <c r="F253">
-        <v>-2.754057650354959</v>
+        <v>-2.75405765035523</v>
       </c>
       <c r="G253">
-        <v>0</v>
+        <v>-2.713385072183883e-13</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -6234,10 +6234,10 @@
         <v>141</v>
       </c>
       <c r="F254">
-        <v>-2.859579514799663</v>
+        <v>-2.860059673078998</v>
       </c>
       <c r="G254">
-        <v>-0.02551778450649422</v>
+        <v>-0.02599794278582923</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -6257,10 +6257,10 @@
         <v>283</v>
       </c>
       <c r="F255">
-        <v>-2.958811360264598</v>
+        <v>-2.960422889495681</v>
       </c>
       <c r="G255">
-        <v>-0.04380213962222745</v>
+        <v>-0.04578967444204585</v>
       </c>
     </row>
     <row r="256" spans="1:7">
@@ -6280,10 +6280,10 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.050313708814578</v>
+        <v>-3.053673118113357</v>
       </c>
       <c r="G256">
-        <v>-0.05548838217275165</v>
+        <v>-0.05903582312151201</v>
       </c>
     </row>
     <row r="257" spans="1:7">
@@ -6303,10 +6303,10 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.136084028574278</v>
+        <v>-3.141807741588365</v>
       </c>
       <c r="G257">
-        <v>-0.06024136341956599</v>
+        <v>-0.06659896183605385</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -6326,10 +6326,10 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.217061700669015</v>
+        <v>-3.22367762687283</v>
       </c>
       <c r="G258">
-        <v>-0.06163801963448479</v>
+        <v>-0.06846476718230954</v>
       </c>
     </row>
     <row r="259" spans="1:7">
@@ -6349,10 +6349,10 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.295131676644201</v>
+        <v>-3.301219619432476</v>
       </c>
       <c r="G259">
-        <v>-0.05880408182004593</v>
+        <v>-0.06543527498148838</v>
       </c>
     </row>
     <row r="260" spans="1:7">
@@ -6372,10 +6372,10 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.367829167640465</v>
+        <v>-3.373050733085449</v>
       </c>
       <c r="G260">
-        <v>-0.05112925886468378</v>
+        <v>-0.05726230869625171</v>
       </c>
     </row>
     <row r="261" spans="1:7">
@@ -6395,10 +6395,10 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.436345395248071</v>
+        <v>-3.439578960212611</v>
       </c>
       <c r="G261">
-        <v>-0.03968679502190919</v>
+        <v>-0.04321905106294766</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -6418,10 +6418,10 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.499487504523403</v>
+        <v>-3.502148491846754</v>
       </c>
       <c r="G262">
-        <v>-0.02294620606559572</v>
+        <v>-0.02578450275888</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -6441,10 +6441,10 @@
         <v>1415</v>
       </c>
       <c r="F263">
-        <v>-3.55693547384834</v>
+        <v>-3.556935473849069</v>
       </c>
       <c r="G263">
-        <v>0</v>
+        <v>-7.287503933639528e-13</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -6464,10 +6464,10 @@
         <v>0</v>
       </c>
       <c r="F264">
-        <v>-2.777331564851756</v>
+        <v>-2.777331564852105</v>
       </c>
       <c r="G264">
-        <v>0</v>
+        <v>-3.486100297322992e-13</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -6487,10 +6487,10 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.88277732051883</v>
+        <v>-2.883623712836216</v>
       </c>
       <c r="G265">
-        <v>-0.02438565895318945</v>
+        <v>-0.02560140123570509</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -6510,10 +6510,10 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.982215394028987</v>
+        <v>-2.984780872604509</v>
       </c>
       <c r="G266">
-        <v>-0.04258180329186079</v>
+        <v>-0.04567420085646967</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -6533,10 +6533,10 @@
         <v>617</v>
       </c>
       <c r="F267">
-        <v>-3.07534771981153</v>
+        <v>-3.079188729776575</v>
       </c>
       <c r="G267">
-        <v>-0.05515668791596151</v>
+        <v>-0.05899769788100717</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -6556,10 +6556,10 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.161598411330683</v>
+        <v>-3.166588136695935</v>
       </c>
       <c r="G268">
-        <v>-0.05976825743771474</v>
+        <v>-0.06570635805161285</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -6579,10 +6579,10 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.243194088622016</v>
+        <v>-3.249308346790897</v>
       </c>
       <c r="G269">
-        <v>-0.0609834098110571</v>
+        <v>-0.06734220799904622</v>
       </c>
     </row>
     <row r="270" spans="1:7">
@@ -6602,10 +6602,10 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.321642388029861</v>
+        <v>-3.327869221786628</v>
       </c>
       <c r="G270">
-        <v>-0.05843500147492464</v>
+        <v>-0.06481872284724788</v>
       </c>
     </row>
     <row r="271" spans="1:7">
@@ -6625,10 +6625,10 @@
         <v>1439</v>
       </c>
       <c r="F271">
-        <v>-3.395451085093607</v>
+        <v>-3.401012162470983</v>
       </c>
       <c r="G271">
-        <v>-0.05122008598462036</v>
+        <v>-0.05727091678284846</v>
       </c>
     </row>
     <row r="272" spans="1:7">
@@ -6648,10 +6648,10 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.464209229948666</v>
+        <v>-3.468238141735037</v>
       </c>
       <c r="G272">
-        <v>-0.0390600039257023</v>
+        <v>-0.04341253589937355</v>
       </c>
     </row>
     <row r="273" spans="1:7">
@@ -6671,10 +6671,10 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.528467235584596</v>
+        <v>-3.531263580488339</v>
       </c>
       <c r="G273">
-        <v>-0.02215783843354158</v>
+        <v>-0.0253536145051475</v>
       </c>
     </row>
     <row r="274" spans="1:7">
@@ -6694,10 +6694,10 @@
         <v>2057</v>
       </c>
       <c r="F274">
-        <v>-3.58699432613072</v>
+        <v>-3.586994326131439</v>
       </c>
       <c r="G274">
-        <v>0</v>
+        <v>-7.189804307472514e-13</v>
       </c>
     </row>
     <row r="275" spans="1:7">
@@ -6717,10 +6717,10 @@
         <v>0</v>
       </c>
       <c r="F275">
-        <v>-2.795675378543732</v>
+        <v>-2.795675378544225</v>
       </c>
       <c r="G275">
-        <v>0</v>
+        <v>-4.929390229335695e-13</v>
       </c>
     </row>
     <row r="276" spans="1:7">
@@ -6740,10 +6740,10 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.901443699658546</v>
+        <v>-2.902589304494746</v>
       </c>
       <c r="G276">
-        <v>-0.02410492755691784</v>
+        <v>-0.02566854828954579</v>
       </c>
     </row>
     <row r="277" spans="1:7">
@@ -6763,10 +6763,10 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.001416184821707</v>
+        <v>-3.003366860659705</v>
       </c>
       <c r="G277">
-        <v>-0.04228245081358217</v>
+        <v>-0.04491665204596718</v>
       </c>
     </row>
     <row r="278" spans="1:7">
@@ -6786,10 +6786,10 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.094833691468409</v>
+        <v>-3.098039836068727</v>
       </c>
       <c r="G278">
-        <v>-0.05464948411930903</v>
+        <v>-0.05806017504645355</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -6809,10 +6809,10 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.181872577828134</v>
+        <v>-3.186897355445425</v>
       </c>
       <c r="G279">
-        <v>-0.05965904936877275</v>
+        <v>-0.06538824201461524</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -6832,10 +6832,10 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.26372487840872</v>
+        <v>-3.269791337516753</v>
       </c>
       <c r="G280">
-        <v>-0.06004439110488713</v>
+        <v>-0.06675277167740656</v>
       </c>
     </row>
     <row r="281" spans="1:7">
@@ -6855,10 +6855,10 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.343020834190786</v>
+        <v>-3.348082887897847</v>
       </c>
       <c r="G281">
-        <v>-0.05779545449823376</v>
+        <v>-0.06351486964996411</v>
       </c>
     </row>
     <row r="282" spans="1:7">
@@ -6878,10 +6878,10 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.417413941893833</v>
+        <v>-3.42213210848631</v>
       </c>
       <c r="G282">
-        <v>-0.05089489200008046</v>
+        <v>-0.0560346378298906</v>
       </c>
     </row>
     <row r="283" spans="1:7">
@@ -6901,10 +6901,10 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.486686237316042</v>
+        <v>-3.490413545904524</v>
       </c>
       <c r="G283">
-        <v>-0.03853052012238201</v>
+        <v>-0.04278662283956813</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -6924,10 +6924,10 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.551564040973521</v>
+        <v>-3.553789523861628</v>
       </c>
       <c r="G284">
-        <v>-0.02225548276206646</v>
+        <v>-0.02463314838813591</v>
       </c>
     </row>
     <row r="285" spans="1:7">
@@ -6947,10 +6947,10 @@
         <v>2869</v>
       </c>
       <c r="F285">
-        <v>-3.610685827882029</v>
+        <v>-3.610685827881414</v>
       </c>
       <c r="G285">
-        <v>0</v>
+        <v>6.146194664324867e-13</v>
       </c>
     </row>
     <row r="286" spans="1:7">
@@ -6970,10 +6970,10 @@
         <v>0</v>
       </c>
       <c r="F286">
-        <v>-2.810502834326656</v>
+        <v>-2.810502834325307</v>
       </c>
       <c r="G286">
-        <v>0</v>
+        <v>1.34869893031464e-12</v>
       </c>
     </row>
     <row r="287" spans="1:7">
@@ -6993,10 +6993,10 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.916697896601635</v>
+        <v>-2.917768090691933</v>
       </c>
       <c r="G287">
-        <v>-0.02403030586568988</v>
+        <v>-0.02535311932536111</v>
       </c>
     </row>
     <row r="288" spans="1:7">
@@ -7016,10 +7016,10 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.01657384583281</v>
+        <v>-3.019116119926947</v>
       </c>
       <c r="G288">
-        <v>-0.04186728267844808</v>
+        <v>-0.04478901152046033</v>
       </c>
     </row>
     <row r="289" spans="1:7">
@@ -7039,10 +7039,10 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.110365763700011</v>
+        <v>-3.114091083524233</v>
       </c>
       <c r="G289">
-        <v>-0.05345523606710678</v>
+        <v>-0.05785183807782968</v>
       </c>
     </row>
     <row r="290" spans="1:7">
@@ -7062,10 +7062,10 @@
         <v>1548</v>
       </c>
       <c r="F290">
-        <v>-3.198300336004285</v>
+        <v>-3.203156986817808</v>
       </c>
       <c r="G290">
-        <v>-0.05934208910956373</v>
+        <v>-0.0650056043314895</v>
       </c>
     </row>
     <row r="291" spans="1:7">
@@ -7085,10 +7085,10 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.280198966464786</v>
+        <v>-3.285837715712817</v>
       </c>
       <c r="G291">
-        <v>-0.05990299769007379</v>
+        <v>-0.06577419618658276</v>
       </c>
     </row>
     <row r="292" spans="1:7">
@@ -7108,10 +7108,10 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.359822163206362</v>
+        <v>-3.365310023999299</v>
       </c>
       <c r="G292">
-        <v>-0.05778634558300988</v>
+        <v>-0.06333436743314813</v>
       </c>
     </row>
     <row r="293" spans="1:7">
@@ -7131,10 +7131,10 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.434533603304953</v>
+        <v>-3.438768877538672</v>
       </c>
       <c r="G293">
-        <v>-0.05040229084891523</v>
+        <v>-0.05488108393260571</v>
       </c>
     </row>
     <row r="294" spans="1:7">
@@ -7154,10 +7154,10 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.504718570703486</v>
+        <v>-3.508176783004854</v>
       </c>
       <c r="G294">
-        <v>-0.03861174703917247</v>
+        <v>-0.04237685235887212</v>
       </c>
     </row>
     <row r="295" spans="1:7">
@@ -7177,10 +7177,10 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.569824402480835</v>
+        <v>-3.572004523720261</v>
       </c>
       <c r="G295">
-        <v>-0.02183006925358355</v>
+        <v>-0.02429245603436292</v>
       </c>
     </row>
     <row r="296" spans="1:7">
@@ -7200,10 +7200,10 @@
         <v>3871</v>
       </c>
       <c r="F296">
-        <v>-3.62983586399465</v>
+        <v>-3.62983586399244</v>
       </c>
       <c r="G296">
-        <v>0</v>
+        <v>2.210676086633612e-12</v>
       </c>
     </row>
     <row r="297" spans="1:7">
@@ -7223,10 +7223,10 @@
         <v>0</v>
       </c>
       <c r="F297">
-        <v>-2.822735089673319</v>
+        <v>-2.822735089670116</v>
       </c>
       <c r="G297">
-        <v>0</v>
+        <v>3.202771381438652e-12</v>
       </c>
     </row>
     <row r="298" spans="1:7">
@@ -7246,10 +7246,10 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.929232203878962</v>
+        <v>-2.930150712318684</v>
       </c>
       <c r="G298">
-        <v>-0.02385052765782003</v>
+        <v>-0.02517428605472638</v>
       </c>
     </row>
     <row r="299" spans="1:7">
@@ -7269,10 +7269,10 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.02910818475723</v>
+        <v>-3.031598174513073</v>
       </c>
       <c r="G299">
-        <v>-0.04112516752593587</v>
+        <v>-0.0443804116584765</v>
       </c>
     </row>
     <row r="300" spans="1:7">
@@ -7292,10 +7292,10 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.123229776992641</v>
+        <v>-3.126553362108349</v>
       </c>
       <c r="G300">
-        <v>-0.05326578981867036</v>
+        <v>-0.05709426266311346</v>
       </c>
     </row>
     <row r="301" spans="1:7">
@@ -7315,10 +7315,10 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.211719724177081</v>
+        <v>-3.215298596544145</v>
       </c>
       <c r="G301">
-        <v>-0.0593133207041987</v>
+        <v>-0.06343626811340775</v>
       </c>
     </row>
     <row r="302" spans="1:7">
@@ -7338,10 +7338,10 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.294469968025844</v>
+        <v>-3.299044224190915</v>
       </c>
       <c r="G302">
-        <v>-0.06023859692640099</v>
+        <v>-0.06494055916953889</v>
       </c>
     </row>
     <row r="303" spans="1:7">
@@ -7361,10 +7361,10 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.374121614949914</v>
+        <v>-3.378130103095616</v>
       </c>
       <c r="G303">
-        <v>-0.0574623048464058</v>
+        <v>-0.06178510148360083</v>
       </c>
     </row>
     <row r="304" spans="1:7">
@@ -7384,10 +7384,10 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.4494885664904</v>
+        <v>-3.453074962658991</v>
       </c>
       <c r="G304">
-        <v>-0.05013096774184156</v>
+        <v>-0.05432673206147376</v>
       </c>
     </row>
     <row r="305" spans="1:7">
@@ -7407,10 +7407,10 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.519557576645006</v>
+        <v>-3.522803052106447</v>
       </c>
       <c r="G305">
-        <v>-0.03844270850177123</v>
+        <v>-0.04181348491829107</v>
       </c>
     </row>
     <row r="306" spans="1:7">
@@ -7430,10 +7430,10 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.585195908341226</v>
+        <v>-3.587216767754723</v>
       </c>
       <c r="G306">
-        <v>-0.02180273327331667</v>
+        <v>-0.02398586397592811</v>
       </c>
     </row>
     <row r="307" spans="1:7">
@@ -7453,10 +7453,10 @@
         <v>5083</v>
       </c>
       <c r="F307">
-        <v>-3.645634132764297</v>
+        <v>-3.645634132762194</v>
       </c>
       <c r="G307">
-        <v>0</v>
+        <v>2.102762408640046e-12</v>
       </c>
     </row>
     <row r="308" spans="1:7">
@@ -7476,10 +7476,10 @@
         <v>0</v>
       </c>
       <c r="F308">
-        <v>-2.832997797461241</v>
+        <v>-2.832997797458318</v>
       </c>
       <c r="G308">
-        <v>0</v>
+        <v>2.922551090023262e-12</v>
       </c>
     </row>
     <row r="309" spans="1:7">
@@ -7499,10 +7499,10 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.939221781027594</v>
+        <v>-2.940407304814413</v>
       </c>
       <c r="G309">
-        <v>-0.02354941484064899</v>
+        <v>-0.02488370567813858</v>
       </c>
     </row>
     <row r="310" spans="1:7">
@@ -7522,10 +7522,10 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.039818930885545</v>
+        <v>-3.042350921711773</v>
       </c>
       <c r="G310">
-        <v>-0.04140220600042799</v>
+        <v>-0.04417494758501173</v>
       </c>
     </row>
     <row r="311" spans="1:7">
@@ -7545,10 +7545,10 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.134475255962764</v>
+        <v>-3.137321672576231</v>
       </c>
       <c r="G311">
-        <v>-0.05335442644850641</v>
+        <v>-0.05661989677443646</v>
       </c>
     </row>
     <row r="312" spans="1:7">
@@ -7568,10 +7568,10 @@
         <v>2610</v>
       </c>
       <c r="F312">
-        <v>-3.223143517040259</v>
+        <v>-3.226816097970815</v>
       </c>
       <c r="G312">
-        <v>-0.05949952362912359</v>
+        <v>-0.06346194717853337</v>
       </c>
     </row>
     <row r="313" spans="1:7">
@@ -7591,10 +7591,10 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.306134144065003</v>
+        <v>-3.310122949175367</v>
       </c>
       <c r="G313">
-        <v>-0.0599024636677512</v>
+        <v>-0.06424299670805111</v>
       </c>
     </row>
     <row r="314" spans="1:7">
@@ -7614,10 +7614,10 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.386046159755509</v>
+        <v>-3.389892753147253</v>
       </c>
       <c r="G314">
-        <v>-0.05724085631689713</v>
+        <v>-0.06136042568945133</v>
       </c>
     </row>
     <row r="315" spans="1:7">
@@ -7637,10 +7637,10 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.461515714368445</v>
+        <v>-3.465248842862806</v>
       </c>
       <c r="G315">
-        <v>-0.05019521705996333</v>
+        <v>-0.05419071372997042</v>
       </c>
     </row>
     <row r="316" spans="1:7">
@@ -7660,10 +7660,10 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.53209113324048</v>
+        <v>-3.534998676077985</v>
       </c>
       <c r="G316">
-        <v>-0.03838062911715767</v>
+        <v>-0.04128817195466283</v>
       </c>
     </row>
     <row r="317" spans="1:7">
@@ -7683,10 +7683,10 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.598056752731856</v>
+        <v>-3.599857296428731</v>
       </c>
       <c r="G317">
-        <v>-0.02166924374122592</v>
+        <v>-0.02362099063037559</v>
       </c>
     </row>
     <row r="318" spans="1:7">
@@ -7706,10 +7706,10 @@
         <v>6525</v>
       </c>
       <c r="F318">
-        <v>-3.658888680788842</v>
+        <v>-3.658888680789056</v>
       </c>
       <c r="G318">
-        <v>0</v>
+        <v>-2.140509991477302e-13</v>
       </c>
     </row>
     <row r="319" spans="1:7">
@@ -7729,10 +7729,10 @@
         <v>0</v>
       </c>
       <c r="F319">
-        <v>-2.8417306772002</v>
+        <v>-2.841730677199684</v>
       </c>
       <c r="G319">
-        <v>0</v>
+        <v>5.155875726359227e-13</v>
       </c>
     </row>
     <row r="320" spans="1:7">
@@ -7752,10 +7752,10 @@
         <v>821</v>
       </c>
       <c r="F320">
-        <v>-2.948047977829589</v>
+        <v>-2.948923751228304</v>
       </c>
       <c r="G320">
-        <v>-0.02342755294048926</v>
+        <v>-0.02441997394645989</v>
       </c>
     </row>
     <row r="321" spans="1:7">
@@ -7775,10 +7775,10 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.048629946401157</v>
+        <v>-3.050794219996431</v>
       </c>
       <c r="G321">
-        <v>-0.04105382393232659</v>
+        <v>-0.04341652277900776</v>
       </c>
     </row>
     <row r="322" spans="1:7">
@@ -7798,10 +7798,10 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.14364356956247</v>
+        <v>-3.14616572135518</v>
       </c>
       <c r="G322">
-        <v>-0.05322942723368751</v>
+        <v>-0.05591410420217802</v>
       </c>
     </row>
     <row r="323" spans="1:7">
@@ -7821,10 +7821,10 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.232551248063721</v>
+        <v>-3.235845882406449</v>
       </c>
       <c r="G323">
-        <v>-0.05939024509142476</v>
+        <v>-0.0628211651718027</v>
       </c>
     </row>
     <row r="324" spans="1:7">
@@ -7844,10 +7844,10 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.316158077987718</v>
+        <v>-3.320001931522911</v>
       </c>
       <c r="G324">
-        <v>-0.05969937581233586</v>
+        <v>-0.0641032943526858</v>
       </c>
     </row>
     <row r="325" spans="1:7">
@@ -7867,10 +7867,10 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.396505072566357</v>
+        <v>-3.399906986430935</v>
       </c>
       <c r="G325">
-        <v>-0.0573351088484626</v>
+        <v>-0.06113442932512947</v>
       </c>
     </row>
     <row r="326" spans="1:7">
@@ -7890,10 +7890,10 @@
         <v>5751</v>
       </c>
       <c r="F326">
-        <v>-3.47172504092641</v>
+        <v>-3.475158652570573</v>
       </c>
       <c r="G326">
-        <v>-0.05002948046087663</v>
+        <v>-0.05361299538312403</v>
       </c>
     </row>
     <row r="327" spans="1:7">
@@ -7913,10 +7913,10 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.542779945524092</v>
+        <v>-3.545233521043671</v>
       </c>
       <c r="G327">
-        <v>-0.03818398641740572</v>
+        <v>-0.04081394392064219</v>
       </c>
     </row>
     <row r="328" spans="1:7">
@@ -7936,10 +7936,10 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.609115289175988</v>
+        <v>-3.610671010373864</v>
       </c>
       <c r="G328">
-        <v>-0.02161330954659391</v>
+        <v>-0.02337751331525639</v>
       </c>
     </row>
     <row r="329" spans="1:7">
@@ -7959,10 +7959,10 @@
         <v>8217</v>
       </c>
       <c r="F329">
-        <v>-3.670167416994187</v>
+        <v>-3.670167416996026</v>
       </c>
       <c r="G329">
-        <v>0</v>
+        <v>-1.838973417989109e-12</v>
       </c>
     </row>
     <row r="330" spans="1:7">
@@ -7982,10 +7982,10 @@
         <v>0</v>
       </c>
       <c r="F330">
-        <v>-2.849251743704464</v>
+        <v>-2.849251743705888</v>
       </c>
       <c r="G330">
-        <v>0</v>
+        <v>-1.424194095989151e-12</v>
       </c>
     </row>
     <row r="331" spans="1:7">
@@ -8005,10 +8005,10 @@
         <v>1017</v>
       </c>
       <c r="F331">
-        <v>-2.955701044017341</v>
+        <v>-2.956700952756041</v>
       </c>
       <c r="G331">
-        <v>-0.02320088256541197</v>
+        <v>-0.02445971888893883</v>
       </c>
     </row>
     <row r="332" spans="1:7">
@@ -8028,10 +8028,10 @@
         <v>2035</v>
       </c>
       <c r="F332">
-        <v>-3.056284045690008</v>
+        <v>-3.058078837091159</v>
       </c>
       <c r="G332">
-        <v>-0.04097171940838695</v>
+        <v>-0.04276651080953853</v>
       </c>
     </row>
     <row r="333" spans="1:7">
@@ -8051,10 +8051,10 @@
         <v>3053</v>
       </c>
       <c r="F333">
-        <v>-3.151668405989521</v>
+        <v>-3.153818088210635</v>
       </c>
       <c r="G333">
-        <v>-0.05301066041208702</v>
+        <v>-0.05543466951449516</v>
       </c>
     </row>
     <row r="334" spans="1:7">
@@ -8074,10 +8074,10 @@
         <v>4071</v>
       </c>
       <c r="F334">
-        <v>-3.241011505640004</v>
+        <v>-3.243538607131324</v>
       </c>
       <c r="G334">
-        <v>-0.05933993847991159</v>
+        <v>-0.06208409602066611</v>
       </c>
     </row>
     <row r="335" spans="1:7">
@@ -8097,10 +8097,10 @@
         <v>5089</v>
       </c>
       <c r="F335">
-        <v>-3.324830828034152</v>
+        <v>-3.327963624302047</v>
       </c>
       <c r="G335">
-        <v>-0.05988781128979959</v>
+        <v>-0.06343802077687055</v>
       </c>
     </row>
     <row r="336" spans="1:7">
@@ -8120,10 +8120,10 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.40488588943183</v>
+        <v>-3.408008386408828</v>
       </c>
       <c r="G336">
-        <v>-0.05704993979205852</v>
+        <v>-0.06041169046913186</v>
       </c>
     </row>
     <row r="337" spans="1:7">
@@ -8143,10 +8143,10 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.481005533010834</v>
+        <v>-3.483774545765198</v>
       </c>
       <c r="G337">
-        <v>-0.05009617315676917</v>
+        <v>-0.0531067574109837</v>
       </c>
     </row>
     <row r="338" spans="1:7">
@@ -8166,10 +8166,10 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.55204219625536</v>
+        <v>-3.554353605204013</v>
       </c>
       <c r="G338">
-        <v>-0.03816435775097549</v>
+        <v>-0.04061472443527936</v>
       </c>
     </row>
     <row r="339" spans="1:7">
@@ -8189,10 +8189,10 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.6184838224893</v>
+        <v>-3.619794823208812</v>
       </c>
       <c r="G339">
-        <v>-0.0216601668275595</v>
+        <v>-0.02298485002555933</v>
       </c>
     </row>
     <row r="340" spans="1:7">
@@ -8212,10 +8212,10 @@
         <v>10179</v>
       </c>
       <c r="F340">
-        <v>-3.679881065597771</v>
+        <v>-3.679881065597996</v>
       </c>
       <c r="G340">
-        <v>0</v>
+        <v>-2.251532293939817e-13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tools to save and restart population instance - also added xyz to Chromo function
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -967,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="F25">
-        <v>-2.510619128483644</v>
+        <v>-2.510674767910714</v>
       </c>
       <c r="G25">
         <v>-0.0394281961407692</v>
@@ -1105,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="F31">
-        <v>-2.598833969446377</v>
+        <v>-2.598915967272181</v>
       </c>
       <c r="G31">
         <v>-0.0526307116085365</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.613138687596258</v>
+        <v>-2.614225430984661</v>
       </c>
       <c r="G32">
         <v>-0.05443337550925675</v>
@@ -1197,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.653950584619783</v>
+        <v>-2.655652815585636</v>
       </c>
       <c r="G35">
         <v>-0.05773910978529906</v>
@@ -1220,7 +1220,7 @@
         <v>20</v>
       </c>
       <c r="F36">
-        <v>-2.669002863219898</v>
+        <v>-2.669520892040688</v>
       </c>
       <c r="G36">
         <v>-0.06028933413625248</v>
@@ -1243,7 +1243,7 @@
         <v>21</v>
       </c>
       <c r="F37">
-        <v>-2.683249197154117</v>
+        <v>-2.684853324023879</v>
       </c>
       <c r="G37">
         <v>-0.06203361382131134</v>
@@ -1266,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="F38">
-        <v>-2.694493225735216</v>
+        <v>-2.697197167713321</v>
       </c>
       <c r="G38">
         <v>-0.06077558815324902</v>
@@ -1312,7 +1312,7 @@
         <v>24</v>
       </c>
       <c r="F40">
-        <v>-2.722128270175237</v>
+        <v>-2.722328439222692</v>
       </c>
       <c r="G40">
         <v>-0.06340652409494751</v>
@@ -1358,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.747363109888908</v>
+        <v>-2.747564798584898</v>
       </c>
       <c r="G42">
         <v>-0.06363725531029729</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.758883633066294</v>
+        <v>-2.761550640180884</v>
       </c>
       <c r="G43">
         <v>-0.06265572423852195</v>
@@ -1404,7 +1404,7 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <v>-2.774019239367364</v>
+        <v>-2.774419984082233</v>
       </c>
       <c r="G44">
         <v>-0.06528927629043091</v>
@@ -1427,7 +1427,7 @@
         <v>29</v>
       </c>
       <c r="F45">
-        <v>-2.784287451853277</v>
+        <v>-2.786938066485461</v>
       </c>
       <c r="G45">
         <v>-0.06305543452718299</v>
@@ -1473,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="F47">
-        <v>-2.810294422838588</v>
+        <v>-2.810485880851243</v>
       </c>
       <c r="G47">
         <v>-0.06405829701417254</v>
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.821803828216897</v>
+        <v>-2.822255432247109</v>
       </c>
       <c r="G48">
         <v>-0.06306564814332039</v>
@@ -1542,7 +1542,7 @@
         <v>34</v>
       </c>
       <c r="F50">
-        <v>-2.844859183468374</v>
+        <v>-2.846520782120486</v>
       </c>
       <c r="G50">
         <v>-0.06111689489647565</v>
@@ -1588,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.865582547235674</v>
+        <v>-2.867142630027837</v>
       </c>
       <c r="G52">
         <v>-0.05683615016545374</v>
@@ -1657,7 +1657,7 @@
         <v>39</v>
       </c>
       <c r="F55">
-        <v>-2.898804332361363</v>
+        <v>-2.899528362103601</v>
       </c>
       <c r="G55">
         <v>-0.05255177254366028</v>
@@ -1680,7 +1680,7 @@
         <v>40</v>
       </c>
       <c r="F56">
-        <v>-2.910902836012063</v>
+        <v>-2.911880314766472</v>
       </c>
       <c r="G56">
         <v>-0.0521482219451993</v>
@@ -1703,7 +1703,7 @@
         <v>41</v>
       </c>
       <c r="F57">
-        <v>-2.920921851951215</v>
+        <v>-2.922516177360457</v>
       </c>
       <c r="G57">
         <v>-0.04966518363519057</v>
@@ -1749,7 +1749,7 @@
         <v>43</v>
       </c>
       <c r="F59">
-        <v>-2.939732790935115</v>
+        <v>-2.942355251643368</v>
       </c>
       <c r="G59">
         <v>-0.04347201412076784</v>
@@ -1772,7 +1772,7 @@
         <v>44</v>
       </c>
       <c r="F60">
-        <v>-2.951314934013007</v>
+        <v>-2.951418869983091</v>
       </c>
       <c r="G60">
         <v>-0.04255210294949902</v>
@@ -1795,7 +1795,7 @@
         <v>45</v>
       </c>
       <c r="F61">
-        <v>-2.959472181713357</v>
+        <v>-2.961806950792357</v>
       </c>
       <c r="G61">
         <v>-0.03820729640068848</v>
@@ -1818,7 +1818,7 @@
         <v>46</v>
       </c>
       <c r="F62">
-        <v>-2.970036936192295</v>
+        <v>-2.97076663316199</v>
       </c>
       <c r="G62">
         <v>-0.03626999663046548</v>
@@ -2140,7 +2140,7 @@
         <v>4</v>
       </c>
       <c r="F76">
-        <v>-2.55658829208103</v>
+        <v>-2.556861307954046</v>
       </c>
       <c r="G76">
         <v>-0.009360433829400439</v>
@@ -2186,7 +2186,7 @@
         <v>6</v>
       </c>
       <c r="F78">
-        <v>-2.570446547806509</v>
+        <v>-2.570693012148761</v>
       </c>
       <c r="G78">
         <v>-0.01319505159429335</v>
@@ -2209,7 +2209,7 @@
         <v>7</v>
       </c>
       <c r="F79">
-        <v>-2.577089384030851</v>
+        <v>-2.577241016596144</v>
       </c>
       <c r="G79">
         <v>-0.01482606883834148</v>
@@ -2232,7 +2232,7 @@
         <v>8</v>
       </c>
       <c r="F80">
-        <v>-2.584008933855023</v>
+        <v>-2.584337919285817</v>
       </c>
       <c r="G80">
         <v>-0.01673379968222033</v>
@@ -2301,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="F83">
-        <v>-2.603101429675862</v>
+        <v>-2.603586702216664</v>
       </c>
       <c r="G83">
         <v>-0.02079083856217956</v>
@@ -2393,7 +2393,7 @@
         <v>15</v>
       </c>
       <c r="F87">
-        <v>-2.630132587503912</v>
+        <v>-2.630256238791675</v>
       </c>
       <c r="G87">
         <v>-0.02777472046905638</v>
@@ -2439,7 +2439,7 @@
         <v>17</v>
       </c>
       <c r="F89">
-        <v>-2.642477829025828</v>
+        <v>-2.643868368001036</v>
       </c>
       <c r="G89">
         <v>-0.03009632403038554</v>
@@ -2462,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="F90">
-        <v>-2.648787341112458</v>
+        <v>-2.649805497745682</v>
       </c>
       <c r="G90">
         <v>-0.03139401713672241</v>
@@ -2508,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.660921109052133</v>
+        <v>-2.661403515032001</v>
       </c>
       <c r="G92">
         <v>-0.0335041471158104</v>
@@ -2554,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="F94">
-        <v>-2.67331428252893</v>
+        <v>-2.673336999509699</v>
       </c>
       <c r="G94">
         <v>-0.03587368263202073</v>
@@ -2577,7 +2577,7 @@
         <v>23</v>
       </c>
       <c r="F95">
-        <v>-2.67997798810731</v>
+        <v>-2.680889056154785</v>
       </c>
       <c r="G95">
         <v>-0.03752556923010752</v>
@@ -2600,7 +2600,7 @@
         <v>24</v>
       </c>
       <c r="F96">
-        <v>-2.685016028083973</v>
+        <v>-2.686484124785737</v>
       </c>
       <c r="G96">
         <v>-0.03755179022647681</v>
@@ -2623,7 +2623,7 @@
         <v>25</v>
       </c>
       <c r="F97">
-        <v>-2.691823863905655</v>
+        <v>-2.693756599497035</v>
       </c>
       <c r="G97">
         <v>-0.03934780706786567</v>
@@ -2646,7 +2646,7 @@
         <v>26</v>
       </c>
       <c r="F98">
-        <v>-2.698560453394495</v>
+        <v>-2.6988436090532</v>
       </c>
       <c r="G98">
         <v>-0.04107257757641181</v>
@@ -2669,7 +2669,7 @@
         <v>27</v>
       </c>
       <c r="F99">
-        <v>-2.704267371005806</v>
+        <v>-2.705729345165447</v>
       </c>
       <c r="G99">
         <v>-0.04176767620742927</v>
@@ -2692,7 +2692,7 @@
         <v>28</v>
       </c>
       <c r="F100">
-        <v>-2.710825702497996</v>
+        <v>-2.711446074175362</v>
       </c>
       <c r="G100">
         <v>-0.04331418871932691</v>
@@ -2715,7 +2715,7 @@
         <v>29</v>
       </c>
       <c r="F101">
-        <v>-2.71682066018195</v>
+        <v>-2.718257034338622</v>
       </c>
       <c r="G101">
         <v>-0.0442973274229872</v>
@@ -2738,7 +2738,7 @@
         <v>30</v>
       </c>
       <c r="F102">
-        <v>-2.722207010508159</v>
+        <v>-2.723178040276345</v>
       </c>
       <c r="G102">
         <v>-0.04467185876890278</v>
@@ -2761,7 +2761,7 @@
         <v>31</v>
       </c>
       <c r="F103">
-        <v>-2.728385957994885</v>
+        <v>-2.728665632831155</v>
       </c>
       <c r="G103">
         <v>-0.04583898727533553</v>
@@ -2830,7 +2830,7 @@
         <v>34</v>
       </c>
       <c r="F106">
-        <v>-2.747956031091275</v>
+        <v>-2.748110608015103</v>
       </c>
       <c r="G106">
         <v>-0.05037360343084574</v>
@@ -2853,7 +2853,7 @@
         <v>35</v>
       </c>
       <c r="F107">
-        <v>-2.752216965129325</v>
+        <v>-2.753040525849177</v>
       </c>
       <c r="G107">
         <v>-0.04962271848860245</v>
@@ -2899,7 +2899,7 @@
         <v>37</v>
       </c>
       <c r="F109">
-        <v>-2.764290973934087</v>
+        <v>-2.764356187341415</v>
       </c>
       <c r="G109">
         <v>-0.05167308933277748</v>
@@ -3014,7 +3014,7 @@
         <v>42</v>
       </c>
       <c r="F114">
-        <v>-2.792910574129658</v>
+        <v>-2.793585720497061</v>
       </c>
       <c r="G114">
         <v>-0.05523359462688138</v>
@@ -3060,7 +3060,7 @@
         <v>44</v>
       </c>
       <c r="F116">
-        <v>-2.80228001301945</v>
+        <v>-2.803909549011701</v>
       </c>
       <c r="G116">
         <v>-0.05457939555608693</v>
@@ -3129,7 +3129,7 @@
         <v>47</v>
       </c>
       <c r="F119">
-        <v>-2.820995416089896</v>
+        <v>-2.821901924650995</v>
       </c>
       <c r="G119">
         <v>-0.05825934168565339</v>
@@ -3152,7 +3152,7 @@
         <v>48</v>
       </c>
       <c r="F120">
-        <v>-2.826867593709021</v>
+        <v>-2.827347095653737</v>
       </c>
       <c r="G120">
         <v>-0.0591197003244841</v>
@@ -3221,7 +3221,7 @@
         <v>51</v>
       </c>
       <c r="F123">
-        <v>-2.843896086242533</v>
+        <v>-2.844845117088864</v>
       </c>
       <c r="G123">
         <v>-0.06111273591711663</v>
@@ -3267,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.854854374240741</v>
+        <v>-2.855698845588972</v>
       </c>
       <c r="G125">
         <v>-0.06204738595473791</v>
@@ -3290,7 +3290,7 @@
         <v>54</v>
       </c>
       <c r="F126">
-        <v>-2.85877391362527</v>
+        <v>-2.860669583370912</v>
       </c>
       <c r="G126">
         <v>-0.06095510635897328</v>
@@ -3359,7 +3359,7 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.876316768237813</v>
+        <v>-2.876998822342203</v>
       </c>
       <c r="G129">
         <v>-0.06346250403063602</v>
@@ -3382,7 +3382,7 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.880750425093523</v>
+        <v>-2.881471769781636</v>
       </c>
       <c r="G130">
         <v>-0.06288434190605274</v>
@@ -3405,7 +3405,7 @@
         <v>59</v>
       </c>
       <c r="F131">
-        <v>-2.885727239966789</v>
+        <v>-2.889732856557247</v>
       </c>
       <c r="G131">
         <v>-0.06284933779902624</v>
@@ -3451,7 +3451,7 @@
         <v>61</v>
       </c>
       <c r="F133">
-        <v>-2.896937220151821</v>
+        <v>-2.897284011026469</v>
       </c>
       <c r="G133">
         <v>-0.06403568002347071</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.902502460634975</v>
+        <v>-2.903265201702387</v>
       </c>
       <c r="G134">
         <v>-0.06458910152633202</v>
@@ -3497,7 +3497,7 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.908689990128642</v>
+        <v>-2.909551665997399</v>
       </c>
       <c r="G135">
         <v>-0.06576481203970608</v>
@@ -3566,7 +3566,7 @@
         <v>66</v>
       </c>
       <c r="F138">
-        <v>-2.922411691118897</v>
+        <v>-2.924340960933909</v>
       </c>
       <c r="G138">
         <v>-0.06445105608908031</v>
@@ -3589,7 +3589,7 @@
         <v>67</v>
       </c>
       <c r="F139">
-        <v>-2.929005421487068</v>
+        <v>-2.929073024893842</v>
       </c>
       <c r="G139">
         <v>-0.06603296747695842</v>
@@ -3612,7 +3612,7 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.935901568346875</v>
+        <v>-2.936312301870653</v>
       </c>
       <c r="G140">
         <v>-0.06791729535647217</v>
@@ -3727,7 +3727,7 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.960524556538067</v>
+        <v>-2.961327082531045</v>
       </c>
       <c r="G145">
         <v>-0.06748118864619723</v>
@@ -3750,7 +3750,7 @@
         <v>74</v>
       </c>
       <c r="F146">
-        <v>-2.964460550580648</v>
+        <v>-2.966895421125398</v>
       </c>
       <c r="G146">
         <v>-0.06640536370848471</v>
@@ -3773,7 +3773,7 @@
         <v>75</v>
       </c>
       <c r="F147">
-        <v>-2.966466238585252</v>
+        <v>-2.971500992812409</v>
       </c>
       <c r="G147">
         <v>-0.06339923273279569</v>
@@ -3819,7 +3819,7 @@
         <v>77</v>
       </c>
       <c r="F149">
-        <v>-2.980597831757254</v>
+        <v>-2.980865937145079</v>
       </c>
       <c r="G149">
         <v>-0.06750718794421084</v>
@@ -3842,7 +3842,7 @@
         <v>78</v>
       </c>
       <c r="F150">
-        <v>-2.985380094830802</v>
+        <v>-2.987824243905864</v>
       </c>
       <c r="G150">
         <v>-0.06727763203746573</v>
@@ -3865,7 +3865,7 @@
         <v>79</v>
       </c>
       <c r="F151">
-        <v>-2.987676672715433</v>
+        <v>-2.98924785916482</v>
       </c>
       <c r="G151">
         <v>-0.06456239094180272</v>
@@ -3911,7 +3911,7 @@
         <v>81</v>
       </c>
       <c r="F153">
-        <v>-2.997925337577441</v>
+        <v>-2.999941932857733</v>
       </c>
       <c r="G153">
         <v>-0.06478741784322395</v>
@@ -3934,7 +3934,7 @@
         <v>82</v>
       </c>
       <c r="F154">
-        <v>-3.004719453832646</v>
+        <v>-3.005368551263645</v>
       </c>
       <c r="G154">
         <v>-0.0665697151181357</v>
@@ -3957,7 +3957,7 @@
         <v>83</v>
       </c>
       <c r="F155">
-        <v>-3.009934275880199</v>
+        <v>-3.013048408361136</v>
       </c>
       <c r="G155">
         <v>-0.0667727181853961</v>
@@ -3980,7 +3980,7 @@
         <v>84</v>
       </c>
       <c r="F156">
-        <v>-3.014200406633095</v>
+        <v>-3.014214275188162</v>
       </c>
       <c r="G156">
         <v>-0.06602702995799836</v>
@@ -4026,7 +4026,7 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.023778383444115</v>
+        <v>-3.025551867870405</v>
       </c>
       <c r="G158">
         <v>-0.06558136880843191</v>
@@ -4072,7 +4072,7 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.033822331398909</v>
+        <v>-3.03418860758944</v>
       </c>
       <c r="G160">
         <v>-0.06560167880263923</v>
@@ -4118,7 +4118,7 @@
         <v>90</v>
       </c>
       <c r="F162">
-        <v>-3.042358212216969</v>
+        <v>-3.042765124386503</v>
       </c>
       <c r="G162">
         <v>-0.06411392166011232</v>
@@ -4187,7 +4187,7 @@
         <v>93</v>
       </c>
       <c r="F165">
-        <v>-3.056034511921426</v>
+        <v>-3.058015604924448</v>
       </c>
       <c r="G165">
         <v>-0.06275476442368888</v>
@@ -4210,7 +4210,7 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.062104677424069</v>
+        <v>-3.063350357814993</v>
       </c>
       <c r="G166">
         <v>-0.06381311094603859</v>
@@ -4256,7 +4256,7 @@
         <v>96</v>
       </c>
       <c r="F168">
-        <v>-3.070393536808382</v>
+        <v>-3.072189571423429</v>
       </c>
       <c r="G168">
         <v>-0.06207833236976512</v>
@@ -4279,7 +4279,7 @@
         <v>97</v>
       </c>
       <c r="F169">
-        <v>-3.073694227466299</v>
+        <v>-3.074709028456249</v>
       </c>
       <c r="G169">
         <v>-0.06036720404738916</v>
@@ -4394,7 +4394,7 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.095696542563779</v>
+        <v>-3.096109639010141</v>
       </c>
       <c r="G174">
         <v>-0.05731042424340216</v>
@@ -4463,7 +4463,7 @@
         <v>105</v>
       </c>
       <c r="F177">
-        <v>-3.109079491314813</v>
+        <v>-3.109238216318147</v>
       </c>
       <c r="G177">
         <v>-0.05565791605355563</v>
@@ -4578,7 +4578,7 @@
         <v>110</v>
       </c>
       <c r="F182">
-        <v>-3.130518399658781</v>
+        <v>-3.130769858361425</v>
       </c>
       <c r="G182">
         <v>-0.05203772949605678</v>
@@ -4601,7 +4601,7 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.134782904058981</v>
+        <v>-3.136277172608858</v>
       </c>
       <c r="G183">
         <v>-0.05129041491596353</v>
@@ -4647,7 +4647,7 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.141966245646907</v>
+        <v>-3.143883992381014</v>
       </c>
       <c r="G185">
         <v>-0.04845011854330328</v>
@@ -4670,7 +4670,7 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.147779738725947</v>
+        <v>-3.148915907549484</v>
       </c>
       <c r="G186">
         <v>-0.04925179264205015</v>
@@ -4693,7 +4693,7 @@
         <v>115</v>
       </c>
       <c r="F187">
-        <v>-3.150898939419395</v>
+        <v>-3.151165440095393</v>
       </c>
       <c r="G187">
         <v>-0.04735917435520443</v>
@@ -4739,7 +4739,7 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.159550649159591</v>
+        <v>-3.160028332170772</v>
       </c>
       <c r="G189">
         <v>-0.04598724613481375</v>
@@ -4762,7 +4762,7 @@
         <v>118</v>
       </c>
       <c r="F190">
-        <v>-3.163724832661905</v>
+        <v>-3.164574729539761</v>
       </c>
       <c r="G190">
         <v>-0.0451496106568342</v>
@@ -4785,7 +4785,7 @@
         <v>119</v>
       </c>
       <c r="F191">
-        <v>-3.168246459210928</v>
+        <v>-3.168479353982149</v>
       </c>
       <c r="G191">
         <v>-0.0446594182255643</v>
@@ -4854,7 +4854,7 @@
         <v>122</v>
       </c>
       <c r="F194">
-        <v>-3.177434961695387</v>
+        <v>-3.17909070356288</v>
       </c>
       <c r="G194">
         <v>-0.03881246376914294</v>
@@ -4969,7 +4969,7 @@
         <v>127</v>
       </c>
       <c r="F199">
-        <v>-3.198319782422274</v>
+        <v>-3.199543714371964</v>
       </c>
       <c r="G199">
         <v>-0.03463818959456333</v>
@@ -5038,7 +5038,7 @@
         <v>130</v>
       </c>
       <c r="F202">
-        <v>-3.209080613784895</v>
+        <v>-3.209937699206235</v>
       </c>
       <c r="G202">
         <v>-0.03036356401630436</v>
@@ -5061,7 +5061,7 @@
         <v>131</v>
       </c>
       <c r="F203">
-        <v>-3.214049241656778</v>
+        <v>-3.215318522628437</v>
       </c>
       <c r="G203">
         <v>-0.03032037290789391</v>
@@ -5084,7 +5084,7 @@
         <v>132</v>
       </c>
       <c r="F204">
-        <v>-3.216143145267341</v>
+        <v>-3.21669829979673</v>
       </c>
       <c r="G204">
         <v>-0.02740245753816334</v>
@@ -5130,7 +5130,7 @@
         <v>134</v>
       </c>
       <c r="F206">
-        <v>-3.222721375028642</v>
+        <v>-3.224483943344608</v>
       </c>
       <c r="G206">
         <v>-0.02395704933887857</v>
@@ -5153,7 +5153,7 @@
         <v>135</v>
       </c>
       <c r="F207">
-        <v>-3.226849402050685</v>
+        <v>-3.227550527467095</v>
       </c>
       <c r="G207">
         <v>-0.02307325738062735</v>
@@ -5199,7 +5199,7 @@
         <v>137</v>
       </c>
       <c r="F209">
-        <v>-3.234302410137776</v>
+        <v>-3.234809940147315</v>
       </c>
       <c r="G209">
         <v>-0.02050262750713219</v>
@@ -5245,7 +5245,7 @@
         <v>139</v>
       </c>
       <c r="F211">
-        <v>-3.240022510593126</v>
+        <v>-3.24053004060266</v>
       </c>
       <c r="G211">
         <v>-0.01619909000189521</v>
@@ -5475,7 +5475,7 @@
         <v>30</v>
       </c>
       <c r="F221">
-        <v>-2.721372130328087</v>
+        <v>-2.722883284473349</v>
       </c>
       <c r="G221">
         <v>-0.02546572494906751</v>
@@ -5498,7 +5498,7 @@
         <v>61</v>
       </c>
       <c r="F222">
-        <v>-2.817925695426455</v>
+        <v>-2.818575215466129</v>
       </c>
       <c r="G222">
         <v>-0.04534263269702832</v>
@@ -5567,7 +5567,7 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.069679093338019</v>
+        <v>-3.071801599347739</v>
       </c>
       <c r="G225">
         <v>-0.06706605855737169</v>
@@ -5590,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.144550909475877</v>
+        <v>-3.145726063804554</v>
       </c>
       <c r="G226">
         <v>-0.06526121734482282</v>
@@ -5613,7 +5613,7 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.213922992188545</v>
+        <v>-3.213980509517109</v>
       </c>
       <c r="G227">
         <v>-0.05795664270708345</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.277980858521302</v>
+        <v>-3.27801322586012</v>
       </c>
       <c r="G228">
         <v>-0.04533785168943294</v>
@@ -5659,7 +5659,7 @@
         <v>278</v>
       </c>
       <c r="F229">
-        <v>-3.334986834440572</v>
+        <v>-3.335516389978159</v>
       </c>
       <c r="G229">
         <v>-0.0256671702582969</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.786019717367762</v>
+        <v>-2.786641162844797</v>
       </c>
       <c r="G232">
         <v>-0.0260504758789617</v>
@@ -5751,7 +5751,7 @@
         <v>112</v>
       </c>
       <c r="F233">
-        <v>-2.88281455592801</v>
+        <v>-2.883619796906685</v>
       </c>
       <c r="G233">
         <v>-0.04479978674570084</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.974334596308505</v>
+        <v>-2.974608852494831</v>
       </c>
       <c r="G234">
         <v>-0.05827429943268769</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.28633820608926</v>
+        <v>-3.287421329286068</v>
       </c>
       <c r="G238">
         <v>-0.05809579843940671</v>
@@ -5889,7 +5889,7 @@
         <v>448</v>
       </c>
       <c r="F239">
-        <v>-3.351195610319622</v>
+        <v>-3.352339576189505</v>
       </c>
       <c r="G239">
         <v>-0.04490767497625925</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.107249243503461</v>
+        <v>-3.107922243180356</v>
       </c>
       <c r="G246">
         <v>-0.06625630939548288</v>
@@ -6073,7 +6073,7 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.188380491166494</v>
+        <v>-3.188642415278473</v>
       </c>
       <c r="G247">
         <v>-0.06824666094787357</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.264882577851401</v>
+        <v>-3.265190832362579</v>
       </c>
       <c r="G248">
         <v>-0.06560785152213766</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.337443151648606</v>
+        <v>-3.337453691927179</v>
       </c>
       <c r="G249">
         <v>-0.05816730207706311</v>
@@ -6280,7 +6280,7 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.053673118113357</v>
+        <v>-3.053733506929513</v>
       </c>
       <c r="G256">
         <v>-0.05903582312151201</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.301219619432476</v>
+        <v>-3.301761604138614</v>
       </c>
       <c r="G259">
         <v>-0.06543527498148838</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.373050733085449</v>
+        <v>-3.373457111455625</v>
       </c>
       <c r="G260">
         <v>-0.05726230869625171</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.439578960212611</v>
+        <v>-3.440265385995371</v>
       </c>
       <c r="G261">
         <v>-0.04321905106294766</v>
@@ -6418,7 +6418,7 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.502148491846754</v>
+        <v>-3.502404158640303</v>
       </c>
       <c r="G262">
         <v>-0.02578450275888</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.883623712836216</v>
+        <v>-2.883834134956935</v>
       </c>
       <c r="G265">
         <v>-0.02560140123570509</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.098039836068727</v>
+        <v>-3.09806165848084</v>
       </c>
       <c r="G278">
         <v>-0.05806017504645355</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.917768090691933</v>
+        <v>-2.917829764749651</v>
       </c>
       <c r="G287">
         <v>-0.02535311932536111</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.438768877538672</v>
+        <v>-3.438925453220398</v>
       </c>
       <c r="G293">
         <v>-0.05488108393260571</v>
@@ -7154,7 +7154,7 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.508176783004854</v>
+        <v>-3.508392204087163</v>
       </c>
       <c r="G294">
         <v>-0.04237685235887212</v>
@@ -7292,7 +7292,7 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.126553362108349</v>
+        <v>-3.126639482795215</v>
       </c>
       <c r="G300">
         <v>-0.05709426266311346</v>
@@ -7315,7 +7315,7 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.215298596544145</v>
+        <v>-3.215341021749714</v>
       </c>
       <c r="G301">
         <v>-0.06343626811340775</v>
@@ -7361,7 +7361,7 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.378130103095616</v>
+        <v>-3.379059655974281</v>
       </c>
       <c r="G303">
         <v>-0.06178510148360083</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.522803052106447</v>
+        <v>-3.522861606902127</v>
       </c>
       <c r="G305">
         <v>-0.04181348491829107</v>
@@ -7568,7 +7568,7 @@
         <v>2610</v>
       </c>
       <c r="F312">
-        <v>-3.226816097970815</v>
+        <v>-3.227025837417122</v>
       </c>
       <c r="G312">
         <v>-0.06346194717853337</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.389892753147253</v>
+        <v>-3.389936322130754</v>
       </c>
       <c r="G314">
         <v>-0.06136042568945133</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.465248842862806</v>
+        <v>-3.465277447682741</v>
       </c>
       <c r="G315">
         <v>-0.05419071372997042</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.534998676077985</v>
+        <v>-3.535262224065824</v>
       </c>
       <c r="G316">
         <v>-0.04128817195466283</v>
@@ -7752,7 +7752,7 @@
         <v>821</v>
       </c>
       <c r="F320">
-        <v>-2.948923751228304</v>
+        <v>-2.949253146015495</v>
       </c>
       <c r="G320">
         <v>-0.02441997394645989</v>
@@ -7775,7 +7775,7 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.050794219996431</v>
+        <v>-3.050969621063596</v>
       </c>
       <c r="G321">
         <v>-0.04341652277900776</v>
@@ -7798,7 +7798,7 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.14616572135518</v>
+        <v>-3.146426033763205</v>
       </c>
       <c r="G322">
         <v>-0.05591410420217802</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.235845882406449</v>
+        <v>-3.236036412347025</v>
       </c>
       <c r="G323">
         <v>-0.0628211651718027</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.545233521043671</v>
+        <v>-3.545417024307139</v>
       </c>
       <c r="G327">
         <v>-0.04081394392064219</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.554353605204013</v>
+        <v>-3.554464161606724</v>
       </c>
       <c r="G338">
         <v>-0.04061472443527936</v>
@@ -8189,7 +8189,7 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.619794823208812</v>
+        <v>-3.619906107633123</v>
       </c>
       <c r="G339">
         <v>-0.02298485002555933</v>

</xml_diff>

<commit_message>
updated data from v1 of c implementation (NOTE: need to check CE calcs)
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>-2.493858972800308</v>
+        <v>-2.495755947894593</v>
       </c>
       <c r="G24">
         <v>-0.03517009470659405</v>
@@ -990,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="F26">
-        <v>-2.524150472668484</v>
+        <v>-2.524925309723143</v>
       </c>
       <c r="G26">
         <v>-0.04045748607644772</v>
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.539769708625962</v>
+        <v>-2.540382347402587</v>
       </c>
       <c r="G27">
         <v>-0.0435746677847646</v>
@@ -1036,7 +1036,7 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <v>-2.554857629083865</v>
+        <v>-2.555895024509102</v>
       </c>
       <c r="G28">
         <v>-0.04616053399350739</v>
@@ -1059,7 +1059,7 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <v>-2.569904932558636</v>
+        <v>-2.569979436581178</v>
       </c>
       <c r="G29">
         <v>-0.04870578321911712</v>
@@ -1105,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="F31">
-        <v>-2.598915967272181</v>
+        <v>-2.599651729792937</v>
       </c>
       <c r="G31">
         <v>-0.0526307116085365</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.614225430984661</v>
+        <v>-2.614335921297939</v>
       </c>
       <c r="G32">
         <v>-0.05443337550925675</v>
@@ -1151,7 +1151,7 @@
         <v>17</v>
       </c>
       <c r="F33">
-        <v>-2.627856346714079</v>
+        <v>-2.628170071715121</v>
       </c>
       <c r="G33">
         <v>-0.05664898037791666</v>
@@ -1174,7 +1174,7 @@
         <v>18</v>
       </c>
       <c r="F34">
-        <v>-2.64176358061228</v>
+        <v>-2.643105066209313</v>
       </c>
       <c r="G34">
         <v>-0.0580541600269564</v>
@@ -1197,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.655652815585636</v>
+        <v>-2.656369164419501</v>
       </c>
       <c r="G35">
         <v>-0.05773910978529906</v>
@@ -1220,7 +1220,7 @@
         <v>20</v>
       </c>
       <c r="F36">
-        <v>-2.669520892040688</v>
+        <v>-2.66987011454032</v>
       </c>
       <c r="G36">
         <v>-0.06028933413625248</v>
@@ -1289,7 +1289,7 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.71015530207535</v>
+        <v>-2.711540019779271</v>
       </c>
       <c r="G39">
         <v>-0.06393561024422234</v>
@@ -1312,7 +1312,7 @@
         <v>24</v>
       </c>
       <c r="F40">
-        <v>-2.722328439222692</v>
+        <v>-2.724326756464124</v>
       </c>
       <c r="G40">
         <v>-0.06340652409494751</v>
@@ -1335,7 +1335,7 @@
         <v>25</v>
       </c>
       <c r="F41">
-        <v>-2.737295759091805</v>
+        <v>-2.737687386151913</v>
       </c>
       <c r="G41">
         <v>-0.06607195876235483</v>
@@ -1358,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.747564798584898</v>
+        <v>-2.749294258234732</v>
       </c>
       <c r="G42">
         <v>-0.06363725531029729</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.761550640180884</v>
+        <v>-2.76231188174176</v>
       </c>
       <c r="G43">
         <v>-0.06265572423852195</v>
@@ -1404,7 +1404,7 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <v>-2.774419984082233</v>
+        <v>-2.775350053409366</v>
       </c>
       <c r="G44">
         <v>-0.06528927629043091</v>
@@ -1427,7 +1427,7 @@
         <v>29</v>
       </c>
       <c r="F45">
-        <v>-2.786938066485461</v>
+        <v>-2.788729517134818</v>
       </c>
       <c r="G45">
         <v>-0.06305543452718299</v>
@@ -1450,7 +1450,7 @@
         <v>30</v>
       </c>
       <c r="F46">
-        <v>-2.797872776822711</v>
+        <v>-2.798738553081813</v>
       </c>
       <c r="G46">
         <v>-0.06413870524745602</v>
@@ -1473,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="F47">
-        <v>-2.810485880851243</v>
+        <v>-2.811585327036044</v>
       </c>
       <c r="G47">
         <v>-0.06405829701417254</v>
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.822255432247109</v>
+        <v>-2.823120060686657</v>
       </c>
       <c r="G48">
         <v>-0.06306564814332039</v>
@@ -1519,7 +1519,7 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.8355716968542</v>
+        <v>-2.835663471362181</v>
       </c>
       <c r="G49">
         <v>-0.06433146253146271</v>
@@ -1565,7 +1565,7 @@
         <v>35</v>
       </c>
       <c r="F51">
-        <v>-2.857482028848871</v>
+        <v>-2.858151952158444</v>
       </c>
       <c r="G51">
         <v>-0.06123768602781177</v>
@@ -1588,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.867142630027837</v>
+        <v>-2.868027122282964</v>
       </c>
       <c r="G52">
         <v>-0.05683615016545374</v>
@@ -1611,7 +1611,7 @@
         <v>37</v>
       </c>
       <c r="F53">
-        <v>-2.87884674053612</v>
+        <v>-2.879788971325359</v>
       </c>
       <c r="G53">
         <v>-0.0575982892167386</v>
@@ -1634,7 +1634,7 @@
         <v>38</v>
       </c>
       <c r="F54">
-        <v>-2.889316676160492</v>
+        <v>-2.890303069259688</v>
       </c>
       <c r="G54">
         <v>-0.05556617059195057</v>
@@ -1657,7 +1657,7 @@
         <v>39</v>
       </c>
       <c r="F55">
-        <v>-2.899528362103601</v>
+        <v>-2.901091692013082</v>
       </c>
       <c r="G55">
         <v>-0.05255177254366028</v>
@@ -1703,7 +1703,7 @@
         <v>41</v>
       </c>
       <c r="F57">
-        <v>-2.922516177360457</v>
+        <v>-2.922606946520343</v>
       </c>
       <c r="G57">
         <v>-0.04966518363519057</v>
@@ -1726,7 +1726,7 @@
         <v>42</v>
       </c>
       <c r="F58">
-        <v>-2.931077214122262</v>
+        <v>-2.932400261829762</v>
       </c>
       <c r="G58">
         <v>-0.04731849155707635</v>
@@ -1749,7 +1749,7 @@
         <v>43</v>
       </c>
       <c r="F59">
-        <v>-2.942355251643368</v>
+        <v>-2.943045038768522</v>
       </c>
       <c r="G59">
         <v>-0.04347201412076784</v>
@@ -1772,7 +1772,7 @@
         <v>44</v>
       </c>
       <c r="F60">
-        <v>-2.951418869983091</v>
+        <v>-2.952991114237355</v>
       </c>
       <c r="G60">
         <v>-0.04255210294949902</v>
@@ -1795,7 +1795,7 @@
         <v>45</v>
       </c>
       <c r="F61">
-        <v>-2.961806950792357</v>
+        <v>-2.961950796606986</v>
       </c>
       <c r="G61">
         <v>-0.03820729640068848</v>
@@ -1841,7 +1841,7 @@
         <v>47</v>
       </c>
       <c r="F63">
-        <v>-2.979726315531624</v>
+        <v>-2.979870161346254</v>
       </c>
       <c r="G63">
         <v>-0.03345732172063337</v>
@@ -2140,7 +2140,7 @@
         <v>4</v>
       </c>
       <c r="F76">
-        <v>-2.556861307954046</v>
+        <v>-2.557134323827063</v>
       </c>
       <c r="G76">
         <v>-0.009360433829400439</v>
@@ -2163,7 +2163,7 @@
         <v>5</v>
       </c>
       <c r="F77">
-        <v>-2.5639287926167</v>
+        <v>-2.564050175924418</v>
       </c>
       <c r="G77">
         <v>-0.01168911538477779</v>
@@ -2186,7 +2186,7 @@
         <v>6</v>
       </c>
       <c r="F78">
-        <v>-2.570693012148761</v>
+        <v>-2.570992579552536</v>
       </c>
       <c r="G78">
         <v>-0.01319505159429335</v>
@@ -2209,7 +2209,7 @@
         <v>7</v>
       </c>
       <c r="F79">
-        <v>-2.577241016596144</v>
+        <v>-2.578060064215193</v>
       </c>
       <c r="G79">
         <v>-0.01482606883834148</v>
@@ -2232,7 +2232,7 @@
         <v>8</v>
       </c>
       <c r="F80">
-        <v>-2.584337919285817</v>
+        <v>-2.584456436097275</v>
       </c>
       <c r="G80">
         <v>-0.01673379968222033</v>
@@ -2255,7 +2255,7 @@
         <v>9</v>
       </c>
       <c r="F81">
-        <v>-2.591033858571673</v>
+        <v>-2.59122065562934</v>
       </c>
       <c r="G81">
         <v>-0.01874690541857671</v>
@@ -2301,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="F83">
-        <v>-2.603586702216664</v>
+        <v>-2.604631409112562</v>
       </c>
       <c r="G83">
         <v>-0.02079083856217956</v>
@@ -2347,7 +2347,7 @@
         <v>13</v>
       </c>
       <c r="F85">
-        <v>-2.616944014812231</v>
+        <v>-2.617617514157474</v>
       </c>
       <c r="G85">
         <v>-0.02460978573796169</v>
@@ -2485,7 +2485,7 @@
         <v>19</v>
       </c>
       <c r="F91">
-        <v>-2.655749325284129</v>
+        <v>-2.656224540195129</v>
       </c>
       <c r="G91">
         <v>-0.03334418232809933</v>
@@ -2508,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.661403515032001</v>
+        <v>-2.662251939564772</v>
       </c>
       <c r="G92">
         <v>-0.0335041471158104</v>
@@ -2554,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="F94">
-        <v>-2.673336999509699</v>
+        <v>-2.674984443720013</v>
       </c>
       <c r="G94">
         <v>-0.03587368263202073</v>
@@ -2600,7 +2600,7 @@
         <v>24</v>
       </c>
       <c r="F96">
-        <v>-2.686484124785737</v>
+        <v>-2.686794200117982</v>
       </c>
       <c r="G96">
         <v>-0.03755179022647681</v>
@@ -2807,7 +2807,7 @@
         <v>33</v>
       </c>
       <c r="F105">
-        <v>-2.740878194225086</v>
+        <v>-2.741020195601559</v>
       </c>
       <c r="G105">
         <v>-0.04830758554495018</v>
@@ -2853,7 +2853,7 @@
         <v>35</v>
       </c>
       <c r="F107">
-        <v>-2.753040525849177</v>
+        <v>-2.753156659747274</v>
       </c>
       <c r="G107">
         <v>-0.04962271848860245</v>
@@ -2876,7 +2876,7 @@
         <v>36</v>
       </c>
       <c r="F108">
-        <v>-2.758853954117912</v>
+        <v>-2.759815823803081</v>
       </c>
       <c r="G108">
         <v>-0.05124788849689588</v>
@@ -2899,7 +2899,7 @@
         <v>37</v>
       </c>
       <c r="F109">
-        <v>-2.764356187341415</v>
+        <v>-2.764483094608916</v>
       </c>
       <c r="G109">
         <v>-0.05167308933277748</v>
@@ -2922,7 +2922,7 @@
         <v>38</v>
       </c>
       <c r="F110">
-        <v>-2.770715044108685</v>
+        <v>-2.771287211404782</v>
       </c>
       <c r="G110">
         <v>-0.05308534052708236</v>
@@ -2945,7 +2945,7 @@
         <v>39</v>
       </c>
       <c r="F111">
-        <v>-2.775735340132129</v>
+        <v>-2.776149239305832</v>
       </c>
       <c r="G111">
         <v>-0.05309381757023268</v>
@@ -2968,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.781446435258457</v>
+        <v>-2.782696320197633</v>
       </c>
       <c r="G112">
         <v>-0.05379309371626739</v>
@@ -3014,7 +3014,7 @@
         <v>42</v>
       </c>
       <c r="F114">
-        <v>-2.793585720497061</v>
+        <v>-2.794010603950464</v>
       </c>
       <c r="G114">
         <v>-0.05523359462688138</v>
@@ -3037,7 +3037,7 @@
         <v>43</v>
       </c>
       <c r="F115">
-        <v>-2.799321249247869</v>
+        <v>-2.799589177480176</v>
       </c>
       <c r="G115">
         <v>-0.05663245076479884</v>
@@ -3060,7 +3060,7 @@
         <v>44</v>
       </c>
       <c r="F116">
-        <v>-2.803909549011701</v>
+        <v>-2.805708441412771</v>
       </c>
       <c r="G116">
         <v>-0.05457939555608693</v>
@@ -3083,7 +3083,7 @@
         <v>45</v>
       </c>
       <c r="F117">
-        <v>-2.810043878293136</v>
+        <v>-2.810532976659868</v>
       </c>
       <c r="G117">
         <v>-0.05733144184947991</v>
@@ -3106,7 +3106,7 @@
         <v>46</v>
       </c>
       <c r="F118">
-        <v>-2.81608535868666</v>
+        <v>-2.816649595955719</v>
       </c>
       <c r="G118">
         <v>-0.05836110326271005</v>
@@ -3152,7 +3152,7 @@
         <v>48</v>
       </c>
       <c r="F120">
-        <v>-2.827347095653737</v>
+        <v>-2.827975820879778</v>
       </c>
       <c r="G120">
         <v>-0.0591197003244841</v>
@@ -3175,7 +3175,7 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.832875603008955</v>
+        <v>-2.833085334345872</v>
       </c>
       <c r="G121">
         <v>-0.06011589064412548</v>
@@ -3221,7 +3221,7 @@
         <v>51</v>
       </c>
       <c r="F123">
-        <v>-2.844845117088864</v>
+        <v>-2.845140152689809</v>
       </c>
       <c r="G123">
         <v>-0.06111273591711663</v>
@@ -3267,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.855698845588972</v>
+        <v>-2.855919870168915</v>
       </c>
       <c r="G125">
         <v>-0.06204738595473791</v>
@@ -3290,7 +3290,7 @@
         <v>54</v>
       </c>
       <c r="F126">
-        <v>-2.860669583370912</v>
+        <v>-2.861677742498329</v>
       </c>
       <c r="G126">
         <v>-0.06095510635897328</v>
@@ -3313,7 +3313,7 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.866402312210238</v>
+        <v>-2.86740541376005</v>
       </c>
       <c r="G127">
         <v>-0.06357168596364748</v>
@@ -3336,7 +3336,7 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.869206086060882</v>
+        <v>-2.872551081569796</v>
       </c>
       <c r="G128">
         <v>-0.06136364083399903</v>
@@ -3359,7 +3359,7 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.876998822342203</v>
+        <v>-2.877887210414418</v>
       </c>
       <c r="G129">
         <v>-0.06346250403063602</v>
@@ -3382,7 +3382,7 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.881471769781636</v>
+        <v>-2.883174545858874</v>
       </c>
       <c r="G130">
         <v>-0.06288434190605274</v>
@@ -3428,7 +3428,7 @@
         <v>60</v>
       </c>
       <c r="F132">
-        <v>-2.893634382373857</v>
+        <v>-2.894902929794221</v>
       </c>
       <c r="G132">
         <v>-0.06574466122580058</v>
@@ -3451,7 +3451,7 @@
         <v>61</v>
       </c>
       <c r="F133">
-        <v>-2.897284011026469</v>
+        <v>-2.899336828010308</v>
       </c>
       <c r="G133">
         <v>-0.06403568002347071</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.903265201702387</v>
+        <v>-2.905332513389349</v>
       </c>
       <c r="G134">
         <v>-0.06458910152633202</v>
@@ -3497,7 +3497,7 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.909551665997399</v>
+        <v>-2.910280538043267</v>
       </c>
       <c r="G135">
         <v>-0.06576481203970608</v>
@@ -3543,7 +3543,7 @@
         <v>65</v>
       </c>
       <c r="F137">
-        <v>-2.920091898552963</v>
+        <v>-2.921014504352457</v>
       </c>
       <c r="G137">
         <v>-0.06714308250343981</v>
@@ -3566,7 +3566,7 @@
         <v>66</v>
       </c>
       <c r="F138">
-        <v>-2.924340960933909</v>
+        <v>-2.92559347818118</v>
       </c>
       <c r="G138">
         <v>-0.06445105608908031</v>
@@ -3589,7 +3589,7 @@
         <v>67</v>
       </c>
       <c r="F139">
-        <v>-2.929073024893842</v>
+        <v>-2.932357879192138</v>
       </c>
       <c r="G139">
         <v>-0.06603296747695842</v>
@@ -3658,7 +3658,7 @@
         <v>70</v>
       </c>
       <c r="F142">
-        <v>-2.945738389721404</v>
+        <v>-2.947583152827628</v>
       </c>
       <c r="G142">
         <v>-0.06773047877041449</v>
@@ -3681,7 +3681,7 @@
         <v>71</v>
       </c>
       <c r="F143">
-        <v>-2.950407938665473</v>
+        <v>-2.95218824026265</v>
       </c>
       <c r="G143">
         <v>-0.06738820873418949</v>
@@ -3727,7 +3727,7 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.961327082531045</v>
+        <v>-2.961959056001634</v>
       </c>
       <c r="G145">
         <v>-0.06748118864619723</v>
@@ -3819,7 +3819,7 @@
         <v>77</v>
       </c>
       <c r="F149">
-        <v>-2.980865937145079</v>
+        <v>-2.981788314171705</v>
       </c>
       <c r="G149">
         <v>-0.06750718794421084</v>
@@ -3865,7 +3865,7 @@
         <v>79</v>
       </c>
       <c r="F151">
-        <v>-2.98924785916482</v>
+        <v>-2.992347745964074</v>
       </c>
       <c r="G151">
         <v>-0.06456239094180272</v>
@@ -3888,7 +3888,7 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.995858882499368</v>
+        <v>-2.997116548710268</v>
       </c>
       <c r="G152">
         <v>-0.06773278174544517</v>
@@ -3911,7 +3911,7 @@
         <v>81</v>
       </c>
       <c r="F153">
-        <v>-2.999941932857733</v>
+        <v>-3.00249512774443</v>
       </c>
       <c r="G153">
         <v>-0.06478741784322395</v>
@@ -3934,7 +3934,7 @@
         <v>82</v>
       </c>
       <c r="F154">
-        <v>-3.005368551263645</v>
+        <v>-3.00584816185901</v>
       </c>
       <c r="G154">
         <v>-0.0665697151181357</v>
@@ -3980,7 +3980,7 @@
         <v>84</v>
       </c>
       <c r="F156">
-        <v>-3.014214275188162</v>
+        <v>-3.016862058843911</v>
       </c>
       <c r="G156">
         <v>-0.06602702995799836</v>
@@ -4003,7 +4003,7 @@
         <v>85</v>
       </c>
       <c r="F157">
-        <v>-3.020874140688279</v>
+        <v>-3.022211961212907</v>
       </c>
       <c r="G157">
         <v>-0.06768894503288925</v>
@@ -4026,7 +4026,7 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.025551867870405</v>
+        <v>-3.026357484602578</v>
       </c>
       <c r="G158">
         <v>-0.06558136880843191</v>
@@ -4049,7 +4049,7 @@
         <v>87</v>
       </c>
       <c r="F159">
-        <v>-3.029083706150644</v>
+        <v>-3.031330986606944</v>
       </c>
       <c r="G159">
         <v>-0.06587487253466695</v>
@@ -4072,7 +4072,7 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.03418860758944</v>
+        <v>-3.034978545336137</v>
       </c>
       <c r="G160">
         <v>-0.06560167880263923</v>
@@ -4095,7 +4095,7 @@
         <v>89</v>
       </c>
       <c r="F161">
-        <v>-3.038560383490193</v>
+        <v>-3.04072894871185</v>
       </c>
       <c r="G161">
         <v>-0.06532791191362941</v>
@@ -4118,7 +4118,7 @@
         <v>90</v>
       </c>
       <c r="F162">
-        <v>-3.042765124386503</v>
+        <v>-3.044954685679027</v>
       </c>
       <c r="G162">
         <v>-0.06411392166011232</v>
@@ -4141,7 +4141,7 @@
         <v>91</v>
       </c>
       <c r="F163">
-        <v>-3.047308026418245</v>
+        <v>-3.04923503691804</v>
       </c>
       <c r="G163">
         <v>-0.06405191688109535</v>
@@ -4187,7 +4187,7 @@
         <v>93</v>
       </c>
       <c r="F165">
-        <v>-3.058015604924448</v>
+        <v>-3.059176702071025</v>
       </c>
       <c r="G165">
         <v>-0.06275476442368888</v>
@@ -4233,7 +4233,7 @@
         <v>95</v>
       </c>
       <c r="F167">
-        <v>-3.066147671850681</v>
+        <v>-3.067260560654754</v>
       </c>
       <c r="G167">
         <v>-0.06284428639235717</v>
@@ -4279,7 +4279,7 @@
         <v>97</v>
       </c>
       <c r="F169">
-        <v>-3.074709028456249</v>
+        <v>-3.076380643854948</v>
       </c>
       <c r="G169">
         <v>-0.06036720404738916</v>
@@ -4302,7 +4302,7 @@
         <v>98</v>
       </c>
       <c r="F170">
-        <v>-3.079984830751882</v>
+        <v>-3.080196145167688</v>
       </c>
       <c r="G170">
         <v>-0.06164598835267909</v>
@@ -4325,7 +4325,7 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.083040039174117</v>
+        <v>-3.085915621611693</v>
       </c>
       <c r="G171">
         <v>-0.05968937779462025</v>
@@ -4371,7 +4371,7 @@
         <v>101</v>
       </c>
       <c r="F173">
-        <v>-3.093976687304298</v>
+        <v>-3.094097007922227</v>
       </c>
       <c r="G173">
         <v>-0.0606023879642148</v>
@@ -4394,7 +4394,7 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.096109639010141</v>
+        <v>-3.098005839385694</v>
       </c>
       <c r="G174">
         <v>-0.05731042424340216</v>
@@ -4440,7 +4440,7 @@
         <v>104</v>
       </c>
       <c r="F176">
-        <v>-3.105425129691536</v>
+        <v>-3.108051807411427</v>
       </c>
       <c r="G176">
         <v>-0.05701537341057217</v>
@@ -4463,7 +4463,7 @@
         <v>105</v>
       </c>
       <c r="F177">
-        <v>-3.109238216318147</v>
+        <v>-3.112464004364122</v>
       </c>
       <c r="G177">
         <v>-0.05565791605355563</v>
@@ -4486,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="F178">
-        <v>-3.114031005796952</v>
+        <v>-3.114847379095872</v>
       </c>
       <c r="G178">
         <v>-0.05559761155540122</v>
@@ -4509,7 +4509,7 @@
         <v>107</v>
       </c>
       <c r="F179">
-        <v>-3.119383826962398</v>
+        <v>-3.120925915000138</v>
       </c>
       <c r="G179">
         <v>-0.05593861374055409</v>
@@ -4555,7 +4555,7 @@
         <v>109</v>
       </c>
       <c r="F181">
-        <v>-3.125869403569847</v>
+        <v>-3.12946943427337</v>
       </c>
       <c r="G181">
         <v>-0.05240055238741648</v>
@@ -4578,7 +4578,7 @@
         <v>110</v>
       </c>
       <c r="F182">
-        <v>-3.130769858361425</v>
+        <v>-3.132794447098449</v>
       </c>
       <c r="G182">
         <v>-0.05203772949605678</v>
@@ -4601,7 +4601,7 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.136277172608858</v>
+        <v>-3.137393101058846</v>
       </c>
       <c r="G183">
         <v>-0.05129041491596353</v>
@@ -4647,7 +4647,7 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.143883992381014</v>
+        <v>-3.145029864284994</v>
       </c>
       <c r="G185">
         <v>-0.04845011854330328</v>
@@ -4670,7 +4670,7 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.148915907549484</v>
+        <v>-3.148943596741501</v>
       </c>
       <c r="G186">
         <v>-0.04925179264205015</v>
@@ -4693,7 +4693,7 @@
         <v>115</v>
       </c>
       <c r="F187">
-        <v>-3.151165440095393</v>
+        <v>-3.153152265441162</v>
       </c>
       <c r="G187">
         <v>-0.04735917435520443</v>
@@ -4716,7 +4716,7 @@
         <v>116</v>
       </c>
       <c r="F188">
-        <v>-3.155012747948987</v>
+        <v>-3.156464680075463</v>
       </c>
       <c r="G188">
         <v>-0.04646116390450361</v>
@@ -4739,7 +4739,7 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.160028332170772</v>
+        <v>-3.161781796442347</v>
       </c>
       <c r="G189">
         <v>-0.04598724613481375</v>
@@ -4762,7 +4762,7 @@
         <v>118</v>
       </c>
       <c r="F190">
-        <v>-3.164574729539761</v>
+        <v>-3.165399485359316</v>
       </c>
       <c r="G190">
         <v>-0.0451496106568342</v>
@@ -4785,7 +4785,7 @@
         <v>119</v>
       </c>
       <c r="F191">
-        <v>-3.168479353982149</v>
+        <v>-3.169240697074989</v>
       </c>
       <c r="G191">
         <v>-0.0446594182255643</v>
@@ -4831,7 +4831,7 @@
         <v>121</v>
       </c>
       <c r="F193">
-        <v>-3.176173472008438</v>
+        <v>-3.176437625820784</v>
       </c>
       <c r="G193">
         <v>-0.04256279306248706</v>
@@ -4854,7 +4854,7 @@
         <v>122</v>
       </c>
       <c r="F194">
-        <v>-3.17909070356288</v>
+        <v>-3.181319681557457</v>
       </c>
       <c r="G194">
         <v>-0.03881246376914294</v>
@@ -4877,7 +4877,7 @@
         <v>123</v>
       </c>
       <c r="F195">
-        <v>-3.183580108248109</v>
+        <v>-3.185369558699013</v>
       </c>
       <c r="G195">
         <v>-0.03994579134157211</v>
@@ -4900,7 +4900,7 @@
         <v>124</v>
       </c>
       <c r="F196">
-        <v>-3.188058576347226</v>
+        <v>-3.189724686115034</v>
       </c>
       <c r="G196">
         <v>-0.03941244046039544</v>
@@ -4923,7 +4923,7 @@
         <v>125</v>
       </c>
       <c r="F197">
-        <v>-3.189936585305512</v>
+        <v>-3.192248379711496</v>
       </c>
       <c r="G197">
         <v>-0.03627863043838803</v>
@@ -4992,7 +4992,7 @@
         <v>128</v>
       </c>
       <c r="F200">
-        <v>-3.202470218677251</v>
+        <v>-3.203331833685932</v>
       </c>
       <c r="G200">
         <v>-0.03377680686924722</v>
@@ -5038,7 +5038,7 @@
         <v>130</v>
       </c>
       <c r="F202">
-        <v>-3.209937699206235</v>
+        <v>-3.210544863271938</v>
       </c>
       <c r="G202">
         <v>-0.03036356401630436</v>
@@ -5084,7 +5084,7 @@
         <v>132</v>
       </c>
       <c r="F204">
-        <v>-3.21669829979673</v>
+        <v>-3.218084110636192</v>
       </c>
       <c r="G204">
         <v>-0.02740245753816334</v>
@@ -5130,7 +5130,7 @@
         <v>134</v>
       </c>
       <c r="F206">
-        <v>-3.224483943344608</v>
+        <v>-3.225722259454766</v>
       </c>
       <c r="G206">
         <v>-0.02395704933887857</v>
@@ -5153,7 +5153,7 @@
         <v>135</v>
       </c>
       <c r="F207">
-        <v>-3.227550527467095</v>
+        <v>-3.228204135007847</v>
       </c>
       <c r="G207">
         <v>-0.02307325738062735</v>
@@ -5199,7 +5199,7 @@
         <v>137</v>
       </c>
       <c r="F209">
-        <v>-3.234809940147315</v>
+        <v>-3.235317470156847</v>
       </c>
       <c r="G209">
         <v>-0.02050262750713219</v>
@@ -5222,7 +5222,7 @@
         <v>138</v>
       </c>
       <c r="F210">
-        <v>-3.237669990374982</v>
+        <v>-3.238177520384523</v>
       </c>
       <c r="G210">
         <v>-0.01885838876404511</v>
@@ -5245,7 +5245,7 @@
         <v>139</v>
       </c>
       <c r="F211">
-        <v>-3.24053004060266</v>
+        <v>-3.241037570612193</v>
       </c>
       <c r="G211">
         <v>-0.01619909000189521</v>
@@ -5268,7 +5268,7 @@
         <v>140</v>
       </c>
       <c r="F212">
-        <v>-3.243390090830335</v>
+        <v>-3.243897620839862</v>
       </c>
       <c r="G212">
         <v>-0.01455485125881051</v>
@@ -5544,7 +5544,7 @@
         <v>123</v>
       </c>
       <c r="F224">
-        <v>-2.991786745210991</v>
+        <v>-2.991851698054141</v>
       </c>
       <c r="G224">
         <v>-0.06585036778075026</v>
@@ -5567,7 +5567,7 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.071801599347739</v>
+        <v>-3.072479080212108</v>
       </c>
       <c r="G225">
         <v>-0.06706605855737169</v>
@@ -5590,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.145726063804554</v>
+        <v>-3.146565938076786</v>
       </c>
       <c r="G226">
         <v>-0.06526121734482282</v>
@@ -5613,7 +5613,7 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.213980509517109</v>
+        <v>-3.214451541346659</v>
       </c>
       <c r="G227">
         <v>-0.05795664270708345</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.27801322586012</v>
+        <v>-3.279026207044959</v>
       </c>
       <c r="G228">
         <v>-0.04533785168943294</v>
@@ -5659,7 +5659,7 @@
         <v>278</v>
       </c>
       <c r="F229">
-        <v>-3.335516389978159</v>
+        <v>-3.336342121179763</v>
       </c>
       <c r="G229">
         <v>-0.0256671702582969</v>
@@ -5797,7 +5797,7 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.05992860600994</v>
+        <v>-3.061133523790462</v>
       </c>
       <c r="G235">
         <v>-0.06582278144061338</v>
@@ -5820,7 +5820,7 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.141646965559532</v>
+        <v>-3.142823936029714</v>
       </c>
       <c r="G236">
         <v>-0.06949561329669662</v>
@@ -5843,7 +5843,7 @@
         <v>336</v>
       </c>
       <c r="F237">
-        <v>-3.216149655374434</v>
+        <v>-3.217457720738783</v>
       </c>
       <c r="G237">
         <v>-0.06595277541808997</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.287421329286068</v>
+        <v>-3.28799411061178</v>
       </c>
       <c r="G238">
         <v>-0.05809579843940671</v>
@@ -6073,7 +6073,7 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.188642415278473</v>
+        <v>-3.189330263160725</v>
       </c>
       <c r="G247">
         <v>-0.06824666094787357</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.265190832362579</v>
+        <v>-3.265605841693848</v>
       </c>
       <c r="G248">
         <v>-0.06560785152213766</v>
@@ -6142,7 +6142,7 @@
         <v>738</v>
       </c>
       <c r="F250">
-        <v>-3.403459083100889</v>
+        <v>-3.403825108517992</v>
       </c>
       <c r="G250">
         <v>-0.04504233741870345</v>
@@ -6165,7 +6165,7 @@
         <v>830</v>
       </c>
       <c r="F251">
-        <v>-3.463723656752894</v>
+        <v>-3.464021387393363</v>
       </c>
       <c r="G251">
         <v>-0.02616601496006538</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.301761604138614</v>
+        <v>-3.301891683843066</v>
       </c>
       <c r="G259">
         <v>-0.06543527498148838</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.373457111455625</v>
+        <v>-3.37378244914177</v>
       </c>
       <c r="G260">
         <v>-0.05726230869625171</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.440265385995371</v>
+        <v>-3.440577904916151</v>
       </c>
       <c r="G261">
         <v>-0.04321905106294766</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.249308346790897</v>
+        <v>-3.249935804537984</v>
       </c>
       <c r="G269">
         <v>-0.06734220799904622</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.327869221786628</v>
+        <v>-3.327974039753514</v>
       </c>
       <c r="G270">
         <v>-0.06481872284724788</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.468238141735037</v>
+        <v>-3.468629416209611</v>
       </c>
       <c r="G272">
         <v>-0.04341253589937355</v>
@@ -6855,7 +6855,7 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.348082887897847</v>
+        <v>-3.348727118902105</v>
       </c>
       <c r="G281">
         <v>-0.06351486964996411</v>
@@ -6878,7 +6878,7 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.42213210848631</v>
+        <v>-3.422448330837314</v>
       </c>
       <c r="G282">
         <v>-0.0560346378298906</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.490413545904524</v>
+        <v>-3.490785261989347</v>
       </c>
       <c r="G283">
         <v>-0.04278662283956813</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.553789523861628</v>
+        <v>-3.553952033217719</v>
       </c>
       <c r="G284">
         <v>-0.02463314838813591</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.285837715712817</v>
+        <v>-3.285963542684351</v>
       </c>
       <c r="G291">
         <v>-0.06577419618658276</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.365310023999299</v>
+        <v>-3.365351565903648</v>
       </c>
       <c r="G292">
         <v>-0.06333436743314813</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.438925453220398</v>
+        <v>-3.43936464679758</v>
       </c>
       <c r="G293">
         <v>-0.05488108393260571</v>
@@ -7154,7 +7154,7 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.508392204087163</v>
+        <v>-3.508522403612005</v>
       </c>
       <c r="G294">
         <v>-0.04237685235887212</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.572004523720261</v>
+        <v>-3.572229444572814</v>
       </c>
       <c r="G295">
         <v>-0.02429245603436292</v>
@@ -7338,7 +7338,7 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.299044224190915</v>
+        <v>-3.299421340991911</v>
       </c>
       <c r="G302">
         <v>-0.06494055916953889</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.453074962658991</v>
+        <v>-3.453398381379759</v>
       </c>
       <c r="G304">
         <v>-0.05432673206147376</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.522861606902127</v>
+        <v>-3.523186693574442</v>
       </c>
       <c r="G305">
         <v>-0.04181348491829107</v>
@@ -7430,7 +7430,7 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.587216767754723</v>
+        <v>-3.587297600076772</v>
       </c>
       <c r="G306">
         <v>-0.02398586397592811</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.389936322130754</v>
+        <v>-3.3902917913971</v>
       </c>
       <c r="G314">
         <v>-0.06136042568945133</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.535262224065824</v>
+        <v>-3.535332709001385</v>
       </c>
       <c r="G316">
         <v>-0.04128817195466283</v>
@@ -7683,7 +7683,7 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.599857296428731</v>
+        <v>-3.600009324462675</v>
       </c>
       <c r="G317">
         <v>-0.02362099063037559</v>
@@ -7890,7 +7890,7 @@
         <v>5751</v>
       </c>
       <c r="F326">
-        <v>-3.475158652570573</v>
+        <v>-3.475207043901229</v>
       </c>
       <c r="G326">
         <v>-0.05361299538312403</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.545417024307139</v>
+        <v>-3.545674978592156</v>
       </c>
       <c r="G327">
         <v>-0.04081394392064219</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.610671010373864</v>
+        <v>-3.610712801335441</v>
       </c>
       <c r="G328">
         <v>-0.02337751331525639</v>
@@ -8120,7 +8120,7 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.408008386408828</v>
+        <v>-3.408173956440033</v>
       </c>
       <c r="G336">
         <v>-0.06041169046913186</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.554464161606724</v>
+        <v>-3.554475767915689</v>
       </c>
       <c r="G338">
         <v>-0.04061472443527936</v>
@@ -8189,7 +8189,7 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.619906107633123</v>
+        <v>-3.620028388592467</v>
       </c>
       <c r="G339">
         <v>-0.02298485002555933</v>

</xml_diff>

<commit_message>
updated data from overnight run
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.540382347402587</v>
+        <v>-2.540474844570503</v>
       </c>
       <c r="G27">
         <v>-0.0435746677847646</v>
@@ -1220,7 +1220,7 @@
         <v>20</v>
       </c>
       <c r="F36">
-        <v>-2.66987011454032</v>
+        <v>-2.670475102966387</v>
       </c>
       <c r="G36">
         <v>-0.06028933413625248</v>
@@ -1266,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="F38">
-        <v>-2.697197167713321</v>
+        <v>-2.697918559728932</v>
       </c>
       <c r="G38">
         <v>-0.06077558815324902</v>
@@ -1358,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.749294258234732</v>
+        <v>-2.750465817882679</v>
       </c>
       <c r="G42">
         <v>-0.06363725531029729</v>
@@ -1450,7 +1450,7 @@
         <v>30</v>
       </c>
       <c r="F46">
-        <v>-2.798738553081813</v>
+        <v>-2.798767128471436</v>
       </c>
       <c r="G46">
         <v>-0.06413870524745602</v>
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.823120060686657</v>
+        <v>-2.823853004773674</v>
       </c>
       <c r="G48">
         <v>-0.06306564814332039</v>
@@ -1588,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.868027122282964</v>
+        <v>-2.868254237674743</v>
       </c>
       <c r="G52">
         <v>-0.05683615016545374</v>
@@ -2163,7 +2163,7 @@
         <v>5</v>
       </c>
       <c r="F77">
-        <v>-2.564050175924418</v>
+        <v>-2.564201808489714</v>
       </c>
       <c r="G77">
         <v>-0.01168911538477779</v>
@@ -2232,7 +2232,7 @@
         <v>8</v>
       </c>
       <c r="F80">
-        <v>-2.584456436097275</v>
+        <v>-2.584824283747256</v>
       </c>
       <c r="G80">
         <v>-0.01673379968222033</v>
@@ -2577,7 +2577,7 @@
         <v>23</v>
       </c>
       <c r="F95">
-        <v>-2.680889056154785</v>
+        <v>-2.681063135759894</v>
       </c>
       <c r="G95">
         <v>-0.03752556923010752</v>
@@ -2600,7 +2600,7 @@
         <v>24</v>
       </c>
       <c r="F96">
-        <v>-2.686794200117982</v>
+        <v>-2.686856484750614</v>
       </c>
       <c r="G96">
         <v>-0.03755179022647681</v>
@@ -2807,7 +2807,7 @@
         <v>33</v>
       </c>
       <c r="F105">
-        <v>-2.741020195601559</v>
+        <v>-2.741076208621173</v>
       </c>
       <c r="G105">
         <v>-0.04830758554495018</v>
@@ -2991,7 +2991,7 @@
         <v>41</v>
       </c>
       <c r="F113">
-        <v>-2.789263077304626</v>
+        <v>-2.789459809392005</v>
       </c>
       <c r="G113">
         <v>-0.0565979167821431</v>
@@ -3313,7 +3313,7 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.86740541376005</v>
+        <v>-2.867662095547192</v>
       </c>
       <c r="G127">
         <v>-0.06357168596364748</v>
@@ -3336,7 +3336,7 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.872551081569796</v>
+        <v>-2.87287318842617</v>
       </c>
       <c r="G128">
         <v>-0.06136364083399903</v>
@@ -3382,7 +3382,7 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.883174545858874</v>
+        <v>-2.883487390046943</v>
       </c>
       <c r="G130">
         <v>-0.06288434190605274</v>
@@ -3635,7 +3635,7 @@
         <v>69</v>
       </c>
       <c r="F141">
-        <v>-2.940935050703278</v>
+        <v>-2.941780385107061</v>
       </c>
       <c r="G141">
         <v>-0.0679389587325816</v>
@@ -3727,7 +3727,7 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.961959056001634</v>
+        <v>-2.962058836287509</v>
       </c>
       <c r="G145">
         <v>-0.06748118864619723</v>
@@ -3819,7 +3819,7 @@
         <v>77</v>
       </c>
       <c r="F149">
-        <v>-2.981788314171705</v>
+        <v>-2.981979035832709</v>
       </c>
       <c r="G149">
         <v>-0.06750718794421084</v>
@@ -4118,7 +4118,7 @@
         <v>90</v>
       </c>
       <c r="F162">
-        <v>-3.044954685679027</v>
+        <v>-3.045358891961728</v>
       </c>
       <c r="G162">
         <v>-0.06411392166011232</v>
@@ -4210,7 +4210,7 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.063350357814993</v>
+        <v>-3.06340521850676</v>
       </c>
       <c r="G166">
         <v>-0.06381311094603859</v>
@@ -4486,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="F178">
-        <v>-3.114847379095872</v>
+        <v>-3.115136646950508</v>
       </c>
       <c r="G178">
         <v>-0.05559761155540122</v>
@@ -4670,7 +4670,7 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.148943596741501</v>
+        <v>-3.149706816182572</v>
       </c>
       <c r="G186">
         <v>-0.04925179264205015</v>
@@ -4785,7 +4785,7 @@
         <v>119</v>
       </c>
       <c r="F191">
-        <v>-3.169240697074989</v>
+        <v>-3.169254765525305</v>
       </c>
       <c r="G191">
         <v>-0.0446594182255643</v>
@@ -4854,7 +4854,7 @@
         <v>122</v>
       </c>
       <c r="F194">
-        <v>-3.181319681557457</v>
+        <v>-3.181396745136484</v>
       </c>
       <c r="G194">
         <v>-0.03881246376914294</v>
@@ -4946,7 +4946,7 @@
         <v>126</v>
       </c>
       <c r="F198">
-        <v>-3.196010794281656</v>
+        <v>-3.19672887167101</v>
       </c>
       <c r="G198">
         <v>-0.03734102043423909</v>
@@ -4992,7 +4992,7 @@
         <v>128</v>
       </c>
       <c r="F200">
-        <v>-3.203331833685932</v>
+        <v>-3.203816678208772</v>
       </c>
       <c r="G200">
         <v>-0.03377680686924722</v>
@@ -5544,7 +5544,7 @@
         <v>123</v>
       </c>
       <c r="F224">
-        <v>-2.991851698054141</v>
+        <v>-2.992003378767224</v>
       </c>
       <c r="G224">
         <v>-0.06585036778075026</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.265605841693848</v>
+        <v>-3.265868722777168</v>
       </c>
       <c r="G248">
         <v>-0.06560785152213766</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.327974039753514</v>
+        <v>-3.32850040435183</v>
       </c>
       <c r="G270">
         <v>-0.06481872284724788</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.468629416209611</v>
+        <v>-3.468659184933812</v>
       </c>
       <c r="G272">
         <v>-0.04341253589937355</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.553952033217719</v>
+        <v>-3.553992063324459</v>
       </c>
       <c r="G284">
         <v>-0.02463314838813591</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.285963542684351</v>
+        <v>-3.286102204651301</v>
       </c>
       <c r="G291">
         <v>-0.06577419618658276</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.453398381379759</v>
+        <v>-3.453466960289215</v>
       </c>
       <c r="G304">
         <v>-0.05432673206147376</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.465277447682741</v>
+        <v>-3.465353046047447</v>
       </c>
       <c r="G315">
         <v>-0.05419071372997042</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.610712801335441</v>
+        <v>-3.610725135587206</v>
       </c>
       <c r="G328">
         <v>-0.02337751331525639</v>

</xml_diff>

<commit_message>
first GA batch run
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -441,7 +441,7 @@
         <v>-1.984661672509521</v>
       </c>
       <c r="G2">
-        <v>-1.77635683940025e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -464,7 +464,7 @@
         <v>-2.042228299641555</v>
       </c>
       <c r="G3">
-        <v>-0.01306052443690664</v>
+        <v>-0.01306052443690531</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -487,7 +487,7 @@
         <v>-2.099794926773589</v>
       </c>
       <c r="G4">
-        <v>-0.02612104887381195</v>
+        <v>-0.02612104887381084</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -510,7 +510,7 @@
         <v>-2.157361553905622</v>
       </c>
       <c r="G5">
-        <v>-0.03918157331071614</v>
+        <v>-0.0391815733107157</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -533,7 +533,7 @@
         <v>-2.214928181037654</v>
       </c>
       <c r="G6">
-        <v>-0.05224209774761879</v>
+        <v>-0.05224209774761857</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -556,7 +556,7 @@
         <v>-2.262929532377208</v>
       </c>
       <c r="G7">
-        <v>-0.05573734639204408</v>
+        <v>-0.05573734639204431</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -579,7 +579,7 @@
         <v>-2.310930883716762</v>
       </c>
       <c r="G8">
-        <v>-0.0592325950364696</v>
+        <v>-0.05923259503647005</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -602,7 +602,7 @@
         <v>-2.358932235056315</v>
       </c>
       <c r="G9">
-        <v>-0.06272784368089335</v>
+        <v>-0.06272784368089435</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -625,7 +625,7 @@
         <v>-2.406933586395867</v>
       </c>
       <c r="G10">
-        <v>-0.06622309232531742</v>
+        <v>-0.06622309232531853</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -648,7 +648,7 @@
         <v>-2.445369661942942</v>
       </c>
       <c r="G11">
-        <v>-0.06015306517726304</v>
+        <v>-0.06015306517726449</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -671,7 +671,7 @@
         <v>-2.483805737490016</v>
       </c>
       <c r="G12">
-        <v>-0.05408303802920789</v>
+        <v>-0.05408303802920994</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -694,7 +694,7 @@
         <v>-2.522241813037089</v>
       </c>
       <c r="G13">
-        <v>-0.04801301088115306</v>
+        <v>-0.04801301088115545</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -717,7 +717,7 @@
         <v>-2.560677888584162</v>
       </c>
       <c r="G14">
-        <v>-0.04194298373309729</v>
+        <v>-0.04194298373309982</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -740,7 +740,7 @@
         <v>-2.563241007546191</v>
       </c>
       <c r="G15">
-        <v>3.108624468950438e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -763,7 +763,7 @@
         <v>-2.358672444100425</v>
       </c>
       <c r="G16">
-        <v>1.332267629550188e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -786,7 +786,7 @@
         <v>-2.378686989554971</v>
       </c>
       <c r="G17">
-        <v>-0.007512491205383665</v>
+        <v>-0.007512491205384997</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -809,7 +809,7 @@
         <v>-2.395730559084579</v>
       </c>
       <c r="G18">
-        <v>-0.0120540064858301</v>
+        <v>-0.01205400648583232</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -832,7 +832,7 @@
         <v>-2.412774128614186</v>
       </c>
       <c r="G19">
-        <v>-0.01659552176627699</v>
+        <v>-0.01659552176627921</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -855,7 +855,7 @@
         <v>-2.429817698143792</v>
       </c>
       <c r="G20">
-        <v>-0.02113703704672254</v>
+        <v>-0.02113703704672432</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -875,10 +875,10 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <v>-2.4468612676734</v>
+        <v>-2.446304268323845</v>
       </c>
       <c r="G21">
-        <v>-0.02567855232716854</v>
+        <v>-0.02512155297761609</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -898,10 +898,10 @@
         <v>6</v>
       </c>
       <c r="F22">
-        <v>-2.463904837203005</v>
+        <v>-2.462427224205399</v>
       </c>
       <c r="G22">
-        <v>-0.03022006760761364</v>
+        <v>-0.02874245461000902</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -921,10 +921,10 @@
         <v>7</v>
       </c>
       <c r="F23">
-        <v>-2.479579712587558</v>
+        <v>-2.477545100240395</v>
       </c>
       <c r="G23">
-        <v>-0.03339288874300506</v>
+        <v>-0.03135827639584443</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -944,10 +944,10 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>-2.495755947894593</v>
+        <v>-2.49290964075193</v>
       </c>
       <c r="G24">
-        <v>-0.03517009470659405</v>
+        <v>-0.03422076265821916</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -967,10 +967,10 @@
         <v>9</v>
       </c>
       <c r="F25">
-        <v>-2.510674767910714</v>
+        <v>-2.510674767910715</v>
       </c>
       <c r="G25">
-        <v>-0.0394281961407692</v>
+        <v>-0.03948383556784352</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -990,10 +990,10 @@
         <v>10</v>
       </c>
       <c r="F26">
-        <v>-2.524925309723143</v>
+        <v>-2.524594621703169</v>
       </c>
       <c r="G26">
-        <v>-0.04045748607644772</v>
+        <v>-0.04090163511113665</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1013,10 +1013,10 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.540474844570503</v>
+        <v>-2.539457802292218</v>
       </c>
       <c r="G27">
-        <v>-0.0435746677847646</v>
+        <v>-0.04326276145102503</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1036,10 +1036,10 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <v>-2.555895024509102</v>
+        <v>-2.555189888564569</v>
       </c>
       <c r="G28">
-        <v>-0.04616053399350739</v>
+        <v>-0.04649279347421498</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1059,10 +1059,10 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <v>-2.569979436581178</v>
+        <v>-2.568573096154417</v>
       </c>
       <c r="G29">
-        <v>-0.04870578321911712</v>
+        <v>-0.04737394681490215</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1082,10 +1082,10 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <v>-2.584899828058029</v>
+        <v>-2.584768113147685</v>
       </c>
       <c r="G30">
-        <v>-0.0511986244693492</v>
+        <v>-0.0510669095590095</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1105,10 +1105,10 @@
         <v>15</v>
       </c>
       <c r="F31">
-        <v>-2.599651729792937</v>
+        <v>-2.597537947112877</v>
       </c>
       <c r="G31">
-        <v>-0.0526307116085365</v>
+        <v>-0.05133468927504103</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1128,10 +1128,10 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.614335921297939</v>
+        <v>-2.61253924598982</v>
       </c>
       <c r="G32">
-        <v>-0.05443337550925675</v>
+        <v>-0.05383393390282332</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1151,10 +1151,10 @@
         <v>17</v>
       </c>
       <c r="F33">
-        <v>-2.628170071715121</v>
+        <v>-2.6267471373837</v>
       </c>
       <c r="G33">
-        <v>-0.05664898037791666</v>
+        <v>-0.05553977104754271</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1174,10 +1174,10 @@
         <v>18</v>
       </c>
       <c r="F34">
-        <v>-2.643105066209313</v>
+        <v>-2.640309169555353</v>
       </c>
       <c r="G34">
-        <v>-0.0580541600269564</v>
+        <v>-0.05659974897003517</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1197,10 +1197,10 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.656369164419501</v>
+        <v>-2.655986789728492</v>
       </c>
       <c r="G35">
-        <v>-0.05773910978529906</v>
+        <v>-0.05977531489401344</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1220,10 +1220,10 @@
         <v>20</v>
       </c>
       <c r="F36">
-        <v>-2.670475102966387</v>
+        <v>-2.668959398600806</v>
       </c>
       <c r="G36">
-        <v>-0.06028933413625248</v>
+        <v>-0.06024586951716659</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1243,10 +1243,10 @@
         <v>21</v>
       </c>
       <c r="F37">
-        <v>-2.684853324023879</v>
+        <v>-2.685610566066039</v>
       </c>
       <c r="G37">
-        <v>-0.06203361382131134</v>
+        <v>-0.06439498273323907</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1266,10 +1266,10 @@
         <v>22</v>
       </c>
       <c r="F38">
-        <v>-2.697918559728932</v>
+        <v>-2.697067098099584</v>
       </c>
       <c r="G38">
-        <v>-0.06077558815324902</v>
+        <v>-0.06334946051762347</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1289,10 +1289,10 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.711540019779271</v>
+        <v>-2.709857285211729</v>
       </c>
       <c r="G39">
-        <v>-0.06393561024422234</v>
+        <v>-0.06363759338060815</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1312,10 +1312,10 @@
         <v>24</v>
       </c>
       <c r="F40">
-        <v>-2.724326756464124</v>
+        <v>-2.723283836822127</v>
       </c>
       <c r="G40">
-        <v>-0.06340652409494751</v>
+        <v>-0.06456209074184449</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1335,10 +1335,10 @@
         <v>25</v>
       </c>
       <c r="F41">
-        <v>-2.737687386151913</v>
+        <v>-2.735913020087091</v>
       </c>
       <c r="G41">
-        <v>-0.06607195876235483</v>
+        <v>-0.06468921975764808</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1358,10 +1358,10 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.750465817882679</v>
+        <v>-2.74705566266379</v>
       </c>
       <c r="G42">
-        <v>-0.06363725531029729</v>
+        <v>-0.06332980808518607</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1381,10 +1381,10 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.76231188174176</v>
+        <v>-2.760142979523824</v>
       </c>
       <c r="G43">
-        <v>-0.06265572423852195</v>
+        <v>-0.06391507069606006</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1404,10 +1404,10 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <v>-2.775350053409366</v>
+        <v>-2.774007077905265</v>
       </c>
       <c r="G44">
-        <v>-0.06528927629043091</v>
+        <v>-0.06527711482833976</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1427,10 +1427,10 @@
         <v>29</v>
       </c>
       <c r="F45">
-        <v>-2.788729517134818</v>
+        <v>-2.786490536389025</v>
       </c>
       <c r="G45">
-        <v>-0.06305543452718299</v>
+        <v>-0.06525851906293978</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1450,10 +1450,10 @@
         <v>30</v>
       </c>
       <c r="F46">
-        <v>-2.798767128471436</v>
+        <v>-2.797612427495173</v>
       </c>
       <c r="G46">
-        <v>-0.06413870524745602</v>
+        <v>-0.06387835591992652</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1473,10 +1473,10 @@
         <v>31</v>
       </c>
       <c r="F47">
-        <v>-2.811585327036044</v>
+        <v>-2.808710017122225</v>
       </c>
       <c r="G47">
-        <v>-0.06405829701417254</v>
+        <v>-0.06247389129781755</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1496,10 +1496,10 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.823853004773674</v>
+        <v>-2.82098743602109</v>
       </c>
       <c r="G48">
-        <v>-0.06306564814332039</v>
+        <v>-0.06224925594752295</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1519,10 +1519,10 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.835663471362181</v>
+        <v>-2.832109733207955</v>
       </c>
       <c r="G49">
-        <v>-0.06433146253146271</v>
+        <v>-0.06086949888522653</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1542,10 +1542,10 @@
         <v>34</v>
       </c>
       <c r="F50">
-        <v>-2.846520782120486</v>
+        <v>-2.845704977870266</v>
       </c>
       <c r="G50">
-        <v>-0.06111689489647565</v>
+        <v>-0.06196268929837656</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1565,10 +1565,10 @@
         <v>35</v>
       </c>
       <c r="F51">
-        <v>-2.858151952158444</v>
+        <v>-2.857196554559008</v>
       </c>
       <c r="G51">
-        <v>-0.06123768602781177</v>
+        <v>-0.06095221173795851</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1588,10 +1588,10 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.868254237674743</v>
+        <v>-2.867976202668343</v>
       </c>
       <c r="G52">
-        <v>-0.05683615016545374</v>
+        <v>-0.05922980559813218</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1611,10 +1611,10 @@
         <v>37</v>
       </c>
       <c r="F53">
-        <v>-2.879788971325359</v>
+        <v>-2.878590044406622</v>
       </c>
       <c r="G53">
-        <v>-0.0575982892167386</v>
+        <v>-0.05734159308725095</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1634,10 +1634,10 @@
         <v>38</v>
       </c>
       <c r="F54">
-        <v>-2.890303069259688</v>
+        <v>-2.889482603130103</v>
       </c>
       <c r="G54">
-        <v>-0.05556617059195057</v>
+        <v>-0.05573209756157105</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1657,10 +1657,10 @@
         <v>39</v>
       </c>
       <c r="F55">
-        <v>-2.901091692013082</v>
+        <v>-2.901122687512842</v>
       </c>
       <c r="G55">
-        <v>-0.05255177254366028</v>
+        <v>-0.05487012769514921</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1680,10 +1680,10 @@
         <v>40</v>
       </c>
       <c r="F56">
-        <v>-2.911880314766472</v>
+        <v>-2.910308070512214</v>
       </c>
       <c r="G56">
-        <v>-0.0521482219451993</v>
+        <v>-0.05155345644536014</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1703,10 +1703,10 @@
         <v>41</v>
       </c>
       <c r="F57">
-        <v>-2.922606946520343</v>
+        <v>-2.921065697765848</v>
       </c>
       <c r="G57">
-        <v>-0.04966518363519057</v>
+        <v>-0.04980902944983412</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1726,10 +1726,10 @@
         <v>42</v>
       </c>
       <c r="F58">
-        <v>-2.932400261829762</v>
+        <v>-2.930209338565391</v>
       </c>
       <c r="G58">
-        <v>-0.04731849155707635</v>
+        <v>-0.04645061600021683</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1749,10 +1749,10 @@
         <v>43</v>
       </c>
       <c r="F59">
-        <v>-2.943045038768522</v>
+        <v>-2.941616640328895</v>
       </c>
       <c r="G59">
-        <v>-0.04347201412076784</v>
+        <v>-0.04535586351456022</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1772,10 +1772,10 @@
         <v>44</v>
       </c>
       <c r="F60">
-        <v>-2.952991114237355</v>
+        <v>-2.951402456055571</v>
       </c>
       <c r="G60">
-        <v>-0.04255210294949902</v>
+        <v>-0.04263962499207485</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1795,10 +1795,10 @@
         <v>45</v>
       </c>
       <c r="F61">
-        <v>-2.961950796606986</v>
+        <v>-2.961108249322421</v>
       </c>
       <c r="G61">
-        <v>-0.03820729640068848</v>
+        <v>-0.03984336400976435</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1818,10 +1818,10 @@
         <v>46</v>
       </c>
       <c r="F62">
-        <v>-2.97076663316199</v>
+        <v>-2.970036936192296</v>
       </c>
       <c r="G62">
-        <v>-0.03626999663046548</v>
+        <v>-0.03626999663047809</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1841,10 +1841,10 @@
         <v>47</v>
       </c>
       <c r="F63">
-        <v>-2.979870161346254</v>
+        <v>-2.979726315531622</v>
       </c>
       <c r="G63">
-        <v>-0.03345732172063337</v>
+        <v>-0.03345732172064375</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1864,10 +1864,10 @@
         <v>48</v>
       </c>
       <c r="F64">
-        <v>-2.988829843715886</v>
+        <v>-2.988685997901257</v>
       </c>
       <c r="G64">
-        <v>-0.03005879565573477</v>
+        <v>-0.02991494984111792</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1887,10 +1887,10 @@
         <v>49</v>
       </c>
       <c r="F65">
-        <v>-2.99778952608552</v>
+        <v>-2.997789526085522</v>
       </c>
       <c r="G65">
-        <v>-0.02651642377620722</v>
+        <v>-0.02651642377622287</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1910,10 +1910,10 @@
         <v>50</v>
       </c>
       <c r="F66">
-        <v>-3.006749208455155</v>
+        <v>-3.006749208455156</v>
       </c>
       <c r="G66">
-        <v>-0.02297405189668139</v>
+        <v>-0.02297405189669574</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1936,7 +1936,7 @@
         <v>-3.015708890824789</v>
       </c>
       <c r="G67">
-        <v>-0.0194316800171547</v>
+        <v>-0.01943168001716766</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -1959,7 +1959,7 @@
         <v>-3.02335302506966</v>
       </c>
       <c r="G68">
-        <v>-0.0145737600128647</v>
+        <v>-0.01457376001287808</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -1982,7 +1982,7 @@
         <v>-3.030997159314529</v>
       </c>
       <c r="G69">
-        <v>-0.009715840008573354</v>
+        <v>-0.009715840008587162</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2005,7 +2005,7 @@
         <v>-3.038641293559397</v>
       </c>
       <c r="G70">
-        <v>-0.004857920004280238</v>
+        <v>-0.004857920004294469</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2028,7 +2028,7 @@
         <v>-3.046285427804264</v>
       </c>
       <c r="G71">
-        <v>1.4210854715202e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2051,7 +2051,7 @@
         <v>-2.527180582330468</v>
       </c>
       <c r="G72">
-        <v>-1.199040866595169e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2074,7 +2074,7 @@
         <v>-2.534669017704617</v>
       </c>
       <c r="G73">
-        <v>-0.002476616393867204</v>
+        <v>-0.002476616393855657</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2097,7 +2097,7 @@
         <v>-2.542157453078766</v>
       </c>
       <c r="G74">
-        <v>-0.004953232787723749</v>
+        <v>-0.004953232787711759</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2117,10 +2117,10 @@
         <v>3</v>
       </c>
       <c r="F75">
-        <v>-2.549645888452914</v>
+        <v>-2.549645888452913</v>
       </c>
       <c r="G75">
-        <v>-0.007429849181578074</v>
+        <v>-0.007429849181566084</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2140,10 +2140,10 @@
         <v>4</v>
       </c>
       <c r="F76">
-        <v>-2.557134323827063</v>
+        <v>-2.556713373115567</v>
       </c>
       <c r="G76">
-        <v>-0.009360433829400439</v>
+        <v>-0.009485514863926792</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2163,10 +2163,10 @@
         <v>5</v>
       </c>
       <c r="F77">
-        <v>-2.564201808489714</v>
+        <v>-2.563777160051407</v>
       </c>
       <c r="G77">
-        <v>-0.01168911538477779</v>
+        <v>-0.01153748281947342</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2186,10 +2186,10 @@
         <v>6</v>
       </c>
       <c r="F78">
-        <v>-2.570992579552536</v>
+        <v>-2.570693012148764</v>
       </c>
       <c r="G78">
-        <v>-0.01319505159429335</v>
+        <v>-0.01344151593653731</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2209,10 +2209,10 @@
         <v>7</v>
       </c>
       <c r="F79">
-        <v>-2.578060064215193</v>
+        <v>-2.577214465065385</v>
       </c>
       <c r="G79">
-        <v>-0.01482606883834148</v>
+        <v>-0.01495114987286561</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2232,10 +2232,10 @@
         <v>8</v>
       </c>
       <c r="F80">
-        <v>-2.584824283747256</v>
+        <v>-2.584251700470463</v>
       </c>
       <c r="G80">
-        <v>-0.01673379968222033</v>
+        <v>-0.01697656629765065</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2255,10 +2255,10 @@
         <v>9</v>
       </c>
       <c r="F81">
-        <v>-2.59122065562934</v>
+        <v>-2.591493671502356</v>
       </c>
       <c r="G81">
-        <v>-0.01874690541857671</v>
+        <v>-0.01920671834924992</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <v>-2.597680392522835</v>
+        <v>-2.597362548723772</v>
       </c>
       <c r="G82">
-        <v>-0.02038162038944558</v>
+        <v>-0.02006377659037284</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2301,10 +2301,10 @@
         <v>11</v>
       </c>
       <c r="F83">
-        <v>-2.604631409112562</v>
+        <v>-2.604783041677857</v>
       </c>
       <c r="G83">
-        <v>-0.02079083856217956</v>
+        <v>-0.02247245056416469</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2324,10 +2324,10 @@
         <v>12</v>
       </c>
       <c r="F84">
-        <v>-2.611293929490623</v>
+        <v>-2.610354619475546</v>
       </c>
       <c r="G84">
-        <v>-0.02397151939664788</v>
+        <v>-0.02303220938156114</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2347,10 +2347,10 @@
         <v>13</v>
       </c>
       <c r="F85">
-        <v>-2.617617514157474</v>
+        <v>-2.615473446191409</v>
       </c>
       <c r="G85">
-        <v>-0.02460978573796169</v>
+        <v>-0.02313921711713052</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2370,10 +2370,10 @@
         <v>14</v>
       </c>
       <c r="F86">
-        <v>-2.624459339543276</v>
+        <v>-2.622653167569458</v>
       </c>
       <c r="G86">
-        <v>-0.02711329148871311</v>
+        <v>-0.02530711951488618</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2393,10 +2393,10 @@
         <v>15</v>
       </c>
       <c r="F87">
-        <v>-2.630256238791675</v>
+        <v>-2.628866613989982</v>
       </c>
       <c r="G87">
-        <v>-0.02777472046905638</v>
+        <v>-0.02650874695511796</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2416,10 +2416,10 @@
         <v>16</v>
       </c>
       <c r="F88">
-        <v>-2.637997222799576</v>
+        <v>-2.636513288796895</v>
       </c>
       <c r="G88">
-        <v>-0.03062753678442665</v>
+        <v>-0.02914360278173733</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2439,10 +2439,10 @@
         <v>17</v>
       </c>
       <c r="F89">
-        <v>-2.643868368001036</v>
+        <v>-2.641131912824005</v>
       </c>
       <c r="G89">
-        <v>-0.03009632403038554</v>
+        <v>-0.02875040782855365</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2462,10 +2462,10 @@
         <v>18</v>
       </c>
       <c r="F90">
-        <v>-2.649805497745682</v>
+        <v>-2.648536988686376</v>
       </c>
       <c r="G90">
-        <v>-0.03139401713672241</v>
+        <v>-0.03114366471063246</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2485,10 +2485,10 @@
         <v>19</v>
       </c>
       <c r="F91">
-        <v>-2.656224540195129</v>
+        <v>-2.654932713960276</v>
       </c>
       <c r="G91">
-        <v>-0.03334418232809933</v>
+        <v>-0.03252757100423942</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2508,10 +2508,10 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.662251939564772</v>
+        <v>-2.660213666698697</v>
       </c>
       <c r="G92">
-        <v>-0.0335041471158104</v>
+        <v>-0.03279670476236696</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2531,10 +2531,10 @@
         <v>21</v>
       </c>
       <c r="F93">
-        <v>-2.669294398769136</v>
+        <v>-2.666267390704045</v>
       </c>
       <c r="G93">
-        <v>-0.03686561785251952</v>
+        <v>-0.0338386097874217</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2554,10 +2554,10 @@
         <v>22</v>
       </c>
       <c r="F94">
-        <v>-2.674984443720013</v>
+        <v>-2.673597520912591</v>
       </c>
       <c r="G94">
-        <v>-0.03587368263202073</v>
+        <v>-0.03615692101567447</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2577,10 +2577,10 @@
         <v>23</v>
       </c>
       <c r="F95">
-        <v>-2.681063135759894</v>
+        <v>-2.680062279369086</v>
       </c>
       <c r="G95">
-        <v>-0.03752556923010752</v>
+        <v>-0.0376098604918762</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2600,10 +2600,10 @@
         <v>24</v>
       </c>
       <c r="F96">
-        <v>-2.686856484750614</v>
+        <v>-2.685958492529633</v>
       </c>
       <c r="G96">
-        <v>-0.03755179022647681</v>
+        <v>-0.03849425467213008</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2623,10 +2623,10 @@
         <v>25</v>
       </c>
       <c r="F97">
-        <v>-2.693756599497035</v>
+        <v>-2.690727542699385</v>
       </c>
       <c r="G97">
-        <v>-0.03934780706786567</v>
+        <v>-0.03825148586158944</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2646,10 +2646,10 @@
         <v>26</v>
       </c>
       <c r="F98">
-        <v>-2.6988436090532</v>
+        <v>-2.696563605339872</v>
       </c>
       <c r="G98">
-        <v>-0.04107257757641181</v>
+        <v>-0.03907572952178295</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2669,10 +2669,10 @@
         <v>27</v>
       </c>
       <c r="F99">
-        <v>-2.705729345165447</v>
+        <v>-2.704609035202683</v>
       </c>
       <c r="G99">
-        <v>-0.04176767620742927</v>
+        <v>-0.04210934040430026</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2692,10 +2692,10 @@
         <v>28</v>
       </c>
       <c r="F100">
-        <v>-2.711446074175362</v>
+        <v>-2.710549838492032</v>
       </c>
       <c r="G100">
-        <v>-0.04331418871932691</v>
+        <v>-0.04303832471335678</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2715,10 +2715,10 @@
         <v>29</v>
       </c>
       <c r="F101">
-        <v>-2.718257034338622</v>
+        <v>-2.715060201262196</v>
       </c>
       <c r="G101">
-        <v>-0.0442973274229872</v>
+        <v>-0.04253686850322724</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -2738,10 +2738,10 @@
         <v>30</v>
       </c>
       <c r="F102">
-        <v>-2.723178040276345</v>
+        <v>-2.722233892144196</v>
       </c>
       <c r="G102">
-        <v>-0.04467185876890278</v>
+        <v>-0.04469874040493416</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2761,10 +2761,10 @@
         <v>31</v>
       </c>
       <c r="F103">
-        <v>-2.728665632831155</v>
+        <v>-2.72794516755145</v>
       </c>
       <c r="G103">
-        <v>-0.04583898727533553</v>
+        <v>-0.04539819683189528</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -2784,10 +2784,10 @@
         <v>32</v>
       </c>
       <c r="F104">
-        <v>-2.735955382133135</v>
+        <v>-2.735043509258003</v>
       </c>
       <c r="G104">
-        <v>-0.04839659243329231</v>
+        <v>-0.04748471955815536</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2807,10 +2807,10 @@
         <v>33</v>
       </c>
       <c r="F105">
-        <v>-2.741076208621173</v>
+        <v>-2.741231268562386</v>
       </c>
       <c r="G105">
-        <v>-0.04830758554495018</v>
+        <v>-0.04866065988224522</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2830,10 +2830,10 @@
         <v>34</v>
       </c>
       <c r="F106">
-        <v>-2.748110608015103</v>
+        <v>-2.747709149568069</v>
       </c>
       <c r="G106">
-        <v>-0.05037360343084574</v>
+        <v>-0.05012672190763467</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -2853,10 +2853,10 @@
         <v>35</v>
       </c>
       <c r="F107">
-        <v>-2.753156659747274</v>
+        <v>-2.752003868543535</v>
       </c>
       <c r="G107">
-        <v>-0.04962271848860245</v>
+        <v>-0.04940962190280773</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2876,10 +2876,10 @@
         <v>36</v>
       </c>
       <c r="F108">
-        <v>-2.759815823803081</v>
+        <v>-2.756812257956874</v>
       </c>
       <c r="G108">
-        <v>-0.05124788849689588</v>
+        <v>-0.04920619233585422</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2899,10 +2899,10 @@
         <v>37</v>
       </c>
       <c r="F109">
-        <v>-2.764483094608916</v>
+        <v>-2.76491329777672</v>
       </c>
       <c r="G109">
-        <v>-0.05167308933277748</v>
+        <v>-0.05229541317540698</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2922,10 +2922,10 @@
         <v>38</v>
       </c>
       <c r="F110">
-        <v>-2.771287211404782</v>
+        <v>-2.769311888944154</v>
       </c>
       <c r="G110">
-        <v>-0.05308534052708236</v>
+        <v>-0.05168218536254798</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2945,10 +2945,10 @@
         <v>39</v>
       </c>
       <c r="F111">
-        <v>-2.776149239305832</v>
+        <v>-2.774925704281841</v>
       </c>
       <c r="G111">
-        <v>-0.05309381757023268</v>
+        <v>-0.05228418171994131</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -2968,10 +2968,10 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.782696320197633</v>
+        <v>-2.780309870683897</v>
       </c>
       <c r="G112">
-        <v>-0.05379309371626739</v>
+        <v>-0.05265652914170493</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2991,10 +2991,10 @@
         <v>41</v>
       </c>
       <c r="F113">
-        <v>-2.789459809392005</v>
+        <v>-2.787099101727094</v>
       </c>
       <c r="G113">
-        <v>-0.0565979167821431</v>
+        <v>-0.05443394120460865</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3014,10 +3014,10 @@
         <v>42</v>
       </c>
       <c r="F114">
-        <v>-2.794010603950464</v>
+        <v>-2.79252639774953</v>
       </c>
       <c r="G114">
-        <v>-0.05523359462688138</v>
+        <v>-0.05484941824675094</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3037,10 +3037,10 @@
         <v>43</v>
       </c>
       <c r="F115">
-        <v>-2.799589177480176</v>
+        <v>-2.798519742704131</v>
       </c>
       <c r="G115">
-        <v>-0.05663245076479884</v>
+        <v>-0.05583094422105916</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3060,10 +3060,10 @@
         <v>44</v>
       </c>
       <c r="F116">
-        <v>-2.805708441412771</v>
+        <v>-2.80399832935169</v>
       </c>
       <c r="G116">
-        <v>-0.05457939555608693</v>
+        <v>-0.05629771188832478</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3083,10 +3083,10 @@
         <v>45</v>
       </c>
       <c r="F117">
-        <v>-2.810532976659868</v>
+        <v>-2.809449469985546</v>
       </c>
       <c r="G117">
-        <v>-0.05733144184947991</v>
+        <v>-0.05673703354188819</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3106,10 +3106,10 @@
         <v>46</v>
       </c>
       <c r="F118">
-        <v>-2.816649595955719</v>
+        <v>-2.816044860002276</v>
       </c>
       <c r="G118">
-        <v>-0.05836110326271005</v>
+        <v>-0.05832060457832489</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3129,10 +3129,10 @@
         <v>47</v>
       </c>
       <c r="F119">
-        <v>-2.821901924650995</v>
+        <v>-2.82301011832586</v>
       </c>
       <c r="G119">
-        <v>-0.05825934168565339</v>
+        <v>-0.06027404392161584</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3152,10 +3152,10 @@
         <v>48</v>
       </c>
       <c r="F120">
-        <v>-2.827975820879778</v>
+        <v>-2.824536013466388</v>
       </c>
       <c r="G120">
-        <v>-0.0591197003244841</v>
+        <v>-0.05678812008185008</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3175,10 +3175,10 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.833085334345872</v>
+        <v>-2.832768823861797</v>
       </c>
       <c r="G121">
-        <v>-0.06011589064412548</v>
+        <v>-0.06000911149696631</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3198,10 +3198,10 @@
         <v>50</v>
       </c>
       <c r="F122">
-        <v>-2.839047481591393</v>
+        <v>-2.837874301520555</v>
       </c>
       <c r="G122">
-        <v>-0.06127595024627008</v>
+        <v>-0.06010277017543042</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3221,10 +3221,10 @@
         <v>51</v>
       </c>
       <c r="F123">
-        <v>-2.845140152689809</v>
+        <v>-2.844506825377259</v>
       </c>
       <c r="G123">
-        <v>-0.06111273591711663</v>
+        <v>-0.06172347505184139</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3244,10 +3244,10 @@
         <v>52</v>
       </c>
       <c r="F124">
-        <v>-2.850292849638052</v>
+        <v>-2.849081799698701</v>
       </c>
       <c r="G124">
-        <v>-0.06249768033234204</v>
+        <v>-0.06128663039299131</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3267,10 +3267,10 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.855919870168915</v>
+        <v>-2.854224371748653</v>
       </c>
       <c r="G125">
-        <v>-0.06204738595473791</v>
+        <v>-0.06141738346264969</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3290,10 +3290,10 @@
         <v>54</v>
       </c>
       <c r="F126">
-        <v>-2.861677742498329</v>
+        <v>-2.858838106987017</v>
       </c>
       <c r="G126">
-        <v>-0.06095510635897328</v>
+        <v>-0.0610192997207204</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3313,10 +3313,10 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.867662095547192</v>
+        <v>-2.865105233882583</v>
       </c>
       <c r="G127">
-        <v>-0.06357168596364748</v>
+        <v>-0.06227460763599346</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3336,10 +3336,10 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.87287318842617</v>
+        <v>-2.869625120603108</v>
       </c>
       <c r="G128">
-        <v>-0.06136364083399903</v>
+        <v>-0.06178267537622562</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3359,10 +3359,10 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.877887210414418</v>
+        <v>-2.875703222970226</v>
       </c>
       <c r="G129">
-        <v>-0.06346250403063602</v>
+        <v>-0.0628489587630503</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3382,10 +3382,10 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.883487390046943</v>
+        <v>-2.881023864806531</v>
       </c>
       <c r="G130">
-        <v>-0.06288434190605274</v>
+        <v>-0.06315778161906183</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3405,10 +3405,10 @@
         <v>59</v>
       </c>
       <c r="F131">
-        <v>-2.889732856557247</v>
+        <v>-2.886881697478125</v>
       </c>
       <c r="G131">
-        <v>-0.06284933779902624</v>
+        <v>-0.06400379531036271</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3428,10 +3428,10 @@
         <v>60</v>
       </c>
       <c r="F132">
-        <v>-2.894902929794221</v>
+        <v>-2.892760930829954</v>
       </c>
       <c r="G132">
-        <v>-0.06574466122580058</v>
+        <v>-0.06487120968189952</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3451,10 +3451,10 @@
         <v>61</v>
       </c>
       <c r="F133">
-        <v>-2.899336828010308</v>
+        <v>-2.899556085513892</v>
       </c>
       <c r="G133">
-        <v>-0.06403568002347071</v>
+        <v>-0.06665454538554338</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3474,10 +3474,10 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.905332513389349</v>
+        <v>-2.901639682666676</v>
       </c>
       <c r="G134">
-        <v>-0.06458910152633202</v>
+        <v>-0.06372632355803498</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3497,10 +3497,10 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.910280538043267</v>
+        <v>-2.906850615773861</v>
       </c>
       <c r="G135">
-        <v>-0.06576481203970608</v>
+        <v>-0.06392543768492631</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3520,10 +3520,10 @@
         <v>64</v>
       </c>
       <c r="F136">
-        <v>-2.91593551636215</v>
+        <v>-2.914986484846605</v>
       </c>
       <c r="G136">
-        <v>-0.06799851929292</v>
+        <v>-0.06704948777737774</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -3543,10 +3543,10 @@
         <v>65</v>
       </c>
       <c r="F137">
-        <v>-2.921014504352457</v>
+        <v>-2.920643281966529</v>
       </c>
       <c r="G137">
-        <v>-0.06714308250343981</v>
+        <v>-0.06769446591700889</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -3566,10 +3566,10 @@
         <v>66</v>
       </c>
       <c r="F138">
-        <v>-2.92559347818118</v>
+        <v>-2.924531650735598</v>
       </c>
       <c r="G138">
-        <v>-0.06445105608908031</v>
+        <v>-0.06657101570578416</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -3589,10 +3589,10 @@
         <v>67</v>
       </c>
       <c r="F139">
-        <v>-2.932357879192138</v>
+        <v>-2.930882657104517</v>
       </c>
       <c r="G139">
-        <v>-0.06603296747695842</v>
+        <v>-0.06791020309441009</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -3612,10 +3612,10 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.936312301870653</v>
+        <v>-2.934563576090229</v>
       </c>
       <c r="G140">
-        <v>-0.06791729535647217</v>
+        <v>-0.06657930309982896</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -3635,10 +3635,10 @@
         <v>69</v>
       </c>
       <c r="F141">
-        <v>-2.941780385107061</v>
+        <v>-2.940079792462224</v>
       </c>
       <c r="G141">
-        <v>-0.0679389587325816</v>
+        <v>-0.06708370049153078</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -3658,10 +3658,10 @@
         <v>70</v>
       </c>
       <c r="F142">
-        <v>-2.947583152827628</v>
+        <v>-2.945805796069576</v>
       </c>
       <c r="G142">
-        <v>-0.06773047877041449</v>
+        <v>-0.06779788511858942</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -3681,10 +3681,10 @@
         <v>71</v>
       </c>
       <c r="F143">
-        <v>-2.95218824026265</v>
+        <v>-2.947522217144268</v>
       </c>
       <c r="G143">
-        <v>-0.06738820873418949</v>
+        <v>-0.06450248721298824</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -3704,10 +3704,10 @@
         <v>72</v>
       </c>
       <c r="F144">
-        <v>-2.956999208266978</v>
+        <v>-2.955359082172823</v>
       </c>
       <c r="G144">
-        <v>-0.06896765935540161</v>
+        <v>-0.06732753326125041</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -3727,10 +3727,10 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.962058836287509</v>
+        <v>-2.95886499975033</v>
       </c>
       <c r="G145">
-        <v>-0.06748118864619723</v>
+        <v>-0.06582163185846457</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -3750,10 +3750,10 @@
         <v>74</v>
       </c>
       <c r="F146">
-        <v>-2.966895421125398</v>
+        <v>-2.965956651104943</v>
       </c>
       <c r="G146">
-        <v>-0.06640536370848471</v>
+        <v>-0.06790146423278398</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -3773,10 +3773,10 @@
         <v>75</v>
       </c>
       <c r="F147">
-        <v>-2.971500992812409</v>
+        <v>-2.970240533670157</v>
       </c>
       <c r="G147">
-        <v>-0.06339923273279569</v>
+        <v>-0.06717352781770547</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -3796,10 +3796,10 @@
         <v>76</v>
       </c>
       <c r="F148">
-        <v>-2.976876368968091</v>
+        <v>-2.976312929408151</v>
       </c>
       <c r="G148">
-        <v>-0.06879754413534145</v>
+        <v>-0.06823410457540602</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -3819,10 +3819,10 @@
         <v>77</v>
       </c>
       <c r="F149">
-        <v>-2.981979035832709</v>
+        <v>-2.979798580267622</v>
       </c>
       <c r="G149">
-        <v>-0.06750718794421084</v>
+        <v>-0.06670793645458395</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -3842,10 +3842,10 @@
         <v>78</v>
       </c>
       <c r="F150">
-        <v>-2.987824243905864</v>
+        <v>-2.986650378176986</v>
       </c>
       <c r="G150">
-        <v>-0.06727763203746573</v>
+        <v>-0.06854791538365457</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -3865,10 +3865,10 @@
         <v>79</v>
       </c>
       <c r="F151">
-        <v>-2.992347745964074</v>
+        <v>-2.989199539033386</v>
       </c>
       <c r="G151">
-        <v>-0.06456239094180272</v>
+        <v>-0.06608525725976122</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -3888,10 +3888,10 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.997116548710268</v>
+        <v>-2.995927960554186</v>
       </c>
       <c r="G152">
-        <v>-0.06773278174544517</v>
+        <v>-0.06780185980026898</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -3911,10 +3911,10 @@
         <v>81</v>
       </c>
       <c r="F153">
-        <v>-3.00249512774443</v>
+        <v>-2.997696423449615</v>
       </c>
       <c r="G153">
-        <v>-0.06478741784322395</v>
+        <v>-0.06455850371540439</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -3934,10 +3934,10 @@
         <v>82</v>
       </c>
       <c r="F154">
-        <v>-3.00584816185901</v>
+        <v>-3.005461249675485</v>
       </c>
       <c r="G154">
-        <v>-0.0665697151181357</v>
+        <v>-0.06731151096098098</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -3957,10 +3957,10 @@
         <v>83</v>
       </c>
       <c r="F155">
-        <v>-3.013048408361136</v>
+        <v>-3.009286787448657</v>
       </c>
       <c r="G155">
-        <v>-0.0667727181853961</v>
+        <v>-0.06612522975386037</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -3980,10 +3980,10 @@
         <v>84</v>
       </c>
       <c r="F156">
-        <v>-3.016862058843911</v>
+        <v>-3.014826701520832</v>
       </c>
       <c r="G156">
-        <v>-0.06602702995799836</v>
+        <v>-0.06665332484574193</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -4003,10 +4003,10 @@
         <v>85</v>
       </c>
       <c r="F157">
-        <v>-3.022211961212907</v>
+        <v>-3.018040862294405</v>
       </c>
       <c r="G157">
-        <v>-0.06768894503288925</v>
+        <v>-0.06485566663902187</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -4026,10 +4026,10 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.026357484602578</v>
+        <v>-3.023943258117787</v>
       </c>
       <c r="G158">
-        <v>-0.06558136880843191</v>
+        <v>-0.06574624348211056</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -4049,10 +4049,10 @@
         <v>87</v>
       </c>
       <c r="F159">
-        <v>-3.031330986606944</v>
+        <v>-3.030893326777961</v>
       </c>
       <c r="G159">
-        <v>-0.06587487253466695</v>
+        <v>-0.06768449316199199</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -4072,10 +4072,10 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.034978545336137</v>
+        <v>-3.032697887756073</v>
       </c>
       <c r="G160">
-        <v>-0.06560167880263923</v>
+        <v>-0.06447723515981063</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -4095,10 +4095,10 @@
         <v>89</v>
       </c>
       <c r="F161">
-        <v>-3.04072894871185</v>
+        <v>-3.03825063639719</v>
       </c>
       <c r="G161">
-        <v>-0.06532791191362941</v>
+        <v>-0.06501816482063427</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -4118,10 +4118,10 @@
         <v>90</v>
       </c>
       <c r="F162">
-        <v>-3.045358891961728</v>
+        <v>-3.043672997008324</v>
       </c>
       <c r="G162">
-        <v>-0.06411392166011232</v>
+        <v>-0.06542870645147514</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -4141,10 +4141,10 @@
         <v>91</v>
       </c>
       <c r="F163">
-        <v>-3.04923503691804</v>
+        <v>-3.049209427558229</v>
       </c>
       <c r="G163">
-        <v>-0.06405191688109535</v>
+        <v>-0.06595331802108673</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -4164,10 +4164,10 @@
         <v>92</v>
       </c>
       <c r="F164">
-        <v>-3.053446742499242</v>
+        <v>-3.053039562562568</v>
       </c>
       <c r="G164">
-        <v>-0.06517881398179826</v>
+        <v>-0.06477163404513264</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -4187,10 +4187,10 @@
         <v>93</v>
       </c>
       <c r="F165">
-        <v>-3.059176702071025</v>
+        <v>-3.057874822442671</v>
       </c>
       <c r="G165">
-        <v>-0.06275476442368888</v>
+        <v>-0.06459507494494299</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -4210,10 +4210,10 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.06340521850676</v>
+        <v>-3.060945828585529</v>
       </c>
       <c r="G166">
-        <v>-0.06381311094603859</v>
+        <v>-0.06265426210750791</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -4233,10 +4233,10 @@
         <v>95</v>
       </c>
       <c r="F167">
-        <v>-3.067260560654754</v>
+        <v>-3.066247275541154</v>
       </c>
       <c r="G167">
-        <v>-0.06284428639235717</v>
+        <v>-0.06294389008283985</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -4256,10 +4256,10 @@
         <v>96</v>
       </c>
       <c r="F168">
-        <v>-3.072189571423429</v>
+        <v>-3.069187029523578</v>
       </c>
       <c r="G168">
-        <v>-0.06207833236976512</v>
+        <v>-0.06087182508497047</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -4279,10 +4279,10 @@
         <v>97</v>
       </c>
       <c r="F169">
-        <v>-3.076380643854948</v>
+        <v>-3.075635874617286</v>
       </c>
       <c r="G169">
-        <v>-0.06036720404738916</v>
+        <v>-0.06230885119838547</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -4302,10 +4302,10 @@
         <v>98</v>
       </c>
       <c r="F170">
-        <v>-3.080196145167688</v>
+        <v>-3.079430700637604</v>
       </c>
       <c r="G170">
-        <v>-0.06164598835267909</v>
+        <v>-0.06109185823841068</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -4325,10 +4325,10 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.085915621611693</v>
+        <v>-3.084791519730381</v>
       </c>
       <c r="G171">
-        <v>-0.05968937779462025</v>
+        <v>-0.06144085835089474</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -4348,10 +4348,10 @@
         <v>100</v>
       </c>
       <c r="F172">
-        <v>-3.089939289968849</v>
+        <v>-3.0887427165684</v>
       </c>
       <c r="G172">
-        <v>-0.06157680960905887</v>
+        <v>-0.06038023620861965</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -4371,10 +4371,10 @@
         <v>101</v>
       </c>
       <c r="F173">
-        <v>-3.094097007922227</v>
+        <v>-3.09196443733838</v>
       </c>
       <c r="G173">
-        <v>-0.0606023879642148</v>
+        <v>-0.05859013799830659</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -4394,10 +4394,10 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.098005839385694</v>
+        <v>-3.096628738555165</v>
       </c>
       <c r="G174">
-        <v>-0.05731042424340216</v>
+        <v>-0.05824262023479909</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -4417,10 +4417,10 @@
         <v>103</v>
       </c>
       <c r="F175">
-        <v>-3.102921715754679</v>
+        <v>-3.101286726821514</v>
       </c>
       <c r="G175">
-        <v>-0.0595237784540088</v>
+        <v>-0.05788878952085452</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -4440,10 +4440,10 @@
         <v>104</v>
       </c>
       <c r="F176">
-        <v>-3.108051807411427</v>
+        <v>-3.106166831824455</v>
       </c>
       <c r="G176">
-        <v>-0.05701537341057217</v>
+        <v>-0.05775707554350284</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -4463,10 +4463,10 @@
         <v>105</v>
       </c>
       <c r="F177">
-        <v>-3.112464004364122</v>
+        <v>-3.110689252978262</v>
       </c>
       <c r="G177">
-        <v>-0.05565791605355563</v>
+        <v>-0.05726767771701669</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -4486,10 +4486,10 @@
         <v>106</v>
       </c>
       <c r="F178">
-        <v>-3.115136646950508</v>
+        <v>-3.114248229247178</v>
       </c>
       <c r="G178">
-        <v>-0.05559761155540122</v>
+        <v>-0.05581483500563944</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -4509,10 +4509,10 @@
         <v>107</v>
       </c>
       <c r="F179">
-        <v>-3.120925915000138</v>
+        <v>-3.118617065905588</v>
       </c>
       <c r="G179">
-        <v>-0.05593861374055409</v>
+        <v>-0.05517185268375624</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -4532,10 +4532,10 @@
         <v>108</v>
       </c>
       <c r="F180">
-        <v>-3.124273964997457</v>
+        <v>-3.1242249942571</v>
       </c>
       <c r="G180">
-        <v>-0.05581693279531974</v>
+        <v>-0.0557679620549747</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -4555,10 +4555,10 @@
         <v>109</v>
       </c>
       <c r="F181">
-        <v>-3.12946943427337</v>
+        <v>-3.127558437683602</v>
       </c>
       <c r="G181">
-        <v>-0.05240055238741648</v>
+        <v>-0.05408958650118412</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -4578,10 +4578,10 @@
         <v>110</v>
       </c>
       <c r="F182">
-        <v>-3.132794447098449</v>
+        <v>-3.132939447210961</v>
       </c>
       <c r="G182">
-        <v>-0.05203772949605678</v>
+        <v>-0.05445877704824975</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -4601,10 +4601,10 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.137393101058846</v>
+        <v>-3.135976321111293</v>
       </c>
       <c r="G183">
-        <v>-0.05129041491596353</v>
+        <v>-0.05248383196828954</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -4624,10 +4624,10 @@
         <v>112</v>
       </c>
       <c r="F184">
-        <v>-3.14087100199626</v>
+        <v>-3.13813708687773</v>
       </c>
       <c r="G184">
-        <v>-0.05236669387295001</v>
+        <v>-0.04963277875443273</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -4647,10 +4647,10 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.145029864284994</v>
+        <v>-3.142254156616289</v>
       </c>
       <c r="G185">
-        <v>-0.04845011854330328</v>
+        <v>-0.04873802951269879</v>
       </c>
     </row>
     <row r="186" spans="1:7">
@@ -4670,10 +4670,10 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.149706816182572</v>
+        <v>-3.147536980199019</v>
       </c>
       <c r="G186">
-        <v>-0.04925179264205015</v>
+        <v>-0.04900903411513546</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -4693,10 +4693,10 @@
         <v>115</v>
       </c>
       <c r="F187">
-        <v>-3.153152265441162</v>
+        <v>-3.152453837310835</v>
       </c>
       <c r="G187">
-        <v>-0.04735917435520443</v>
+        <v>-0.04891407224665856</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -4716,10 +4716,10 @@
         <v>116</v>
       </c>
       <c r="F188">
-        <v>-3.156464680075463</v>
+        <v>-3.156219508673063</v>
       </c>
       <c r="G188">
-        <v>-0.04646116390450361</v>
+        <v>-0.04766792462859348</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -4739,10 +4739,10 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.161781796442347</v>
+        <v>-3.158365444796538</v>
       </c>
       <c r="G189">
-        <v>-0.04598724613481375</v>
+        <v>-0.0448020417717746</v>
       </c>
     </row>
     <row r="190" spans="1:7">
@@ -4762,10 +4762,10 @@
         <v>118</v>
       </c>
       <c r="F190">
-        <v>-3.165399485359316</v>
+        <v>-3.163952397055203</v>
       </c>
       <c r="G190">
-        <v>-0.0451496106568342</v>
+        <v>-0.04537717505014682</v>
       </c>
     </row>
     <row r="191" spans="1:7">
@@ -4785,10 +4785,10 @@
         <v>119</v>
       </c>
       <c r="F191">
-        <v>-3.169254765525305</v>
+        <v>-3.168977772165204</v>
       </c>
       <c r="G191">
-        <v>-0.0446594182255643</v>
+        <v>-0.04539073117985515</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -4808,10 +4808,10 @@
         <v>120</v>
       </c>
       <c r="F192">
-        <v>-3.173435111890394</v>
+        <v>-3.172927394559157</v>
       </c>
       <c r="G192">
-        <v>-0.044836251924737</v>
+        <v>-0.04432853459351432</v>
       </c>
     </row>
     <row r="193" spans="1:7">
@@ -4831,10 +4831,10 @@
         <v>121</v>
       </c>
       <c r="F193">
-        <v>-3.176437625820784</v>
+        <v>-3.177157787923274</v>
       </c>
       <c r="G193">
-        <v>-0.04256279306248706</v>
+        <v>-0.0435471089773386</v>
       </c>
     </row>
     <row r="194" spans="1:7">
@@ -4854,10 +4854,10 @@
         <v>122</v>
       </c>
       <c r="F194">
-        <v>-3.181396745136484</v>
+        <v>-3.179788708903259</v>
       </c>
       <c r="G194">
-        <v>-0.03881246376914294</v>
+        <v>-0.04116621097703005</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -4877,10 +4877,10 @@
         <v>123</v>
       </c>
       <c r="F195">
-        <v>-3.185369558699013</v>
+        <v>-3.182358158345255</v>
       </c>
       <c r="G195">
-        <v>-0.03994579134157211</v>
+        <v>-0.03872384143873364</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -4900,10 +4900,10 @@
         <v>124</v>
       </c>
       <c r="F196">
-        <v>-3.189724686115034</v>
+        <v>-3.185158707349343</v>
       </c>
       <c r="G196">
-        <v>-0.03941244046039544</v>
+        <v>-0.03651257146252856</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -4923,10 +4923,10 @@
         <v>125</v>
       </c>
       <c r="F197">
-        <v>-3.192248379711496</v>
+        <v>-3.191518139969665</v>
       </c>
       <c r="G197">
-        <v>-0.03627863043838803</v>
+        <v>-0.03786018510255756</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -4946,10 +4946,10 @@
         <v>126</v>
       </c>
       <c r="F198">
-        <v>-3.19672887167101</v>
+        <v>-3.19398984278846</v>
       </c>
       <c r="G198">
-        <v>-0.03734102043423909</v>
+        <v>-0.03532006894105899</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -4969,10 +4969,10 @@
         <v>127</v>
       </c>
       <c r="F199">
-        <v>-3.199543714371964</v>
+        <v>-3.199718311870945</v>
       </c>
       <c r="G199">
-        <v>-0.03463818959456333</v>
+        <v>-0.03603671904325106</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -4992,10 +4992,10 @@
         <v>128</v>
       </c>
       <c r="F200">
-        <v>-3.203816678208772</v>
+        <v>-3.201667904242333</v>
       </c>
       <c r="G200">
-        <v>-0.03377680686924722</v>
+        <v>-0.03297449243434603</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -5015,10 +5015,10 @@
         <v>129</v>
       </c>
       <c r="F201">
-        <v>-3.207967688723123</v>
+        <v>-3.206672737644993</v>
       </c>
       <c r="G201">
-        <v>-0.03426245793482557</v>
+        <v>-0.03296750685671307</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -5038,10 +5038,10 @@
         <v>130</v>
       </c>
       <c r="F202">
-        <v>-3.210544863271938</v>
+        <v>-3.210110834742801</v>
       </c>
       <c r="G202">
-        <v>-0.03036356401630436</v>
+        <v>-0.03139378497422746</v>
       </c>
     </row>
     <row r="203" spans="1:7">
@@ -5061,10 +5061,10 @@
         <v>131</v>
       </c>
       <c r="F203">
-        <v>-3.215318522628437</v>
+        <v>-3.213748245542063</v>
       </c>
       <c r="G203">
-        <v>-0.03032037290789391</v>
+        <v>-0.03001937679319677</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -5084,10 +5084,10 @@
         <v>132</v>
       </c>
       <c r="F204">
-        <v>-3.218084110636192</v>
+        <v>-3.218892636760453</v>
       </c>
       <c r="G204">
-        <v>-0.02740245753816334</v>
+        <v>-0.03015194903129287</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -5107,10 +5107,10 @@
         <v>133</v>
       </c>
       <c r="F205">
-        <v>-3.221752686988122</v>
+        <v>-3.220749041614699</v>
       </c>
       <c r="G205">
-        <v>-0.02800018027865142</v>
+        <v>-0.02699653490524634</v>
       </c>
     </row>
     <row r="206" spans="1:7">
@@ -5130,10 +5130,10 @@
         <v>134</v>
       </c>
       <c r="F206">
-        <v>-3.225722259454766</v>
+        <v>-3.223867708449949</v>
       </c>
       <c r="G206">
-        <v>-0.02395704933887857</v>
+        <v>-0.02510338276020257</v>
       </c>
     </row>
     <row r="207" spans="1:7">
@@ -5153,10 +5153,10 @@
         <v>135</v>
       </c>
       <c r="F207">
-        <v>-3.228204135007847</v>
+        <v>-3.227773783558185</v>
       </c>
       <c r="G207">
-        <v>-0.02307325738062735</v>
+        <v>-0.02399763888814654</v>
       </c>
     </row>
     <row r="208" spans="1:7">
@@ -5176,10 +5176,10 @@
         <v>136</v>
       </c>
       <c r="F208">
-        <v>-3.231949889919643</v>
+        <v>-3.231648893804923</v>
       </c>
       <c r="G208">
-        <v>-0.02316192626929275</v>
+        <v>-0.02286093015459117</v>
       </c>
     </row>
     <row r="209" spans="1:7">
@@ -5199,10 +5199,10 @@
         <v>137</v>
       </c>
       <c r="F209">
-        <v>-3.235317470156847</v>
+        <v>-3.234809940147318</v>
       </c>
       <c r="G209">
-        <v>-0.02050262750713219</v>
+        <v>-0.02101015751669322</v>
       </c>
     </row>
     <row r="210" spans="1:7">
@@ -5222,10 +5222,10 @@
         <v>138</v>
       </c>
       <c r="F210">
-        <v>-3.238177520384523</v>
+        <v>-3.236638208159643</v>
       </c>
       <c r="G210">
-        <v>-0.01885838876404511</v>
+        <v>-0.01782660654872453</v>
       </c>
     </row>
     <row r="211" spans="1:7">
@@ -5245,10 +5245,10 @@
         <v>139</v>
       </c>
       <c r="F211">
-        <v>-3.241037570612193</v>
+        <v>-3.24103757061219</v>
       </c>
       <c r="G211">
-        <v>-0.01619909000189521</v>
+        <v>-0.01721415002097867</v>
       </c>
     </row>
     <row r="212" spans="1:7">
@@ -5268,10 +5268,10 @@
         <v>140</v>
       </c>
       <c r="F212">
-        <v>-3.243897620839862</v>
+        <v>-3.243897620839866</v>
       </c>
       <c r="G212">
-        <v>-0.01455485125881051</v>
+        <v>-0.01506238126836154</v>
       </c>
     </row>
     <row r="213" spans="1:7">
@@ -5294,7 +5294,7 @@
         <v>-3.246757671067538</v>
       </c>
       <c r="G213">
-        <v>-0.0129106125157203</v>
+        <v>-0.0129106125157398</v>
       </c>
     </row>
     <row r="214" spans="1:7">
@@ -5314,10 +5314,10 @@
         <v>142</v>
       </c>
       <c r="F214">
-        <v>-3.249617721295208</v>
+        <v>-3.249617721295209</v>
       </c>
       <c r="G214">
-        <v>-0.01075884376309759</v>
+        <v>-0.01075884376311806</v>
       </c>
     </row>
     <row r="215" spans="1:7">
@@ -5337,10 +5337,10 @@
         <v>143</v>
       </c>
       <c r="F215">
-        <v>-3.252477771522878</v>
+        <v>-3.252477771522879</v>
       </c>
       <c r="G215">
-        <v>-0.008607075010473988</v>
+        <v>-0.008607075010494528</v>
       </c>
     </row>
     <row r="216" spans="1:7">
@@ -5363,7 +5363,7 @@
         <v>-3.255337821750548</v>
       </c>
       <c r="G216">
-        <v>-0.006455306257851269</v>
+        <v>-0.006455306257871454</v>
       </c>
     </row>
     <row r="217" spans="1:7">
@@ -5386,7 +5386,7 @@
         <v>-3.258197871978218</v>
       </c>
       <c r="G217">
-        <v>-0.004303537505227224</v>
+        <v>-0.00430353750524793</v>
       </c>
     </row>
     <row r="218" spans="1:7">
@@ -5409,7 +5409,7 @@
         <v>-3.261057922205887</v>
       </c>
       <c r="G218">
-        <v>-0.002151768752603176</v>
+        <v>-0.002151768752623965</v>
       </c>
     </row>
     <row r="219" spans="1:7">
@@ -5432,7 +5432,7 @@
         <v>-3.263917972433557</v>
       </c>
       <c r="G219">
-        <v>2.087219286295294e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:7">
@@ -5455,7 +5455,7 @@
         <v>-2.621703188588206</v>
       </c>
       <c r="G220">
-        <v>9.769962616701378e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:7">
@@ -5475,10 +5475,10 @@
         <v>30</v>
       </c>
       <c r="F221">
-        <v>-2.722883284473349</v>
+        <v>-2.721510722131381</v>
       </c>
       <c r="G221">
-        <v>-0.02546572494906751</v>
+        <v>-0.02560431675245223</v>
       </c>
     </row>
     <row r="222" spans="1:7">
@@ -5498,10 +5498,10 @@
         <v>61</v>
       </c>
       <c r="F222">
-        <v>-2.818575215466129</v>
+        <v>-2.816450490858558</v>
       </c>
       <c r="G222">
-        <v>-0.04534263269702832</v>
+        <v>-0.04386742812921618</v>
       </c>
     </row>
     <row r="223" spans="1:7">
@@ -5521,10 +5521,10 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.908422681011093</v>
+        <v>-2.906543125733036</v>
       </c>
       <c r="G223">
-        <v>-0.05916296093125939</v>
+        <v>-0.05728340565328049</v>
       </c>
     </row>
     <row r="224" spans="1:7">
@@ -5544,10 +5544,10 @@
         <v>123</v>
       </c>
       <c r="F224">
-        <v>-2.992003378767224</v>
+        <v>-2.99171354786893</v>
       </c>
       <c r="G224">
-        <v>-0.06585036778075026</v>
+        <v>-0.06577717043876063</v>
       </c>
     </row>
     <row r="225" spans="1:7">
@@ -5567,10 +5567,10 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.072479080212108</v>
+        <v>-3.071125763879544</v>
       </c>
       <c r="G225">
-        <v>-0.06706605855737169</v>
+        <v>-0.06851272909896111</v>
       </c>
     </row>
     <row r="226" spans="1:7">
@@ -5590,10 +5590,10 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.146565938076786</v>
+        <v>-3.146782647157709</v>
       </c>
       <c r="G226">
-        <v>-0.06526121734482282</v>
+        <v>-0.06749295502671293</v>
       </c>
     </row>
     <row r="227" spans="1:7">
@@ -5613,10 +5613,10 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.214451541346659</v>
+        <v>-3.213330466850168</v>
       </c>
       <c r="G227">
-        <v>-0.05795664270708345</v>
+        <v>-0.05736411736875813</v>
       </c>
     </row>
     <row r="228" spans="1:7">
@@ -5636,10 +5636,10 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.279026207044959</v>
+        <v>-3.277196299859827</v>
       </c>
       <c r="G228">
-        <v>-0.04533785168943294</v>
+        <v>-0.04455329302800359</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -5659,10 +5659,10 @@
         <v>278</v>
       </c>
       <c r="F229">
-        <v>-3.336342121179763</v>
+        <v>-3.336305831800731</v>
       </c>
       <c r="G229">
-        <v>-0.0256671702582969</v>
+        <v>-0.02698616761849393</v>
       </c>
     </row>
     <row r="230" spans="1:7">
@@ -5685,7 +5685,7 @@
         <v>-3.38599632153265</v>
       </c>
       <c r="G230">
-        <v>3.241851231905457e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:7">
@@ -5708,7 +5708,7 @@
         <v>-2.681923713795318</v>
       </c>
       <c r="G231">
-        <v>-2.708944180085382e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="232" spans="1:7">
@@ -5728,10 +5728,10 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.786641162844797</v>
+        <v>-2.785241004952843</v>
       </c>
       <c r="G232">
-        <v>-0.0260504758789617</v>
+        <v>-0.02527176346397342</v>
       </c>
     </row>
     <row r="233" spans="1:7">
@@ -5751,10 +5751,10 @@
         <v>112</v>
       </c>
       <c r="F233">
-        <v>-2.883619796906685</v>
+        <v>-2.88178318501804</v>
       </c>
       <c r="G233">
-        <v>-0.04479978674570084</v>
+        <v>-0.04376841583561886</v>
       </c>
     </row>
     <row r="234" spans="1:7">
@@ -5774,10 +5774,10 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.974608852494831</v>
+        <v>-2.974016186751373</v>
       </c>
       <c r="G234">
-        <v>-0.05827429943268769</v>
+        <v>-0.05795588987540001</v>
       </c>
     </row>
     <row r="235" spans="1:7">
@@ -5797,10 +5797,10 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.061133523790462</v>
+        <v>-3.059513041857866</v>
       </c>
       <c r="G235">
-        <v>-0.06582278144061338</v>
+        <v>-0.06540721728834087</v>
       </c>
     </row>
     <row r="236" spans="1:7">
@@ -5820,10 +5820,10 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.142823936029714</v>
+        <v>-3.141468331645823</v>
       </c>
       <c r="G236">
-        <v>-0.06949561329669662</v>
+        <v>-0.06931697938274617</v>
       </c>
     </row>
     <row r="237" spans="1:7">
@@ -5843,10 +5843,10 @@
         <v>336</v>
       </c>
       <c r="F237">
-        <v>-3.217457720738783</v>
+        <v>-3.216518542399338</v>
       </c>
       <c r="G237">
-        <v>-0.06595277541808997</v>
+        <v>-0.06632166244271054</v>
       </c>
     </row>
     <row r="238" spans="1:7">
@@ -5866,10 +5866,10 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.28799411061178</v>
+        <v>-3.286245268625959</v>
       </c>
       <c r="G238">
-        <v>-0.05809579843940671</v>
+        <v>-0.05800286097577989</v>
       </c>
     </row>
     <row r="239" spans="1:7">
@@ -5889,10 +5889,10 @@
         <v>448</v>
       </c>
       <c r="F239">
-        <v>-3.352339576189505</v>
+        <v>-3.351027618502251</v>
       </c>
       <c r="G239">
-        <v>-0.04490767497625925</v>
+        <v>-0.04473968315851939</v>
       </c>
     </row>
     <row r="240" spans="1:7">
@@ -5912,10 +5912,10 @@
         <v>504</v>
       </c>
       <c r="F240">
-        <v>-3.411836790186109</v>
+        <v>-3.411452841865691</v>
       </c>
       <c r="G240">
-        <v>-0.0275033271492377</v>
+        <v>-0.02711937882840842</v>
       </c>
     </row>
     <row r="241" spans="1:7">
@@ -5938,7 +5938,7 @@
         <v>-3.463772660868219</v>
       </c>
       <c r="G241">
-        <v>-4.547473508864641e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:7">
@@ -5961,7 +5961,7 @@
         <v>-2.723569122533946</v>
       </c>
       <c r="G242">
-        <v>-1.749711486809247e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:7">
@@ -5981,10 +5981,10 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.82912645721084</v>
+        <v>-2.827740477309618</v>
       </c>
       <c r="G243">
-        <v>-0.02641643856642695</v>
+        <v>-0.0250304586649932</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -6004,10 +6004,10 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.927573942591553</v>
+        <v>-2.925399438424117</v>
       </c>
       <c r="G244">
-        <v>-0.04572302783649684</v>
+        <v>-0.04354852366881445</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -6027,10 +6027,10 @@
         <v>276</v>
       </c>
       <c r="F245">
-        <v>-3.020058596200119</v>
+        <v>-3.018224530215806</v>
       </c>
       <c r="G245">
-        <v>-0.05906678533442067</v>
+        <v>-0.05723271934982499</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -6050,10 +6050,10 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.107922243180356</v>
+        <v>-3.105821067673915</v>
       </c>
       <c r="G246">
-        <v>-0.06625630939548288</v>
+        <v>-0.06482813356561712</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -6073,10 +6073,10 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.189330263160725</v>
+        <v>-3.188184808981283</v>
       </c>
       <c r="G247">
-        <v>-0.06824666094787357</v>
+        <v>-0.06805097876230648</v>
       </c>
     </row>
     <row r="248" spans="1:7">
@@ -6096,10 +6096,10 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.265868722777168</v>
+        <v>-3.266093010389055</v>
       </c>
       <c r="G248">
-        <v>-0.06560785152213766</v>
+        <v>-0.06681828405940005</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -6119,10 +6119,10 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.337453691927179</v>
+        <v>-3.336877591286729</v>
       </c>
       <c r="G249">
-        <v>-0.05816730207706311</v>
+        <v>-0.05760174171475763</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -6142,10 +6142,10 @@
         <v>738</v>
       </c>
       <c r="F250">
-        <v>-3.403825108517992</v>
+        <v>-3.403517360526654</v>
       </c>
       <c r="G250">
-        <v>-0.04504233741870345</v>
+        <v>-0.04510061484400452</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -6165,10 +6165,10 @@
         <v>830</v>
       </c>
       <c r="F251">
-        <v>-3.464021387393363</v>
+        <v>-3.463582307346689</v>
       </c>
       <c r="G251">
-        <v>-0.02616601496006538</v>
+        <v>-0.02602466555336047</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -6191,7 +6191,7 @@
         <v>-3.517558765035645</v>
       </c>
       <c r="G252">
-        <v>-5.364597654988756e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -6214,7 +6214,7 @@
         <v>-2.75405765035523</v>
       </c>
       <c r="G253">
-        <v>-2.713385072183883e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -6234,10 +6234,10 @@
         <v>141</v>
       </c>
       <c r="F254">
-        <v>-2.860059673078998</v>
+        <v>-2.858243375323748</v>
       </c>
       <c r="G254">
-        <v>-0.02599794278582923</v>
+        <v>-0.0241816450302621</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -6257,10 +6257,10 @@
         <v>283</v>
       </c>
       <c r="F255">
-        <v>-2.960422889495681</v>
+        <v>-2.95827432598797</v>
       </c>
       <c r="G255">
-        <v>-0.04578967444204585</v>
+        <v>-0.04364111093397272</v>
       </c>
     </row>
     <row r="256" spans="1:7">
@@ -6280,10 +6280,10 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.053733506929513</v>
+        <v>-3.051876142218384</v>
       </c>
       <c r="G256">
-        <v>-0.05903582312151201</v>
+        <v>-0.05723884722613048</v>
       </c>
     </row>
     <row r="257" spans="1:7">
@@ -6303,10 +6303,10 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.141807741588365</v>
+        <v>-3.140443944612575</v>
       </c>
       <c r="G257">
-        <v>-0.06659896183605385</v>
+        <v>-0.06523516485980907</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -6326,10 +6326,10 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.22367762687283</v>
+        <v>-3.223560836956544</v>
       </c>
       <c r="G258">
-        <v>-0.06846476718230954</v>
+        <v>-0.06834797726552355</v>
       </c>
     </row>
     <row r="259" spans="1:7">
@@ -6349,10 +6349,10 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.301891683843066</v>
+        <v>-3.300776031133399</v>
       </c>
       <c r="G259">
-        <v>-0.06543527498148838</v>
+        <v>-0.06499168668186583</v>
       </c>
     </row>
     <row r="260" spans="1:7">
@@ -6372,10 +6372,10 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.37378244914177</v>
+        <v>-3.373227744413447</v>
       </c>
       <c r="G260">
-        <v>-0.05726230869625171</v>
+        <v>-0.05743932002365837</v>
       </c>
     </row>
     <row r="261" spans="1:7">
@@ -6395,10 +6395,10 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.440577904916151</v>
+        <v>-3.440303181694261</v>
       </c>
       <c r="G261">
-        <v>-0.04321905106294766</v>
+        <v>-0.04394327254395969</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -6418,10 +6418,10 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.502404158640303</v>
+        <v>-3.50162754945332</v>
       </c>
       <c r="G262">
-        <v>-0.02578450275888</v>
+        <v>-0.0252635603647639</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -6444,7 +6444,7 @@
         <v>-3.556935473849069</v>
       </c>
       <c r="G263">
-        <v>-7.287503933639528e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -6467,7 +6467,7 @@
         <v>-2.777331564852105</v>
       </c>
       <c r="G264">
-        <v>-3.486100297322992e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -6487,10 +6487,10 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.883834134956935</v>
+        <v>-2.882085517278409</v>
       </c>
       <c r="G265">
-        <v>-0.02560140123570509</v>
+        <v>-0.0240632056775123</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -6510,10 +6510,10 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.984780872604509</v>
+        <v>-2.982419887251812</v>
       </c>
       <c r="G266">
-        <v>-0.04567420085646967</v>
+        <v>-0.04331321550334977</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -6533,10 +6533,10 @@
         <v>617</v>
       </c>
       <c r="F267">
-        <v>-3.079188729776575</v>
+        <v>-3.076507397946806</v>
       </c>
       <c r="G267">
-        <v>-0.05899769788100717</v>
+        <v>-0.05631636605077839</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -6556,10 +6556,10 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.166588136695935</v>
+        <v>-3.165436669974895</v>
       </c>
       <c r="G268">
-        <v>-0.06570635805161285</v>
+        <v>-0.06455489133007597</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -6579,10 +6579,10 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.249935804537984</v>
+        <v>-3.249772890711616</v>
       </c>
       <c r="G269">
-        <v>-0.06734220799904622</v>
+        <v>-0.06780675191923091</v>
       </c>
     </row>
     <row r="270" spans="1:7">
@@ -6602,10 +6602,10 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.32850040435183</v>
+        <v>-3.327248020091443</v>
       </c>
       <c r="G270">
-        <v>-0.06481872284724788</v>
+        <v>-0.06419752115149246</v>
       </c>
     </row>
     <row r="271" spans="1:7">
@@ -6625,10 +6625,10 @@
         <v>1439</v>
       </c>
       <c r="F271">
-        <v>-3.401012162470983</v>
+        <v>-3.400622653892166</v>
       </c>
       <c r="G271">
-        <v>-0.05727091678284846</v>
+        <v>-0.05688140820342391</v>
       </c>
     </row>
     <row r="272" spans="1:7">
@@ -6648,10 +6648,10 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.468659184933812</v>
+        <v>-3.468702984681467</v>
       </c>
       <c r="G272">
-        <v>-0.04341253589937355</v>
+        <v>-0.04387737884515908</v>
       </c>
     </row>
     <row r="273" spans="1:7">
@@ -6671,10 +6671,10 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.531263580488339</v>
+        <v>-3.530575857990558</v>
       </c>
       <c r="G273">
-        <v>-0.0253536145051475</v>
+        <v>-0.02466589200668384</v>
       </c>
     </row>
     <row r="274" spans="1:7">
@@ -6697,7 +6697,7 @@
         <v>-3.586994326131439</v>
       </c>
       <c r="G274">
-        <v>-7.189804307472514e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="275" spans="1:7">
@@ -6720,7 +6720,7 @@
         <v>-2.795675378544225</v>
       </c>
       <c r="G275">
-        <v>-4.929390229335695e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="276" spans="1:7">
@@ -6740,10 +6740,10 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.902589304494746</v>
+        <v>-2.900989963076124</v>
       </c>
       <c r="G276">
-        <v>-0.02566854828954579</v>
+        <v>-0.02406920687054059</v>
       </c>
     </row>
     <row r="277" spans="1:7">
@@ -6763,10 +6763,10 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.003366860659705</v>
+        <v>-3.000726409056423</v>
       </c>
       <c r="G277">
-        <v>-0.04491665204596718</v>
+        <v>-0.04227620044241398</v>
       </c>
     </row>
     <row r="278" spans="1:7">
@@ -6786,10 +6786,10 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.09806165848084</v>
+        <v>-3.096058483857597</v>
       </c>
       <c r="G278">
-        <v>-0.05806017504645355</v>
+        <v>-0.05607882283516297</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -6809,10 +6809,10 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.186897355445425</v>
+        <v>-3.184691001597194</v>
       </c>
       <c r="G279">
-        <v>-0.06538824201461524</v>
+        <v>-0.06318188816633419</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -6832,10 +6832,10 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.269791337516753</v>
+        <v>-3.269256825465189</v>
       </c>
       <c r="G280">
-        <v>-0.06675277167740656</v>
+        <v>-0.06621825962590311</v>
       </c>
     </row>
     <row r="281" spans="1:7">
@@ -6855,10 +6855,10 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.348727118902105</v>
+        <v>-3.348557961400317</v>
       </c>
       <c r="G281">
-        <v>-0.06351486964996411</v>
+        <v>-0.06398994315260564</v>
       </c>
     </row>
     <row r="282" spans="1:7">
@@ -6878,10 +6878,10 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.422448330837314</v>
+        <v>-3.422224973593063</v>
       </c>
       <c r="G282">
-        <v>-0.0560346378298906</v>
+        <v>-0.05612750293692592</v>
       </c>
     </row>
     <row r="283" spans="1:7">
@@ -6901,10 +6901,10 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.490785261989347</v>
+        <v>-3.49058572605642</v>
       </c>
       <c r="G283">
-        <v>-0.04278662283956813</v>
+        <v>-0.04295880299185728</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -6924,10 +6924,10 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.553992063324459</v>
+        <v>-3.553629376809089</v>
       </c>
       <c r="G284">
-        <v>-0.02463314838813591</v>
+        <v>-0.0244730013361007</v>
       </c>
     </row>
     <row r="285" spans="1:7">
@@ -6950,7 +6950,7 @@
         <v>-3.610685827881414</v>
       </c>
       <c r="G285">
-        <v>6.146194664324867e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:7">
@@ -6973,7 +6973,7 @@
         <v>-2.810502834325307</v>
       </c>
       <c r="G286">
-        <v>1.34869893031464e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:7">
@@ -6993,10 +6993,10 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.917829764749651</v>
+        <v>-2.916094948776097</v>
       </c>
       <c r="G287">
-        <v>-0.02535311932536111</v>
+        <v>-0.02367997741095973</v>
       </c>
     </row>
     <row r="288" spans="1:7">
@@ -7016,10 +7016,10 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.019116119926947</v>
+        <v>-3.016840117319153</v>
       </c>
       <c r="G288">
-        <v>-0.04478901152046033</v>
+        <v>-0.04251300891418719</v>
       </c>
     </row>
     <row r="289" spans="1:7">
@@ -7039,10 +7039,10 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.114091083524233</v>
+        <v>-3.111757161510439</v>
       </c>
       <c r="G289">
-        <v>-0.05785183807782968</v>
+        <v>-0.05551791606564294</v>
       </c>
     </row>
     <row r="290" spans="1:7">
@@ -7062,10 +7062,10 @@
         <v>1548</v>
       </c>
       <c r="F290">
-        <v>-3.203156986817808</v>
+        <v>-3.201150424798553</v>
       </c>
       <c r="G290">
-        <v>-0.0650056043314895</v>
+        <v>-0.06299904231392772</v>
       </c>
     </row>
     <row r="291" spans="1:7">
@@ -7085,10 +7085,10 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.286102204651301</v>
+        <v>-3.28564389761307</v>
       </c>
       <c r="G291">
-        <v>-0.06577419618658276</v>
+        <v>-0.0655803780886155</v>
       </c>
     </row>
     <row r="292" spans="1:7">
@@ -7108,10 +7108,10 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.365351565903648</v>
+        <v>-3.365015206725004</v>
       </c>
       <c r="G292">
-        <v>-0.06333436743314813</v>
+        <v>-0.06303955016071905</v>
       </c>
     </row>
     <row r="293" spans="1:7">
@@ -7131,10 +7131,10 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.43936464679758</v>
+        <v>-3.439037917844733</v>
       </c>
       <c r="G293">
-        <v>-0.05488108393260571</v>
+        <v>-0.05515012424061883</v>
       </c>
     </row>
     <row r="294" spans="1:7">
@@ -7154,10 +7154,10 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.508522403612005</v>
+        <v>-3.508167108257353</v>
       </c>
       <c r="G294">
-        <v>-0.04237685235887212</v>
+        <v>-0.04236717761340913</v>
       </c>
     </row>
     <row r="295" spans="1:7">
@@ -7177,10 +7177,10 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.572229444572814</v>
+        <v>-3.572203588368217</v>
       </c>
       <c r="G295">
-        <v>-0.02429245603436292</v>
+        <v>-0.02449152068444382</v>
       </c>
     </row>
     <row r="296" spans="1:7">
@@ -7203,7 +7203,7 @@
         <v>-3.62983586399244</v>
       </c>
       <c r="G296">
-        <v>2.210676086633612e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="297" spans="1:7">
@@ -7226,7 +7226,7 @@
         <v>-2.822735089670116</v>
       </c>
       <c r="G297">
-        <v>3.202771381438652e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298" spans="1:7">
@@ -7246,10 +7246,10 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.930150712318684</v>
+        <v>-2.928550245428536</v>
       </c>
       <c r="G298">
-        <v>-0.02517428605472638</v>
+        <v>-0.02357381916767043</v>
       </c>
     </row>
     <row r="299" spans="1:7">
@@ -7269,10 +7269,10 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.031598174513073</v>
+        <v>-3.029230465649422</v>
       </c>
       <c r="G299">
-        <v>-0.0443804116584765</v>
+        <v>-0.04201270279780811</v>
       </c>
     </row>
     <row r="300" spans="1:7">
@@ -7292,10 +7292,10 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.126639482795215</v>
+        <v>-3.123766442911127</v>
       </c>
       <c r="G300">
-        <v>-0.05709426266311346</v>
+        <v>-0.0543073434687642</v>
       </c>
     </row>
     <row r="301" spans="1:7">
@@ -7315,10 +7315,10 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.215341021749714</v>
+        <v>-3.214053777474791</v>
       </c>
       <c r="G301">
-        <v>-0.06343626811340775</v>
+        <v>-0.06219144904681673</v>
       </c>
     </row>
     <row r="302" spans="1:7">
@@ -7338,10 +7338,10 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.299421340991911</v>
+        <v>-3.299142821772032</v>
       </c>
       <c r="G302">
-        <v>-0.06494055916953889</v>
+        <v>-0.06503915675330885</v>
       </c>
     </row>
     <row r="303" spans="1:7">
@@ -7361,10 +7361,10 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.379059655974281</v>
+        <v>-3.378714907612919</v>
       </c>
       <c r="G303">
-        <v>-0.06178510148360083</v>
+        <v>-0.06236990600344705</v>
       </c>
     </row>
     <row r="304" spans="1:7">
@@ -7384,10 +7384,10 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.453466960289215</v>
+        <v>-3.453395595239973</v>
       </c>
       <c r="G304">
-        <v>-0.05432673206147376</v>
+        <v>-0.05464736464488806</v>
       </c>
     </row>
     <row r="305" spans="1:7">
@@ -7407,10 +7407,10 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.523186693574442</v>
+        <v>-3.523194756241369</v>
       </c>
       <c r="G305">
-        <v>-0.04181348491829107</v>
+        <v>-0.04220518905553605</v>
       </c>
     </row>
     <row r="306" spans="1:7">
@@ -7430,10 +7430,10 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.587297600076772</v>
+        <v>-3.587182006673184</v>
       </c>
       <c r="G306">
-        <v>-0.02398586397592811</v>
+        <v>-0.02395110289660207</v>
       </c>
     </row>
     <row r="307" spans="1:7">
@@ -7456,7 +7456,7 @@
         <v>-3.645634132762194</v>
       </c>
       <c r="G307">
-        <v>2.102762408640046e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="308" spans="1:7">
@@ -7479,7 +7479,7 @@
         <v>-2.832997797458318</v>
       </c>
       <c r="G308">
-        <v>2.922551090023262e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="309" spans="1:7">
@@ -7499,10 +7499,10 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.940407304814413</v>
+        <v>-2.938908684353428</v>
       </c>
       <c r="G309">
-        <v>-0.02488370567813858</v>
+        <v>-0.02338508521976257</v>
       </c>
     </row>
     <row r="310" spans="1:7">
@@ -7522,10 +7522,10 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.042350921711773</v>
+        <v>-3.039465975634541</v>
       </c>
       <c r="G310">
-        <v>-0.04417494758501173</v>
+        <v>-0.04129000151007567</v>
       </c>
     </row>
     <row r="311" spans="1:7">
@@ -7545,10 +7545,10 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.137321672576231</v>
+        <v>-3.134907091146637</v>
       </c>
       <c r="G311">
-        <v>-0.05661989677443646</v>
+        <v>-0.05420531534682338</v>
       </c>
     </row>
     <row r="312" spans="1:7">
@@ -7568,10 +7568,10 @@
         <v>2610</v>
       </c>
       <c r="F312">
-        <v>-3.227025837417122</v>
+        <v>-3.224950462906559</v>
       </c>
       <c r="G312">
-        <v>-0.06346194717853337</v>
+        <v>-0.06159631211594552</v>
       </c>
     </row>
     <row r="313" spans="1:7">
@@ -7591,10 +7591,10 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.310122949175367</v>
+        <v>-3.309853324480303</v>
       </c>
       <c r="G313">
-        <v>-0.06424299670805111</v>
+        <v>-0.06397337201434161</v>
       </c>
     </row>
     <row r="314" spans="1:7">
@@ -7614,10 +7614,10 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.3902917913971</v>
+        <v>-3.389970993876977</v>
       </c>
       <c r="G314">
-        <v>-0.06136042568945133</v>
+        <v>-0.061438666420216</v>
       </c>
     </row>
     <row r="315" spans="1:7">
@@ -7637,10 +7637,10 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.465353046047447</v>
+        <v>-3.465049183776194</v>
       </c>
       <c r="G315">
-        <v>-0.05419071372997042</v>
+        <v>-0.05399105464408593</v>
       </c>
     </row>
     <row r="316" spans="1:7">
@@ -7660,10 +7660,10 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.535332709001385</v>
+        <v>-3.535028743434018</v>
       </c>
       <c r="G316">
-        <v>-0.04128817195466283</v>
+        <v>-0.0413182393111089</v>
       </c>
     </row>
     <row r="317" spans="1:7">
@@ -7683,10 +7683,10 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.600009324462675</v>
+        <v>-3.599959312422064</v>
       </c>
       <c r="G317">
-        <v>-0.02362099063037559</v>
+        <v>-0.02372300662380827</v>
       </c>
     </row>
     <row r="318" spans="1:7">
@@ -7709,7 +7709,7 @@
         <v>-3.658888680789056</v>
       </c>
       <c r="G318">
-        <v>-2.140509991477302e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:7">
@@ -7732,7 +7732,7 @@
         <v>-2.841730677199684</v>
       </c>
       <c r="G319">
-        <v>5.155875726359227e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="320" spans="1:7">
@@ -7752,10 +7752,10 @@
         <v>821</v>
       </c>
       <c r="F320">
-        <v>-2.949253146015495</v>
+        <v>-2.947885710296204</v>
       </c>
       <c r="G320">
-        <v>-0.02441997394645989</v>
+        <v>-0.0233819330146412</v>
       </c>
     </row>
     <row r="321" spans="1:7">
@@ -7775,10 +7775,10 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.050969621063596</v>
+        <v>-3.048636987068577</v>
       </c>
       <c r="G321">
-        <v>-0.04341652277900776</v>
+        <v>-0.0412592898511992</v>
       </c>
     </row>
     <row r="322" spans="1:7">
@@ -7798,10 +7798,10 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.146426033763205</v>
+        <v>-3.143577998573606</v>
       </c>
       <c r="G322">
-        <v>-0.05591410420217802</v>
+        <v>-0.05332638142041324</v>
       </c>
     </row>
     <row r="323" spans="1:7">
@@ -7821,10 +7821,10 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.236036412347025</v>
+        <v>-3.23402273830819</v>
       </c>
       <c r="G323">
-        <v>-0.0628211651718027</v>
+        <v>-0.06099802107311758</v>
       </c>
     </row>
     <row r="324" spans="1:7">
@@ -7844,10 +7844,10 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.320001931522911</v>
+        <v>-3.319427249167131</v>
       </c>
       <c r="G324">
-        <v>-0.0641032943526858</v>
+        <v>-0.06352861199624371</v>
       </c>
     </row>
     <row r="325" spans="1:7">
@@ -7867,10 +7867,10 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.399906986430935</v>
+        <v>-3.399732419225027</v>
       </c>
       <c r="G325">
-        <v>-0.06113442932512947</v>
+        <v>-0.06095986211832471</v>
       </c>
     </row>
     <row r="326" spans="1:7">
@@ -7890,10 +7890,10 @@
         <v>5751</v>
       </c>
       <c r="F326">
-        <v>-3.475207043901229</v>
+        <v>-3.475186578979213</v>
       </c>
       <c r="G326">
-        <v>-0.05361299538312403</v>
+        <v>-0.05364092179063251</v>
       </c>
     </row>
     <row r="327" spans="1:7">
@@ -7913,10 +7913,10 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.545674978592156</v>
+        <v>-3.545289680831317</v>
       </c>
       <c r="G327">
-        <v>-0.04081394392064219</v>
+        <v>-0.04087010370692101</v>
       </c>
     </row>
     <row r="328" spans="1:7">
@@ -7936,10 +7936,10 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.610725135587206</v>
+        <v>-3.610687399680431</v>
       </c>
       <c r="G328">
-        <v>-0.02337751331525639</v>
+        <v>-0.02339390262022029</v>
       </c>
     </row>
     <row r="329" spans="1:7">
@@ -7962,7 +7962,7 @@
         <v>-3.670167416996026</v>
       </c>
       <c r="G329">
-        <v>-1.838973417989109e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="330" spans="1:7">
@@ -7985,7 +7985,7 @@
         <v>-2.849251743705888</v>
       </c>
       <c r="G330">
-        <v>-1.424194095989151e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331" spans="1:7">
@@ -8005,10 +8005,10 @@
         <v>1017</v>
       </c>
       <c r="F331">
-        <v>-2.956700952756041</v>
+        <v>-2.955287275856456</v>
       </c>
       <c r="G331">
-        <v>-0.02445971888893883</v>
+        <v>-0.02304604198804938</v>
       </c>
     </row>
     <row r="332" spans="1:7">
@@ -8028,10 +8028,10 @@
         <v>2035</v>
       </c>
       <c r="F332">
-        <v>-3.058078837091159</v>
+        <v>-3.056157781381454</v>
       </c>
       <c r="G332">
-        <v>-0.04276651080953853</v>
+        <v>-0.04084545509864856</v>
       </c>
     </row>
     <row r="333" spans="1:7">
@@ -8051,10 +8051,10 @@
         <v>3053</v>
       </c>
       <c r="F333">
-        <v>-3.153818088210635</v>
+        <v>-3.151555598695108</v>
       </c>
       <c r="G333">
-        <v>-0.05543466951449516</v>
+        <v>-0.05317217999790391</v>
       </c>
     </row>
     <row r="334" spans="1:7">
@@ -8074,10 +8074,10 @@
         <v>4071</v>
       </c>
       <c r="F334">
-        <v>-3.243538607131324</v>
+        <v>-3.242025773038145</v>
       </c>
       <c r="G334">
-        <v>-0.06208409602066611</v>
+        <v>-0.06057126192654172</v>
       </c>
     </row>
     <row r="335" spans="1:7">
@@ -8097,10 +8097,10 @@
         <v>5089</v>
       </c>
       <c r="F335">
-        <v>-3.327963624302047</v>
+        <v>-3.327312774157283</v>
       </c>
       <c r="G335">
-        <v>-0.06343802077687055</v>
+        <v>-0.06278717063128125</v>
       </c>
     </row>
     <row r="336" spans="1:7">
@@ -8120,10 +8120,10 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.408173956440033</v>
+        <v>-3.408101752218418</v>
       </c>
       <c r="G336">
-        <v>-0.06041169046913186</v>
+        <v>-0.06050505627801783</v>
       </c>
     </row>
     <row r="337" spans="1:7">
@@ -8143,10 +8143,10 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.483774545765198</v>
+        <v>-3.483532286888218</v>
       </c>
       <c r="G337">
-        <v>-0.0531067574109837</v>
+        <v>-0.05286449853341879</v>
       </c>
     </row>
     <row r="338" spans="1:7">
@@ -8166,10 +8166,10 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.554475767915689</v>
+        <v>-3.554270606692177</v>
       </c>
       <c r="G338">
-        <v>-0.04061472443527936</v>
+        <v>-0.04053172592297882</v>
       </c>
     </row>
     <row r="339" spans="1:7">
@@ -8189,10 +8189,10 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.620028388592467</v>
+        <v>-3.619917485418374</v>
       </c>
       <c r="G339">
-        <v>-0.02298485002555933</v>
+        <v>-0.02310751223477731</v>
       </c>
     </row>
     <row r="340" spans="1:7">
@@ -8215,7 +8215,7 @@
         <v>-3.679881065597996</v>
       </c>
       <c r="G340">
-        <v>-2.251532293939817e-13</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data from 02.24.2019
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -875,7 +875,7 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <v>-2.446304268323845</v>
+        <v>-2.446861267673398</v>
       </c>
       <c r="G21">
         <v>-0.02512155297761609</v>
@@ -898,7 +898,7 @@
         <v>6</v>
       </c>
       <c r="F22">
-        <v>-2.462427224205399</v>
+        <v>-2.463904837203008</v>
       </c>
       <c r="G22">
         <v>-0.02874245461000902</v>
@@ -921,7 +921,7 @@
         <v>7</v>
       </c>
       <c r="F23">
-        <v>-2.477545100240395</v>
+        <v>-2.479022713238004</v>
       </c>
       <c r="G23">
         <v>-0.03135827639584443</v>
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>-2.49290964075193</v>
+        <v>-2.494387253749535</v>
       </c>
       <c r="G24">
         <v>-0.03422076265821916</v>
@@ -990,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="F26">
-        <v>-2.524594621703169</v>
+        <v>-2.524816390870587</v>
       </c>
       <c r="G26">
         <v>-0.04090163511113665</v>
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.539457802292218</v>
+        <v>-2.540382347402589</v>
       </c>
       <c r="G27">
         <v>-0.04326276145102503</v>
@@ -1059,7 +1059,7 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <v>-2.568573096154417</v>
+        <v>-2.5698312999862</v>
       </c>
       <c r="G29">
         <v>-0.04737394681490215</v>
@@ -1082,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <v>-2.584768113147685</v>
+        <v>-2.584897468056439</v>
       </c>
       <c r="G30">
         <v>-0.0510669095590095</v>
@@ -1105,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="F31">
-        <v>-2.597537947112877</v>
+        <v>-2.599575654309668</v>
       </c>
       <c r="G31">
         <v>-0.05133468927504103</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.61253924598982</v>
+        <v>-2.612952376921871</v>
       </c>
       <c r="G32">
         <v>-0.05383393390282332</v>
@@ -1151,7 +1151,7 @@
         <v>17</v>
       </c>
       <c r="F33">
-        <v>-2.6267471373837</v>
+        <v>-2.62832467198693</v>
       </c>
       <c r="G33">
         <v>-0.05553977104754271</v>
@@ -1174,7 +1174,7 @@
         <v>18</v>
       </c>
       <c r="F34">
-        <v>-2.640309169555353</v>
+        <v>-2.641710308943922</v>
       </c>
       <c r="G34">
         <v>-0.05659974897003517</v>
@@ -1220,7 +1220,7 @@
         <v>20</v>
       </c>
       <c r="F36">
-        <v>-2.668959398600806</v>
+        <v>-2.670698443594537</v>
       </c>
       <c r="G36">
         <v>-0.06024586951716659</v>
@@ -1266,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="F38">
-        <v>-2.697067098099584</v>
+        <v>-2.698171662420433</v>
       </c>
       <c r="G38">
         <v>-0.06334946051762347</v>
@@ -1289,7 +1289,7 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.709857285211729</v>
+        <v>-2.710478063328874</v>
       </c>
       <c r="G39">
         <v>-0.06363759338060815</v>
@@ -1312,7 +1312,7 @@
         <v>24</v>
       </c>
       <c r="F40">
-        <v>-2.723283836822127</v>
+        <v>-2.723348593903957</v>
       </c>
       <c r="G40">
         <v>-0.06456209074184449</v>
@@ -1335,7 +1335,7 @@
         <v>25</v>
       </c>
       <c r="F41">
-        <v>-2.735913020087091</v>
+        <v>-2.736788718405263</v>
       </c>
       <c r="G41">
         <v>-0.06468921975764808</v>
@@ -1358,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.74705566266379</v>
+        <v>-2.749073675741039</v>
       </c>
       <c r="G42">
         <v>-0.06332980808518607</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.760142979523824</v>
+        <v>-2.762216332470147</v>
       </c>
       <c r="G43">
         <v>-0.06391507069606006</v>
@@ -1427,7 +1427,7 @@
         <v>29</v>
       </c>
       <c r="F45">
-        <v>-2.786490536389025</v>
+        <v>-2.786789765434675</v>
       </c>
       <c r="G45">
         <v>-0.06525851906293978</v>
@@ -1450,7 +1450,7 @@
         <v>30</v>
       </c>
       <c r="F46">
-        <v>-2.797612427495173</v>
+        <v>-2.798883286202902</v>
       </c>
       <c r="G46">
         <v>-0.06387835591992652</v>
@@ -1473,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="F47">
-        <v>-2.808710017122225</v>
+        <v>-2.810595484048786</v>
       </c>
       <c r="G47">
         <v>-0.06247389129781755</v>
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.82098743602109</v>
+        <v>-2.822759225816332</v>
       </c>
       <c r="G48">
         <v>-0.06224925594752295</v>
@@ -1519,7 +1519,7 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.832109733207955</v>
+        <v>-2.832956532957937</v>
       </c>
       <c r="G49">
         <v>-0.06086949888522653</v>
@@ -1542,7 +1542,7 @@
         <v>34</v>
       </c>
       <c r="F50">
-        <v>-2.845704977870266</v>
+        <v>-2.846633632435351</v>
       </c>
       <c r="G50">
         <v>-0.06196268929837656</v>
@@ -1565,7 +1565,7 @@
         <v>35</v>
       </c>
       <c r="F51">
-        <v>-2.857196554559008</v>
+        <v>-2.857331486028856</v>
       </c>
       <c r="G51">
         <v>-0.06095221173795851</v>
@@ -1588,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.867976202668343</v>
+        <v>-2.868067032127506</v>
       </c>
       <c r="G52">
         <v>-0.05922980559813218</v>
@@ -1634,7 +1634,7 @@
         <v>38</v>
       </c>
       <c r="F54">
-        <v>-2.889482603130103</v>
+        <v>-2.8904558294191</v>
       </c>
       <c r="G54">
         <v>-0.05573209756157105</v>
@@ -1680,7 +1680,7 @@
         <v>40</v>
       </c>
       <c r="F56">
-        <v>-2.910308070512214</v>
+        <v>-2.911971083926363</v>
       </c>
       <c r="G56">
         <v>-0.05155345644536014</v>
@@ -1703,7 +1703,7 @@
         <v>41</v>
       </c>
       <c r="F57">
-        <v>-2.921065697765848</v>
+        <v>-2.921908245050409</v>
       </c>
       <c r="G57">
         <v>-0.04980902944983412</v>
@@ -1726,7 +1726,7 @@
         <v>42</v>
       </c>
       <c r="F58">
-        <v>-2.930209338565391</v>
+        <v>-2.931719389049388</v>
       </c>
       <c r="G58">
         <v>-0.04645061600021683</v>
@@ -1749,7 +1749,7 @@
         <v>43</v>
       </c>
       <c r="F59">
-        <v>-2.941616640328895</v>
+        <v>-2.942211405828743</v>
       </c>
       <c r="G59">
         <v>-0.04535586351456022</v>
@@ -1772,7 +1772,7 @@
         <v>44</v>
       </c>
       <c r="F60">
-        <v>-2.951402456055571</v>
+        <v>-2.952261417267655</v>
       </c>
       <c r="G60">
         <v>-0.04263962499207485</v>
@@ -1795,7 +1795,7 @@
         <v>45</v>
       </c>
       <c r="F61">
-        <v>-2.961108249322421</v>
+        <v>-2.961806950792357</v>
       </c>
       <c r="G61">
         <v>-0.03984336400976435</v>
@@ -1818,7 +1818,7 @@
         <v>46</v>
       </c>
       <c r="F62">
-        <v>-2.970036936192296</v>
+        <v>-2.970766633161993</v>
       </c>
       <c r="G62">
         <v>-0.03626999663047809</v>
@@ -1864,7 +1864,7 @@
         <v>48</v>
       </c>
       <c r="F64">
-        <v>-2.988685997901257</v>
+        <v>-2.988829843715888</v>
       </c>
       <c r="G64">
         <v>-0.02991494984111792</v>
@@ -2163,7 +2163,7 @@
         <v>5</v>
       </c>
       <c r="F77">
-        <v>-2.563777160051407</v>
+        <v>-2.564076727455178</v>
       </c>
       <c r="G77">
         <v>-0.01153748281947342</v>
@@ -2186,7 +2186,7 @@
         <v>6</v>
       </c>
       <c r="F78">
-        <v>-2.570693012148764</v>
+        <v>-2.57071956367952</v>
       </c>
       <c r="G78">
         <v>-0.01344151593653731</v>
@@ -2209,7 +2209,7 @@
         <v>7</v>
       </c>
       <c r="F79">
-        <v>-2.577214465065385</v>
+        <v>-2.577661967307641</v>
       </c>
       <c r="G79">
         <v>-0.01495114987286561</v>
@@ -2232,7 +2232,7 @@
         <v>8</v>
       </c>
       <c r="F80">
-        <v>-2.584251700470463</v>
+        <v>-2.584577819404997</v>
       </c>
       <c r="G80">
         <v>-0.01697656629765065</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <v>-2.597362548723772</v>
+        <v>-2.597590475980668</v>
       </c>
       <c r="G82">
         <v>-0.02006377659037284</v>
@@ -2301,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="F83">
-        <v>-2.604783041677857</v>
+        <v>-2.605025808293304</v>
       </c>
       <c r="G83">
         <v>-0.02247245056416469</v>
@@ -2324,7 +2324,7 @@
         <v>12</v>
       </c>
       <c r="F84">
-        <v>-2.610354619475546</v>
+        <v>-2.610802121717799</v>
       </c>
       <c r="G84">
         <v>-0.02303220938156114</v>
@@ -2347,7 +2347,7 @@
         <v>13</v>
       </c>
       <c r="F85">
-        <v>-2.615473446191409</v>
+        <v>-2.617220728412067</v>
       </c>
       <c r="G85">
         <v>-0.02313921711713052</v>
@@ -2370,7 +2370,7 @@
         <v>14</v>
       </c>
       <c r="F86">
-        <v>-2.622653167569458</v>
+        <v>-2.62326409200272</v>
       </c>
       <c r="G86">
         <v>-0.02530711951488618</v>
@@ -2393,7 +2393,7 @@
         <v>15</v>
       </c>
       <c r="F87">
-        <v>-2.628866613989982</v>
+        <v>-2.630884699251327</v>
       </c>
       <c r="G87">
         <v>-0.02650874695511796</v>
@@ -2416,7 +2416,7 @@
         <v>16</v>
       </c>
       <c r="F88">
-        <v>-2.636513288796895</v>
+        <v>-2.636775642969768</v>
       </c>
       <c r="G88">
         <v>-0.02914360278173733</v>
@@ -2439,7 +2439,7 @@
         <v>17</v>
       </c>
       <c r="F89">
-        <v>-2.641131912824005</v>
+        <v>-2.642327393259413</v>
       </c>
       <c r="G89">
         <v>-0.02875040782855365</v>
@@ -2462,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="F90">
-        <v>-2.648536988686376</v>
+        <v>-2.649258199078582</v>
       </c>
       <c r="G90">
         <v>-0.03114366471063246</v>
@@ -2485,7 +2485,7 @@
         <v>19</v>
       </c>
       <c r="F91">
-        <v>-2.654932713960276</v>
+        <v>-2.656231428174714</v>
       </c>
       <c r="G91">
         <v>-0.03252757100423942</v>
@@ -2508,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.660213666698697</v>
+        <v>-2.661230894164726</v>
       </c>
       <c r="G92">
         <v>-0.03279670476236696</v>
@@ -2531,7 +2531,7 @@
         <v>21</v>
       </c>
       <c r="F93">
-        <v>-2.666267390704045</v>
+        <v>-2.667951659094491</v>
       </c>
       <c r="G93">
         <v>-0.0338386097874217</v>
@@ -2577,7 +2577,7 @@
         <v>23</v>
       </c>
       <c r="F95">
-        <v>-2.680062279369086</v>
+        <v>-2.680564242120132</v>
       </c>
       <c r="G95">
         <v>-0.0376098604918762</v>
@@ -2600,7 +2600,7 @@
         <v>24</v>
       </c>
       <c r="F96">
-        <v>-2.685958492529633</v>
+        <v>-2.6862469887413</v>
       </c>
       <c r="G96">
         <v>-0.03849425467213008</v>
@@ -2623,7 +2623,7 @@
         <v>25</v>
       </c>
       <c r="F97">
-        <v>-2.690727542699385</v>
+        <v>-2.692656297317452</v>
       </c>
       <c r="G97">
         <v>-0.03825148586158944</v>
@@ -2646,7 +2646,7 @@
         <v>26</v>
       </c>
       <c r="F98">
-        <v>-2.696563605339872</v>
+        <v>-2.698894327306781</v>
       </c>
       <c r="G98">
         <v>-0.03907572952178295</v>
@@ -2715,7 +2715,7 @@
         <v>29</v>
       </c>
       <c r="F101">
-        <v>-2.715060201262196</v>
+        <v>-2.717517562597841</v>
       </c>
       <c r="G101">
         <v>-0.04253686850322724</v>
@@ -2738,7 +2738,7 @@
         <v>30</v>
       </c>
       <c r="F102">
-        <v>-2.722233892144196</v>
+        <v>-2.72225596236469</v>
       </c>
       <c r="G102">
         <v>-0.04469874040493416</v>
@@ -2761,7 +2761,7 @@
         <v>31</v>
       </c>
       <c r="F103">
-        <v>-2.72794516755145</v>
+        <v>-2.72858095934013</v>
       </c>
       <c r="G103">
         <v>-0.04539819683189528</v>
@@ -2853,7 +2853,7 @@
         <v>35</v>
       </c>
       <c r="F107">
-        <v>-2.752003868543535</v>
+        <v>-2.752549955996056</v>
       </c>
       <c r="G107">
         <v>-0.04940962190280773</v>
@@ -2876,7 +2876,7 @@
         <v>36</v>
       </c>
       <c r="F108">
-        <v>-2.756812257956874</v>
+        <v>-2.760172023271265</v>
       </c>
       <c r="G108">
         <v>-0.04920619233585422</v>
@@ -2922,7 +2922,7 @@
         <v>38</v>
       </c>
       <c r="F110">
-        <v>-2.769311888944154</v>
+        <v>-2.77016950951556</v>
       </c>
       <c r="G110">
         <v>-0.05168218536254798</v>
@@ -2945,7 +2945,7 @@
         <v>39</v>
       </c>
       <c r="F111">
-        <v>-2.774925704281841</v>
+        <v>-2.776161777894426</v>
       </c>
       <c r="G111">
         <v>-0.05228418171994131</v>
@@ -2968,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.780309870683897</v>
+        <v>-2.782321950372386</v>
       </c>
       <c r="G112">
         <v>-0.05265652914170493</v>
@@ -2991,7 +2991,7 @@
         <v>41</v>
       </c>
       <c r="F113">
-        <v>-2.787099101727094</v>
+        <v>-2.787495426092556</v>
       </c>
       <c r="G113">
         <v>-0.05443394120460865</v>
@@ -3014,7 +3014,7 @@
         <v>42</v>
       </c>
       <c r="F114">
-        <v>-2.79252639774953</v>
+        <v>-2.794376066736298</v>
       </c>
       <c r="G114">
         <v>-0.05484941824675094</v>
@@ -3037,7 +3037,7 @@
         <v>43</v>
       </c>
       <c r="F115">
-        <v>-2.798519742704131</v>
+        <v>-2.799586717938548</v>
       </c>
       <c r="G115">
         <v>-0.05583094422105916</v>
@@ -3083,7 +3083,7 @@
         <v>45</v>
       </c>
       <c r="F117">
-        <v>-2.809449469985546</v>
+        <v>-2.81045962199248</v>
       </c>
       <c r="G117">
         <v>-0.05673703354188819</v>
@@ -3106,7 +3106,7 @@
         <v>46</v>
       </c>
       <c r="F118">
-        <v>-2.816044860002276</v>
+        <v>-2.816470236668416</v>
       </c>
       <c r="G118">
         <v>-0.05832060457832489</v>
@@ -3152,7 +3152,7 @@
         <v>48</v>
       </c>
       <c r="F120">
-        <v>-2.824536013466388</v>
+        <v>-2.827503614459652</v>
       </c>
       <c r="G120">
         <v>-0.05678812008185008</v>
@@ -3175,7 +3175,7 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.832768823861797</v>
+        <v>-2.833475543034154</v>
       </c>
       <c r="G121">
         <v>-0.06000911149696631</v>
@@ -3198,7 +3198,7 @@
         <v>50</v>
       </c>
       <c r="F122">
-        <v>-2.837874301520555</v>
+        <v>-2.838705670062885</v>
       </c>
       <c r="G122">
         <v>-0.06010277017543042</v>
@@ -3244,7 +3244,7 @@
         <v>52</v>
       </c>
       <c r="F124">
-        <v>-2.849081799698701</v>
+        <v>-2.849436604266412</v>
       </c>
       <c r="G124">
         <v>-0.06128663039299131</v>
@@ -3267,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.854224371748653</v>
+        <v>-2.855727620921819</v>
       </c>
       <c r="G125">
         <v>-0.06141738346264969</v>
@@ -3290,7 +3290,7 @@
         <v>54</v>
       </c>
       <c r="F126">
-        <v>-2.858838106987017</v>
+        <v>-2.860604829993085</v>
       </c>
       <c r="G126">
         <v>-0.0610192997207204</v>
@@ -3313,7 +3313,7 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.865105233882583</v>
+        <v>-2.866440875372655</v>
       </c>
       <c r="G127">
         <v>-0.06227460763599346</v>
@@ -3336,7 +3336,7 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.869625120603108</v>
+        <v>-2.872472075462798</v>
       </c>
       <c r="G128">
         <v>-0.06178267537622562</v>
@@ -3359,7 +3359,7 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.875703222970226</v>
+        <v>-2.878582029843677</v>
       </c>
       <c r="G129">
         <v>-0.0628489587630503</v>
@@ -3382,7 +3382,7 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.881023864806531</v>
+        <v>-2.884569497790821</v>
       </c>
       <c r="G130">
         <v>-0.06315778161906183</v>
@@ -3405,7 +3405,7 @@
         <v>59</v>
       </c>
       <c r="F131">
-        <v>-2.886881697478125</v>
+        <v>-2.888062742161599</v>
       </c>
       <c r="G131">
         <v>-0.06400379531036271</v>
@@ -3428,7 +3428,7 @@
         <v>60</v>
       </c>
       <c r="F132">
-        <v>-2.892760930829954</v>
+        <v>-2.893118469000448</v>
       </c>
       <c r="G132">
         <v>-0.06487120968189952</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.901639682666676</v>
+        <v>-2.903474408615333</v>
       </c>
       <c r="G134">
         <v>-0.06372632355803498</v>
@@ -3497,7 +3497,7 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.906850615773861</v>
+        <v>-2.909328199519948</v>
       </c>
       <c r="G135">
         <v>-0.06392543768492631</v>
@@ -3566,7 +3566,7 @@
         <v>66</v>
       </c>
       <c r="F138">
-        <v>-2.924531650735598</v>
+        <v>-2.925240382044629</v>
       </c>
       <c r="G138">
         <v>-0.06657101570578416</v>
@@ -3589,7 +3589,7 @@
         <v>67</v>
       </c>
       <c r="F139">
-        <v>-2.930882657104517</v>
+        <v>-2.93144802874842</v>
       </c>
       <c r="G139">
         <v>-0.06791020309441009</v>
@@ -3612,7 +3612,7 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.934563576090229</v>
+        <v>-2.935686307104717</v>
       </c>
       <c r="G140">
         <v>-0.06657930309982896</v>
@@ -3635,7 +3635,7 @@
         <v>69</v>
       </c>
       <c r="F141">
-        <v>-2.940079792462224</v>
+        <v>-2.941524145065613</v>
       </c>
       <c r="G141">
         <v>-0.06708370049153078</v>
@@ -3658,7 +3658,7 @@
         <v>70</v>
       </c>
       <c r="F142">
-        <v>-2.945805796069576</v>
+        <v>-2.947608015262093</v>
       </c>
       <c r="G142">
         <v>-0.06779788511858942</v>
@@ -3681,7 +3681,7 @@
         <v>71</v>
       </c>
       <c r="F143">
-        <v>-2.947522217144268</v>
+        <v>-2.951484518146378</v>
       </c>
       <c r="G143">
         <v>-0.06450248721298824</v>
@@ -3704,7 +3704,7 @@
         <v>72</v>
       </c>
       <c r="F144">
-        <v>-2.955359082172823</v>
+        <v>-2.956102687736116</v>
       </c>
       <c r="G144">
         <v>-0.06732753326125041</v>
@@ -3727,7 +3727,7 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.95886499975033</v>
+        <v>-2.961279999590877</v>
       </c>
       <c r="G145">
         <v>-0.06582163185846457</v>
@@ -3750,7 +3750,7 @@
         <v>74</v>
       </c>
       <c r="F146">
-        <v>-2.965956651104943</v>
+        <v>-2.967027395138442</v>
       </c>
       <c r="G146">
         <v>-0.06790146423278398</v>
@@ -3773,7 +3773,7 @@
         <v>75</v>
       </c>
       <c r="F147">
-        <v>-2.970240533670157</v>
+        <v>-2.971341762296957</v>
       </c>
       <c r="G147">
         <v>-0.06717352781770547</v>
@@ -3796,7 +3796,7 @@
         <v>76</v>
       </c>
       <c r="F148">
-        <v>-2.976312929408151</v>
+        <v>-2.976855218327667</v>
       </c>
       <c r="G148">
         <v>-0.06823410457540602</v>
@@ -3819,7 +3819,7 @@
         <v>77</v>
       </c>
       <c r="F149">
-        <v>-2.979798580267622</v>
+        <v>-2.982159992646322</v>
       </c>
       <c r="G149">
         <v>-0.06670793645458395</v>
@@ -3865,7 +3865,7 @@
         <v>79</v>
       </c>
       <c r="F151">
-        <v>-2.989199539033386</v>
+        <v>-2.992850267538294</v>
       </c>
       <c r="G151">
         <v>-0.06608525725976122</v>
@@ -3888,7 +3888,7 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.995927960554186</v>
+        <v>-2.996063818351252</v>
       </c>
       <c r="G152">
         <v>-0.06780185980026898</v>
@@ -3911,7 +3911,7 @@
         <v>81</v>
       </c>
       <c r="F153">
-        <v>-2.997696423449615</v>
+        <v>-3.002176294718225</v>
       </c>
       <c r="G153">
         <v>-0.06455850371540439</v>
@@ -3934,7 +3934,7 @@
         <v>82</v>
       </c>
       <c r="F154">
-        <v>-3.005461249675485</v>
+        <v>-3.005936233845047</v>
       </c>
       <c r="G154">
         <v>-0.06731151096098098</v>
@@ -3957,7 +3957,7 @@
         <v>83</v>
       </c>
       <c r="F155">
-        <v>-3.009286787448657</v>
+        <v>-3.010524771102745</v>
       </c>
       <c r="G155">
         <v>-0.06612522975386037</v>
@@ -4003,7 +4003,7 @@
         <v>85</v>
       </c>
       <c r="F157">
-        <v>-3.018040862294405</v>
+        <v>-3.019988911721621</v>
       </c>
       <c r="G157">
         <v>-0.06485566663902187</v>
@@ -4026,7 +4026,7 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.023943258117787</v>
+        <v>-3.025253967463569</v>
       </c>
       <c r="G158">
         <v>-0.06574624348211056</v>
@@ -4072,7 +4072,7 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.032697887756073</v>
+        <v>-3.034310629195259</v>
       </c>
       <c r="G160">
         <v>-0.06447723515981063</v>
@@ -4187,7 +4187,7 @@
         <v>93</v>
       </c>
       <c r="F165">
-        <v>-3.057874822442671</v>
+        <v>-3.059367225593587</v>
       </c>
       <c r="G165">
         <v>-0.06459507494494299</v>
@@ -4210,7 +4210,7 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.060945828585529</v>
+        <v>-3.062579727792436</v>
       </c>
       <c r="G166">
         <v>-0.06265426210750791</v>
@@ -4233,7 +4233,7 @@
         <v>95</v>
       </c>
       <c r="F167">
-        <v>-3.066247275541154</v>
+        <v>-3.066793143194778</v>
       </c>
       <c r="G167">
         <v>-0.06294389008283985</v>
@@ -4256,7 +4256,7 @@
         <v>96</v>
       </c>
       <c r="F168">
-        <v>-3.069187029523578</v>
+        <v>-3.070750927340897</v>
       </c>
       <c r="G168">
         <v>-0.06087182508497047</v>
@@ -4279,7 +4279,7 @@
         <v>97</v>
       </c>
       <c r="F169">
-        <v>-3.075635874617286</v>
+        <v>-3.077749901712157</v>
       </c>
       <c r="G169">
         <v>-0.06230885119838547</v>
@@ -4302,7 +4302,7 @@
         <v>98</v>
       </c>
       <c r="F170">
-        <v>-3.079430700637604</v>
+        <v>-3.081073717901897</v>
       </c>
       <c r="G170">
         <v>-0.06109185823841068</v>
@@ -4325,7 +4325,7 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.084791519730381</v>
+        <v>-3.085623373035919</v>
       </c>
       <c r="G171">
         <v>-0.06144085835089474</v>
@@ -4371,7 +4371,7 @@
         <v>101</v>
       </c>
       <c r="F173">
-        <v>-3.09196443733838</v>
+        <v>-3.09404606678751</v>
       </c>
       <c r="G173">
         <v>-0.05859013799830659</v>
@@ -4394,7 +4394,7 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.096628738555165</v>
+        <v>-3.098819617308678</v>
       </c>
       <c r="G174">
         <v>-0.05824262023479909</v>
@@ -4417,7 +4417,7 @@
         <v>103</v>
       </c>
       <c r="F175">
-        <v>-3.101286726821514</v>
+        <v>-3.103003873808356</v>
       </c>
       <c r="G175">
         <v>-0.05788878952085452</v>
@@ -4440,7 +4440,7 @@
         <v>104</v>
       </c>
       <c r="F176">
-        <v>-3.106166831824455</v>
+        <v>-3.1073544608549</v>
       </c>
       <c r="G176">
         <v>-0.05775707554350284</v>
@@ -4486,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="F178">
-        <v>-3.114248229247178</v>
+        <v>-3.115619699724924</v>
       </c>
       <c r="G178">
         <v>-0.05581483500563944</v>
@@ -4601,7 +4601,7 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.135976321111293</v>
+        <v>-3.136007763768681</v>
       </c>
       <c r="G183">
         <v>-0.05248383196828954</v>
@@ -4624,7 +4624,7 @@
         <v>112</v>
       </c>
       <c r="F184">
-        <v>-3.13813708687773</v>
+        <v>-3.140938719361097</v>
       </c>
       <c r="G184">
         <v>-0.04963277875443273</v>
@@ -4647,7 +4647,7 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.142254156616289</v>
+        <v>-3.145505707148269</v>
       </c>
       <c r="G185">
         <v>-0.04873802951269879</v>
@@ -4670,7 +4670,7 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.147536980199019</v>
+        <v>-3.149157034993176</v>
       </c>
       <c r="G186">
         <v>-0.04900903411513546</v>
@@ -4716,7 +4716,7 @@
         <v>116</v>
       </c>
       <c r="F188">
-        <v>-3.156219508673063</v>
+        <v>-3.156883588056143</v>
       </c>
       <c r="G188">
         <v>-0.04766792462859348</v>
@@ -4739,7 +4739,7 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.158365444796538</v>
+        <v>-3.160152375518529</v>
       </c>
       <c r="G189">
         <v>-0.0448020417717746</v>
@@ -4762,7 +4762,7 @@
         <v>118</v>
       </c>
       <c r="F190">
-        <v>-3.163952397055203</v>
+        <v>-3.164530400511254</v>
       </c>
       <c r="G190">
         <v>-0.04537717505014682</v>
@@ -4808,7 +4808,7 @@
         <v>120</v>
       </c>
       <c r="F192">
-        <v>-3.172927394559157</v>
+        <v>-3.17370797116319</v>
       </c>
       <c r="G192">
         <v>-0.04432853459351432</v>
@@ -4854,7 +4854,7 @@
         <v>122</v>
       </c>
       <c r="F194">
-        <v>-3.179788708903259</v>
+        <v>-3.181320952143119</v>
       </c>
       <c r="G194">
         <v>-0.04116621097703005</v>
@@ -4877,7 +4877,7 @@
         <v>123</v>
       </c>
       <c r="F195">
-        <v>-3.182358158345255</v>
+        <v>-3.18518725597489</v>
       </c>
       <c r="G195">
         <v>-0.03872384143873364</v>
@@ -4900,7 +4900,7 @@
         <v>124</v>
       </c>
       <c r="F196">
-        <v>-3.185158707349343</v>
+        <v>-3.18857125185235</v>
       </c>
       <c r="G196">
         <v>-0.03651257146252856</v>
@@ -4923,7 +4923,7 @@
         <v>125</v>
       </c>
       <c r="F197">
-        <v>-3.191518139969665</v>
+        <v>-3.19363076122327</v>
       </c>
       <c r="G197">
         <v>-0.03786018510255756</v>
@@ -4946,7 +4946,7 @@
         <v>126</v>
       </c>
       <c r="F198">
-        <v>-3.19398984278846</v>
+        <v>-3.195395560351626</v>
       </c>
       <c r="G198">
         <v>-0.03532006894105899</v>
@@ -4992,7 +4992,7 @@
         <v>128</v>
       </c>
       <c r="F200">
-        <v>-3.201667904242333</v>
+        <v>-3.203085892108148</v>
       </c>
       <c r="G200">
         <v>-0.03297449243434603</v>
@@ -5015,7 +5015,7 @@
         <v>129</v>
       </c>
       <c r="F201">
-        <v>-3.206672737644993</v>
+        <v>-3.206756323989463</v>
       </c>
       <c r="G201">
         <v>-0.03296750685671307</v>
@@ -5038,7 +5038,7 @@
         <v>130</v>
       </c>
       <c r="F202">
-        <v>-3.210110834742801</v>
+        <v>-3.210681661419583</v>
       </c>
       <c r="G202">
         <v>-0.03139378497422746</v>
@@ -5061,7 +5061,7 @@
         <v>131</v>
       </c>
       <c r="F203">
-        <v>-3.213748245542063</v>
+        <v>-3.21424153288638</v>
       </c>
       <c r="G203">
         <v>-0.03001937679319677</v>
@@ -5107,7 +5107,7 @@
         <v>133</v>
       </c>
       <c r="F205">
-        <v>-3.220749041614699</v>
+        <v>-3.221546153093309</v>
       </c>
       <c r="G205">
         <v>-0.02699653490524634</v>
@@ -5130,7 +5130,7 @@
         <v>134</v>
       </c>
       <c r="F206">
-        <v>-3.223867708449949</v>
+        <v>-3.225722259454766</v>
       </c>
       <c r="G206">
         <v>-0.02510338276020257</v>
@@ -5153,7 +5153,7 @@
         <v>135</v>
       </c>
       <c r="F207">
-        <v>-3.227773783558185</v>
+        <v>-3.228359053591354</v>
       </c>
       <c r="G207">
         <v>-0.02399763888814654</v>
@@ -5222,7 +5222,7 @@
         <v>138</v>
       </c>
       <c r="F210">
-        <v>-3.236638208159643</v>
+        <v>-3.237669990374989</v>
       </c>
       <c r="G210">
         <v>-0.01782660654872453</v>
@@ -5544,7 +5544,7 @@
         <v>123</v>
       </c>
       <c r="F224">
-        <v>-2.99171354786893</v>
+        <v>-2.992002848431156</v>
       </c>
       <c r="G224">
         <v>-0.06577717043876063</v>
@@ -5567,7 +5567,7 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.071125763879544</v>
+        <v>-3.07267002638519</v>
       </c>
       <c r="G225">
         <v>-0.06851272909896111</v>
@@ -5590,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.146782647157709</v>
+        <v>-3.146829227176161</v>
       </c>
       <c r="G226">
         <v>-0.06749295502671293</v>
@@ -5613,7 +5613,7 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.213330466850168</v>
+        <v>-3.215467582571681</v>
       </c>
       <c r="G227">
         <v>-0.05736411736875813</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.277196299859827</v>
+        <v>-3.277979120281306</v>
       </c>
       <c r="G228">
         <v>-0.04455329302800359</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.785241004952843</v>
+        <v>-2.785254690851337</v>
       </c>
       <c r="G232">
         <v>-0.02527176346397342</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.974016186751373</v>
+        <v>-2.975220099357068</v>
       </c>
       <c r="G234">
         <v>-0.05795588987540001</v>
@@ -5797,7 +5797,7 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.059513041857866</v>
+        <v>-3.059691081603795</v>
       </c>
       <c r="G235">
         <v>-0.06540721728834087</v>
@@ -5820,7 +5820,7 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.141468331645823</v>
+        <v>-3.141786382797472</v>
       </c>
       <c r="G236">
         <v>-0.06931697938274617</v>
@@ -5843,7 +5843,7 @@
         <v>336</v>
       </c>
       <c r="F237">
-        <v>-3.216518542399338</v>
+        <v>-3.217263988450917</v>
       </c>
       <c r="G237">
         <v>-0.06632166244271054</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.286245268625959</v>
+        <v>-3.286681348060005</v>
       </c>
       <c r="G238">
         <v>-0.05800286097577989</v>
@@ -5889,7 +5889,7 @@
         <v>448</v>
       </c>
       <c r="F239">
-        <v>-3.351027618502251</v>
+        <v>-3.351440169516465</v>
       </c>
       <c r="G239">
         <v>-0.04473968315851939</v>
@@ -5981,7 +5981,7 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.827740477309618</v>
+        <v>-2.828156229082379</v>
       </c>
       <c r="G243">
         <v>-0.0250304586649932</v>
@@ -6004,7 +6004,7 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.925399438424117</v>
+        <v>-2.925754748791487</v>
       </c>
       <c r="G244">
         <v>-0.04354852366881445</v>
@@ -6027,7 +6027,7 @@
         <v>276</v>
       </c>
       <c r="F245">
-        <v>-3.018224530215806</v>
+        <v>-3.018538024520988</v>
       </c>
       <c r="G245">
         <v>-0.05723271934982499</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.105821067673915</v>
+        <v>-3.107482042026098</v>
       </c>
       <c r="G246">
         <v>-0.06482813356561712</v>
@@ -6073,7 +6073,7 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.188184808981283</v>
+        <v>-3.188994721802795</v>
       </c>
       <c r="G247">
         <v>-0.06805097876230648</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.336877591286729</v>
+        <v>-3.337986942140626</v>
       </c>
       <c r="G249">
         <v>-0.05760174171475763</v>
@@ -6165,7 +6165,7 @@
         <v>830</v>
       </c>
       <c r="F251">
-        <v>-3.463582307346689</v>
+        <v>-3.463683301626151</v>
       </c>
       <c r="G251">
         <v>-0.02602466555336047</v>
@@ -6234,7 +6234,7 @@
         <v>141</v>
       </c>
       <c r="F254">
-        <v>-2.858243375323748</v>
+        <v>-2.858263277145572</v>
       </c>
       <c r="G254">
         <v>-0.0241816450302621</v>
@@ -6257,7 +6257,7 @@
         <v>283</v>
       </c>
       <c r="F255">
-        <v>-2.95827432598797</v>
+        <v>-2.958839467334881</v>
       </c>
       <c r="G255">
         <v>-0.04364111093397272</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.140443944612575</v>
+        <v>-3.140840251813976</v>
       </c>
       <c r="G257">
         <v>-0.06523516485980907</v>
@@ -6326,7 +6326,7 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.223560836956544</v>
+        <v>-3.223614842514555</v>
       </c>
       <c r="G258">
         <v>-0.06834797726552355</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.300776031133399</v>
+        <v>-3.301700032185678</v>
       </c>
       <c r="G259">
         <v>-0.06499168668186583</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.373227744413447</v>
+        <v>-3.373470496044969</v>
       </c>
       <c r="G260">
         <v>-0.05743932002365837</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.440303181694261</v>
+        <v>-3.440987681625689</v>
       </c>
       <c r="G261">
         <v>-0.04394327254395969</v>
@@ -6418,7 +6418,7 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.50162754945332</v>
+        <v>-3.502079272778104</v>
       </c>
       <c r="G262">
         <v>-0.0252635603647639</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.882085517278409</v>
+        <v>-2.882393499096431</v>
       </c>
       <c r="G265">
         <v>-0.0240632056775123</v>
@@ -6533,7 +6533,7 @@
         <v>617</v>
       </c>
       <c r="F267">
-        <v>-3.076507397946806</v>
+        <v>-3.076750932100177</v>
       </c>
       <c r="G267">
         <v>-0.05631636605077839</v>
@@ -6556,7 +6556,7 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.165436669974895</v>
+        <v>-3.166342564638918</v>
       </c>
       <c r="G268">
         <v>-0.06455489133007597</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.249772890711616</v>
+        <v>-3.249813231931348</v>
       </c>
       <c r="G269">
         <v>-0.06780675191923091</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.327248020091443</v>
+        <v>-3.328056441038416</v>
       </c>
       <c r="G270">
         <v>-0.06419752115149246</v>
@@ -6625,7 +6625,7 @@
         <v>1439</v>
       </c>
       <c r="F271">
-        <v>-3.400622653892166</v>
+        <v>-3.400774446050496</v>
       </c>
       <c r="G271">
         <v>-0.05688140820342391</v>
@@ -6671,7 +6671,7 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.530575857990558</v>
+        <v>-3.531142133428199</v>
       </c>
       <c r="G273">
         <v>-0.02466589200668384</v>
@@ -6763,7 +6763,7 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.000726409056423</v>
+        <v>-3.001412315953363</v>
       </c>
       <c r="G277">
         <v>-0.04227620044241398</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.096058483857597</v>
+        <v>-3.09630213826145</v>
       </c>
       <c r="G278">
         <v>-0.05607882283516297</v>
@@ -6809,7 +6809,7 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.184691001597194</v>
+        <v>-3.185386860303748</v>
       </c>
       <c r="G279">
         <v>-0.06318188816633419</v>
@@ -6832,7 +6832,7 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.269256825465189</v>
+        <v>-3.269857694946573</v>
       </c>
       <c r="G280">
         <v>-0.06621825962590311</v>
@@ -6878,7 +6878,7 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.422224973593063</v>
+        <v>-3.422422739655839</v>
       </c>
       <c r="G282">
         <v>-0.05612750293692592</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.49058572605642</v>
+        <v>-3.490639832882349</v>
       </c>
       <c r="G283">
         <v>-0.04295880299185728</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.553629376809089</v>
+        <v>-3.553999852508709</v>
       </c>
       <c r="G284">
         <v>-0.0244730013361007</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.916094948776097</v>
+        <v>-2.916382420020435</v>
       </c>
       <c r="G287">
         <v>-0.02367997741095973</v>
@@ -7062,7 +7062,7 @@
         <v>1548</v>
       </c>
       <c r="F290">
-        <v>-3.201150424798553</v>
+        <v>-3.201503651527488</v>
       </c>
       <c r="G290">
         <v>-0.06299904231392772</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.365015206725004</v>
+        <v>-3.365356781376585</v>
       </c>
       <c r="G292">
         <v>-0.06303955016071905</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.439037917844733</v>
+        <v>-3.439358653266375</v>
       </c>
       <c r="G293">
         <v>-0.05515012424061883</v>
@@ -7154,7 +7154,7 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.508167108257353</v>
+        <v>-3.508297556637264</v>
       </c>
       <c r="G294">
         <v>-0.04236717761340913</v>
@@ -7246,7 +7246,7 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.928550245428536</v>
+        <v>-2.928926664795901</v>
       </c>
       <c r="G298">
         <v>-0.02357381916767043</v>
@@ -7269,7 +7269,7 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.029230465649422</v>
+        <v>-3.029361128074739</v>
       </c>
       <c r="G299">
         <v>-0.04201270279780811</v>
@@ -7292,7 +7292,7 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.123766442911127</v>
+        <v>-3.124217593665675</v>
       </c>
       <c r="G300">
         <v>-0.0543073434687642</v>
@@ -7315,7 +7315,7 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.214053777474791</v>
+        <v>-3.214391226947151</v>
       </c>
       <c r="G301">
         <v>-0.06219144904681673</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.453395595239973</v>
+        <v>-3.453589010283106</v>
       </c>
       <c r="G304">
         <v>-0.05464736464488806</v>
@@ -7430,7 +7430,7 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.587182006673184</v>
+        <v>-3.587352753748192</v>
       </c>
       <c r="G306">
         <v>-0.02395110289660207</v>
@@ -7499,7 +7499,7 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.938908684353428</v>
+        <v>-2.939171862367354</v>
       </c>
       <c r="G309">
         <v>-0.02338508521976257</v>
@@ -7522,7 +7522,7 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.039465975634541</v>
+        <v>-3.03971666525752</v>
       </c>
       <c r="G310">
         <v>-0.04129000151007567</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.134907091146637</v>
+        <v>-3.134988281561666</v>
       </c>
       <c r="G311">
         <v>-0.05420531534682338</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.309853324480303</v>
+        <v>-3.310154341880595</v>
       </c>
       <c r="G313">
         <v>-0.06397337201434161</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.389970993876977</v>
+        <v>-3.39036391909549</v>
       </c>
       <c r="G314">
         <v>-0.061438666420216</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.465049183776194</v>
+        <v>-3.465276702676325</v>
       </c>
       <c r="G315">
         <v>-0.05399105464408593</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.535028743434018</v>
+        <v>-3.535252120536945</v>
       </c>
       <c r="G316">
         <v>-0.0413182393111089</v>
@@ -7798,7 +7798,7 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.143577998573606</v>
+        <v>-3.144109425256732</v>
       </c>
       <c r="G322">
         <v>-0.05332638142041324</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.23402273830819</v>
+        <v>-3.234239548246836</v>
       </c>
       <c r="G323">
         <v>-0.06099802107311758</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.319427249167131</v>
+        <v>-3.31945553665359</v>
       </c>
       <c r="G324">
         <v>-0.06352861199624371</v>
@@ -7867,7 +7867,7 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.399732419225027</v>
+        <v>-3.399778101971039</v>
       </c>
       <c r="G325">
         <v>-0.06095986211832471</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.545289680831317</v>
+        <v>-3.545568933448949</v>
       </c>
       <c r="G327">
         <v>-0.04087010370692101</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.610687399680431</v>
+        <v>-3.610877899281044</v>
       </c>
       <c r="G328">
         <v>-0.02339390262022029</v>
@@ -8005,7 +8005,7 @@
         <v>1017</v>
       </c>
       <c r="F331">
-        <v>-2.955287275856456</v>
+        <v>-2.955427732058425</v>
       </c>
       <c r="G331">
         <v>-0.02304604198804938</v>
@@ -8051,7 +8051,7 @@
         <v>3053</v>
       </c>
       <c r="F333">
-        <v>-3.151555598695108</v>
+        <v>-3.151609263122812</v>
       </c>
       <c r="G333">
         <v>-0.05317217999790391</v>
@@ -8120,7 +8120,7 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.408101752218418</v>
+        <v>-3.408117256727448</v>
       </c>
       <c r="G336">
         <v>-0.06050505627801783</v>
@@ -8143,7 +8143,7 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.483532286888218</v>
+        <v>-3.483864630190737</v>
       </c>
       <c r="G337">
         <v>-0.05286449853341879</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.554270606692177</v>
+        <v>-3.554433724879317</v>
       </c>
       <c r="G338">
         <v>-0.04053172592297882</v>

</xml_diff>

<commit_message>
updated data from night of 02.25.2019
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -990,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="F26">
-        <v>-2.524816390870587</v>
+        <v>-2.525537948499767</v>
       </c>
       <c r="G26">
         <v>-0.04090163511113665</v>
@@ -1036,7 +1036,7 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <v>-2.555189888564569</v>
+        <v>-2.555282385732477</v>
       </c>
       <c r="G28">
         <v>-0.04649279347421498</v>
@@ -1059,7 +1059,7 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <v>-2.5698312999862</v>
+        <v>-2.569944150301068</v>
       </c>
       <c r="G29">
         <v>-0.04737394681490215</v>
@@ -1082,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <v>-2.584897468056439</v>
+        <v>-2.584953107483507</v>
       </c>
       <c r="G30">
         <v>-0.0510669095590095</v>
@@ -1105,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="F31">
-        <v>-2.599575654309668</v>
+        <v>-2.59966815147758</v>
       </c>
       <c r="G31">
         <v>-0.05133468927504103</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.612952376921871</v>
+        <v>-2.613044874089788</v>
       </c>
       <c r="G32">
         <v>-0.05383393390282332</v>
@@ -1197,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.655986789728492</v>
+        <v>-2.656121036853345</v>
       </c>
       <c r="G35">
         <v>-0.05977531489401344</v>
@@ -1289,7 +1289,7 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.710478063328874</v>
+        <v>-2.711373890038922</v>
       </c>
       <c r="G39">
         <v>-0.06363759338060815</v>
@@ -1312,7 +1312,7 @@
         <v>24</v>
       </c>
       <c r="F40">
-        <v>-2.723348593903957</v>
+        <v>-2.723461444218823</v>
       </c>
       <c r="G40">
         <v>-0.06456209074184449</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.762216332470147</v>
+        <v>-2.762785566926954</v>
       </c>
       <c r="G43">
         <v>-0.06391507069606006</v>
@@ -1404,7 +1404,7 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <v>-2.774007077905265</v>
+        <v>-2.775328977602483</v>
       </c>
       <c r="G44">
         <v>-0.06527711482833976</v>
@@ -1565,7 +1565,7 @@
         <v>35</v>
       </c>
       <c r="F51">
-        <v>-2.857331486028856</v>
+        <v>-2.858061182998552</v>
       </c>
       <c r="G51">
         <v>-0.06095221173795851</v>
@@ -1611,7 +1611,7 @@
         <v>37</v>
       </c>
       <c r="F53">
-        <v>-2.878590044406622</v>
+        <v>-2.878802578226157</v>
       </c>
       <c r="G53">
         <v>-0.05734159308725095</v>
@@ -1680,7 +1680,7 @@
         <v>40</v>
       </c>
       <c r="F56">
-        <v>-2.911971083926363</v>
+        <v>-2.912123844085772</v>
       </c>
       <c r="G56">
         <v>-0.05155345644536014</v>
@@ -1726,7 +1726,7 @@
         <v>42</v>
       </c>
       <c r="F58">
-        <v>-2.931719389049388</v>
+        <v>-2.933395569273737</v>
       </c>
       <c r="G58">
         <v>-0.04645061600021683</v>
@@ -1795,7 +1795,7 @@
         <v>45</v>
       </c>
       <c r="F61">
-        <v>-2.961806950792357</v>
+        <v>-2.961950796606986</v>
       </c>
       <c r="G61">
         <v>-0.03984336400976435</v>
@@ -1841,7 +1841,7 @@
         <v>47</v>
       </c>
       <c r="F63">
-        <v>-2.979726315531622</v>
+        <v>-2.979870161346251</v>
       </c>
       <c r="G63">
         <v>-0.03345732172064375</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <v>-2.597590475980668</v>
+        <v>-2.597988572888221</v>
       </c>
       <c r="G82">
         <v>-0.02006377659037284</v>
@@ -2347,7 +2347,7 @@
         <v>13</v>
       </c>
       <c r="F85">
-        <v>-2.617220728412067</v>
+        <v>-2.617508322953553</v>
       </c>
       <c r="G85">
         <v>-0.02313921711713052</v>
@@ -2393,7 +2393,7 @@
         <v>15</v>
       </c>
       <c r="F87">
-        <v>-2.630884699251327</v>
+        <v>-2.631157715124343</v>
       </c>
       <c r="G87">
         <v>-0.02650874695511796</v>
@@ -2439,7 +2439,7 @@
         <v>17</v>
       </c>
       <c r="F89">
-        <v>-2.642327393259413</v>
+        <v>-2.643094408998108</v>
       </c>
       <c r="G89">
         <v>-0.02875040782855365</v>
@@ -2462,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="F90">
-        <v>-2.649258199078582</v>
+        <v>-2.649271656835363</v>
       </c>
       <c r="G90">
         <v>-0.03114366471063246</v>
@@ -2508,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.661230894164726</v>
+        <v>-2.66184276986176</v>
       </c>
       <c r="G92">
         <v>-0.03279670476236696</v>
@@ -2531,7 +2531,7 @@
         <v>21</v>
       </c>
       <c r="F93">
-        <v>-2.667951659094491</v>
+        <v>-2.668130273391605</v>
       </c>
       <c r="G93">
         <v>-0.0338386097874217</v>
@@ -2554,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="F94">
-        <v>-2.673597520912591</v>
+        <v>-2.67384172282893</v>
       </c>
       <c r="G94">
         <v>-0.03615692101567447</v>
@@ -2577,7 +2577,7 @@
         <v>23</v>
       </c>
       <c r="F95">
-        <v>-2.680564242120132</v>
+        <v>-2.68111979946261</v>
       </c>
       <c r="G95">
         <v>-0.0376098604918762</v>
@@ -2600,7 +2600,7 @@
         <v>24</v>
       </c>
       <c r="F96">
-        <v>-2.6862469887413</v>
+        <v>-2.686994654148593</v>
       </c>
       <c r="G96">
         <v>-0.03849425467213008</v>
@@ -2623,7 +2623,7 @@
         <v>25</v>
       </c>
       <c r="F97">
-        <v>-2.692656297317452</v>
+        <v>-2.693252072224326</v>
       </c>
       <c r="G97">
         <v>-0.03825148586158944</v>
@@ -2646,7 +2646,7 @@
         <v>26</v>
       </c>
       <c r="F98">
-        <v>-2.698894327306781</v>
+        <v>-2.699524197210764</v>
       </c>
       <c r="G98">
         <v>-0.03907572952178295</v>
@@ -2669,7 +2669,7 @@
         <v>27</v>
       </c>
       <c r="F99">
-        <v>-2.704609035202683</v>
+        <v>-2.705108742005925</v>
       </c>
       <c r="G99">
         <v>-0.04210934040430026</v>
@@ -2715,7 +2715,7 @@
         <v>29</v>
       </c>
       <c r="F101">
-        <v>-2.717517562597841</v>
+        <v>-2.717945745593173</v>
       </c>
       <c r="G101">
         <v>-0.04253686850322724</v>
@@ -2738,7 +2738,7 @@
         <v>30</v>
       </c>
       <c r="F102">
-        <v>-2.72225596236469</v>
+        <v>-2.722774319837313</v>
       </c>
       <c r="G102">
         <v>-0.04469874040493416</v>
@@ -2761,7 +2761,7 @@
         <v>31</v>
       </c>
       <c r="F103">
-        <v>-2.72858095934013</v>
+        <v>-2.728636498696848</v>
       </c>
       <c r="G103">
         <v>-0.04539819683189528</v>
@@ -2807,7 +2807,7 @@
         <v>33</v>
       </c>
       <c r="F105">
-        <v>-2.741231268562386</v>
+        <v>-2.741522054280629</v>
       </c>
       <c r="G105">
         <v>-0.04866065988224522</v>
@@ -2830,7 +2830,7 @@
         <v>34</v>
       </c>
       <c r="F106">
-        <v>-2.747709149568069</v>
+        <v>-2.748081793206684</v>
       </c>
       <c r="G106">
         <v>-0.05012672190763467</v>
@@ -2876,7 +2876,7 @@
         <v>36</v>
       </c>
       <c r="F108">
-        <v>-2.760172023271265</v>
+        <v>-2.760566422452002</v>
       </c>
       <c r="G108">
         <v>-0.04920619233585422</v>
@@ -2899,7 +2899,7 @@
         <v>37</v>
       </c>
       <c r="F109">
-        <v>-2.76491329777672</v>
+        <v>-2.765396098433242</v>
       </c>
       <c r="G109">
         <v>-0.05229541317540698</v>
@@ -2922,7 +2922,7 @@
         <v>38</v>
       </c>
       <c r="F110">
-        <v>-2.77016950951556</v>
+        <v>-2.770515427754134</v>
       </c>
       <c r="G110">
         <v>-0.05168218536254798</v>
@@ -2945,7 +2945,7 @@
         <v>39</v>
       </c>
       <c r="F111">
-        <v>-2.776161777894426</v>
+        <v>-2.776217317251142</v>
       </c>
       <c r="G111">
         <v>-0.05228418171994131</v>
@@ -2968,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.782321950372386</v>
+        <v>-2.782625645704036</v>
       </c>
       <c r="G112">
         <v>-0.05265652914170493</v>
@@ -3037,7 +3037,7 @@
         <v>43</v>
       </c>
       <c r="F115">
-        <v>-2.799586717938548</v>
+        <v>-2.800191385123631</v>
       </c>
       <c r="G115">
         <v>-0.05583094422105916</v>
@@ -3060,7 +3060,7 @@
         <v>44</v>
       </c>
       <c r="F116">
-        <v>-2.80399832935169</v>
+        <v>-2.806017669833766</v>
       </c>
       <c r="G116">
         <v>-0.05629771188832478</v>
@@ -3083,7 +3083,7 @@
         <v>45</v>
       </c>
       <c r="F117">
-        <v>-2.81045962199248</v>
+        <v>-2.811209954592179</v>
       </c>
       <c r="G117">
         <v>-0.05673703354188819</v>
@@ -3106,7 +3106,7 @@
         <v>46</v>
       </c>
       <c r="F118">
-        <v>-2.816470236668416</v>
+        <v>-2.816936589341345</v>
       </c>
       <c r="G118">
         <v>-0.05832060457832489</v>
@@ -3129,7 +3129,7 @@
         <v>47</v>
       </c>
       <c r="F119">
-        <v>-2.82301011832586</v>
+        <v>-2.823801251983955</v>
       </c>
       <c r="G119">
         <v>-0.06027404392161584</v>
@@ -3175,7 +3175,7 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.833475543034154</v>
+        <v>-2.83401037603045</v>
       </c>
       <c r="G121">
         <v>-0.06000911149696631</v>
@@ -3198,7 +3198,7 @@
         <v>50</v>
       </c>
       <c r="F122">
-        <v>-2.838705670062885</v>
+        <v>-2.838978997118416</v>
       </c>
       <c r="G122">
         <v>-0.06010277017543042</v>
@@ -3221,7 +3221,7 @@
         <v>51</v>
       </c>
       <c r="F123">
-        <v>-2.844506825377259</v>
+        <v>-2.84532322984614</v>
       </c>
       <c r="G123">
         <v>-0.06172347505184139</v>
@@ -3244,7 +3244,7 @@
         <v>52</v>
       </c>
       <c r="F124">
-        <v>-2.849436604266412</v>
+        <v>-2.85025554793902</v>
       </c>
       <c r="G124">
         <v>-0.06128663039299131</v>
@@ -3313,7 +3313,7 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.866440875372655</v>
+        <v>-2.866759499480688</v>
       </c>
       <c r="G127">
         <v>-0.06227460763599346</v>
@@ -3336,7 +3336,7 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.872472075462798</v>
+        <v>-2.872687936797506</v>
       </c>
       <c r="G128">
         <v>-0.06178267537622562</v>
@@ -3359,7 +3359,7 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.878582029843677</v>
+        <v>-2.878774949605554</v>
       </c>
       <c r="G129">
         <v>-0.0628489587630503</v>
@@ -3428,7 +3428,7 @@
         <v>60</v>
       </c>
       <c r="F132">
-        <v>-2.893118469000448</v>
+        <v>-2.894051155315235</v>
       </c>
       <c r="G132">
         <v>-0.06487120968189952</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.903474408615333</v>
+        <v>-2.903809790610806</v>
       </c>
       <c r="G134">
         <v>-0.06372632355803498</v>
@@ -3497,7 +3497,7 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.909328199519948</v>
+        <v>-2.909994630219312</v>
       </c>
       <c r="G135">
         <v>-0.06392543768492631</v>
@@ -3520,7 +3520,7 @@
         <v>64</v>
       </c>
       <c r="F136">
-        <v>-2.914986484846605</v>
+        <v>-2.917632046275433</v>
       </c>
       <c r="G136">
         <v>-0.06704948777737774</v>
@@ -3543,7 +3543,7 @@
         <v>65</v>
       </c>
       <c r="F137">
-        <v>-2.920643281966529</v>
+        <v>-2.921462703550947</v>
       </c>
       <c r="G137">
         <v>-0.06769446591700889</v>
@@ -3589,7 +3589,7 @@
         <v>67</v>
       </c>
       <c r="F139">
-        <v>-2.93144802874842</v>
+        <v>-2.931472624041096</v>
       </c>
       <c r="G139">
         <v>-0.06791020309441009</v>
@@ -3612,7 +3612,7 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.935686307104717</v>
+        <v>-2.936403561658945</v>
       </c>
       <c r="G140">
         <v>-0.06657930309982896</v>
@@ -3635,7 +3635,7 @@
         <v>69</v>
       </c>
       <c r="F141">
-        <v>-2.941524145065613</v>
+        <v>-2.94200408010642</v>
       </c>
       <c r="G141">
         <v>-0.06708370049153078</v>
@@ -3681,7 +3681,7 @@
         <v>71</v>
       </c>
       <c r="F143">
-        <v>-2.951484518146378</v>
+        <v>-2.951615683346875</v>
       </c>
       <c r="G143">
         <v>-0.06450248721298824</v>
@@ -3704,7 +3704,7 @@
         <v>72</v>
       </c>
       <c r="F144">
-        <v>-2.956102687736116</v>
+        <v>-2.956126583628377</v>
       </c>
       <c r="G144">
         <v>-0.06732753326125041</v>
@@ -3727,7 +3727,7 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.961279999590877</v>
+        <v>-2.961407180252653</v>
       </c>
       <c r="G145">
         <v>-0.06582163185846457</v>
@@ -3750,7 +3750,7 @@
         <v>74</v>
       </c>
       <c r="F146">
-        <v>-2.967027395138442</v>
+        <v>-2.96739315953787</v>
       </c>
       <c r="G146">
         <v>-0.06790146423278398</v>
@@ -3773,7 +3773,7 @@
         <v>75</v>
       </c>
       <c r="F147">
-        <v>-2.971341762296957</v>
+        <v>-2.971590631594759</v>
       </c>
       <c r="G147">
         <v>-0.06717352781770547</v>
@@ -3888,7 +3888,7 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.996063818351252</v>
+        <v>-2.996152760644822</v>
       </c>
       <c r="G152">
         <v>-0.06780185980026898</v>
@@ -3934,7 +3934,7 @@
         <v>82</v>
       </c>
       <c r="F154">
-        <v>-3.005936233845047</v>
+        <v>-3.006187623249666</v>
       </c>
       <c r="G154">
         <v>-0.06731151096098098</v>
@@ -3980,7 +3980,7 @@
         <v>84</v>
       </c>
       <c r="F156">
-        <v>-3.014826701520832</v>
+        <v>-3.015001859457396</v>
       </c>
       <c r="G156">
         <v>-0.06665332484574193</v>
@@ -4072,7 +4072,7 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.034310629195259</v>
+        <v>-3.035014009120696</v>
       </c>
       <c r="G160">
         <v>-0.06447723515981063</v>
@@ -4141,7 +4141,7 @@
         <v>91</v>
       </c>
       <c r="F163">
-        <v>-3.049209427558229</v>
+        <v>-3.050030487114018</v>
       </c>
       <c r="G163">
         <v>-0.06595331802108673</v>
@@ -4164,7 +4164,7 @@
         <v>92</v>
       </c>
       <c r="F164">
-        <v>-3.053039562562568</v>
+        <v>-3.053528711057775</v>
       </c>
       <c r="G164">
         <v>-0.06477163404513264</v>
@@ -4187,7 +4187,7 @@
         <v>93</v>
       </c>
       <c r="F165">
-        <v>-3.059367225593587</v>
+        <v>-3.059511802916689</v>
       </c>
       <c r="G165">
         <v>-0.06459507494494299</v>
@@ -4256,7 +4256,7 @@
         <v>96</v>
       </c>
       <c r="F168">
-        <v>-3.070750927340897</v>
+        <v>-3.071142906206022</v>
       </c>
       <c r="G168">
         <v>-0.06087182508497047</v>
@@ -4302,7 +4302,7 @@
         <v>98</v>
       </c>
       <c r="F170">
-        <v>-3.081073717901897</v>
+        <v>-3.0820211183379</v>
       </c>
       <c r="G170">
         <v>-0.06109185823841068</v>
@@ -4371,7 +4371,7 @@
         <v>101</v>
       </c>
       <c r="F173">
-        <v>-3.09404606678751</v>
+        <v>-3.095367613248914</v>
       </c>
       <c r="G173">
         <v>-0.05859013799830659</v>
@@ -4394,7 +4394,7 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.098819617308678</v>
+        <v>-3.098917913719822</v>
       </c>
       <c r="G174">
         <v>-0.05824262023479909</v>
@@ -4417,7 +4417,7 @@
         <v>103</v>
       </c>
       <c r="F175">
-        <v>-3.103003873808356</v>
+        <v>-3.103833402550027</v>
       </c>
       <c r="G175">
         <v>-0.05788878952085452</v>
@@ -4440,7 +4440,7 @@
         <v>104</v>
       </c>
       <c r="F176">
-        <v>-3.1073544608549</v>
+        <v>-3.107626152349118</v>
       </c>
       <c r="G176">
         <v>-0.05775707554350284</v>
@@ -4486,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="F178">
-        <v>-3.115619699724924</v>
+        <v>-3.116207549514336</v>
       </c>
       <c r="G178">
         <v>-0.05581483500563944</v>
@@ -4509,7 +4509,7 @@
         <v>107</v>
       </c>
       <c r="F179">
-        <v>-3.118617065905588</v>
+        <v>-3.119194927189529</v>
       </c>
       <c r="G179">
         <v>-0.05517185268375624</v>
@@ -4532,7 +4532,7 @@
         <v>108</v>
       </c>
       <c r="F180">
-        <v>-3.1242249942571</v>
+        <v>-3.124470624963318</v>
       </c>
       <c r="G180">
         <v>-0.0557679620549747</v>
@@ -4647,7 +4647,7 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.145505707148269</v>
+        <v>-3.146014365222033</v>
       </c>
       <c r="G185">
         <v>-0.04873802951269879</v>
@@ -4670,7 +4670,7 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.149157034993176</v>
+        <v>-3.149695287544229</v>
       </c>
       <c r="G186">
         <v>-0.04900903411513546</v>
@@ -4693,7 +4693,7 @@
         <v>115</v>
       </c>
       <c r="F187">
-        <v>-3.152453837310835</v>
+        <v>-3.152716864678379</v>
       </c>
       <c r="G187">
         <v>-0.04891407224665856</v>
@@ -4739,7 +4739,7 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.160152375518529</v>
+        <v>-3.16049151181362</v>
       </c>
       <c r="G189">
         <v>-0.0448020417717746</v>
@@ -4762,7 +4762,7 @@
         <v>118</v>
       </c>
       <c r="F190">
-        <v>-3.164530400511254</v>
+        <v>-3.16510425589877</v>
       </c>
       <c r="G190">
         <v>-0.04537717505014682</v>
@@ -4831,7 +4831,7 @@
         <v>121</v>
       </c>
       <c r="F193">
-        <v>-3.177157787923274</v>
+        <v>-3.177622953530636</v>
       </c>
       <c r="G193">
         <v>-0.0435471089773386</v>
@@ -4900,7 +4900,7 @@
         <v>124</v>
       </c>
       <c r="F196">
-        <v>-3.18857125185235</v>
+        <v>-3.189111423044547</v>
       </c>
       <c r="G196">
         <v>-0.03651257146252856</v>
@@ -5130,7 +5130,7 @@
         <v>134</v>
       </c>
       <c r="F206">
-        <v>-3.225722259454766</v>
+        <v>-3.2262297894643</v>
       </c>
       <c r="G206">
         <v>-0.02510338276020257</v>
@@ -5176,7 +5176,7 @@
         <v>136</v>
       </c>
       <c r="F208">
-        <v>-3.231648893804923</v>
+        <v>-3.232457419929176</v>
       </c>
       <c r="G208">
         <v>-0.02286093015459117</v>
@@ -5222,7 +5222,7 @@
         <v>138</v>
       </c>
       <c r="F210">
-        <v>-3.237669990374989</v>
+        <v>-3.238177520384518</v>
       </c>
       <c r="G210">
         <v>-0.01782660654872453</v>
@@ -5475,7 +5475,7 @@
         <v>30</v>
       </c>
       <c r="F221">
-        <v>-2.721510722131381</v>
+        <v>-2.721729468088695</v>
       </c>
       <c r="G221">
         <v>-0.02560431675245223</v>
@@ -5498,7 +5498,7 @@
         <v>61</v>
       </c>
       <c r="F222">
-        <v>-2.816450490858558</v>
+        <v>-2.817106634341454</v>
       </c>
       <c r="G222">
         <v>-0.04386742812921618</v>
@@ -5521,7 +5521,7 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.906543125733036</v>
+        <v>-2.906957990495776</v>
       </c>
       <c r="G223">
         <v>-0.05728340565328049</v>
@@ -5567,7 +5567,7 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.07267002638519</v>
+        <v>-3.07334638953181</v>
       </c>
       <c r="G225">
         <v>-0.06851272909896111</v>
@@ -5590,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.146829227176161</v>
+        <v>-3.147328074376943</v>
       </c>
       <c r="G226">
         <v>-0.06749295502671293</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.277979120281306</v>
+        <v>-3.278007373686587</v>
       </c>
       <c r="G228">
         <v>-0.04455329302800359</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.785254690851337</v>
+        <v>-2.785465779935326</v>
       </c>
       <c r="G232">
         <v>-0.02527176346397342</v>
@@ -5751,7 +5751,7 @@
         <v>112</v>
       </c>
       <c r="F233">
-        <v>-2.88178318501804</v>
+        <v>-2.882212288148072</v>
       </c>
       <c r="G233">
         <v>-0.04376841583561886</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.975220099357068</v>
+        <v>-2.97545774266125</v>
       </c>
       <c r="G234">
         <v>-0.05795588987540001</v>
@@ -5797,7 +5797,7 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.059691081603795</v>
+        <v>-3.0597795102224</v>
       </c>
       <c r="G235">
         <v>-0.06540721728834087</v>
@@ -5820,7 +5820,7 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.141786382797472</v>
+        <v>-3.142199875457754</v>
       </c>
       <c r="G236">
         <v>-0.06931697938274617</v>
@@ -5843,7 +5843,7 @@
         <v>336</v>
       </c>
       <c r="F237">
-        <v>-3.217263988450917</v>
+        <v>-3.217414775683589</v>
       </c>
       <c r="G237">
         <v>-0.06632166244271054</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.286681348060005</v>
+        <v>-3.287163187852923</v>
       </c>
       <c r="G238">
         <v>-0.05800286097577989</v>
@@ -5889,7 +5889,7 @@
         <v>448</v>
       </c>
       <c r="F239">
-        <v>-3.351440169516465</v>
+        <v>-3.351831843524696</v>
       </c>
       <c r="G239">
         <v>-0.04473968315851939</v>
@@ -5912,7 +5912,7 @@
         <v>504</v>
       </c>
       <c r="F240">
-        <v>-3.411452841865691</v>
+        <v>-3.411628903919411</v>
       </c>
       <c r="G240">
         <v>-0.02711937882840842</v>
@@ -5981,7 +5981,7 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.828156229082379</v>
+        <v>-2.828533199099743</v>
       </c>
       <c r="G243">
         <v>-0.0250304586649932</v>
@@ -6004,7 +6004,7 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.925754748791487</v>
+        <v>-2.926171870329461</v>
       </c>
       <c r="G244">
         <v>-0.04354852366881445</v>
@@ -6027,7 +6027,7 @@
         <v>276</v>
       </c>
       <c r="F245">
-        <v>-3.018538024520988</v>
+        <v>-3.018624987323443</v>
       </c>
       <c r="G245">
         <v>-0.05723271934982499</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.107482042026098</v>
+        <v>-3.108310053919059</v>
       </c>
       <c r="G246">
         <v>-0.06482813356561712</v>
@@ -6073,7 +6073,7 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.188994721802795</v>
+        <v>-3.190171603828873</v>
       </c>
       <c r="G247">
         <v>-0.06805097876230648</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.266093010389055</v>
+        <v>-3.266758536966854</v>
       </c>
       <c r="G248">
         <v>-0.06681828405940005</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.337986942140626</v>
+        <v>-3.338389455690561</v>
       </c>
       <c r="G249">
         <v>-0.05760174171475763</v>
@@ -6142,7 +6142,7 @@
         <v>738</v>
       </c>
       <c r="F250">
-        <v>-3.403517360526654</v>
+        <v>-3.404252093427187</v>
       </c>
       <c r="G250">
         <v>-0.04510061484400452</v>
@@ -6165,7 +6165,7 @@
         <v>830</v>
       </c>
       <c r="F251">
-        <v>-3.463683301626151</v>
+        <v>-3.464181639065342</v>
       </c>
       <c r="G251">
         <v>-0.02602466555336047</v>
@@ -6234,7 +6234,7 @@
         <v>141</v>
       </c>
       <c r="F254">
-        <v>-2.858263277145572</v>
+        <v>-2.858623322430484</v>
       </c>
       <c r="G254">
         <v>-0.0241816450302621</v>
@@ -6257,7 +6257,7 @@
         <v>283</v>
       </c>
       <c r="F255">
-        <v>-2.958839467334881</v>
+        <v>-2.959116687715872</v>
       </c>
       <c r="G255">
         <v>-0.04364111093397272</v>
@@ -6280,7 +6280,7 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.051876142218384</v>
+        <v>-3.052753171251637</v>
       </c>
       <c r="G256">
         <v>-0.05723884722613048</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.140840251813976</v>
+        <v>-3.141582105107187</v>
       </c>
       <c r="G257">
         <v>-0.06523516485980907</v>
@@ -6326,7 +6326,7 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.223614842514555</v>
+        <v>-3.224653950096374</v>
       </c>
       <c r="G258">
         <v>-0.06834797726552355</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.301700032185678</v>
+        <v>-3.303298628607456</v>
       </c>
       <c r="G259">
         <v>-0.06499168668186583</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.373470496044969</v>
+        <v>-3.375294742817646</v>
       </c>
       <c r="G260">
         <v>-0.05743932002365837</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.440987681625689</v>
+        <v>-3.441916739694034</v>
       </c>
       <c r="G261">
         <v>-0.04394327254395969</v>
@@ -6418,7 +6418,7 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.502079272778104</v>
+        <v>-3.502623495605347</v>
       </c>
       <c r="G262">
         <v>-0.0252635603647639</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.882393499096431</v>
+        <v>-2.882753836884993</v>
       </c>
       <c r="G265">
         <v>-0.0240632056775123</v>
@@ -6510,7 +6510,7 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.982419887251812</v>
+        <v>-2.982934689945172</v>
       </c>
       <c r="G266">
         <v>-0.04331321550334977</v>
@@ -6533,7 +6533,7 @@
         <v>617</v>
       </c>
       <c r="F267">
-        <v>-3.076750932100177</v>
+        <v>-3.077896571705333</v>
       </c>
       <c r="G267">
         <v>-0.05631636605077839</v>
@@ -6556,7 +6556,7 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.166342564638918</v>
+        <v>-3.167583822026921</v>
       </c>
       <c r="G268">
         <v>-0.06455489133007597</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.249813231931348</v>
+        <v>-3.251305594258885</v>
       </c>
       <c r="G269">
         <v>-0.06780675191923091</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.328056441038416</v>
+        <v>-3.330715530744679</v>
       </c>
       <c r="G270">
         <v>-0.06419752115149246</v>
@@ -6625,7 +6625,7 @@
         <v>1439</v>
       </c>
       <c r="F271">
-        <v>-3.400774446050496</v>
+        <v>-3.402765276113812</v>
       </c>
       <c r="G271">
         <v>-0.05688140820342391</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.468702984681467</v>
+        <v>-3.470384589899591</v>
       </c>
       <c r="G272">
         <v>-0.04387737884515908</v>
@@ -6671,7 +6671,7 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.531142133428199</v>
+        <v>-3.531834329867634</v>
       </c>
       <c r="G273">
         <v>-0.02466589200668384</v>
@@ -6740,7 +6740,7 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.900989963076124</v>
+        <v>-2.901353445396789</v>
       </c>
       <c r="G276">
         <v>-0.02406920687054059</v>
@@ -6763,7 +6763,7 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.001412315953363</v>
+        <v>-3.001906182634051</v>
       </c>
       <c r="G277">
         <v>-0.04227620044241398</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.09630213826145</v>
+        <v>-3.097718421551724</v>
       </c>
       <c r="G278">
         <v>-0.05607882283516297</v>
@@ -6809,7 +6809,7 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.185386860303748</v>
+        <v>-3.187629474947174</v>
       </c>
       <c r="G279">
         <v>-0.06318188816633419</v>
@@ -6832,7 +6832,7 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.269857694946573</v>
+        <v>-3.272596820551765</v>
       </c>
       <c r="G280">
         <v>-0.06621825962590311</v>
@@ -6855,7 +6855,7 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.348557961400317</v>
+        <v>-3.351791532868845</v>
       </c>
       <c r="G281">
         <v>-0.06398994315260564</v>
@@ -6878,7 +6878,7 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.422422739655839</v>
+        <v>-3.425119950847487</v>
       </c>
       <c r="G282">
         <v>-0.05612750293692592</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.490639832882349</v>
+        <v>-3.492399678604969</v>
       </c>
       <c r="G283">
         <v>-0.04295880299185728</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.553999852508709</v>
+        <v>-3.554874228601493</v>
       </c>
       <c r="G284">
         <v>-0.0244730013361007</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.916382420020435</v>
+        <v>-2.916675103103247</v>
       </c>
       <c r="G287">
         <v>-0.02367997741095973</v>
@@ -7016,7 +7016,7 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.016840117319153</v>
+        <v>-3.017622009757004</v>
       </c>
       <c r="G288">
         <v>-0.04251300891418719</v>
@@ -7039,7 +7039,7 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.111757161510439</v>
+        <v>-3.113677070659592</v>
       </c>
       <c r="G289">
         <v>-0.05551791606564294</v>
@@ -7062,7 +7062,7 @@
         <v>1548</v>
       </c>
       <c r="F290">
-        <v>-3.201503651527488</v>
+        <v>-3.204339678774593</v>
       </c>
       <c r="G290">
         <v>-0.06299904231392772</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.28564389761307</v>
+        <v>-3.28932044900224</v>
       </c>
       <c r="G291">
         <v>-0.0655803780886155</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.365356781376585</v>
+        <v>-3.368894258297968</v>
       </c>
       <c r="G292">
         <v>-0.06303955016071905</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.439358653266375</v>
+        <v>-3.442431535213945</v>
       </c>
       <c r="G293">
         <v>-0.05515012424061883</v>
@@ -7154,7 +7154,7 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.508297556637264</v>
+        <v>-3.510742992195424</v>
       </c>
       <c r="G294">
         <v>-0.04236717761340913</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.572203588368217</v>
+        <v>-3.573311827673294</v>
       </c>
       <c r="G295">
         <v>-0.02449152068444382</v>
@@ -7246,7 +7246,7 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.928926664795901</v>
+        <v>-2.929119222088884</v>
       </c>
       <c r="G298">
         <v>-0.02357381916767043</v>
@@ -7269,7 +7269,7 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.029361128074739</v>
+        <v>-3.03055267499326</v>
       </c>
       <c r="G299">
         <v>-0.04201270279780811</v>
@@ -7292,7 +7292,7 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.124217593665675</v>
+        <v>-3.126877317882713</v>
       </c>
       <c r="G300">
         <v>-0.0543073434687642</v>
@@ -7315,7 +7315,7 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.214391226947151</v>
+        <v>-3.217784402036398</v>
       </c>
       <c r="G301">
         <v>-0.06219144904681673</v>
@@ -7338,7 +7338,7 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.299142821772032</v>
+        <v>-3.303176176223764</v>
       </c>
       <c r="G302">
         <v>-0.06503915675330885</v>
@@ -7361,7 +7361,7 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.378714907612919</v>
+        <v>-3.38273532195491</v>
       </c>
       <c r="G303">
         <v>-0.06236990600344705</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.453589010283106</v>
+        <v>-3.457371496651011</v>
       </c>
       <c r="G304">
         <v>-0.05464736464488806</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.523194756241369</v>
+        <v>-3.52571168893542</v>
       </c>
       <c r="G305">
         <v>-0.04220518905553605</v>
@@ -7430,7 +7430,7 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.587352753748192</v>
+        <v>-3.588475545632808</v>
       </c>
       <c r="G306">
         <v>-0.02395110289660207</v>
@@ -7499,7 +7499,7 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.939171862367354</v>
+        <v>-2.939502050526279</v>
       </c>
       <c r="G309">
         <v>-0.02338508521976257</v>
@@ -7522,7 +7522,7 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.03971666525752</v>
+        <v>-3.041301204178368</v>
       </c>
       <c r="G310">
         <v>-0.04129000151007567</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.134988281561666</v>
+        <v>-3.138028678381241</v>
       </c>
       <c r="G311">
         <v>-0.05420531534682338</v>
@@ -7568,7 +7568,7 @@
         <v>2610</v>
       </c>
       <c r="F312">
-        <v>-3.224950462906559</v>
+        <v>-3.228854273413367</v>
       </c>
       <c r="G312">
         <v>-0.06159631211594552</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.310154341880595</v>
+        <v>-3.3144075862108</v>
       </c>
       <c r="G313">
         <v>-0.06397337201434161</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.39036391909549</v>
+        <v>-3.394757037903488</v>
       </c>
       <c r="G314">
         <v>-0.061438666420216</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.465276702676325</v>
+        <v>-3.468956934684792</v>
       </c>
       <c r="G315">
         <v>-0.05399105464408593</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.535252120536945</v>
+        <v>-3.538189380448835</v>
       </c>
       <c r="G316">
         <v>-0.0413182393111089</v>
@@ -7683,7 +7683,7 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.599959312422064</v>
+        <v>-3.601173136993015</v>
       </c>
       <c r="G317">
         <v>-0.02372300662380827</v>
@@ -7752,7 +7752,7 @@
         <v>821</v>
       </c>
       <c r="F320">
-        <v>-2.947885710296204</v>
+        <v>-2.948295291869554</v>
       </c>
       <c r="G320">
         <v>-0.0233819330146412</v>
@@ -7775,7 +7775,7 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.048636987068577</v>
+        <v>-3.050301686199274</v>
       </c>
       <c r="G321">
         <v>-0.0412592898511992</v>
@@ -7798,7 +7798,7 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.144109425256732</v>
+        <v>-3.14738127792324</v>
       </c>
       <c r="G322">
         <v>-0.05332638142041324</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.234239548246836</v>
+        <v>-3.23827236163357</v>
       </c>
       <c r="G323">
         <v>-0.06099802107311758</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.31945553665359</v>
+        <v>-3.324263017962735</v>
       </c>
       <c r="G324">
         <v>-0.06352861199624371</v>
@@ -7867,7 +7867,7 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.399778101971039</v>
+        <v>-3.404333248923183</v>
       </c>
       <c r="G325">
         <v>-0.06095986211832471</v>
@@ -7890,7 +7890,7 @@
         <v>5751</v>
       </c>
       <c r="F326">
-        <v>-3.475186578979213</v>
+        <v>-3.47933785083631</v>
       </c>
       <c r="G326">
         <v>-0.05364092179063251</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.545568933448949</v>
+        <v>-3.548240382816604</v>
       </c>
       <c r="G327">
         <v>-0.04087010370692101</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.610877899281044</v>
+        <v>-3.612230915524306</v>
       </c>
       <c r="G328">
         <v>-0.02339390262022029</v>
@@ -8005,7 +8005,7 @@
         <v>1017</v>
       </c>
       <c r="F331">
-        <v>-2.955427732058425</v>
+        <v>-2.956056144997122</v>
       </c>
       <c r="G331">
         <v>-0.02304604198804938</v>
@@ -8028,7 +8028,7 @@
         <v>2035</v>
       </c>
       <c r="F332">
-        <v>-3.056157781381454</v>
+        <v>-3.05824364257423</v>
       </c>
       <c r="G332">
         <v>-0.04084545509864856</v>
@@ -8051,7 +8051,7 @@
         <v>3053</v>
       </c>
       <c r="F333">
-        <v>-3.151609263122812</v>
+        <v>-3.155090689209559</v>
       </c>
       <c r="G333">
         <v>-0.05317217999790391</v>
@@ -8074,7 +8074,7 @@
         <v>4071</v>
       </c>
       <c r="F334">
-        <v>-3.242025773038145</v>
+        <v>-3.246319023253284</v>
       </c>
       <c r="G334">
         <v>-0.06057126192654172</v>
@@ -8097,7 +8097,7 @@
         <v>5089</v>
       </c>
       <c r="F335">
-        <v>-3.327312774157283</v>
+        <v>-3.332130557403822</v>
       </c>
       <c r="G335">
         <v>-0.06278717063128125</v>
@@ -8120,7 +8120,7 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.408117256727448</v>
+        <v>-3.412878355089753</v>
       </c>
       <c r="G336">
         <v>-0.06050505627801783</v>
@@ -8143,7 +8143,7 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.483864630190737</v>
+        <v>-3.487839886350137</v>
       </c>
       <c r="G337">
         <v>-0.05286449853341879</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.554433724879317</v>
+        <v>-3.557352462816103</v>
       </c>
       <c r="G338">
         <v>-0.04053172592297882</v>
@@ -8189,7 +8189,7 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.619917485418374</v>
+        <v>-3.621296743720847</v>
       </c>
       <c r="G339">
         <v>-0.02310751223477731</v>

</xml_diff>

<commit_message>
updated data from 02.28.2019
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -921,7 +921,7 @@
         <v>7</v>
       </c>
       <c r="F23">
-        <v>-2.479022713238004</v>
+        <v>-2.479579712587558</v>
       </c>
       <c r="G23">
         <v>-0.03135827639584443</v>
@@ -1197,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.656121036853345</v>
+        <v>-2.65713207387985</v>
       </c>
       <c r="G35">
         <v>-0.05977531489401344</v>
@@ -1289,7 +1289,7 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.711373890038922</v>
+        <v>-2.711461412081488</v>
       </c>
       <c r="G39">
         <v>-0.06363759338060815</v>
@@ -1358,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.749073675741039</v>
+        <v>-2.750108230129674</v>
       </c>
       <c r="G42">
         <v>-0.06332980808518607</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.762785566926954</v>
+        <v>-2.762864174624738</v>
       </c>
       <c r="G43">
         <v>-0.06391507069606006</v>
@@ -1404,7 +1404,7 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <v>-2.775328977602483</v>
+        <v>-2.776419509442502</v>
       </c>
       <c r="G44">
         <v>-0.06527711482833976</v>
@@ -1450,7 +1450,7 @@
         <v>30</v>
       </c>
       <c r="F46">
-        <v>-2.798883286202902</v>
+        <v>-2.799531128357493</v>
       </c>
       <c r="G46">
         <v>-0.06387835591992652</v>
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.822759225816332</v>
+        <v>-2.822925355556685</v>
       </c>
       <c r="G48">
         <v>-0.06224925594752295</v>
@@ -1588,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.868067032127506</v>
+        <v>-2.868157801287395</v>
       </c>
       <c r="G52">
         <v>-0.05922980559813218</v>
@@ -1611,7 +1611,7 @@
         <v>37</v>
       </c>
       <c r="F53">
-        <v>-2.878802578226157</v>
+        <v>-2.879059274355655</v>
       </c>
       <c r="G53">
         <v>-0.05734159308725095</v>
@@ -2140,7 +2140,7 @@
         <v>4</v>
       </c>
       <c r="F76">
-        <v>-2.556713373115567</v>
+        <v>-2.557134323827063</v>
       </c>
       <c r="G76">
         <v>-0.009485514863926792</v>
@@ -2186,7 +2186,7 @@
         <v>6</v>
       </c>
       <c r="F78">
-        <v>-2.57071956367952</v>
+        <v>-2.571019131083296</v>
       </c>
       <c r="G78">
         <v>-0.01344151593653731</v>
@@ -2209,7 +2209,7 @@
         <v>7</v>
       </c>
       <c r="F79">
-        <v>-2.577661967307641</v>
+        <v>-2.577961534711414</v>
       </c>
       <c r="G79">
         <v>-0.01495114987286561</v>
@@ -2232,7 +2232,7 @@
         <v>8</v>
       </c>
       <c r="F80">
-        <v>-2.584577819404997</v>
+        <v>-2.584702900439534</v>
       </c>
       <c r="G80">
         <v>-0.01697656629765065</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <v>-2.597988572888221</v>
+        <v>-2.5981365077267</v>
       </c>
       <c r="G82">
         <v>-0.02006377659037284</v>
@@ -2324,7 +2324,7 @@
         <v>12</v>
       </c>
       <c r="F84">
-        <v>-2.610802121717799</v>
+        <v>-2.611534950521496</v>
       </c>
       <c r="G84">
         <v>-0.02303220938156114</v>
@@ -2370,7 +2370,7 @@
         <v>14</v>
       </c>
       <c r="F86">
-        <v>-2.62326409200272</v>
+        <v>-2.624521055566408</v>
       </c>
       <c r="G86">
         <v>-0.02530711951488618</v>
@@ -2393,7 +2393,7 @@
         <v>15</v>
       </c>
       <c r="F87">
-        <v>-2.631157715124343</v>
+        <v>-2.631465895489727</v>
       </c>
       <c r="G87">
         <v>-0.02650874695511796</v>
@@ -2462,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="F90">
-        <v>-2.649271656835363</v>
+        <v>-2.64959662870154</v>
       </c>
       <c r="G90">
         <v>-0.03114366471063246</v>
@@ -2485,7 +2485,7 @@
         <v>19</v>
       </c>
       <c r="F91">
-        <v>-2.656231428174714</v>
+        <v>-2.656375051848741</v>
       </c>
       <c r="G91">
         <v>-0.03252757100423942</v>
@@ -2508,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.66184276986176</v>
+        <v>-2.662228729950169</v>
       </c>
       <c r="G92">
         <v>-0.03279670476236696</v>
@@ -2531,7 +2531,7 @@
         <v>21</v>
       </c>
       <c r="F93">
-        <v>-2.668130273391605</v>
+        <v>-2.668906254976394</v>
       </c>
       <c r="G93">
         <v>-0.0338386097874217</v>
@@ -2554,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="F94">
-        <v>-2.67384172282893</v>
+        <v>-2.674158875917362</v>
       </c>
       <c r="G94">
         <v>-0.03615692101567447</v>
@@ -2577,7 +2577,7 @@
         <v>23</v>
       </c>
       <c r="F95">
-        <v>-2.68111979946261</v>
+        <v>-2.682110284505121</v>
       </c>
       <c r="G95">
         <v>-0.0376098604918762</v>
@@ -2623,7 +2623,7 @@
         <v>25</v>
       </c>
       <c r="F97">
-        <v>-2.693252072224326</v>
+        <v>-2.693498536566583</v>
       </c>
       <c r="G97">
         <v>-0.03825148586158944</v>
@@ -2669,7 +2669,7 @@
         <v>27</v>
       </c>
       <c r="F99">
-        <v>-2.705108742005925</v>
+        <v>-2.705143474693888</v>
       </c>
       <c r="G99">
         <v>-0.04210934040430026</v>
@@ -2692,7 +2692,7 @@
         <v>28</v>
       </c>
       <c r="F100">
-        <v>-2.710549838492032</v>
+        <v>-2.711486699410311</v>
       </c>
       <c r="G100">
         <v>-0.04303832471335678</v>
@@ -2715,7 +2715,7 @@
         <v>29</v>
       </c>
       <c r="F101">
-        <v>-2.717945745593173</v>
+        <v>-2.718368561806627</v>
       </c>
       <c r="G101">
         <v>-0.04253686850322724</v>
@@ -2738,7 +2738,7 @@
         <v>30</v>
       </c>
       <c r="F102">
-        <v>-2.722774319837313</v>
+        <v>-2.723818139658242</v>
       </c>
       <c r="G102">
         <v>-0.04469874040493416</v>
@@ -2761,7 +2761,7 @@
         <v>31</v>
       </c>
       <c r="F103">
-        <v>-2.728636498696848</v>
+        <v>-2.728981498097013</v>
       </c>
       <c r="G103">
         <v>-0.04539819683189528</v>
@@ -2784,7 +2784,7 @@
         <v>32</v>
       </c>
       <c r="F104">
-        <v>-2.735043509258003</v>
+        <v>-2.735969503946624</v>
       </c>
       <c r="G104">
         <v>-0.04748471955815536</v>
@@ -2807,7 +2807,7 @@
         <v>33</v>
       </c>
       <c r="F105">
-        <v>-2.741522054280629</v>
+        <v>-2.741743484855521</v>
       </c>
       <c r="G105">
         <v>-0.04866065988224522</v>
@@ -2853,7 +2853,7 @@
         <v>35</v>
       </c>
       <c r="F107">
-        <v>-2.752549955996056</v>
+        <v>-2.753164643948289</v>
       </c>
       <c r="G107">
         <v>-0.04940962190280773</v>
@@ -2922,7 +2922,7 @@
         <v>38</v>
       </c>
       <c r="F110">
-        <v>-2.770515427754134</v>
+        <v>-2.771515004902781</v>
       </c>
       <c r="G110">
         <v>-0.05168218536254798</v>
@@ -2945,7 +2945,7 @@
         <v>39</v>
       </c>
       <c r="F111">
-        <v>-2.776217317251142</v>
+        <v>-2.776630282283806</v>
       </c>
       <c r="G111">
         <v>-0.05228418171994131</v>
@@ -2968,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.782625645704036</v>
+        <v>-2.782998115473368</v>
       </c>
       <c r="G112">
         <v>-0.05265652914170493</v>
@@ -2991,7 +2991,7 @@
         <v>41</v>
       </c>
       <c r="F113">
-        <v>-2.787495426092556</v>
+        <v>-2.788275095314994</v>
       </c>
       <c r="G113">
         <v>-0.05443394120460865</v>
@@ -3014,7 +3014,7 @@
         <v>42</v>
       </c>
       <c r="F114">
-        <v>-2.794376066736298</v>
+        <v>-2.795076685920944</v>
       </c>
       <c r="G114">
         <v>-0.05484941824675094</v>
@@ -3060,7 +3060,7 @@
         <v>44</v>
       </c>
       <c r="F116">
-        <v>-2.806017669833766</v>
+        <v>-2.806595723585162</v>
       </c>
       <c r="G116">
         <v>-0.05629771188832478</v>
@@ -3083,7 +3083,7 @@
         <v>45</v>
       </c>
       <c r="F117">
-        <v>-2.811209954592179</v>
+        <v>-2.812261084476657</v>
       </c>
       <c r="G117">
         <v>-0.05673703354188819</v>
@@ -3106,7 +3106,7 @@
         <v>46</v>
       </c>
       <c r="F118">
-        <v>-2.816936589341345</v>
+        <v>-2.817503724539682</v>
       </c>
       <c r="G118">
         <v>-0.05832060457832489</v>
@@ -3129,7 +3129,7 @@
         <v>47</v>
       </c>
       <c r="F119">
-        <v>-2.823801251983955</v>
+        <v>-2.824058167066811</v>
       </c>
       <c r="G119">
         <v>-0.06027404392161584</v>
@@ -3152,7 +3152,7 @@
         <v>48</v>
       </c>
       <c r="F120">
-        <v>-2.827503614459652</v>
+        <v>-2.830051491611046</v>
       </c>
       <c r="G120">
         <v>-0.05678812008185008</v>
@@ -3175,7 +3175,7 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.83401037603045</v>
+        <v>-2.834338931260185</v>
       </c>
       <c r="G121">
         <v>-0.06000911149696631</v>
@@ -3198,7 +3198,7 @@
         <v>50</v>
       </c>
       <c r="F122">
-        <v>-2.838978997118416</v>
+        <v>-2.839426316124094</v>
       </c>
       <c r="G122">
         <v>-0.06010277017543042</v>
@@ -3244,7 +3244,7 @@
         <v>52</v>
       </c>
       <c r="F124">
-        <v>-2.85025554793902</v>
+        <v>-2.851020932746203</v>
       </c>
       <c r="G124">
         <v>-0.06128663039299131</v>
@@ -3267,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.855727620921819</v>
+        <v>-2.856546668540866</v>
       </c>
       <c r="G125">
         <v>-0.06141738346264969</v>
@@ -3290,7 +3290,7 @@
         <v>54</v>
       </c>
       <c r="F126">
-        <v>-2.860604829993085</v>
+        <v>-2.861995839860281</v>
       </c>
       <c r="G126">
         <v>-0.0610192997207204</v>
@@ -3313,7 +3313,7 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.866759499480688</v>
+        <v>-2.867073125934038</v>
       </c>
       <c r="G127">
         <v>-0.06227460763599346</v>
@@ -3336,7 +3336,7 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.872687936797506</v>
+        <v>-2.873829094865831</v>
       </c>
       <c r="G128">
         <v>-0.06178267537622562</v>
@@ -3359,7 +3359,7 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.878774949605554</v>
+        <v>-2.881078259951218</v>
       </c>
       <c r="G129">
         <v>-0.0628489587630503</v>
@@ -3382,7 +3382,7 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.884569497790821</v>
+        <v>-2.884921139917135</v>
       </c>
       <c r="G130">
         <v>-0.06315778161906183</v>
@@ -3405,7 +3405,7 @@
         <v>59</v>
       </c>
       <c r="F131">
-        <v>-2.888062742161599</v>
+        <v>-2.888482594611272</v>
       </c>
       <c r="G131">
         <v>-0.06400379531036271</v>
@@ -3428,7 +3428,7 @@
         <v>60</v>
       </c>
       <c r="F132">
-        <v>-2.894051155315235</v>
+        <v>-2.895010105185572</v>
       </c>
       <c r="G132">
         <v>-0.06487120968189952</v>
@@ -3451,7 +3451,7 @@
         <v>61</v>
       </c>
       <c r="F133">
-        <v>-2.899556085513892</v>
+        <v>-2.900110629721547</v>
       </c>
       <c r="G133">
         <v>-0.06665454538554338</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.903809790610806</v>
+        <v>-2.90476199420082</v>
       </c>
       <c r="G134">
         <v>-0.06372632355803498</v>
@@ -3497,7 +3497,7 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.909994630219312</v>
+        <v>-2.910382771364809</v>
       </c>
       <c r="G135">
         <v>-0.06392543768492631</v>
@@ -3520,7 +3520,7 @@
         <v>64</v>
       </c>
       <c r="F136">
-        <v>-2.917632046275433</v>
+        <v>-2.917810300294328</v>
       </c>
       <c r="G136">
         <v>-0.06704948777737774</v>
@@ -3543,7 +3543,7 @@
         <v>65</v>
       </c>
       <c r="F137">
-        <v>-2.921462703550947</v>
+        <v>-2.922715609602384</v>
       </c>
       <c r="G137">
         <v>-0.06769446591700889</v>
@@ -3566,7 +3566,7 @@
         <v>66</v>
       </c>
       <c r="F138">
-        <v>-2.925240382044629</v>
+        <v>-2.925492280066375</v>
       </c>
       <c r="G138">
         <v>-0.06657101570578416</v>
@@ -3589,7 +3589,7 @@
         <v>67</v>
       </c>
       <c r="F139">
-        <v>-2.931472624041096</v>
+        <v>-2.932102139760855</v>
       </c>
       <c r="G139">
         <v>-0.06791020309441009</v>
@@ -3612,7 +3612,7 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.936403561658945</v>
+        <v>-2.937402763206419</v>
       </c>
       <c r="G140">
         <v>-0.06657930309982896</v>
@@ -3635,7 +3635,7 @@
         <v>69</v>
       </c>
       <c r="F141">
-        <v>-2.94200408010642</v>
+        <v>-2.9421098940919</v>
       </c>
       <c r="G141">
         <v>-0.06708370049153078</v>
@@ -3658,7 +3658,7 @@
         <v>70</v>
       </c>
       <c r="F142">
-        <v>-2.947608015262093</v>
+        <v>-2.948280120868618</v>
       </c>
       <c r="G142">
         <v>-0.06779788511858942</v>
@@ -3681,7 +3681,7 @@
         <v>71</v>
       </c>
       <c r="F143">
-        <v>-2.951615683346875</v>
+        <v>-2.953106408647871</v>
       </c>
       <c r="G143">
         <v>-0.06450248721298824</v>
@@ -3704,7 +3704,7 @@
         <v>72</v>
       </c>
       <c r="F144">
-        <v>-2.956126583628377</v>
+        <v>-2.957392898478543</v>
       </c>
       <c r="G144">
         <v>-0.06732753326125041</v>
@@ -3727,7 +3727,7 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.961407180252653</v>
+        <v>-2.962125493304821</v>
       </c>
       <c r="G145">
         <v>-0.06582163185846457</v>
@@ -3750,7 +3750,7 @@
         <v>74</v>
       </c>
       <c r="F146">
-        <v>-2.96739315953787</v>
+        <v>-2.967506962887702</v>
       </c>
       <c r="G146">
         <v>-0.06790146423278398</v>
@@ -3796,7 +3796,7 @@
         <v>76</v>
       </c>
       <c r="F148">
-        <v>-2.976855218327667</v>
+        <v>-2.977602202825011</v>
       </c>
       <c r="G148">
         <v>-0.06823410457540602</v>
@@ -3819,7 +3819,7 @@
         <v>77</v>
       </c>
       <c r="F149">
-        <v>-2.982159992646322</v>
+        <v>-2.982478986268691</v>
       </c>
       <c r="G149">
         <v>-0.06670793645458395</v>
@@ -3842,7 +3842,7 @@
         <v>78</v>
       </c>
       <c r="F150">
-        <v>-2.986650378176986</v>
+        <v>-2.986994974492911</v>
       </c>
       <c r="G150">
         <v>-0.06854791538365457</v>
@@ -3888,7 +3888,7 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.996152760644822</v>
+        <v>-2.997305876974929</v>
       </c>
       <c r="G152">
         <v>-0.06780185980026898</v>
@@ -3911,7 +3911,7 @@
         <v>81</v>
       </c>
       <c r="F153">
-        <v>-3.002176294718225</v>
+        <v>-3.002645253762812</v>
       </c>
       <c r="G153">
         <v>-0.06455850371540439</v>
@@ -3934,7 +3934,7 @@
         <v>82</v>
       </c>
       <c r="F154">
-        <v>-3.006187623249666</v>
+        <v>-3.006778206336128</v>
       </c>
       <c r="G154">
         <v>-0.06731151096098098</v>
@@ -3957,7 +3957,7 @@
         <v>83</v>
       </c>
       <c r="F155">
-        <v>-3.010524771102745</v>
+        <v>-3.010926011316208</v>
       </c>
       <c r="G155">
         <v>-0.06612522975386037</v>
@@ -3980,7 +3980,7 @@
         <v>84</v>
       </c>
       <c r="F156">
-        <v>-3.015001859457396</v>
+        <v>-3.015680591900383</v>
       </c>
       <c r="G156">
         <v>-0.06665332484574193</v>
@@ -4003,7 +4003,7 @@
         <v>85</v>
       </c>
       <c r="F157">
-        <v>-3.019988911721621</v>
+        <v>-3.020508169087034</v>
       </c>
       <c r="G157">
         <v>-0.06485566663902187</v>
@@ -4026,7 +4026,7 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.025253967463569</v>
+        <v>-3.026200663894586</v>
       </c>
       <c r="G158">
         <v>-0.06574624348211056</v>
@@ -4049,7 +4049,7 @@
         <v>87</v>
       </c>
       <c r="F159">
-        <v>-3.030893326777961</v>
+        <v>-3.031169144325665</v>
       </c>
       <c r="G159">
         <v>-0.06768449316199199</v>
@@ -4072,7 +4072,7 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.035014009120696</v>
+        <v>-3.035995264110954</v>
       </c>
       <c r="G160">
         <v>-0.06447723515981063</v>
@@ -4095,7 +4095,7 @@
         <v>89</v>
       </c>
       <c r="F161">
-        <v>-3.03825063639719</v>
+        <v>-3.0382908681829</v>
       </c>
       <c r="G161">
         <v>-0.06501816482063427</v>
@@ -4118,7 +4118,7 @@
         <v>90</v>
       </c>
       <c r="F162">
-        <v>-3.043672997008324</v>
+        <v>-3.04477441877759</v>
       </c>
       <c r="G162">
         <v>-0.06542870645147514</v>
@@ -4141,7 +4141,7 @@
         <v>91</v>
       </c>
       <c r="F163">
-        <v>-3.050030487114018</v>
+        <v>-3.050328364043296</v>
       </c>
       <c r="G163">
         <v>-0.06595331802108673</v>
@@ -4164,7 +4164,7 @@
         <v>92</v>
       </c>
       <c r="F164">
-        <v>-3.053528711057775</v>
+        <v>-3.053741715275098</v>
       </c>
       <c r="G164">
         <v>-0.06477163404513264</v>
@@ -4210,7 +4210,7 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.062579727792436</v>
+        <v>-3.062784217926058</v>
       </c>
       <c r="G166">
         <v>-0.06265426210750791</v>
@@ -4233,7 +4233,7 @@
         <v>95</v>
       </c>
       <c r="F167">
-        <v>-3.066793143194778</v>
+        <v>-3.068395256206483</v>
       </c>
       <c r="G167">
         <v>-0.06294389008283985</v>
@@ -4256,7 +4256,7 @@
         <v>96</v>
       </c>
       <c r="F168">
-        <v>-3.071142906206022</v>
+        <v>-3.073248305309884</v>
       </c>
       <c r="G168">
         <v>-0.06087182508497047</v>
@@ -4302,7 +4302,7 @@
         <v>98</v>
       </c>
       <c r="F170">
-        <v>-3.0820211183379</v>
+        <v>-3.082422253946845</v>
       </c>
       <c r="G170">
         <v>-0.06109185823841068</v>
@@ -4325,7 +4325,7 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.085623373035919</v>
+        <v>-3.086267065344651</v>
       </c>
       <c r="G171">
         <v>-0.06144085835089474</v>
@@ -4394,7 +4394,7 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.098917913719822</v>
+        <v>-3.098948154703767</v>
       </c>
       <c r="G174">
         <v>-0.05824262023479909</v>
@@ -4463,7 +4463,7 @@
         <v>105</v>
       </c>
       <c r="F177">
-        <v>-3.110689252978262</v>
+        <v>-3.111004000825581</v>
       </c>
       <c r="G177">
         <v>-0.05726767771701669</v>
@@ -4486,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="F178">
-        <v>-3.116207549514336</v>
+        <v>-3.116477709570204</v>
       </c>
       <c r="G178">
         <v>-0.05581483500563944</v>
@@ -4509,7 +4509,7 @@
         <v>107</v>
       </c>
       <c r="F179">
-        <v>-3.119194927189529</v>
+        <v>-3.120140937522577</v>
       </c>
       <c r="G179">
         <v>-0.05517185268375624</v>
@@ -4532,7 +4532,7 @@
         <v>108</v>
       </c>
       <c r="F180">
-        <v>-3.124470624963318</v>
+        <v>-3.125046931304443</v>
       </c>
       <c r="G180">
         <v>-0.0557679620549747</v>
@@ -4555,7 +4555,7 @@
         <v>109</v>
       </c>
       <c r="F181">
-        <v>-3.127558437683602</v>
+        <v>-3.12802642779326</v>
       </c>
       <c r="G181">
         <v>-0.05408958650118412</v>
@@ -4578,7 +4578,7 @@
         <v>110</v>
       </c>
       <c r="F182">
-        <v>-3.132939447210961</v>
+        <v>-3.134269113601619</v>
       </c>
       <c r="G182">
         <v>-0.05445877704824975</v>
@@ -4601,7 +4601,7 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.136007763768681</v>
+        <v>-3.137118014112034</v>
       </c>
       <c r="G183">
         <v>-0.05248383196828954</v>
@@ -4624,7 +4624,7 @@
         <v>112</v>
       </c>
       <c r="F184">
-        <v>-3.140938719361097</v>
+        <v>-3.141477214232125</v>
       </c>
       <c r="G184">
         <v>-0.04963277875443273</v>
@@ -4647,7 +4647,7 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.146014365222033</v>
+        <v>-3.146523023295797</v>
       </c>
       <c r="G185">
         <v>-0.04873802951269879</v>
@@ -4670,7 +4670,7 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.149695287544229</v>
+        <v>-3.150085495573549</v>
       </c>
       <c r="G186">
         <v>-0.04900903411513546</v>
@@ -4739,7 +4739,7 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.16049151181362</v>
+        <v>-3.160822187448525</v>
       </c>
       <c r="G189">
         <v>-0.0448020417717746</v>
@@ -4762,7 +4762,7 @@
         <v>118</v>
       </c>
       <c r="F190">
-        <v>-3.16510425589877</v>
+        <v>-3.165612913972534</v>
       </c>
       <c r="G190">
         <v>-0.04537717505014682</v>
@@ -4785,7 +4785,7 @@
         <v>119</v>
       </c>
       <c r="F191">
-        <v>-3.168977772165204</v>
+        <v>-3.169556957827944</v>
       </c>
       <c r="G191">
         <v>-0.04539073117985515</v>
@@ -4808,7 +4808,7 @@
         <v>120</v>
       </c>
       <c r="F192">
-        <v>-3.17370797116319</v>
+        <v>-3.174111066248696</v>
       </c>
       <c r="G192">
         <v>-0.04432853459351432</v>
@@ -4877,7 +4877,7 @@
         <v>123</v>
       </c>
       <c r="F195">
-        <v>-3.18518725597489</v>
+        <v>-3.185508347967865</v>
       </c>
       <c r="G195">
         <v>-0.03872384143873364</v>
@@ -4900,7 +4900,7 @@
         <v>124</v>
       </c>
       <c r="F196">
-        <v>-3.189111423044547</v>
+        <v>-3.190126354363985</v>
       </c>
       <c r="G196">
         <v>-0.03651257146252856</v>
@@ -4946,7 +4946,7 @@
         <v>126</v>
       </c>
       <c r="F198">
-        <v>-3.195395560351626</v>
+        <v>-3.195962709948929</v>
       </c>
       <c r="G198">
         <v>-0.03532006894105899</v>
@@ -4992,7 +4992,7 @@
         <v>128</v>
       </c>
       <c r="F200">
-        <v>-3.203085892108148</v>
+        <v>-3.204153034839979</v>
       </c>
       <c r="G200">
         <v>-0.03297449243434603</v>
@@ -5015,7 +5015,7 @@
         <v>129</v>
       </c>
       <c r="F201">
-        <v>-3.206756323989463</v>
+        <v>-3.20709268062067</v>
       </c>
       <c r="G201">
         <v>-0.03296750685671307</v>
@@ -5038,7 +5038,7 @@
         <v>130</v>
       </c>
       <c r="F202">
-        <v>-3.210681661419583</v>
+        <v>-3.211412447520205</v>
       </c>
       <c r="G202">
         <v>-0.03139378497422746</v>
@@ -5153,7 +5153,7 @@
         <v>135</v>
       </c>
       <c r="F207">
-        <v>-3.228359053591354</v>
+        <v>-3.228582309682441</v>
       </c>
       <c r="G207">
         <v>-0.02399763888814654</v>
@@ -5199,7 +5199,7 @@
         <v>137</v>
       </c>
       <c r="F209">
-        <v>-3.234809940147318</v>
+        <v>-3.23531747015685</v>
       </c>
       <c r="G209">
         <v>-0.02101015751669322</v>
@@ -5475,7 +5475,7 @@
         <v>30</v>
       </c>
       <c r="F221">
-        <v>-2.721729468088695</v>
+        <v>-2.72229098479988</v>
       </c>
       <c r="G221">
         <v>-0.02560431675245223</v>
@@ -5498,7 +5498,7 @@
         <v>61</v>
       </c>
       <c r="F222">
-        <v>-2.817106634341454</v>
+        <v>-2.818027126507107</v>
       </c>
       <c r="G222">
         <v>-0.04386742812921618</v>
@@ -5521,7 +5521,7 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.906957990495776</v>
+        <v>-2.907088556863</v>
       </c>
       <c r="G223">
         <v>-0.05728340565328049</v>
@@ -5544,7 +5544,7 @@
         <v>123</v>
       </c>
       <c r="F224">
-        <v>-2.992002848431156</v>
+        <v>-2.992755358524738</v>
       </c>
       <c r="G224">
         <v>-0.06577717043876063</v>
@@ -5567,7 +5567,7 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.07334638953181</v>
+        <v>-3.073843689921</v>
       </c>
       <c r="G225">
         <v>-0.06851272909896111</v>
@@ -5590,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.147328074376943</v>
+        <v>-3.147803739418754</v>
       </c>
       <c r="G226">
         <v>-0.06749295502671293</v>
@@ -5613,7 +5613,7 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.215467582571681</v>
+        <v>-3.2160999406124</v>
       </c>
       <c r="G227">
         <v>-0.05736411736875813</v>
@@ -5659,7 +5659,7 @@
         <v>278</v>
       </c>
       <c r="F229">
-        <v>-3.336305831800731</v>
+        <v>-3.336348063458273</v>
       </c>
       <c r="G229">
         <v>-0.02698616761849393</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.785465779935326</v>
+        <v>-2.786147729031592</v>
       </c>
       <c r="G232">
         <v>-0.02527176346397342</v>
@@ -5751,7 +5751,7 @@
         <v>112</v>
       </c>
       <c r="F233">
-        <v>-2.882212288148072</v>
+        <v>-2.882579645320932</v>
       </c>
       <c r="G233">
         <v>-0.04376841583561886</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.97545774266125</v>
+        <v>-2.975773110198728</v>
       </c>
       <c r="G234">
         <v>-0.05795588987540001</v>
@@ -5797,7 +5797,7 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.0597795102224</v>
+        <v>-3.059851049140998</v>
       </c>
       <c r="G235">
         <v>-0.06540721728834087</v>
@@ -5820,7 +5820,7 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.142199875457754</v>
+        <v>-3.142565422629807</v>
       </c>
       <c r="G236">
         <v>-0.06931697938274617</v>
@@ -5843,7 +5843,7 @@
         <v>336</v>
       </c>
       <c r="F237">
-        <v>-3.217414775683589</v>
+        <v>-3.217638002679049</v>
       </c>
       <c r="G237">
         <v>-0.06632166244271054</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.287163187852923</v>
+        <v>-3.287273832229776</v>
       </c>
       <c r="G238">
         <v>-0.05800286097577989</v>
@@ -5981,7 +5981,7 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.828533199099743</v>
+        <v>-2.82920117972315</v>
       </c>
       <c r="G243">
         <v>-0.0250304586649932</v>
@@ -6004,7 +6004,7 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.926171870329461</v>
+        <v>-2.92626371924288</v>
       </c>
       <c r="G244">
         <v>-0.04354852366881445</v>
@@ -6027,7 +6027,7 @@
         <v>276</v>
       </c>
       <c r="F245">
-        <v>-3.018624987323443</v>
+        <v>-3.018668468724671</v>
       </c>
       <c r="G245">
         <v>-0.05723271934982499</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.108310053919059</v>
+        <v>-3.108448371160833</v>
       </c>
       <c r="G246">
         <v>-0.06482813356561712</v>
@@ -6073,7 +6073,7 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.190171603828873</v>
+        <v>-3.190285688701083</v>
       </c>
       <c r="G247">
         <v>-0.06805097876230648</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.266758536966854</v>
+        <v>-3.266845499769308</v>
       </c>
       <c r="G248">
         <v>-0.06681828405940005</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.338389455690561</v>
+        <v>-3.338485811014014</v>
       </c>
       <c r="G249">
         <v>-0.05760174171475763</v>
@@ -6165,7 +6165,7 @@
         <v>830</v>
       </c>
       <c r="F251">
-        <v>-3.464181639065342</v>
+        <v>-3.464306102521145</v>
       </c>
       <c r="G251">
         <v>-0.02602466555336047</v>
@@ -6234,7 +6234,7 @@
         <v>141</v>
       </c>
       <c r="F254">
-        <v>-2.858623322430484</v>
+        <v>-2.858856743806128</v>
       </c>
       <c r="G254">
         <v>-0.0241816450302621</v>
@@ -6257,7 +6257,7 @@
         <v>283</v>
       </c>
       <c r="F255">
-        <v>-2.959116687715872</v>
+        <v>-2.959203160009108</v>
       </c>
       <c r="G255">
         <v>-0.04364111093397272</v>
@@ -6280,7 +6280,7 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.052753171251637</v>
+        <v>-3.052809337315142</v>
       </c>
       <c r="G256">
         <v>-0.05723884722613048</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.141582105107187</v>
+        <v>-3.14174123101849</v>
       </c>
       <c r="G257">
         <v>-0.06523516485980907</v>
@@ -6326,7 +6326,7 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.224653950096374</v>
+        <v>-3.224826629755423</v>
       </c>
       <c r="G258">
         <v>-0.06834797726552355</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.303298628607456</v>
+        <v>-3.303507220660733</v>
       </c>
       <c r="G259">
         <v>-0.06499168668186583</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.375294742817646</v>
+        <v>-3.375324167192619</v>
       </c>
       <c r="G260">
         <v>-0.05743932002365837</v>
@@ -6418,7 +6418,7 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.502623495605347</v>
+        <v>-3.502643840541766</v>
       </c>
       <c r="G262">
         <v>-0.0252635603647639</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.882753836884993</v>
+        <v>-2.882946807602409</v>
       </c>
       <c r="G265">
         <v>-0.0240632056775123</v>
@@ -6510,7 +6510,7 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.982934689945172</v>
+        <v>-2.983254722231226</v>
       </c>
       <c r="G266">
         <v>-0.04331321550334977</v>
@@ -6533,7 +6533,7 @@
         <v>617</v>
       </c>
       <c r="F267">
-        <v>-3.077896571705333</v>
+        <v>-3.078246401913582</v>
       </c>
       <c r="G267">
         <v>-0.05631636605077839</v>
@@ -6556,7 +6556,7 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.167583822026921</v>
+        <v>-3.167854221881214</v>
       </c>
       <c r="G268">
         <v>-0.06455489133007597</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.251305594258885</v>
+        <v>-3.251520090452157</v>
       </c>
       <c r="G269">
         <v>-0.06780675191923091</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.330715530744679</v>
+        <v>-3.330929582189078</v>
       </c>
       <c r="G270">
         <v>-0.06419752115149246</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.470384589899591</v>
+        <v>-3.470536114371271</v>
       </c>
       <c r="G272">
         <v>-0.04387737884515908</v>
@@ -6671,7 +6671,7 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.531834329867634</v>
+        <v>-3.53191432878926</v>
       </c>
       <c r="G273">
         <v>-0.02466589200668384</v>
@@ -6740,7 +6740,7 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.901353445396789</v>
+        <v>-2.901482897902854</v>
       </c>
       <c r="G276">
         <v>-0.02406920687054059</v>
@@ -6763,7 +6763,7 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.001906182634051</v>
+        <v>-3.002140624103695</v>
       </c>
       <c r="G277">
         <v>-0.04227620044241398</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.097718421551724</v>
+        <v>-3.097783316229176</v>
       </c>
       <c r="G278">
         <v>-0.05607882283516297</v>
@@ -6809,7 +6809,7 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.187629474947174</v>
+        <v>-3.187876057929453</v>
       </c>
       <c r="G279">
         <v>-0.06318188816633419</v>
@@ -6832,7 +6832,7 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.272596820551765</v>
+        <v>-3.272903786512736</v>
       </c>
       <c r="G280">
         <v>-0.06621825962590311</v>
@@ -6855,7 +6855,7 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.351791532868845</v>
+        <v>-3.352205624672247</v>
       </c>
       <c r="G281">
         <v>-0.06398994315260564</v>
@@ -6878,7 +6878,7 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.425119950847487</v>
+        <v>-3.425569404379988</v>
       </c>
       <c r="G282">
         <v>-0.05612750293692592</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.492399678604969</v>
+        <v>-3.492777865089028</v>
       </c>
       <c r="G283">
         <v>-0.04295880299185728</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.554874228601493</v>
+        <v>-3.555021461264616</v>
       </c>
       <c r="G284">
         <v>-0.0244730013361007</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.916675103103247</v>
+        <v>-2.916941444266158</v>
       </c>
       <c r="G287">
         <v>-0.02367997741095973</v>
@@ -7016,7 +7016,7 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.017622009757004</v>
+        <v>-3.017691305283781</v>
       </c>
       <c r="G288">
         <v>-0.04251300891418719</v>
@@ -7039,7 +7039,7 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.113677070659592</v>
+        <v>-3.113868671160673</v>
       </c>
       <c r="G289">
         <v>-0.05551791606564294</v>
@@ -7062,7 +7062,7 @@
         <v>1548</v>
       </c>
       <c r="F290">
-        <v>-3.204339678774593</v>
+        <v>-3.204771157617794</v>
       </c>
       <c r="G290">
         <v>-0.06299904231392772</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.28932044900224</v>
+        <v>-3.289690025780672</v>
       </c>
       <c r="G291">
         <v>-0.0655803780886155</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.368894258297968</v>
+        <v>-3.369536530513567</v>
       </c>
       <c r="G292">
         <v>-0.06303955016071905</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.442431535213945</v>
+        <v>-3.443116424555875</v>
       </c>
       <c r="G293">
         <v>-0.05515012424061883</v>
@@ -7154,7 +7154,7 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.510742992195424</v>
+        <v>-3.511174259827198</v>
       </c>
       <c r="G294">
         <v>-0.04236717761340913</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.573311827673294</v>
+        <v>-3.573377639242001</v>
       </c>
       <c r="G295">
         <v>-0.02449152068444382</v>
@@ -7246,7 +7246,7 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.929119222088884</v>
+        <v>-2.929305380983764</v>
       </c>
       <c r="G298">
         <v>-0.02357381916767043</v>
@@ -7269,7 +7269,7 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.03055267499326</v>
+        <v>-3.030685550306855</v>
       </c>
       <c r="G299">
         <v>-0.04201270279780811</v>
@@ -7292,7 +7292,7 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.126877317882713</v>
+        <v>-3.127191833883172</v>
       </c>
       <c r="G300">
         <v>-0.0543073434687642</v>
@@ -7315,7 +7315,7 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.217784402036398</v>
+        <v>-3.218291057772684</v>
       </c>
       <c r="G301">
         <v>-0.06219144904681673</v>
@@ -7338,7 +7338,7 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.303176176223764</v>
+        <v>-3.303966242601376</v>
       </c>
       <c r="G302">
         <v>-0.06503915675330885</v>
@@ -7361,7 +7361,7 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.38273532195491</v>
+        <v>-3.383605153169666</v>
       </c>
       <c r="G303">
         <v>-0.06236990600344705</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.457371496651011</v>
+        <v>-3.458298090038189</v>
       </c>
       <c r="G304">
         <v>-0.05464736464488806</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.52571168893542</v>
+        <v>-3.526369809228998</v>
       </c>
       <c r="G305">
         <v>-0.04220518905553605</v>
@@ -7430,7 +7430,7 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.588475545632808</v>
+        <v>-3.588716447193514</v>
       </c>
       <c r="G306">
         <v>-0.02395110289660207</v>
@@ -7499,7 +7499,7 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.939502050526279</v>
+        <v>-2.939694004878652</v>
       </c>
       <c r="G309">
         <v>-0.02338508521976257</v>
@@ -7522,7 +7522,7 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.041301204178368</v>
+        <v>-3.041495676422547</v>
       </c>
       <c r="G310">
         <v>-0.04129000151007567</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.138028678381241</v>
+        <v>-3.13847205729284</v>
       </c>
       <c r="G311">
         <v>-0.05420531534682338</v>
@@ -7568,7 +7568,7 @@
         <v>2610</v>
       </c>
       <c r="F312">
-        <v>-3.228854273413367</v>
+        <v>-3.229759206086767</v>
       </c>
       <c r="G312">
         <v>-0.06159631211594552</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.3144075862108</v>
+        <v>-3.315386998485069</v>
       </c>
       <c r="G313">
         <v>-0.06397337201434161</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.394757037903488</v>
+        <v>-3.396251702933894</v>
       </c>
       <c r="G314">
         <v>-0.061438666420216</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.468956934684792</v>
+        <v>-3.470244786953842</v>
       </c>
       <c r="G315">
         <v>-0.05399105464408593</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.538189380448835</v>
+        <v>-3.538995317477704</v>
       </c>
       <c r="G316">
         <v>-0.0413182393111089</v>
@@ -7683,7 +7683,7 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.601173136993015</v>
+        <v>-3.601465079277375</v>
       </c>
       <c r="G317">
         <v>-0.02372300662380827</v>
@@ -7752,7 +7752,7 @@
         <v>821</v>
       </c>
       <c r="F320">
-        <v>-2.948295291869554</v>
+        <v>-2.948353902067926</v>
       </c>
       <c r="G320">
         <v>-0.0233819330146412</v>
@@ -7775,7 +7775,7 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.050301686199274</v>
+        <v>-3.050544519531514</v>
       </c>
       <c r="G321">
         <v>-0.0412592898511992</v>
@@ -7798,7 +7798,7 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.14738127792324</v>
+        <v>-3.147994627343824</v>
       </c>
       <c r="G322">
         <v>-0.05332638142041324</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.23827236163357</v>
+        <v>-3.23939404245551</v>
       </c>
       <c r="G323">
         <v>-0.06099802107311758</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.324263017962735</v>
+        <v>-3.32561250971933</v>
       </c>
       <c r="G324">
         <v>-0.06352861199624371</v>
@@ -7867,7 +7867,7 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.404333248923183</v>
+        <v>-3.406131182695687</v>
       </c>
       <c r="G325">
         <v>-0.06095986211832471</v>
@@ -7890,7 +7890,7 @@
         <v>5751</v>
       </c>
       <c r="F326">
-        <v>-3.47933785083631</v>
+        <v>-3.481000859790254</v>
       </c>
       <c r="G326">
         <v>-0.05364092179063251</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.548240382816604</v>
+        <v>-3.549396217465975</v>
       </c>
       <c r="G327">
         <v>-0.04087010370692101</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.612230915524306</v>
+        <v>-3.612645085952099</v>
       </c>
       <c r="G328">
         <v>-0.02339390262022029</v>
@@ -8005,7 +8005,7 @@
         <v>1017</v>
       </c>
       <c r="F331">
-        <v>-2.956056144997122</v>
+        <v>-2.956135910407875</v>
       </c>
       <c r="G331">
         <v>-0.02304604198804938</v>
@@ -8028,7 +8028,7 @@
         <v>2035</v>
       </c>
       <c r="F332">
-        <v>-3.05824364257423</v>
+        <v>-3.058648904743516</v>
       </c>
       <c r="G332">
         <v>-0.04084545509864856</v>
@@ -8051,7 +8051,7 @@
         <v>3053</v>
       </c>
       <c r="F333">
-        <v>-3.155090689209559</v>
+        <v>-3.155844359088574</v>
       </c>
       <c r="G333">
         <v>-0.05317217999790391</v>
@@ -8074,7 +8074,7 @@
         <v>4071</v>
       </c>
       <c r="F334">
-        <v>-3.246319023253284</v>
+        <v>-3.247754457165829</v>
       </c>
       <c r="G334">
         <v>-0.06057126192654172</v>
@@ -8097,7 +8097,7 @@
         <v>5089</v>
       </c>
       <c r="F335">
-        <v>-3.332130557403822</v>
+        <v>-3.33436889827686</v>
       </c>
       <c r="G335">
         <v>-0.06278717063128125</v>
@@ -8120,7 +8120,7 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.412878355089753</v>
+        <v>-3.414985217608911</v>
       </c>
       <c r="G336">
         <v>-0.06050505627801783</v>
@@ -8143,7 +8143,7 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.487839886350137</v>
+        <v>-3.489777944869828</v>
       </c>
       <c r="G337">
         <v>-0.05286449853341879</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.557352462816103</v>
+        <v>-3.558690544624951</v>
       </c>
       <c r="G338">
         <v>-0.04053172592297882</v>
@@ -8189,7 +8189,7 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.621296743720847</v>
+        <v>-3.621825275949748</v>
       </c>
       <c r="G339">
         <v>-0.02310751223477731</v>

</xml_diff>

<commit_message>
updated data from 03.03.2019
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>-2.494387253749535</v>
+        <v>-2.494442893176611</v>
       </c>
       <c r="G24">
         <v>-0.03422076265821916</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.613044874089788</v>
+        <v>-2.613532591755807</v>
       </c>
       <c r="G32">
         <v>-0.05383393390282332</v>
@@ -1450,7 +1450,7 @@
         <v>30</v>
       </c>
       <c r="F46">
-        <v>-2.799531128357493</v>
+        <v>-2.79977586579563</v>
       </c>
       <c r="G46">
         <v>-0.06387835591992652</v>
@@ -1473,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="F47">
-        <v>-2.810595484048786</v>
+        <v>-2.812136732803287</v>
       </c>
       <c r="G47">
         <v>-0.06247389129781755</v>
@@ -1519,7 +1519,7 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.832956532957937</v>
+        <v>-2.834607384909984</v>
       </c>
       <c r="G49">
         <v>-0.06086949888522653</v>
@@ -2301,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="F83">
-        <v>-2.605025808293304</v>
+        <v>-2.605078911354817</v>
       </c>
       <c r="G83">
         <v>-0.02247245056416469</v>
@@ -2347,7 +2347,7 @@
         <v>13</v>
       </c>
       <c r="F85">
-        <v>-2.617508322953553</v>
+        <v>-2.617843054849695</v>
       </c>
       <c r="G85">
         <v>-0.02313921711713052</v>
@@ -2439,7 +2439,7 @@
         <v>17</v>
       </c>
       <c r="F89">
-        <v>-2.643094408998108</v>
+        <v>-2.643806651977909</v>
       </c>
       <c r="G89">
         <v>-0.02875040782855365</v>
@@ -2462,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="F90">
-        <v>-2.64959662870154</v>
+        <v>-2.649798004427677</v>
       </c>
       <c r="G90">
         <v>-0.03114366471063246</v>
@@ -2508,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.662228729950169</v>
+        <v>-2.66243633207324</v>
       </c>
       <c r="G92">
         <v>-0.03279670476236696</v>
@@ -2531,7 +2531,7 @@
         <v>21</v>
       </c>
       <c r="F93">
-        <v>-2.668906254976394</v>
+        <v>-2.669076951243897</v>
       </c>
       <c r="G93">
         <v>-0.0338386097874217</v>
@@ -2554,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="F94">
-        <v>-2.674158875917362</v>
+        <v>-2.675521418758289</v>
       </c>
       <c r="G94">
         <v>-0.03615692101567447</v>
@@ -2623,7 +2623,7 @@
         <v>25</v>
       </c>
       <c r="F97">
-        <v>-2.693498536566583</v>
+        <v>-2.694432220033696</v>
       </c>
       <c r="G97">
         <v>-0.03825148586158944</v>
@@ -2738,7 +2738,7 @@
         <v>30</v>
       </c>
       <c r="F102">
-        <v>-2.723818139658242</v>
+        <v>-2.724057856540847</v>
       </c>
       <c r="G102">
         <v>-0.04469874040493416</v>
@@ -2761,7 +2761,7 @@
         <v>31</v>
       </c>
       <c r="F103">
-        <v>-2.728981498097013</v>
+        <v>-2.729256205602705</v>
       </c>
       <c r="G103">
         <v>-0.04539819683189528</v>
@@ -2784,7 +2784,7 @@
         <v>32</v>
       </c>
       <c r="F104">
-        <v>-2.735969503946624</v>
+        <v>-2.736155970979087</v>
       </c>
       <c r="G104">
         <v>-0.04748471955815536</v>
@@ -2853,7 +2853,7 @@
         <v>35</v>
       </c>
       <c r="F107">
-        <v>-2.753164643948289</v>
+        <v>-2.753252728265598</v>
       </c>
       <c r="G107">
         <v>-0.04940962190280773</v>
@@ -2876,7 +2876,7 @@
         <v>36</v>
       </c>
       <c r="F108">
-        <v>-2.760566422452002</v>
+        <v>-2.76096979435579</v>
       </c>
       <c r="G108">
         <v>-0.04920619233585422</v>
@@ -2945,7 +2945,7 @@
         <v>39</v>
       </c>
       <c r="F111">
-        <v>-2.776630282283806</v>
+        <v>-2.776803670391222</v>
       </c>
       <c r="G111">
         <v>-0.05228418171994131</v>
@@ -2968,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.782998115473368</v>
+        <v>-2.783099863433906</v>
       </c>
       <c r="G112">
         <v>-0.05265652914170493</v>
@@ -2991,7 +2991,7 @@
         <v>41</v>
       </c>
       <c r="F113">
-        <v>-2.788275095314994</v>
+        <v>-2.789194802063853</v>
       </c>
       <c r="G113">
         <v>-0.05443394120460865</v>
@@ -3037,7 +3037,7 @@
         <v>43</v>
       </c>
       <c r="F115">
-        <v>-2.800191385123631</v>
+        <v>-2.800672003119718</v>
       </c>
       <c r="G115">
         <v>-0.05583094422105916</v>
@@ -3106,7 +3106,7 @@
         <v>46</v>
       </c>
       <c r="F118">
-        <v>-2.817503724539682</v>
+        <v>-2.817681875015227</v>
       </c>
       <c r="G118">
         <v>-0.05832060457832489</v>
@@ -3221,7 +3221,7 @@
         <v>51</v>
       </c>
       <c r="F123">
-        <v>-2.84532322984614</v>
+        <v>-2.845978069606061</v>
       </c>
       <c r="G123">
         <v>-0.06172347505184139</v>
@@ -3244,7 +3244,7 @@
         <v>52</v>
       </c>
       <c r="F124">
-        <v>-2.851020932746203</v>
+        <v>-2.851750119233269</v>
       </c>
       <c r="G124">
         <v>-0.06128663039299131</v>
@@ -3267,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.856546668540866</v>
+        <v>-2.856908227229114</v>
       </c>
       <c r="G125">
         <v>-0.06141738346264969</v>
@@ -3359,7 +3359,7 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.881078259951218</v>
+        <v>-2.881279635677355</v>
       </c>
       <c r="G129">
         <v>-0.0628489587630503</v>
@@ -3428,7 +3428,7 @@
         <v>60</v>
       </c>
       <c r="F132">
-        <v>-2.895010105185572</v>
+        <v>-2.895356023424147</v>
       </c>
       <c r="G132">
         <v>-0.06487120968189952</v>
@@ -3451,7 +3451,7 @@
         <v>61</v>
       </c>
       <c r="F133">
-        <v>-2.900110629721547</v>
+        <v>-2.900317726011542</v>
       </c>
       <c r="G133">
         <v>-0.06665454538554338</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.90476199420082</v>
+        <v>-2.905157701136438</v>
       </c>
       <c r="G134">
         <v>-0.06372632355803498</v>
@@ -3497,7 +3497,7 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.910382771364809</v>
+        <v>-2.910488765484706</v>
       </c>
       <c r="G135">
         <v>-0.06392543768492631</v>
@@ -3543,7 +3543,7 @@
         <v>65</v>
       </c>
       <c r="F137">
-        <v>-2.922715609602384</v>
+        <v>-2.923056032258541</v>
       </c>
       <c r="G137">
         <v>-0.06769446591700889</v>
@@ -3566,7 +3566,7 @@
         <v>66</v>
       </c>
       <c r="F138">
-        <v>-2.925492280066375</v>
+        <v>-2.926806772077847</v>
       </c>
       <c r="G138">
         <v>-0.06657101570578416</v>
@@ -3612,7 +3612,7 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.937402763206419</v>
+        <v>-2.937633125717735</v>
       </c>
       <c r="G140">
         <v>-0.06657930309982896</v>
@@ -3635,7 +3635,7 @@
         <v>69</v>
       </c>
       <c r="F141">
-        <v>-2.9421098940919</v>
+        <v>-2.943609446751588</v>
       </c>
       <c r="G141">
         <v>-0.06708370049153078</v>
@@ -3658,7 +3658,7 @@
         <v>70</v>
       </c>
       <c r="F142">
-        <v>-2.948280120868618</v>
+        <v>-2.948553136741634</v>
       </c>
       <c r="G142">
         <v>-0.06779788511858942</v>
@@ -3681,7 +3681,7 @@
         <v>71</v>
       </c>
       <c r="F143">
-        <v>-2.953106408647871</v>
+        <v>-2.953123447678578</v>
       </c>
       <c r="G143">
         <v>-0.06450248721298824</v>
@@ -3773,7 +3773,7 @@
         <v>75</v>
       </c>
       <c r="F147">
-        <v>-2.971590631594759</v>
+        <v>-2.971935422715746</v>
       </c>
       <c r="G147">
         <v>-0.06717352781770547</v>
@@ -3796,7 +3796,7 @@
         <v>76</v>
       </c>
       <c r="F148">
-        <v>-2.977602202825011</v>
+        <v>-2.977896336549297</v>
       </c>
       <c r="G148">
         <v>-0.06823410457540602</v>
@@ -3865,7 +3865,7 @@
         <v>79</v>
       </c>
       <c r="F151">
-        <v>-2.992850267538294</v>
+        <v>-2.993289451945098</v>
       </c>
       <c r="G151">
         <v>-0.06608525725976122</v>
@@ -3934,7 +3934,7 @@
         <v>82</v>
       </c>
       <c r="F154">
-        <v>-3.006778206336128</v>
+        <v>-3.007060784823164</v>
       </c>
       <c r="G154">
         <v>-0.06731151096098098</v>
@@ -3957,7 +3957,7 @@
         <v>83</v>
       </c>
       <c r="F155">
-        <v>-3.010926011316208</v>
+        <v>-3.011134211911406</v>
       </c>
       <c r="G155">
         <v>-0.06612522975386037</v>
@@ -4003,7 +4003,7 @@
         <v>85</v>
       </c>
       <c r="F157">
-        <v>-3.020508169087034</v>
+        <v>-3.021285961458676</v>
       </c>
       <c r="G157">
         <v>-0.06485566663902187</v>
@@ -4026,7 +4026,7 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.026200663894586</v>
+        <v>-3.026437180748415</v>
       </c>
       <c r="G158">
         <v>-0.06574624348211056</v>
@@ -4072,7 +4072,7 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.035995264110954</v>
+        <v>-3.036187401049683</v>
       </c>
       <c r="G160">
         <v>-0.06447723515981063</v>
@@ -4095,7 +4095,7 @@
         <v>89</v>
       </c>
       <c r="F161">
-        <v>-3.0382908681829</v>
+        <v>-3.03860610696284</v>
       </c>
       <c r="G161">
         <v>-0.06501816482063427</v>
@@ -4118,7 +4118,7 @@
         <v>90</v>
       </c>
       <c r="F162">
-        <v>-3.04477441877759</v>
+        <v>-3.044975286333649</v>
       </c>
       <c r="G162">
         <v>-0.06542870645147514</v>
@@ -4210,7 +4210,7 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.062784217926058</v>
+        <v>-3.063029848632278</v>
       </c>
       <c r="G166">
         <v>-0.06265426210750791</v>
@@ -4233,7 +4233,7 @@
         <v>95</v>
       </c>
       <c r="F167">
-        <v>-3.068395256206483</v>
+        <v>-3.068807926024766</v>
       </c>
       <c r="G167">
         <v>-0.06294389008283985</v>
@@ -4302,7 +4302,7 @@
         <v>98</v>
       </c>
       <c r="F170">
-        <v>-3.082422253946845</v>
+        <v>-3.082667884653064</v>
       </c>
       <c r="G170">
         <v>-0.06109185823841068</v>
@@ -4325,7 +4325,7 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.086267065344651</v>
+        <v>-3.086544160038232</v>
       </c>
       <c r="G171">
         <v>-0.06144085835089474</v>
@@ -4348,7 +4348,7 @@
         <v>100</v>
       </c>
       <c r="F172">
-        <v>-3.0887427165684</v>
+        <v>-3.088840574504851</v>
       </c>
       <c r="G172">
         <v>-0.06038023620861965</v>
@@ -4394,7 +4394,7 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.098948154703767</v>
+        <v>-3.099188794660562</v>
       </c>
       <c r="G174">
         <v>-0.05824262023479909</v>
@@ -4417,7 +4417,7 @@
         <v>103</v>
       </c>
       <c r="F175">
-        <v>-3.103833402550027</v>
+        <v>-3.104187155842564</v>
       </c>
       <c r="G175">
         <v>-0.05788878952085452</v>
@@ -4463,7 +4463,7 @@
         <v>105</v>
       </c>
       <c r="F177">
-        <v>-3.111004000825581</v>
+        <v>-3.111351985947977</v>
       </c>
       <c r="G177">
         <v>-0.05726767771701669</v>
@@ -4486,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="F178">
-        <v>-3.116477709570204</v>
+        <v>-3.117051907008043</v>
       </c>
       <c r="G178">
         <v>-0.05581483500563944</v>
@@ -4555,7 +4555,7 @@
         <v>109</v>
       </c>
       <c r="F181">
-        <v>-3.12802642779326</v>
+        <v>-3.128342586088457</v>
       </c>
       <c r="G181">
         <v>-0.05408958650118412</v>
@@ -4601,7 +4601,7 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.137118014112034</v>
+        <v>-3.137328459640947</v>
       </c>
       <c r="G183">
         <v>-0.05248383196828954</v>
@@ -4624,7 +4624,7 @@
         <v>112</v>
       </c>
       <c r="F184">
-        <v>-3.141477214232125</v>
+        <v>-3.141991734757872</v>
       </c>
       <c r="G184">
         <v>-0.04963277875443273</v>
@@ -4647,7 +4647,7 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.146523023295797</v>
+        <v>-3.146688619624995</v>
       </c>
       <c r="G185">
         <v>-0.04873802951269879</v>
@@ -4716,7 +4716,7 @@
         <v>116</v>
       </c>
       <c r="F188">
-        <v>-3.156883588056143</v>
+        <v>-3.157452269768656</v>
       </c>
       <c r="G188">
         <v>-0.04766792462859348</v>
@@ -4831,7 +4831,7 @@
         <v>121</v>
       </c>
       <c r="F193">
-        <v>-3.177622953530636</v>
+        <v>-3.178193334391923</v>
       </c>
       <c r="G193">
         <v>-0.0435471089773386</v>
@@ -5107,7 +5107,7 @@
         <v>133</v>
       </c>
       <c r="F205">
-        <v>-3.221546153093309</v>
+        <v>-3.222053683102841</v>
       </c>
       <c r="G205">
         <v>-0.02699653490524634</v>
@@ -5498,7 +5498,7 @@
         <v>61</v>
       </c>
       <c r="F222">
-        <v>-2.818027126507107</v>
+        <v>-2.818238076813503</v>
       </c>
       <c r="G222">
         <v>-0.04386742812921618</v>
@@ -5521,7 +5521,7 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.907088556863</v>
+        <v>-2.907555937780125</v>
       </c>
       <c r="G223">
         <v>-0.05728340565328049</v>
@@ -5544,7 +5544,7 @@
         <v>123</v>
       </c>
       <c r="F224">
-        <v>-2.992755358524738</v>
+        <v>-2.992911881867078</v>
       </c>
       <c r="G224">
         <v>-0.06577717043876063</v>
@@ -5567,7 +5567,7 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.073843689921</v>
+        <v>-3.07387858022364</v>
       </c>
       <c r="G225">
         <v>-0.06851272909896111</v>
@@ -5590,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.147803739418754</v>
+        <v>-3.1479033063511</v>
       </c>
       <c r="G226">
         <v>-0.06749295502671293</v>
@@ -5613,7 +5613,7 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.2160999406124</v>
+        <v>-3.216142221479354</v>
       </c>
       <c r="G227">
         <v>-0.05736411736875813</v>
@@ -5659,7 +5659,7 @@
         <v>278</v>
       </c>
       <c r="F229">
-        <v>-3.336348063458273</v>
+        <v>-3.336567320252117</v>
       </c>
       <c r="G229">
         <v>-0.02698616761849393</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.786147729031592</v>
+        <v>-2.786281745642369</v>
       </c>
       <c r="G232">
         <v>-0.02527176346397342</v>
@@ -5751,7 +5751,7 @@
         <v>112</v>
       </c>
       <c r="F233">
-        <v>-2.882579645320932</v>
+        <v>-2.882655612525247</v>
       </c>
       <c r="G233">
         <v>-0.04376841583561886</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.975773110198728</v>
+        <v>-2.975811274160444</v>
       </c>
       <c r="G234">
         <v>-0.05795588987540001</v>
@@ -5797,7 +5797,7 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.059851049140998</v>
+        <v>-3.060197640919311</v>
       </c>
       <c r="G235">
         <v>-0.06540721728834087</v>
@@ -5820,7 +5820,7 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.142565422629807</v>
+        <v>-3.142582119869091</v>
       </c>
       <c r="G236">
         <v>-0.06931697938274617</v>
@@ -5843,7 +5843,7 @@
         <v>336</v>
       </c>
       <c r="F237">
-        <v>-3.217638002679049</v>
+        <v>-3.217973454648345</v>
       </c>
       <c r="G237">
         <v>-0.06632166244271054</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.287273832229776</v>
+        <v>-3.287416910066971</v>
       </c>
       <c r="G238">
         <v>-0.05800286097577989</v>
@@ -5889,7 +5889,7 @@
         <v>448</v>
       </c>
       <c r="F239">
-        <v>-3.351831843524696</v>
+        <v>-3.351986264091969</v>
       </c>
       <c r="G239">
         <v>-0.04473968315851939</v>
@@ -5981,7 +5981,7 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.82920117972315</v>
+        <v>-2.82940084529449</v>
       </c>
       <c r="G243">
         <v>-0.0250304586649932</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.108448371160833</v>
+        <v>-3.108844603936353</v>
       </c>
       <c r="G246">
         <v>-0.06482813356561712</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.266845499769308</v>
+        <v>-3.267086763155016</v>
       </c>
       <c r="G248">
         <v>-0.06681828405940005</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.338485811014014</v>
+        <v>-3.338550914228639</v>
       </c>
       <c r="G249">
         <v>-0.05760174171475763</v>
@@ -6165,7 +6165,7 @@
         <v>830</v>
       </c>
       <c r="F251">
-        <v>-3.464306102521145</v>
+        <v>-3.464318394231113</v>
       </c>
       <c r="G251">
         <v>-0.02602466555336047</v>
@@ -6234,7 +6234,7 @@
         <v>141</v>
       </c>
       <c r="F254">
-        <v>-2.858856743806128</v>
+        <v>-2.858929754882972</v>
       </c>
       <c r="G254">
         <v>-0.0241816450302621</v>
@@ -6257,7 +6257,7 @@
         <v>283</v>
       </c>
       <c r="F255">
-        <v>-2.959203160009108</v>
+        <v>-2.959444738217551</v>
       </c>
       <c r="G255">
         <v>-0.04364111093397272</v>
@@ -6280,7 +6280,7 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.052809337315142</v>
+        <v>-3.052983463057705</v>
       </c>
       <c r="G256">
         <v>-0.05723884722613048</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.14174123101849</v>
+        <v>-3.141769593798231</v>
       </c>
       <c r="G257">
         <v>-0.06523516485980907</v>
@@ -6326,7 +6326,7 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.224826629755423</v>
+        <v>-3.224855664051356</v>
       </c>
       <c r="G258">
         <v>-0.06834797726552355</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.441916739694034</v>
+        <v>-3.44197804009431</v>
       </c>
       <c r="G261">
         <v>-0.04394327254395969</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.882946807602409</v>
+        <v>-2.882977154379477</v>
       </c>
       <c r="G265">
         <v>-0.0240632056775123</v>
@@ -6510,7 +6510,7 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.983254722231226</v>
+        <v>-2.983283171548391</v>
       </c>
       <c r="G266">
         <v>-0.04331321550334977</v>
@@ -6533,7 +6533,7 @@
         <v>617</v>
       </c>
       <c r="F267">
-        <v>-3.078246401913582</v>
+        <v>-3.078285687347898</v>
       </c>
       <c r="G267">
         <v>-0.05631636605077839</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.251520090452157</v>
+        <v>-3.251569089215711</v>
       </c>
       <c r="G269">
         <v>-0.06780675191923091</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.330929582189078</v>
+        <v>-3.331157842693474</v>
       </c>
       <c r="G270">
         <v>-0.06419752115149246</v>
@@ -6625,7 +6625,7 @@
         <v>1439</v>
       </c>
       <c r="F271">
-        <v>-3.402765276113812</v>
+        <v>-3.402895947856657</v>
       </c>
       <c r="G271">
         <v>-0.05688140820342391</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.470536114371271</v>
+        <v>-3.470673391683279</v>
       </c>
       <c r="G272">
         <v>-0.04387737884515908</v>
@@ -6740,7 +6740,7 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.901482897902854</v>
+        <v>-2.901570811868176</v>
       </c>
       <c r="G276">
         <v>-0.02406920687054059</v>
@@ -6763,7 +6763,7 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.002140624103695</v>
+        <v>-3.002168601331533</v>
       </c>
       <c r="G277">
         <v>-0.04227620044241398</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.097783316229176</v>
+        <v>-3.097951179596199</v>
       </c>
       <c r="G278">
         <v>-0.05607882283516297</v>
@@ -6809,7 +6809,7 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.187876057929453</v>
+        <v>-3.187918023771209</v>
       </c>
       <c r="G279">
         <v>-0.06318188816633419</v>
@@ -6832,7 +6832,7 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.272903786512736</v>
+        <v>-3.27301618989266</v>
       </c>
       <c r="G280">
         <v>-0.06621825962590311</v>
@@ -6855,7 +6855,7 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.352205624672247</v>
+        <v>-3.352451285889274</v>
       </c>
       <c r="G281">
         <v>-0.06398994315260564</v>
@@ -6878,7 +6878,7 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.425569404379988</v>
+        <v>-3.425583392993906</v>
       </c>
       <c r="G282">
         <v>-0.05612750293692592</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.492777865089028</v>
+        <v>-3.492791853702947</v>
       </c>
       <c r="G283">
         <v>-0.04295880299185728</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.916941444266158</v>
+        <v>-2.916971290190819</v>
       </c>
       <c r="G287">
         <v>-0.02367997741095973</v>
@@ -7016,7 +7016,7 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.017691305283781</v>
+        <v>-3.017729191179332</v>
       </c>
       <c r="G288">
         <v>-0.04251300891418719</v>
@@ -7039,7 +7039,7 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.113868671160673</v>
+        <v>-3.113896189364843</v>
       </c>
       <c r="G289">
         <v>-0.05551791606564294</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.289690025780672</v>
+        <v>-3.289786790423084</v>
       </c>
       <c r="G291">
         <v>-0.0655803780886155</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.369536530513567</v>
+        <v>-3.369670012197032</v>
       </c>
       <c r="G292">
         <v>-0.06303955016071905</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.443116424555875</v>
+        <v>-3.443159803905059</v>
       </c>
       <c r="G293">
         <v>-0.05515012424061883</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.573377639242001</v>
+        <v>-3.5733900553575</v>
       </c>
       <c r="G295">
         <v>-0.02449152068444382</v>
@@ -7246,7 +7246,7 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.929305380983764</v>
+        <v>-2.929318117317237</v>
       </c>
       <c r="G298">
         <v>-0.02357381916767043</v>
@@ -7269,7 +7269,7 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.030685550306855</v>
+        <v>-3.030815166800251</v>
       </c>
       <c r="G299">
         <v>-0.04201270279780811</v>
@@ -7292,7 +7292,7 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.127191833883172</v>
+        <v>-3.127220859322134</v>
       </c>
       <c r="G300">
         <v>-0.0543073434687642</v>
@@ -7315,7 +7315,7 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.218291057772684</v>
+        <v>-3.218301683459285</v>
       </c>
       <c r="G301">
         <v>-0.06219144904681673</v>
@@ -7361,7 +7361,7 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.383605153169666</v>
+        <v>-3.383636735568512</v>
       </c>
       <c r="G303">
         <v>-0.06236990600344705</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.458298090038189</v>
+        <v>-3.458334328378897</v>
       </c>
       <c r="G304">
         <v>-0.05464736464488806</v>
@@ -7499,7 +7499,7 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.939694004878652</v>
+        <v>-2.939738119188486</v>
       </c>
       <c r="G309">
         <v>-0.02338508521976257</v>
@@ -7522,7 +7522,7 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.041495676422547</v>
+        <v>-3.041639216086596</v>
       </c>
       <c r="G310">
         <v>-0.04129000151007567</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.13847205729284</v>
+        <v>-3.138539990616749</v>
       </c>
       <c r="G311">
         <v>-0.05420531534682338</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.315386998485069</v>
+        <v>-3.315410783528948</v>
       </c>
       <c r="G313">
         <v>-0.06397337201434161</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.396251702933894</v>
+        <v>-3.396270155041174</v>
       </c>
       <c r="G314">
         <v>-0.061438666420216</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.538995317477704</v>
+        <v>-3.539039582883659</v>
       </c>
       <c r="G316">
         <v>-0.0413182393111089</v>
@@ -7752,7 +7752,7 @@
         <v>821</v>
       </c>
       <c r="F320">
-        <v>-2.948353902067926</v>
+        <v>-2.948417396449492</v>
       </c>
       <c r="G320">
         <v>-0.0233819330146412</v>
@@ -7798,7 +7798,7 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.147994627343824</v>
+        <v>-3.148062193464878</v>
       </c>
       <c r="G322">
         <v>-0.05332638142041324</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.23939404245551</v>
+        <v>-3.239404359669467</v>
       </c>
       <c r="G323">
         <v>-0.06099802107311758</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.32561250971933</v>
+        <v>-3.325623033671495</v>
       </c>
       <c r="G324">
         <v>-0.06352861199624371</v>
@@ -7867,7 +7867,7 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.406131182695687</v>
+        <v>-3.406248316925786</v>
       </c>
       <c r="G325">
         <v>-0.06095986211832471</v>
@@ -7890,7 +7890,7 @@
         <v>5751</v>
       </c>
       <c r="F326">
-        <v>-3.481000859790254</v>
+        <v>-3.481088537206477</v>
       </c>
       <c r="G326">
         <v>-0.05364092179063251</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.549396217465975</v>
+        <v>-3.549424104950625</v>
       </c>
       <c r="G327">
         <v>-0.04087010370692101</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.612645085952099</v>
+        <v>-3.612665606572998</v>
       </c>
       <c r="G328">
         <v>-0.02339390262022029</v>
@@ -8005,7 +8005,7 @@
         <v>1017</v>
       </c>
       <c r="F331">
-        <v>-2.956135910407875</v>
+        <v>-2.956233365286864</v>
       </c>
       <c r="G331">
         <v>-0.02304604198804938</v>
@@ -8028,7 +8028,7 @@
         <v>2035</v>
       </c>
       <c r="F332">
-        <v>-3.058648904743516</v>
+        <v>-3.058661468656175</v>
       </c>
       <c r="G332">
         <v>-0.04084545509864856</v>
@@ -8051,7 +8051,7 @@
         <v>3053</v>
       </c>
       <c r="F333">
-        <v>-3.155844359088574</v>
+        <v>-3.155908250782195</v>
       </c>
       <c r="G333">
         <v>-0.05317217999790391</v>
@@ -8074,7 +8074,7 @@
         <v>4071</v>
       </c>
       <c r="F334">
-        <v>-3.247754457165829</v>
+        <v>-3.247814837371238</v>
       </c>
       <c r="G334">
         <v>-0.06057126192654172</v>
@@ -8097,7 +8097,7 @@
         <v>5089</v>
       </c>
       <c r="F335">
-        <v>-3.33436889827686</v>
+        <v>-3.334563161944447</v>
       </c>
       <c r="G335">
         <v>-0.06278717063128125</v>
@@ -8120,7 +8120,7 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.414985217608911</v>
+        <v>-3.415118697430842</v>
       </c>
       <c r="G336">
         <v>-0.06050505627801783</v>
@@ -8143,7 +8143,7 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.489777944869828</v>
+        <v>-3.489838410936327</v>
       </c>
       <c r="G337">
         <v>-0.05286449853341879</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.558690544624951</v>
+        <v>-3.558775099056283</v>
       </c>
       <c r="G338">
         <v>-0.04053172592297882</v>
@@ -8189,7 +8189,7 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.621825275949748</v>
+        <v>-3.621835751483296</v>
       </c>
       <c r="G339">
         <v>-0.02310751223477731</v>

</xml_diff>

<commit_message>
updated GA data from 03.05.2019
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -990,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="F26">
-        <v>-2.525537948499767</v>
+        <v>-2.525574806240608</v>
       </c>
       <c r="G26">
         <v>-0.04090163511113665</v>
@@ -1082,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <v>-2.584953107483507</v>
+        <v>-2.585399616519781</v>
       </c>
       <c r="G30">
         <v>-0.0510669095590095</v>
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.822925355556685</v>
+        <v>-2.823880753156115</v>
       </c>
       <c r="G48">
         <v>-0.06224925594752295</v>
@@ -1519,7 +1519,7 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.834607384909984</v>
+        <v>-2.834729149569632</v>
       </c>
       <c r="G49">
         <v>-0.06086949888522653</v>
@@ -2232,7 +2232,7 @@
         <v>8</v>
       </c>
       <c r="F80">
-        <v>-2.584702900439534</v>
+        <v>-2.584877386808773</v>
       </c>
       <c r="G80">
         <v>-0.01697656629765065</v>
@@ -2255,7 +2255,7 @@
         <v>9</v>
       </c>
       <c r="F81">
-        <v>-2.591493671502356</v>
+        <v>-2.591520223033114</v>
       </c>
       <c r="G81">
         <v>-0.01920671834924992</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <v>-2.5981365077267</v>
+        <v>-2.598382972068958</v>
       </c>
       <c r="G82">
         <v>-0.02006377659037284</v>
@@ -2784,7 +2784,7 @@
         <v>32</v>
       </c>
       <c r="F104">
-        <v>-2.736155970979087</v>
+        <v>-2.736342458985815</v>
       </c>
       <c r="G104">
         <v>-0.04748471955815536</v>
@@ -2945,7 +2945,7 @@
         <v>39</v>
       </c>
       <c r="F111">
-        <v>-2.776803670391222</v>
+        <v>-2.776949913597027</v>
       </c>
       <c r="G111">
         <v>-0.05228418171994131</v>
@@ -2968,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.783099863433906</v>
+        <v>-2.783922445609977</v>
       </c>
       <c r="G112">
         <v>-0.05265652914170493</v>
@@ -3175,7 +3175,7 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.834338931260185</v>
+        <v>-2.834703566007532</v>
       </c>
       <c r="G121">
         <v>-0.06000911149696631</v>
@@ -3267,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.856908227229114</v>
+        <v>-2.857211922560765</v>
       </c>
       <c r="G125">
         <v>-0.06141738346264969</v>
@@ -3313,7 +3313,7 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.867073125934038</v>
+        <v>-2.867275420498586</v>
       </c>
       <c r="G127">
         <v>-0.06227460763599346</v>
@@ -3405,7 +3405,7 @@
         <v>59</v>
       </c>
       <c r="F131">
-        <v>-2.888482594611272</v>
+        <v>-2.888749790923737</v>
       </c>
       <c r="G131">
         <v>-0.06400379531036271</v>
@@ -3451,7 +3451,7 @@
         <v>61</v>
       </c>
       <c r="F133">
-        <v>-2.900317726011542</v>
+        <v>-2.901210938214826</v>
       </c>
       <c r="G133">
         <v>-0.06665454538554338</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.905157701136438</v>
+        <v>-2.905281168628177</v>
       </c>
       <c r="G134">
         <v>-0.06372632355803498</v>
@@ -3681,7 +3681,7 @@
         <v>71</v>
       </c>
       <c r="F143">
-        <v>-2.953123447678578</v>
+        <v>-2.95326172042358</v>
       </c>
       <c r="G143">
         <v>-0.06450248721298824</v>
@@ -3888,7 +3888,7 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.997305876974929</v>
+        <v>-2.997697015357584</v>
       </c>
       <c r="G152">
         <v>-0.06780185980026898</v>
@@ -4003,7 +4003,7 @@
         <v>85</v>
       </c>
       <c r="F157">
-        <v>-3.021285961458676</v>
+        <v>-3.022719520336881</v>
       </c>
       <c r="G157">
         <v>-0.06485566663902187</v>
@@ -4072,7 +4072,7 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.036187401049683</v>
+        <v>-3.036429737464065</v>
       </c>
       <c r="G160">
         <v>-0.06447723515981063</v>
@@ -4095,7 +4095,7 @@
         <v>89</v>
       </c>
       <c r="F161">
-        <v>-3.03860610696284</v>
+        <v>-3.038976980772308</v>
       </c>
       <c r="G161">
         <v>-0.06501816482063427</v>
@@ -4279,7 +4279,7 @@
         <v>97</v>
       </c>
       <c r="F169">
-        <v>-3.077749901712157</v>
+        <v>-3.07826736478147</v>
       </c>
       <c r="G169">
         <v>-0.06230885119838547</v>
@@ -4325,7 +4325,7 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.086544160038232</v>
+        <v>-3.086561556699558</v>
       </c>
       <c r="G171">
         <v>-0.06144085835089474</v>
@@ -4348,7 +4348,7 @@
         <v>100</v>
       </c>
       <c r="F172">
-        <v>-3.088840574504851</v>
+        <v>-3.089335949781305</v>
       </c>
       <c r="G172">
         <v>-0.06038023620861965</v>
@@ -4555,7 +4555,7 @@
         <v>109</v>
       </c>
       <c r="F181">
-        <v>-3.128342586088457</v>
+        <v>-3.128615601961473</v>
       </c>
       <c r="G181">
         <v>-0.05408958650118412</v>
@@ -4601,7 +4601,7 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.137328459640947</v>
+        <v>-3.137711315373395</v>
       </c>
       <c r="G183">
         <v>-0.05248383196828954</v>
@@ -4647,7 +4647,7 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.146688619624995</v>
+        <v>-3.146822838016389</v>
       </c>
       <c r="G185">
         <v>-0.04873802951269879</v>
@@ -4785,7 +4785,7 @@
         <v>119</v>
       </c>
       <c r="F191">
-        <v>-3.169556957827944</v>
+        <v>-3.169743831429527</v>
       </c>
       <c r="G191">
         <v>-0.04539073117985515</v>
@@ -4808,7 +4808,7 @@
         <v>120</v>
       </c>
       <c r="F192">
-        <v>-3.174111066248696</v>
+        <v>-3.174649561119725</v>
       </c>
       <c r="G192">
         <v>-0.04432853459351432</v>
@@ -4969,7 +4969,7 @@
         <v>127</v>
       </c>
       <c r="F199">
-        <v>-3.199718311870945</v>
+        <v>-3.19983286307691</v>
       </c>
       <c r="G199">
         <v>-0.03603671904325106</v>
@@ -5498,7 +5498,7 @@
         <v>61</v>
       </c>
       <c r="F222">
-        <v>-2.818238076813503</v>
+        <v>-2.81854787055259</v>
       </c>
       <c r="G222">
         <v>-0.04386742812921618</v>
@@ -5521,7 +5521,7 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.907555937780125</v>
+        <v>-2.907865059960086</v>
       </c>
       <c r="G223">
         <v>-0.05728340565328049</v>
@@ -5613,7 +5613,7 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.216142221479354</v>
+        <v>-3.216198779595988</v>
       </c>
       <c r="G227">
         <v>-0.05736411736875813</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.786281745642369</v>
+        <v>-2.786353284560966</v>
       </c>
       <c r="G232">
         <v>-0.02527176346397342</v>
@@ -5797,7 +5797,7 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.060197640919311</v>
+        <v>-3.060292734501858</v>
       </c>
       <c r="G235">
         <v>-0.06540721728834087</v>
@@ -5889,7 +5889,7 @@
         <v>448</v>
       </c>
       <c r="F239">
-        <v>-3.351986264091969</v>
+        <v>-3.352006352667231</v>
       </c>
       <c r="G239">
         <v>-0.04473968315851939</v>
@@ -5981,7 +5981,7 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.82940084529449</v>
+        <v>-2.829459261146031</v>
       </c>
       <c r="G243">
         <v>-0.0250304586649932</v>
@@ -6004,7 +6004,7 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.92626371924288</v>
+        <v>-2.926335530363728</v>
       </c>
       <c r="G244">
         <v>-0.04354852366881445</v>
@@ -6027,7 +6027,7 @@
         <v>276</v>
       </c>
       <c r="F245">
-        <v>-3.018668468724671</v>
+        <v>-3.019056598279157</v>
       </c>
       <c r="G245">
         <v>-0.05723271934982499</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.108844603936353</v>
+        <v>-3.108888085337582</v>
       </c>
       <c r="G246">
         <v>-0.06482813356561712</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.338550914228639</v>
+        <v>-3.338725597586517</v>
       </c>
       <c r="G249">
         <v>-0.05760174171475763</v>
@@ -6234,7 +6234,7 @@
         <v>141</v>
       </c>
       <c r="F254">
-        <v>-2.858929754882972</v>
+        <v>-2.85896390400346</v>
       </c>
       <c r="G254">
         <v>-0.0241816450302621</v>
@@ -6280,7 +6280,7 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.052983463057705</v>
+        <v>-3.053031016123247</v>
       </c>
       <c r="G256">
         <v>-0.05723884722613048</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.141769593798231</v>
+        <v>-3.141855223936979</v>
       </c>
       <c r="G257">
         <v>-0.06523516485980907</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.303507220660733</v>
+        <v>-3.303548978242894</v>
       </c>
       <c r="G259">
         <v>-0.06499168668186583</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.44197804009431</v>
+        <v>-3.442034520148211</v>
       </c>
       <c r="G261">
         <v>-0.04394327254395969</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.882977154379477</v>
+        <v>-2.883161880891549</v>
       </c>
       <c r="G265">
         <v>-0.0240632056775123</v>
@@ -6510,7 +6510,7 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.983283171548391</v>
+        <v>-2.983322192776716</v>
       </c>
       <c r="G266">
         <v>-0.04331321550334977</v>
@@ -6533,7 +6533,7 @@
         <v>617</v>
       </c>
       <c r="F267">
-        <v>-3.078285687347898</v>
+        <v>-3.078373737307547</v>
       </c>
       <c r="G267">
         <v>-0.05631636605077839</v>
@@ -6625,7 +6625,7 @@
         <v>1439</v>
       </c>
       <c r="F271">
-        <v>-3.402895947856657</v>
+        <v>-3.402919144450092</v>
       </c>
       <c r="G271">
         <v>-0.05688140820342391</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.470673391683279</v>
+        <v>-3.470699926882973</v>
       </c>
       <c r="G272">
         <v>-0.04387737884515908</v>
@@ -6671,7 +6671,7 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.53191432878926</v>
+        <v>-3.531934137652331</v>
       </c>
       <c r="G273">
         <v>-0.02466589200668384</v>
@@ -6740,7 +6740,7 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.901570811868176</v>
+        <v>-2.901584800482094</v>
       </c>
       <c r="G276">
         <v>-0.02406920687054059</v>
@@ -6763,7 +6763,7 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.002168601331533</v>
+        <v>-3.002182589945451</v>
       </c>
       <c r="G277">
         <v>-0.04227620044241398</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.097951179596199</v>
+        <v>-3.09802729482115</v>
       </c>
       <c r="G278">
         <v>-0.05607882283516297</v>
@@ -6809,7 +6809,7 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.187918023771209</v>
+        <v>-3.187963133482202</v>
       </c>
       <c r="G279">
         <v>-0.06318188816633419</v>
@@ -6855,7 +6855,7 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.352451285889274</v>
+        <v>-3.352465274503192</v>
       </c>
       <c r="G281">
         <v>-0.06398994315260564</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.492791853702947</v>
+        <v>-3.492805842316865</v>
       </c>
       <c r="G283">
         <v>-0.04295880299185728</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.916971290190819</v>
+        <v>-2.916995148990574</v>
       </c>
       <c r="G287">
         <v>-0.02367997741095973</v>
@@ -7016,7 +7016,7 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.017729191179332</v>
+        <v>-3.017747137437067</v>
       </c>
       <c r="G288">
         <v>-0.04251300891418719</v>
@@ -7039,7 +7039,7 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.113896189364843</v>
+        <v>-3.113906557056224</v>
       </c>
       <c r="G289">
         <v>-0.05551791606564294</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.289786790423084</v>
+        <v>-3.289870221482005</v>
       </c>
       <c r="G291">
         <v>-0.0655803780886155</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.369670012197032</v>
+        <v>-3.369749187996073</v>
       </c>
       <c r="G292">
         <v>-0.06303955016071905</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.5733900553575</v>
+        <v>-3.573426585177015</v>
       </c>
       <c r="G295">
         <v>-0.02449152068444382</v>
@@ -7269,7 +7269,7 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.030815166800251</v>
+        <v>-3.030836123512497</v>
       </c>
       <c r="G299">
         <v>-0.04201270279780811</v>
@@ -7292,7 +7292,7 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.127220859322134</v>
+        <v>-3.127251554473209</v>
       </c>
       <c r="G300">
         <v>-0.0543073434687642</v>
@@ -7315,7 +7315,7 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.218301683459285</v>
+        <v>-3.218315796108344</v>
       </c>
       <c r="G301">
         <v>-0.06219144904681673</v>
@@ -7338,7 +7338,7 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.303966242601376</v>
+        <v>-3.303998145998349</v>
       </c>
       <c r="G302">
         <v>-0.06503915675330885</v>
@@ -7361,7 +7361,7 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.383636735568512</v>
+        <v>-3.38364689440433</v>
       </c>
       <c r="G303">
         <v>-0.06236990600344705</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.526369809228998</v>
+        <v>-3.526386556019768</v>
       </c>
       <c r="G305">
         <v>-0.04220518905553605</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.138539990616749</v>
+        <v>-3.138552292021602</v>
       </c>
       <c r="G311">
         <v>-0.05420531534682338</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.315410783528948</v>
+        <v>-3.31542465464907</v>
       </c>
       <c r="G313">
         <v>-0.06397337201434161</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.470244786953842</v>
+        <v>-3.470299396594158</v>
       </c>
       <c r="G315">
         <v>-0.05399105464408593</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.539039582883659</v>
+        <v>-3.539051884288511</v>
       </c>
       <c r="G316">
         <v>-0.0413182393111089</v>
@@ -7775,7 +7775,7 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.050544519531514</v>
+        <v>-3.050556066313728</v>
       </c>
       <c r="G321">
         <v>-0.0412592898511992</v>
@@ -7798,7 +7798,7 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.148062193464878</v>
+        <v>-3.14809638274726</v>
       </c>
       <c r="G322">
         <v>-0.05332638142041324</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.239404359669467</v>
+        <v>-3.23942499409738</v>
       </c>
       <c r="G323">
         <v>-0.06099802107311758</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.325623033671495</v>
+        <v>-3.325668235780154</v>
       </c>
       <c r="G324">
         <v>-0.06352861199624371</v>
@@ -7867,7 +7867,7 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.406248316925786</v>
+        <v>-3.406258634139743</v>
       </c>
       <c r="G325">
         <v>-0.06095986211832471</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.549424104950625</v>
+        <v>-3.549434679112862</v>
       </c>
       <c r="G327">
         <v>-0.04087010370692101</v>
@@ -8005,7 +8005,7 @@
         <v>1017</v>
       </c>
       <c r="F331">
-        <v>-2.956233365286864</v>
+        <v>-2.956253710334245</v>
       </c>
       <c r="G331">
         <v>-0.02304604198804938</v>
@@ -8074,7 +8074,7 @@
         <v>4071</v>
       </c>
       <c r="F334">
-        <v>-3.247814837371238</v>
+        <v>-3.247826832349809</v>
       </c>
       <c r="G334">
         <v>-0.06057126192654172</v>
@@ -8120,7 +8120,7 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.415118697430842</v>
+        <v>-3.415132895232571</v>
       </c>
       <c r="G336">
         <v>-0.06050505627801783</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.558775099056283</v>
+        <v>-3.558842915543228</v>
       </c>
       <c r="G338">
         <v>-0.04053172592297882</v>

</xml_diff>

<commit_message>
updated data from 03.07.2019
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -1059,7 +1059,7 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <v>-2.569944150301068</v>
+        <v>-2.570092286896046</v>
       </c>
       <c r="G29">
         <v>-0.04737394681490215</v>
@@ -1197,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.65713207387985</v>
+        <v>-2.657411053935069</v>
       </c>
       <c r="G35">
         <v>-0.05977531489401344</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.762864174624738</v>
+        <v>-2.763785329607089</v>
       </c>
       <c r="G43">
         <v>-0.06391507069606006</v>
@@ -1519,7 +1519,7 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.834729149569632</v>
+        <v>-2.835641390207203</v>
       </c>
       <c r="G49">
         <v>-0.06086949888522653</v>
@@ -2347,7 +2347,7 @@
         <v>13</v>
       </c>
       <c r="F85">
-        <v>-2.617843054849695</v>
+        <v>-2.618670715430355</v>
       </c>
       <c r="G85">
         <v>-0.02313921711713052</v>
@@ -2554,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="F94">
-        <v>-2.675521418758289</v>
+        <v>-2.675607637573642</v>
       </c>
       <c r="G94">
         <v>-0.03615692101567447</v>
@@ -2669,7 +2669,7 @@
         <v>27</v>
       </c>
       <c r="F99">
-        <v>-2.705143474693888</v>
+        <v>-2.705155522254721</v>
       </c>
       <c r="G99">
         <v>-0.04210934040430026</v>
@@ -2715,7 +2715,7 @@
         <v>29</v>
       </c>
       <c r="F101">
-        <v>-2.718368561806627</v>
+        <v>-2.718512185480655</v>
       </c>
       <c r="G101">
         <v>-0.04253686850322724</v>
@@ -2761,7 +2761,7 @@
         <v>31</v>
       </c>
       <c r="F103">
-        <v>-2.729256205602705</v>
+        <v>-2.729458201780353</v>
       </c>
       <c r="G103">
         <v>-0.04539819683189528</v>
@@ -2784,7 +2784,7 @@
         <v>32</v>
       </c>
       <c r="F104">
-        <v>-2.736342458985815</v>
+        <v>-2.736497674914668</v>
       </c>
       <c r="G104">
         <v>-0.04748471955815536</v>
@@ -3175,7 +3175,7 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.834703566007532</v>
+        <v>-2.834759416546765</v>
       </c>
       <c r="G121">
         <v>-0.06000911149696631</v>
@@ -3198,7 +3198,7 @@
         <v>50</v>
       </c>
       <c r="F122">
-        <v>-2.839426316124094</v>
+        <v>-2.839957477100891</v>
       </c>
       <c r="G122">
         <v>-0.06010277017543042</v>
@@ -3313,7 +3313,7 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.867275420498586</v>
+        <v>-2.867440799714733</v>
       </c>
       <c r="G127">
         <v>-0.06227460763599346</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.905281168628177</v>
+        <v>-2.905804992440557</v>
       </c>
       <c r="G134">
         <v>-0.06372632355803498</v>
@@ -3497,7 +3497,7 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.910488765484706</v>
+        <v>-2.910520702831482</v>
       </c>
       <c r="G135">
         <v>-0.06392543768492631</v>
@@ -3566,7 +3566,7 @@
         <v>66</v>
       </c>
       <c r="F138">
-        <v>-2.926806772077847</v>
+        <v>-2.9268219772449</v>
       </c>
       <c r="G138">
         <v>-0.06657101570578416</v>
@@ -3658,7 +3658,7 @@
         <v>70</v>
       </c>
       <c r="F142">
-        <v>-2.948553136741634</v>
+        <v>-2.948868375521574</v>
       </c>
       <c r="G142">
         <v>-0.06779788511858942</v>
@@ -3727,7 +3727,7 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.962125493304821</v>
+        <v>-2.962975415944975</v>
       </c>
       <c r="G145">
         <v>-0.06582163185846457</v>
@@ -3865,7 +3865,7 @@
         <v>79</v>
       </c>
       <c r="F151">
-        <v>-2.993289451945098</v>
+        <v>-2.993545441583025</v>
       </c>
       <c r="G151">
         <v>-0.06608525725976122</v>
@@ -3888,7 +3888,7 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.997697015357584</v>
+        <v>-2.997753908275254</v>
       </c>
       <c r="G152">
         <v>-0.06780185980026898</v>
@@ -3911,7 +3911,7 @@
         <v>81</v>
       </c>
       <c r="F153">
-        <v>-3.002645253762812</v>
+        <v>-3.002744275072772</v>
       </c>
       <c r="G153">
         <v>-0.06455850371540439</v>
@@ -4026,7 +4026,7 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.026437180748415</v>
+        <v>-3.026589975741185</v>
       </c>
       <c r="G158">
         <v>-0.06574624348211056</v>
@@ -4325,7 +4325,7 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.086561556699558</v>
+        <v>-3.086632029469215</v>
       </c>
       <c r="G171">
         <v>-0.06144085835089474</v>
@@ -4371,7 +4371,7 @@
         <v>101</v>
       </c>
       <c r="F173">
-        <v>-3.095367613248914</v>
+        <v>-3.095486063293359</v>
       </c>
       <c r="G173">
         <v>-0.05859013799830659</v>
@@ -4762,7 +4762,7 @@
         <v>118</v>
       </c>
       <c r="F190">
-        <v>-3.165612913972534</v>
+        <v>-3.166224738107228</v>
       </c>
       <c r="G190">
         <v>-0.04537717505014682</v>
@@ -4785,7 +4785,7 @@
         <v>119</v>
       </c>
       <c r="F191">
-        <v>-3.169743831429527</v>
+        <v>-3.169981330185832</v>
       </c>
       <c r="G191">
         <v>-0.04539073117985515</v>
@@ -4808,7 +4808,7 @@
         <v>120</v>
       </c>
       <c r="F192">
-        <v>-3.174649561119725</v>
+        <v>-3.174762256796305</v>
       </c>
       <c r="G192">
         <v>-0.04432853459351432</v>
@@ -4900,7 +4900,7 @@
         <v>124</v>
       </c>
       <c r="F196">
-        <v>-3.190126354363985</v>
+        <v>-3.190738178498679</v>
       </c>
       <c r="G196">
         <v>-0.03651257146252856</v>
@@ -4969,7 +4969,7 @@
         <v>127</v>
       </c>
       <c r="F199">
-        <v>-3.19983286307691</v>
+        <v>-3.200133859191629</v>
       </c>
       <c r="G199">
         <v>-0.03603671904325106</v>
@@ -5084,7 +5084,7 @@
         <v>132</v>
       </c>
       <c r="F204">
-        <v>-3.218892636760453</v>
+        <v>-3.219193632875172</v>
       </c>
       <c r="G204">
         <v>-0.03015194903129287</v>
@@ -5475,7 +5475,7 @@
         <v>30</v>
       </c>
       <c r="F221">
-        <v>-2.72229098479988</v>
+        <v>-2.723656845986538</v>
       </c>
       <c r="G221">
         <v>-0.02560431675245223</v>
@@ -5498,7 +5498,7 @@
         <v>61</v>
       </c>
       <c r="F222">
-        <v>-2.81854787055259</v>
+        <v>-2.818607375122417</v>
       </c>
       <c r="G222">
         <v>-0.04386742812921618</v>
@@ -5521,7 +5521,7 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.907865059960086</v>
+        <v>-2.907913736277271</v>
       </c>
       <c r="G223">
         <v>-0.05728340565328049</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.278007373686587</v>
+        <v>-3.278266012121108</v>
       </c>
       <c r="G228">
         <v>-0.04455329302800359</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.786353284560966</v>
+        <v>-2.786503127290418</v>
       </c>
       <c r="G232">
         <v>-0.02527176346397342</v>
@@ -5751,7 +5751,7 @@
         <v>112</v>
       </c>
       <c r="F233">
-        <v>-2.882655612525247</v>
+        <v>-2.882797962767977</v>
       </c>
       <c r="G233">
         <v>-0.04376841583561886</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.975811274160444</v>
+        <v>-2.975941843619013</v>
       </c>
       <c r="G234">
         <v>-0.05795588987540001</v>
@@ -5820,7 +5820,7 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.142582119869091</v>
+        <v>-3.142683249924229</v>
       </c>
       <c r="G236">
         <v>-0.06931697938274617</v>
@@ -5912,7 +5912,7 @@
         <v>504</v>
       </c>
       <c r="F240">
-        <v>-3.411628903919411</v>
+        <v>-3.411728863050773</v>
       </c>
       <c r="G240">
         <v>-0.02711937882840842</v>
@@ -5981,7 +5981,7 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.829459261146031</v>
+        <v>-2.829502742547259</v>
       </c>
       <c r="G243">
         <v>-0.0250304586649932</v>
@@ -6004,7 +6004,7 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.926335530363728</v>
+        <v>-2.926551333478266</v>
       </c>
       <c r="G244">
         <v>-0.04354852366881445</v>
@@ -6073,7 +6073,7 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.190285688701083</v>
+        <v>-3.190298015122594</v>
       </c>
       <c r="G247">
         <v>-0.06805097876230648</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.338725597586517</v>
+        <v>-3.338769078987744</v>
       </c>
       <c r="G249">
         <v>-0.05760174171475763</v>
@@ -6234,7 +6234,7 @@
         <v>141</v>
       </c>
       <c r="F254">
-        <v>-2.85896390400346</v>
+        <v>-2.859022385229573</v>
       </c>
       <c r="G254">
         <v>-0.0241816450302621</v>
@@ -6257,7 +6257,7 @@
         <v>283</v>
       </c>
       <c r="F255">
-        <v>-2.959444738217551</v>
+        <v>-2.959473100997292</v>
       </c>
       <c r="G255">
         <v>-0.04364111093397272</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.375324167192619</v>
+        <v>-3.375349342777718</v>
       </c>
       <c r="G260">
         <v>-0.05743932002365837</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.883161880891549</v>
+        <v>-2.883195782478849</v>
       </c>
       <c r="G265">
         <v>-0.0240632056775123</v>
@@ -6510,7 +6510,7 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.983322192776716</v>
+        <v>-2.983340495676592</v>
       </c>
       <c r="G266">
         <v>-0.04331321550334977</v>
@@ -6556,7 +6556,7 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.167854221881214</v>
+        <v>-3.167873732495376</v>
       </c>
       <c r="G268">
         <v>-0.06455489133007597</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.251569089215711</v>
+        <v>-3.251608110444038</v>
       </c>
       <c r="G269">
         <v>-0.06780675191923091</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.331157842693474</v>
+        <v>-3.331177353307637</v>
       </c>
       <c r="G270">
         <v>-0.06419752115149246</v>
@@ -6625,7 +6625,7 @@
         <v>1439</v>
       </c>
       <c r="F271">
-        <v>-3.402919144450092</v>
+        <v>-3.402992630218043</v>
       </c>
       <c r="G271">
         <v>-0.05688140820342391</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.09802729482115</v>
+        <v>-3.0980740975509</v>
       </c>
       <c r="G278">
         <v>-0.05607882283516297</v>
@@ -6832,7 +6832,7 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.27301618989266</v>
+        <v>-3.273035933631117</v>
       </c>
       <c r="G280">
         <v>-0.06621825962590311</v>
@@ -6855,7 +6855,7 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.352465274503192</v>
+        <v>-3.352528063933899</v>
       </c>
       <c r="G281">
         <v>-0.06398994315260564</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.492805842316865</v>
+        <v>-3.492819830930784</v>
       </c>
       <c r="G283">
         <v>-0.04295880299185728</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.555021461264616</v>
+        <v>-3.55503584210588</v>
       </c>
       <c r="G284">
         <v>-0.0244730013361007</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.916995148990574</v>
+        <v>-2.917031869843392</v>
       </c>
       <c r="G287">
         <v>-0.02367997741095973</v>
@@ -7039,7 +7039,7 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.113906557056224</v>
+        <v>-3.113948027821744</v>
       </c>
       <c r="G289">
         <v>-0.05551791606564294</v>
@@ -7062,7 +7062,7 @@
         <v>1548</v>
       </c>
       <c r="F290">
-        <v>-3.204771157617794</v>
+        <v>-3.204795038623368</v>
       </c>
       <c r="G290">
         <v>-0.06299904231392772</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.289870221482005</v>
+        <v>-3.289882190957003</v>
       </c>
       <c r="G291">
         <v>-0.0655803780886155</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.369749187996073</v>
+        <v>-3.369779036285709</v>
       </c>
       <c r="G292">
         <v>-0.06303955016071905</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.443159803905059</v>
+        <v>-3.44317017159644</v>
       </c>
       <c r="G293">
         <v>-0.05515012424061883</v>
@@ -7246,7 +7246,7 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.929318117317237</v>
+        <v>-2.929349301208876</v>
       </c>
       <c r="G298">
         <v>-0.02357381916767043</v>
@@ -7269,7 +7269,7 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.030836123512497</v>
+        <v>-3.030879309779817</v>
       </c>
       <c r="G299">
         <v>-0.04201270279780811</v>
@@ -7338,7 +7338,7 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.303998145998349</v>
+        <v>-3.304054594288487</v>
       </c>
       <c r="G302">
         <v>-0.06503915675330885</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.458334328378897</v>
+        <v>-3.45834923233055</v>
       </c>
       <c r="G304">
         <v>-0.05464736464488806</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.526386556019768</v>
+        <v>-3.526402002354607</v>
       </c>
       <c r="G305">
         <v>-0.04220518905553605</v>
@@ -7499,7 +7499,7 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.939738119188486</v>
+        <v>-2.939759593641992</v>
       </c>
       <c r="G309">
         <v>-0.02338508521976257</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.31542465464907</v>
+        <v>-3.315439718700854</v>
       </c>
       <c r="G313">
         <v>-0.06397337201434161</v>
@@ -7683,7 +7683,7 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.601465079277375</v>
+        <v>-3.6014934184512</v>
       </c>
       <c r="G317">
         <v>-0.02372300662380827</v>
@@ -7775,7 +7775,7 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.050556066313728</v>
+        <v>-3.05057071886332</v>
       </c>
       <c r="G321">
         <v>-0.0412592898511992</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.23942499409738</v>
+        <v>-3.239435237463776</v>
       </c>
       <c r="G323">
         <v>-0.06099802107311758</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.325668235780154</v>
+        <v>-3.325694099330758</v>
       </c>
       <c r="G324">
         <v>-0.06352861199624371</v>
@@ -8028,7 +8028,7 @@
         <v>2035</v>
       </c>
       <c r="F332">
-        <v>-3.058661468656175</v>
+        <v>-3.058678315404536</v>
       </c>
       <c r="G332">
         <v>-0.04084545509864856</v>
@@ -8143,7 +8143,7 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.489838410936327</v>
+        <v>-3.489858674897246</v>
       </c>
       <c r="G337">
         <v>-0.05286449853341879</v>
@@ -8189,7 +8189,7 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.621835751483296</v>
+        <v>-3.621847992123753</v>
       </c>
       <c r="G339">
         <v>-0.02310751223477731</v>

</xml_diff>

<commit_message>
updated data from 03.09.2019
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -921,7 +921,7 @@
         <v>7</v>
       </c>
       <c r="F23">
-        <v>-2.479579712587558</v>
+        <v>-2.480948406732614</v>
       </c>
       <c r="G23">
         <v>-0.03135827639584443</v>
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>-2.494442893176611</v>
+        <v>-2.495811587321665</v>
       </c>
       <c r="G24">
         <v>-0.03422076265821916</v>
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.540382347402589</v>
+        <v>-2.540437986829659</v>
       </c>
       <c r="G27">
         <v>-0.04326276145102503</v>
@@ -1036,7 +1036,7 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <v>-2.555282385732477</v>
+        <v>-2.555338025159549</v>
       </c>
       <c r="G28">
         <v>-0.04649279347421498</v>
@@ -1059,7 +1059,7 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <v>-2.570092286896046</v>
+        <v>-2.570795062838994</v>
       </c>
       <c r="G29">
         <v>-0.04737394681490215</v>
@@ -1082,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <v>-2.585399616519781</v>
+        <v>-2.585621385687204</v>
       </c>
       <c r="G30">
         <v>-0.0510669095590095</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.613532591755807</v>
+        <v>-2.615180828584095</v>
       </c>
       <c r="G32">
         <v>-0.05383393390282332</v>
@@ -1151,7 +1151,7 @@
         <v>17</v>
       </c>
       <c r="F33">
-        <v>-2.62832467198693</v>
+        <v>-2.629988369746072</v>
       </c>
       <c r="G33">
         <v>-0.05553977104754271</v>
@@ -1174,7 +1174,7 @@
         <v>18</v>
       </c>
       <c r="F34">
-        <v>-2.641710308943922</v>
+        <v>-2.644795910908055</v>
       </c>
       <c r="G34">
         <v>-0.05659974897003517</v>
@@ -1197,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.657411053935069</v>
+        <v>-2.658785691723474</v>
       </c>
       <c r="G35">
         <v>-0.05977531489401344</v>
@@ -1220,7 +1220,7 @@
         <v>20</v>
       </c>
       <c r="F36">
-        <v>-2.670698443594537</v>
+        <v>-2.672738930219503</v>
       </c>
       <c r="G36">
         <v>-0.06024586951716659</v>
@@ -1243,7 +1243,7 @@
         <v>21</v>
       </c>
       <c r="F37">
-        <v>-2.685610566066039</v>
+        <v>-2.686540635393171</v>
       </c>
       <c r="G37">
         <v>-0.06439498273323907</v>
@@ -1266,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="F38">
-        <v>-2.698171662420433</v>
+        <v>-2.7004938738892</v>
       </c>
       <c r="G38">
         <v>-0.06334946051762347</v>
@@ -1289,7 +1289,7 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.711461412081488</v>
+        <v>-2.714371345724047</v>
       </c>
       <c r="G39">
         <v>-0.06363759338060815</v>
@@ -1312,7 +1312,7 @@
         <v>24</v>
       </c>
       <c r="F40">
-        <v>-2.723461444218823</v>
+        <v>-2.726926917861679</v>
       </c>
       <c r="G40">
         <v>-0.06456209074184449</v>
@@ -1335,7 +1335,7 @@
         <v>25</v>
       </c>
       <c r="F41">
-        <v>-2.736788718405263</v>
+        <v>-2.739482489999309</v>
       </c>
       <c r="G41">
         <v>-0.06468921975764808</v>
@@ -1358,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.750108230129674</v>
+        <v>-2.752038062136941</v>
       </c>
       <c r="G42">
         <v>-0.06332980808518607</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.763785329607089</v>
+        <v>-2.764511779459467</v>
       </c>
       <c r="G43">
         <v>-0.06391507069606006</v>
@@ -1404,7 +1404,7 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <v>-2.776419509442502</v>
+        <v>-2.777149206412203</v>
       </c>
       <c r="G44">
         <v>-0.06527711482833976</v>
@@ -1427,7 +1427,7 @@
         <v>29</v>
       </c>
       <c r="F45">
-        <v>-2.786789765434675</v>
+        <v>-2.789622923734727</v>
       </c>
       <c r="G45">
         <v>-0.06525851906293978</v>
@@ -1450,7 +1450,7 @@
         <v>30</v>
       </c>
       <c r="F46">
-        <v>-2.79977586579563</v>
+        <v>-2.802178495872356</v>
       </c>
       <c r="G46">
         <v>-0.06387835591992652</v>
@@ -1473,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="F47">
-        <v>-2.812136732803287</v>
+        <v>-2.812535057408017</v>
       </c>
       <c r="G47">
         <v>-0.06247389129781755</v>
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.823880753156115</v>
+        <v>-2.824235920798979</v>
       </c>
       <c r="G48">
         <v>-0.06224925594752295</v>
@@ -1519,7 +1519,7 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.835641390207203</v>
+        <v>-2.836483937491767</v>
       </c>
       <c r="G49">
         <v>-0.06086949888522653</v>
@@ -1588,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.868157801287395</v>
+        <v>-2.868310561446806</v>
       </c>
       <c r="G52">
         <v>-0.05922980559813218</v>
@@ -1611,7 +1611,7 @@
         <v>37</v>
       </c>
       <c r="F53">
-        <v>-2.879059274355655</v>
+        <v>-2.879819966825119</v>
       </c>
       <c r="G53">
         <v>-0.05734159308725095</v>
@@ -1634,7 +1634,7 @@
         <v>38</v>
       </c>
       <c r="F54">
-        <v>-2.8904558294191</v>
+        <v>-2.89057759407875</v>
       </c>
       <c r="G54">
         <v>-0.05573209756157105</v>
@@ -1657,7 +1657,7 @@
         <v>39</v>
       </c>
       <c r="F55">
-        <v>-2.901122687512842</v>
+        <v>-2.901487981491791</v>
       </c>
       <c r="G55">
         <v>-0.05487012769514921</v>
@@ -1703,7 +1703,7 @@
         <v>41</v>
       </c>
       <c r="F57">
-        <v>-2.921908245050409</v>
+        <v>-2.922759706679757</v>
       </c>
       <c r="G57">
         <v>-0.04980902944983412</v>
@@ -1749,7 +1749,7 @@
         <v>43</v>
       </c>
       <c r="F59">
-        <v>-2.942211405828743</v>
+        <v>-2.944031431867719</v>
       </c>
       <c r="G59">
         <v>-0.04535586351456022</v>
@@ -1772,7 +1772,7 @@
         <v>44</v>
       </c>
       <c r="F60">
-        <v>-2.952261417267655</v>
+        <v>-2.952991114237353</v>
       </c>
       <c r="G60">
         <v>-0.04263962499207485</v>
@@ -1818,7 +1818,7 @@
         <v>46</v>
       </c>
       <c r="F62">
-        <v>-2.970766633161993</v>
+        <v>-2.970910478976624</v>
       </c>
       <c r="G62">
         <v>-0.03626999663047809</v>
@@ -2163,7 +2163,7 @@
         <v>5</v>
       </c>
       <c r="F77">
-        <v>-2.564076727455178</v>
+        <v>-2.564201808489716</v>
       </c>
       <c r="G77">
         <v>-0.01153748281947342</v>
@@ -2186,7 +2186,7 @@
         <v>6</v>
       </c>
       <c r="F78">
-        <v>-2.571019131083296</v>
+        <v>-2.571269293152369</v>
       </c>
       <c r="G78">
         <v>-0.01344151593653731</v>
@@ -2209,7 +2209,7 @@
         <v>7</v>
       </c>
       <c r="F79">
-        <v>-2.577961534711414</v>
+        <v>-2.578086615745953</v>
       </c>
       <c r="G79">
         <v>-0.01495114987286561</v>
@@ -2232,7 +2232,7 @@
         <v>8</v>
       </c>
       <c r="F80">
-        <v>-2.584877386808773</v>
+        <v>-2.584903938339531</v>
       </c>
       <c r="G80">
         <v>-0.01697656629765065</v>
@@ -2255,7 +2255,7 @@
         <v>9</v>
       </c>
       <c r="F81">
-        <v>-2.591520223033114</v>
+        <v>-2.59179323890613</v>
       </c>
       <c r="G81">
         <v>-0.01920671834924992</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <v>-2.598382972068958</v>
+        <v>-2.598682539472732</v>
       </c>
       <c r="G82">
         <v>-0.02006377659037284</v>
@@ -2301,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="F83">
-        <v>-2.605078911354817</v>
+        <v>-2.605325375697078</v>
       </c>
       <c r="G83">
         <v>-0.02247245056416469</v>
@@ -2324,7 +2324,7 @@
         <v>12</v>
       </c>
       <c r="F84">
-        <v>-2.611534950521496</v>
+        <v>-2.612214676263675</v>
       </c>
       <c r="G84">
         <v>-0.02303220938156114</v>
@@ -2347,7 +2347,7 @@
         <v>13</v>
       </c>
       <c r="F85">
-        <v>-2.618670715430355</v>
+        <v>-2.618982593522559</v>
       </c>
       <c r="G85">
         <v>-0.02313921711713052</v>
@@ -2370,7 +2370,7 @@
         <v>14</v>
       </c>
       <c r="F86">
-        <v>-2.624521055566408</v>
+        <v>-2.625378965404642</v>
       </c>
       <c r="G86">
         <v>-0.02530711951488618</v>
@@ -2393,7 +2393,7 @@
         <v>15</v>
       </c>
       <c r="F87">
-        <v>-2.631465895489727</v>
+        <v>-2.631960085605857</v>
       </c>
       <c r="G87">
         <v>-0.02650874695511796</v>
@@ -2416,7 +2416,7 @@
         <v>16</v>
       </c>
       <c r="F88">
-        <v>-2.636775642969768</v>
+        <v>-2.638143108899523</v>
       </c>
       <c r="G88">
         <v>-0.02914360278173733</v>
@@ -2439,7 +2439,7 @@
         <v>17</v>
       </c>
       <c r="F89">
-        <v>-2.643806651977909</v>
+        <v>-2.644747082904678</v>
       </c>
       <c r="G89">
         <v>-0.02875040782855365</v>
@@ -2462,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="F90">
-        <v>-2.649798004427677</v>
+        <v>-2.651328203105894</v>
       </c>
       <c r="G90">
         <v>-0.03114366471063246</v>
@@ -2485,7 +2485,7 @@
         <v>19</v>
       </c>
       <c r="F91">
-        <v>-2.656375051848741</v>
+        <v>-2.657599493953442</v>
       </c>
       <c r="G91">
         <v>-0.03252757100423942</v>
@@ -2508,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.66243633207324</v>
+        <v>-2.663990119370176</v>
       </c>
       <c r="G92">
         <v>-0.03279670476236696</v>
@@ -2531,7 +2531,7 @@
         <v>21</v>
       </c>
       <c r="F93">
-        <v>-2.669076951243897</v>
+        <v>-2.670505825821447</v>
       </c>
       <c r="G93">
         <v>-0.0338386097874217</v>
@@ -2554,7 +2554,7 @@
         <v>22</v>
       </c>
       <c r="F94">
-        <v>-2.675607637573642</v>
+        <v>-2.676902197703534</v>
       </c>
       <c r="G94">
         <v>-0.03615692101567447</v>
@@ -2577,7 +2577,7 @@
         <v>23</v>
       </c>
       <c r="F95">
-        <v>-2.682110284505121</v>
+        <v>-2.68330431605097</v>
       </c>
       <c r="G95">
         <v>-0.0376098604918762</v>
@@ -2600,7 +2600,7 @@
         <v>24</v>
       </c>
       <c r="F96">
-        <v>-2.686994654148593</v>
+        <v>-2.689421925594689</v>
       </c>
       <c r="G96">
         <v>-0.03849425467213008</v>
@@ -2623,7 +2623,7 @@
         <v>25</v>
       </c>
       <c r="F97">
-        <v>-2.694432220033696</v>
+        <v>-2.695978543003676</v>
       </c>
       <c r="G97">
         <v>-0.03825148586158944</v>
@@ -2646,7 +2646,7 @@
         <v>26</v>
       </c>
       <c r="F98">
-        <v>-2.699524197210764</v>
+        <v>-2.701858491417203</v>
       </c>
       <c r="G98">
         <v>-0.03907572952178295</v>
@@ -2669,7 +2669,7 @@
         <v>27</v>
       </c>
       <c r="F99">
-        <v>-2.705155522254721</v>
+        <v>-2.708430589164842</v>
       </c>
       <c r="G99">
         <v>-0.04210934040430026</v>
@@ -2692,7 +2692,7 @@
         <v>28</v>
       </c>
       <c r="F100">
-        <v>-2.711486699410311</v>
+        <v>-2.7142499686236</v>
       </c>
       <c r="G100">
         <v>-0.04303832471335678</v>
@@ -2715,7 +2715,7 @@
         <v>29</v>
       </c>
       <c r="F101">
-        <v>-2.718512185480655</v>
+        <v>-2.720838067772605</v>
       </c>
       <c r="G101">
         <v>-0.04253686850322724</v>
@@ -2738,7 +2738,7 @@
         <v>30</v>
       </c>
       <c r="F102">
-        <v>-2.724057856540847</v>
+        <v>-2.726497375573735</v>
       </c>
       <c r="G102">
         <v>-0.04469874040493416</v>
@@ -2761,7 +2761,7 @@
         <v>31</v>
       </c>
       <c r="F103">
-        <v>-2.729458201780353</v>
+        <v>-2.732710734945769</v>
       </c>
       <c r="G103">
         <v>-0.04539819683189528</v>
@@ -2784,7 +2784,7 @@
         <v>32</v>
       </c>
       <c r="F104">
-        <v>-2.736497674914668</v>
+        <v>-2.73832829209616</v>
       </c>
       <c r="G104">
         <v>-0.04748471955815536</v>
@@ -2807,7 +2807,7 @@
         <v>33</v>
       </c>
       <c r="F105">
-        <v>-2.741743484855521</v>
+        <v>-2.744203392741494</v>
       </c>
       <c r="G105">
         <v>-0.04866065988224522</v>
@@ -2830,7 +2830,7 @@
         <v>34</v>
       </c>
       <c r="F106">
-        <v>-2.748081793206684</v>
+        <v>-2.7500110843698</v>
       </c>
       <c r="G106">
         <v>-0.05012672190763467</v>
@@ -2853,7 +2853,7 @@
         <v>35</v>
       </c>
       <c r="F107">
-        <v>-2.753252728265598</v>
+        <v>-2.756890388738615</v>
       </c>
       <c r="G107">
         <v>-0.04940962190280773</v>
@@ -2876,7 +2876,7 @@
         <v>36</v>
       </c>
       <c r="F108">
-        <v>-2.76096979435579</v>
+        <v>-2.762709421003938</v>
       </c>
       <c r="G108">
         <v>-0.04920619233585422</v>
@@ -2899,7 +2899,7 @@
         <v>37</v>
       </c>
       <c r="F109">
-        <v>-2.765396098433242</v>
+        <v>-2.768356420523097</v>
       </c>
       <c r="G109">
         <v>-0.05229541317540698</v>
@@ -2922,7 +2922,7 @@
         <v>38</v>
       </c>
       <c r="F110">
-        <v>-2.771515004902781</v>
+        <v>-2.774566789668315</v>
       </c>
       <c r="G110">
         <v>-0.05168218536254798</v>
@@ -2945,7 +2945,7 @@
         <v>39</v>
       </c>
       <c r="F111">
-        <v>-2.776949913597027</v>
+        <v>-2.779703616457609</v>
       </c>
       <c r="G111">
         <v>-0.05228418171994131</v>
@@ -2968,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.783922445609977</v>
+        <v>-2.786180584828454</v>
       </c>
       <c r="G112">
         <v>-0.05265652914170493</v>
@@ -2991,7 +2991,7 @@
         <v>41</v>
       </c>
       <c r="F113">
-        <v>-2.789194802063853</v>
+        <v>-2.791674803910853</v>
       </c>
       <c r="G113">
         <v>-0.05443394120460865</v>
@@ -3014,7 +3014,7 @@
         <v>42</v>
       </c>
       <c r="F114">
-        <v>-2.795076685920944</v>
+        <v>-2.797646616612941</v>
       </c>
       <c r="G114">
         <v>-0.05484941824675094</v>
@@ -3037,7 +3037,7 @@
         <v>43</v>
       </c>
       <c r="F115">
-        <v>-2.800672003119718</v>
+        <v>-2.80345334059629</v>
       </c>
       <c r="G115">
         <v>-0.05583094422105916</v>
@@ -3060,7 +3060,7 @@
         <v>44</v>
       </c>
       <c r="F116">
-        <v>-2.806595723585162</v>
+        <v>-2.8090707238774</v>
       </c>
       <c r="G116">
         <v>-0.05629771188832478</v>
@@ -3083,7 +3083,7 @@
         <v>45</v>
       </c>
       <c r="F117">
-        <v>-2.812261084476657</v>
+        <v>-2.814937027490379</v>
       </c>
       <c r="G117">
         <v>-0.05673703354188819</v>
@@ -3106,7 +3106,7 @@
         <v>46</v>
       </c>
       <c r="F118">
-        <v>-2.817681875015227</v>
+        <v>-2.820773049937077</v>
       </c>
       <c r="G118">
         <v>-0.05832060457832489</v>
@@ -3129,7 +3129,7 @@
         <v>47</v>
       </c>
       <c r="F119">
-        <v>-2.824058167066811</v>
+        <v>-2.826669908491075</v>
       </c>
       <c r="G119">
         <v>-0.06027404392161584</v>
@@ -3152,7 +3152,7 @@
         <v>48</v>
       </c>
       <c r="F120">
-        <v>-2.830051491611046</v>
+        <v>-2.832349104366217</v>
       </c>
       <c r="G120">
         <v>-0.05678812008185008</v>
@@ -3175,7 +3175,7 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.834759416546765</v>
+        <v>-2.838281850944878</v>
       </c>
       <c r="G121">
         <v>-0.06000911149696631</v>
@@ -3198,7 +3198,7 @@
         <v>50</v>
       </c>
       <c r="F122">
-        <v>-2.839957477100891</v>
+        <v>-2.843891234250655</v>
       </c>
       <c r="G122">
         <v>-0.06010277017543042</v>
@@ -3221,7 +3221,7 @@
         <v>51</v>
       </c>
       <c r="F123">
-        <v>-2.845978069606061</v>
+        <v>-2.849626764669363</v>
       </c>
       <c r="G123">
         <v>-0.06172347505184139</v>
@@ -3244,7 +3244,7 @@
         <v>52</v>
       </c>
       <c r="F124">
-        <v>-2.851750119233269</v>
+        <v>-2.855362295088061</v>
       </c>
       <c r="G124">
         <v>-0.06128663039299131</v>
@@ -3267,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="F125">
-        <v>-2.857211922560765</v>
+        <v>-2.860435729367782</v>
       </c>
       <c r="G125">
         <v>-0.06141738346264969</v>
@@ -3290,7 +3290,7 @@
         <v>54</v>
       </c>
       <c r="F126">
-        <v>-2.861995839860281</v>
+        <v>-2.866115961197832</v>
       </c>
       <c r="G126">
         <v>-0.0610192997207204</v>
@@ -3313,7 +3313,7 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.867440799714733</v>
+        <v>-2.872052151372194</v>
       </c>
       <c r="G127">
         <v>-0.06227460763599346</v>
@@ -3336,7 +3336,7 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.873829094865831</v>
+        <v>-2.87723769598627</v>
       </c>
       <c r="G128">
         <v>-0.06178267537622562</v>
@@ -3359,7 +3359,7 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.881279635677355</v>
+        <v>-2.883745603918092</v>
       </c>
       <c r="G129">
         <v>-0.0628489587630503</v>
@@ -3382,7 +3382,7 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.884921139917135</v>
+        <v>-2.88791067186791</v>
       </c>
       <c r="G130">
         <v>-0.06315778161906183</v>
@@ -3405,7 +3405,7 @@
         <v>59</v>
       </c>
       <c r="F131">
-        <v>-2.888749790923737</v>
+        <v>-2.893516139964121</v>
       </c>
       <c r="G131">
         <v>-0.06400379531036271</v>
@@ -3428,7 +3428,7 @@
         <v>60</v>
       </c>
       <c r="F132">
-        <v>-2.895356023424147</v>
+        <v>-2.898719460327705</v>
       </c>
       <c r="G132">
         <v>-0.06487120968189952</v>
@@ -3451,7 +3451,7 @@
         <v>61</v>
       </c>
       <c r="F133">
-        <v>-2.901210938214826</v>
+        <v>-2.906088307413654</v>
       </c>
       <c r="G133">
         <v>-0.06665454538554338</v>
@@ -3474,7 +3474,7 @@
         <v>62</v>
       </c>
       <c r="F134">
-        <v>-2.905804992440557</v>
+        <v>-2.909806772873404</v>
       </c>
       <c r="G134">
         <v>-0.06372632355803498</v>
@@ -3497,7 +3497,7 @@
         <v>63</v>
       </c>
       <c r="F135">
-        <v>-2.910520702831482</v>
+        <v>-2.915162960423494</v>
       </c>
       <c r="G135">
         <v>-0.06392543768492631</v>
@@ -3520,7 +3520,7 @@
         <v>64</v>
       </c>
       <c r="F136">
-        <v>-2.917810300294328</v>
+        <v>-2.922001232583722</v>
       </c>
       <c r="G136">
         <v>-0.06704948777737774</v>
@@ -3543,7 +3543,7 @@
         <v>65</v>
       </c>
       <c r="F137">
-        <v>-2.923056032258541</v>
+        <v>-2.925936365543709</v>
       </c>
       <c r="G137">
         <v>-0.06769446591700889</v>
@@ -3566,7 +3566,7 @@
         <v>66</v>
       </c>
       <c r="F138">
-        <v>-2.9268219772449</v>
+        <v>-2.930184274115561</v>
       </c>
       <c r="G138">
         <v>-0.06657101570578416</v>
@@ -3589,7 +3589,7 @@
         <v>67</v>
       </c>
       <c r="F139">
-        <v>-2.932102139760855</v>
+        <v>-2.936869877356833</v>
       </c>
       <c r="G139">
         <v>-0.06791020309441009</v>
@@ -3612,7 +3612,7 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.937633125717735</v>
+        <v>-2.941363769757977</v>
       </c>
       <c r="G140">
         <v>-0.06657930309982896</v>
@@ -3635,7 +3635,7 @@
         <v>69</v>
       </c>
       <c r="F141">
-        <v>-2.943609446751588</v>
+        <v>-2.94729518779757</v>
       </c>
       <c r="G141">
         <v>-0.06708370049153078</v>
@@ -3658,7 +3658,7 @@
         <v>70</v>
       </c>
       <c r="F142">
-        <v>-2.948868375521574</v>
+        <v>-2.951994429287164</v>
       </c>
       <c r="G142">
         <v>-0.06779788511858942</v>
@@ -3681,7 +3681,7 @@
         <v>71</v>
       </c>
       <c r="F143">
-        <v>-2.95326172042358</v>
+        <v>-2.957170685008337</v>
       </c>
       <c r="G143">
         <v>-0.06450248721298824</v>
@@ -3704,7 +3704,7 @@
         <v>72</v>
       </c>
       <c r="F144">
-        <v>-2.957392898478543</v>
+        <v>-2.961531104097487</v>
       </c>
       <c r="G144">
         <v>-0.06732753326125041</v>
@@ -3727,7 +3727,7 @@
         <v>73</v>
       </c>
       <c r="F145">
-        <v>-2.962975415944975</v>
+        <v>-2.967084264587558</v>
       </c>
       <c r="G145">
         <v>-0.06582163185846457</v>
@@ -3750,7 +3750,7 @@
         <v>74</v>
       </c>
       <c r="F146">
-        <v>-2.967506962887702</v>
+        <v>-2.97234712985043</v>
       </c>
       <c r="G146">
         <v>-0.06790146423278398</v>
@@ -3773,7 +3773,7 @@
         <v>75</v>
       </c>
       <c r="F147">
-        <v>-2.971935422715746</v>
+        <v>-2.976809940618336</v>
       </c>
       <c r="G147">
         <v>-0.06717352781770547</v>
@@ -3796,7 +3796,7 @@
         <v>76</v>
       </c>
       <c r="F148">
-        <v>-2.977896336549297</v>
+        <v>-2.98287582831025</v>
       </c>
       <c r="G148">
         <v>-0.06823410457540602</v>
@@ -3819,7 +3819,7 @@
         <v>77</v>
       </c>
       <c r="F149">
-        <v>-2.982478986268691</v>
+        <v>-2.986165900791791</v>
       </c>
       <c r="G149">
         <v>-0.06670793645458395</v>
@@ -3842,7 +3842,7 @@
         <v>78</v>
       </c>
       <c r="F150">
-        <v>-2.986994974492911</v>
+        <v>-2.99122011473872</v>
       </c>
       <c r="G150">
         <v>-0.06854791538365457</v>
@@ -3865,7 +3865,7 @@
         <v>79</v>
       </c>
       <c r="F151">
-        <v>-2.993545441583025</v>
+        <v>-2.996508119895559</v>
       </c>
       <c r="G151">
         <v>-0.06608525725976122</v>
@@ -3888,7 +3888,7 @@
         <v>80</v>
       </c>
       <c r="F152">
-        <v>-2.997753908275254</v>
+        <v>-3.001736790820815</v>
       </c>
       <c r="G152">
         <v>-0.06780185980026898</v>
@@ -3911,7 +3911,7 @@
         <v>81</v>
       </c>
       <c r="F153">
-        <v>-3.002744275072772</v>
+        <v>-3.005493430325944</v>
       </c>
       <c r="G153">
         <v>-0.06455850371540439</v>
@@ -3934,7 +3934,7 @@
         <v>82</v>
       </c>
       <c r="F154">
-        <v>-3.007060784823164</v>
+        <v>-3.009369826897697</v>
       </c>
       <c r="G154">
         <v>-0.06731151096098098</v>
@@ -3957,7 +3957,7 @@
         <v>83</v>
       </c>
       <c r="F155">
-        <v>-3.011134211911406</v>
+        <v>-3.015286455249842</v>
       </c>
       <c r="G155">
         <v>-0.06612522975386037</v>
@@ -3980,7 +3980,7 @@
         <v>84</v>
       </c>
       <c r="F156">
-        <v>-3.015680591900383</v>
+        <v>-3.019492489277283</v>
       </c>
       <c r="G156">
         <v>-0.06665332484574193</v>
@@ -4003,7 +4003,7 @@
         <v>85</v>
       </c>
       <c r="F157">
-        <v>-3.022719520336881</v>
+        <v>-3.02480175063726</v>
       </c>
       <c r="G157">
         <v>-0.06485566663902187</v>
@@ -4026,7 +4026,7 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.026589975741185</v>
+        <v>-3.028777124162508</v>
       </c>
       <c r="G158">
         <v>-0.06574624348211056</v>
@@ -4049,7 +4049,7 @@
         <v>87</v>
       </c>
       <c r="F159">
-        <v>-3.031169144325665</v>
+        <v>-3.033613529361189</v>
       </c>
       <c r="G159">
         <v>-0.06768449316199199</v>
@@ -4072,7 +4072,7 @@
         <v>88</v>
       </c>
       <c r="F160">
-        <v>-3.036429737464065</v>
+        <v>-3.037712799762173</v>
       </c>
       <c r="G160">
         <v>-0.06447723515981063</v>
@@ -4095,7 +4095,7 @@
         <v>89</v>
       </c>
       <c r="F161">
-        <v>-3.038976980772308</v>
+        <v>-3.042988035675671</v>
       </c>
       <c r="G161">
         <v>-0.06501816482063427</v>
@@ -4118,7 +4118,7 @@
         <v>90</v>
       </c>
       <c r="F162">
-        <v>-3.044975286333649</v>
+        <v>-3.047431065392828</v>
       </c>
       <c r="G162">
         <v>-0.06542870645147514</v>
@@ -4141,7 +4141,7 @@
         <v>91</v>
       </c>
       <c r="F163">
-        <v>-3.050328364043296</v>
+        <v>-3.052226540803412</v>
       </c>
       <c r="G163">
         <v>-0.06595331802108673</v>
@@ -4164,7 +4164,7 @@
         <v>92</v>
       </c>
       <c r="F164">
-        <v>-3.053741715275098</v>
+        <v>-3.056749396571728</v>
       </c>
       <c r="G164">
         <v>-0.06477163404513264</v>
@@ -4187,7 +4187,7 @@
         <v>93</v>
       </c>
       <c r="F165">
-        <v>-3.059511802916689</v>
+        <v>-3.061272252340038</v>
       </c>
       <c r="G165">
         <v>-0.06459507494494299</v>
@@ -4210,7 +4210,7 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.063029848632278</v>
+        <v>-3.064979301670365</v>
       </c>
       <c r="G166">
         <v>-0.06265426210750791</v>
@@ -4233,7 +4233,7 @@
         <v>95</v>
       </c>
       <c r="F167">
-        <v>-3.068807926024766</v>
+        <v>-3.070230980570038</v>
       </c>
       <c r="G167">
         <v>-0.06294389008283985</v>
@@ -4256,7 +4256,7 @@
         <v>96</v>
       </c>
       <c r="F168">
-        <v>-3.073248305309884</v>
+        <v>-3.074684249693051</v>
       </c>
       <c r="G168">
         <v>-0.06087182508497047</v>
@@ -4279,7 +4279,7 @@
         <v>97</v>
       </c>
       <c r="F169">
-        <v>-3.07826736478147</v>
+        <v>-3.079241898784014</v>
       </c>
       <c r="G169">
         <v>-0.06230885119838547</v>
@@ -4302,7 +4302,7 @@
         <v>98</v>
       </c>
       <c r="F170">
-        <v>-3.082667884653064</v>
+        <v>-3.083695167907024</v>
       </c>
       <c r="G170">
         <v>-0.06109185823841068</v>
@@ -4325,7 +4325,7 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.086632029469215</v>
+        <v>-3.088218023675337</v>
       </c>
       <c r="G171">
         <v>-0.06144085835089474</v>
@@ -4348,7 +4348,7 @@
         <v>100</v>
       </c>
       <c r="F172">
-        <v>-3.089335949781305</v>
+        <v>-3.092671292798344</v>
       </c>
       <c r="G172">
         <v>-0.06038023620861965</v>
@@ -4371,7 +4371,7 @@
         <v>101</v>
       </c>
       <c r="F173">
-        <v>-3.095486063293359</v>
+        <v>-3.097159355244004</v>
       </c>
       <c r="G173">
         <v>-0.05859013799830659</v>
@@ -4394,7 +4394,7 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.099188794660562</v>
+        <v>-3.101664814350992</v>
       </c>
       <c r="G174">
         <v>-0.05824262023479909</v>
@@ -4417,7 +4417,7 @@
         <v>103</v>
       </c>
       <c r="F175">
-        <v>-3.104187155842564</v>
+        <v>-3.106152876796651</v>
       </c>
       <c r="G175">
         <v>-0.05788878952085452</v>
@@ -4440,7 +4440,7 @@
         <v>104</v>
       </c>
       <c r="F176">
-        <v>-3.107626152349118</v>
+        <v>-3.110658335903637</v>
       </c>
       <c r="G176">
         <v>-0.05775707554350284</v>
@@ -4463,7 +4463,7 @@
         <v>105</v>
       </c>
       <c r="F177">
-        <v>-3.111351985947977</v>
+        <v>-3.115034986034474</v>
       </c>
       <c r="G177">
         <v>-0.05726767771701669</v>
@@ -4486,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="F178">
-        <v>-3.117051907008043</v>
+        <v>-3.119148608797763</v>
       </c>
       <c r="G178">
         <v>-0.05581483500563944</v>
@@ -4509,7 +4509,7 @@
         <v>107</v>
       </c>
       <c r="F179">
-        <v>-3.120140937522577</v>
+        <v>-3.123519849513359</v>
       </c>
       <c r="G179">
         <v>-0.05517185268375624</v>
@@ -4532,7 +4532,7 @@
         <v>108</v>
       </c>
       <c r="F180">
-        <v>-3.125046931304443</v>
+        <v>-3.128025308620344</v>
       </c>
       <c r="G180">
         <v>-0.0557679620549747</v>
@@ -4555,7 +4555,7 @@
         <v>109</v>
       </c>
       <c r="F181">
-        <v>-3.128615601961473</v>
+        <v>-3.13289241722954</v>
       </c>
       <c r="G181">
         <v>-0.05408958650118412</v>
@@ -4578,7 +4578,7 @@
         <v>110</v>
       </c>
       <c r="F182">
-        <v>-3.134269113601619</v>
+        <v>-3.136871821601439</v>
       </c>
       <c r="G182">
         <v>-0.05445877704824975</v>
@@ -4601,7 +4601,7 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.137711315373395</v>
+        <v>-3.140459389629641</v>
       </c>
       <c r="G183">
         <v>-0.05248383196828954</v>
@@ -4624,7 +4624,7 @@
         <v>112</v>
       </c>
       <c r="F184">
-        <v>-3.141991734757872</v>
+        <v>-3.14443879400154</v>
       </c>
       <c r="G184">
         <v>-0.04963277875443273</v>
@@ -4647,7 +4647,7 @@
         <v>113</v>
       </c>
       <c r="F185">
-        <v>-3.146822838016389</v>
+        <v>-3.148026362029742</v>
       </c>
       <c r="G185">
         <v>-0.04873802951269879</v>
@@ -4670,7 +4670,7 @@
         <v>114</v>
       </c>
       <c r="F186">
-        <v>-3.150085495573549</v>
+        <v>-3.152789439089032</v>
       </c>
       <c r="G186">
         <v>-0.04900903411513546</v>
@@ -4693,7 +4693,7 @@
         <v>115</v>
       </c>
       <c r="F187">
-        <v>-3.152716864678379</v>
+        <v>-3.15676884346093</v>
       </c>
       <c r="G187">
         <v>-0.04891407224665856</v>
@@ -4716,7 +4716,7 @@
         <v>116</v>
       </c>
       <c r="F188">
-        <v>-3.157452269768656</v>
+        <v>-3.160748247832828</v>
       </c>
       <c r="G188">
         <v>-0.04766792462859348</v>
@@ -4739,7 +4739,7 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.160822187448525</v>
+        <v>-3.163943979517335</v>
       </c>
       <c r="G189">
         <v>-0.0448020417717746</v>
@@ -4762,7 +4762,7 @@
         <v>118</v>
       </c>
       <c r="F190">
-        <v>-3.166224738107228</v>
+        <v>-3.168315220232929</v>
       </c>
       <c r="G190">
         <v>-0.04537717505014682</v>
@@ -4785,7 +4785,7 @@
         <v>119</v>
       </c>
       <c r="F191">
-        <v>-3.169981330185832</v>
+        <v>-3.172686460948523</v>
       </c>
       <c r="G191">
         <v>-0.04539073117985515</v>
@@ -4808,7 +4808,7 @@
         <v>120</v>
       </c>
       <c r="F192">
-        <v>-3.174762256796305</v>
+        <v>-3.176665865320421</v>
       </c>
       <c r="G192">
         <v>-0.04432853459351432</v>
@@ -4831,7 +4831,7 @@
         <v>121</v>
       </c>
       <c r="F193">
-        <v>-3.178193334391923</v>
+        <v>-3.180645269692319</v>
       </c>
       <c r="G193">
         <v>-0.0435471089773386</v>
@@ -4854,7 +4854,7 @@
         <v>122</v>
       </c>
       <c r="F194">
-        <v>-3.181320952143119</v>
+        <v>-3.184313846044246</v>
       </c>
       <c r="G194">
         <v>-0.04116621097703005</v>
@@ -4877,7 +4877,7 @@
         <v>123</v>
       </c>
       <c r="F195">
-        <v>-3.185508347967865</v>
+        <v>-3.187982422396172</v>
       </c>
       <c r="G195">
         <v>-0.03872384143873364</v>
@@ -4900,7 +4900,7 @@
         <v>124</v>
       </c>
       <c r="F196">
-        <v>-3.190738178498679</v>
+        <v>-3.191650998748095</v>
       </c>
       <c r="G196">
         <v>-0.03651257146252856</v>
@@ -4923,7 +4923,7 @@
         <v>125</v>
       </c>
       <c r="F197">
-        <v>-3.19363076122327</v>
+        <v>-3.195319575100019</v>
       </c>
       <c r="G197">
         <v>-0.03786018510255756</v>
@@ -4946,7 +4946,7 @@
         <v>126</v>
       </c>
       <c r="F198">
-        <v>-3.195962709948929</v>
+        <v>-3.198988151451942</v>
       </c>
       <c r="G198">
         <v>-0.03532006894105899</v>
@@ -4969,7 +4969,7 @@
         <v>127</v>
       </c>
       <c r="F199">
-        <v>-3.200133859191629</v>
+        <v>-3.202656727803864</v>
       </c>
       <c r="G199">
         <v>-0.03603671904325106</v>
@@ -4992,7 +4992,7 @@
         <v>128</v>
       </c>
       <c r="F200">
-        <v>-3.204153034839979</v>
+        <v>-3.20602430804107</v>
       </c>
       <c r="G200">
         <v>-0.03297449243434603</v>
@@ -5015,7 +5015,7 @@
         <v>129</v>
       </c>
       <c r="F201">
-        <v>-3.20709268062067</v>
+        <v>-3.209391888278276</v>
       </c>
       <c r="G201">
         <v>-0.03296750685671307</v>
@@ -5038,7 +5038,7 @@
         <v>130</v>
       </c>
       <c r="F202">
-        <v>-3.211412447520205</v>
+        <v>-3.212759468515483</v>
       </c>
       <c r="G202">
         <v>-0.03139378497422746</v>
@@ -5061,7 +5061,7 @@
         <v>131</v>
       </c>
       <c r="F203">
-        <v>-3.21424153288638</v>
+        <v>-3.216127048752689</v>
       </c>
       <c r="G203">
         <v>-0.03001937679319677</v>
@@ -5084,7 +5084,7 @@
         <v>132</v>
       </c>
       <c r="F204">
-        <v>-3.219193632875172</v>
+        <v>-3.219494628989893</v>
       </c>
       <c r="G204">
         <v>-0.03015194903129287</v>
@@ -5107,7 +5107,7 @@
         <v>133</v>
       </c>
       <c r="F205">
-        <v>-3.222053683102841</v>
+        <v>-3.222862209227097</v>
       </c>
       <c r="G205">
         <v>-0.02699653490524634</v>
@@ -5153,7 +5153,7 @@
         <v>135</v>
       </c>
       <c r="F207">
-        <v>-3.228582309682441</v>
+        <v>-3.229597369701504</v>
       </c>
       <c r="G207">
         <v>-0.02399763888814654</v>
@@ -5475,7 +5475,7 @@
         <v>30</v>
       </c>
       <c r="F221">
-        <v>-2.723656845986538</v>
+        <v>-2.726382951277858</v>
       </c>
       <c r="G221">
         <v>-0.02560431675245223</v>
@@ -5498,7 +5498,7 @@
         <v>61</v>
       </c>
       <c r="F222">
-        <v>-2.818607375122417</v>
+        <v>-2.82160700976125</v>
       </c>
       <c r="G222">
         <v>-0.04386742812921618</v>
@@ -5521,7 +5521,7 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.907913736277271</v>
+        <v>-2.913247058229718</v>
       </c>
       <c r="G223">
         <v>-0.05728340565328049</v>
@@ -5544,7 +5544,7 @@
         <v>123</v>
       </c>
       <c r="F224">
-        <v>-2.992911881867078</v>
+        <v>-2.997931634120476</v>
       </c>
       <c r="G224">
         <v>-0.06577717043876063</v>
@@ -5567,7 +5567,7 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.07387858022364</v>
+        <v>-3.076902673708512</v>
       </c>
       <c r="G225">
         <v>-0.06851272909896111</v>
@@ -5590,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.1479033063511</v>
+        <v>-3.150904134009064</v>
       </c>
       <c r="G226">
         <v>-0.06749295502671293</v>
@@ -5613,7 +5613,7 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.216198779595988</v>
+        <v>-3.217850332889162</v>
       </c>
       <c r="G227">
         <v>-0.05736411736875813</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.278266012121108</v>
+        <v>-3.280542670767227</v>
       </c>
       <c r="G228">
         <v>-0.04455329302800359</v>
@@ -5659,7 +5659,7 @@
         <v>278</v>
       </c>
       <c r="F229">
-        <v>-3.336567320252117</v>
+        <v>-3.336943235324647</v>
       </c>
       <c r="G229">
         <v>-0.02698616761849393</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.786503127290418</v>
+        <v>-2.790013498592089</v>
       </c>
       <c r="G232">
         <v>-0.02527176346397342</v>
@@ -5751,7 +5751,7 @@
         <v>112</v>
       </c>
       <c r="F233">
-        <v>-2.882797962767977</v>
+        <v>-2.887230566625838</v>
       </c>
       <c r="G233">
         <v>-0.04376841583561886</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.975941843619013</v>
+        <v>-2.979650874432433</v>
       </c>
       <c r="G234">
         <v>-0.05795588987540001</v>
@@ -5797,7 +5797,7 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.060292734501858</v>
+        <v>-3.066215640758489</v>
       </c>
       <c r="G235">
         <v>-0.06540721728834087</v>
@@ -5820,7 +5820,7 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.142683249924229</v>
+        <v>-3.147255395055307</v>
       </c>
       <c r="G236">
         <v>-0.06931697938274617</v>
@@ -5843,7 +5843,7 @@
         <v>336</v>
       </c>
       <c r="F237">
-        <v>-3.217973454648345</v>
+        <v>-3.224023189232544</v>
       </c>
       <c r="G237">
         <v>-0.06632166244271054</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.287416910066971</v>
+        <v>-3.291330448086803</v>
       </c>
       <c r="G238">
         <v>-0.05800286097577989</v>
@@ -5889,7 +5889,7 @@
         <v>448</v>
       </c>
       <c r="F239">
-        <v>-3.352006352667231</v>
+        <v>-3.355501881764296</v>
       </c>
       <c r="G239">
         <v>-0.04473968315851939</v>
@@ -5912,7 +5912,7 @@
         <v>504</v>
       </c>
       <c r="F240">
-        <v>-3.411728863050773</v>
+        <v>-3.413380605602728</v>
       </c>
       <c r="G240">
         <v>-0.02711937882840842</v>
@@ -5981,7 +5981,7 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.829502742547259</v>
+        <v>-2.832910615195931</v>
       </c>
       <c r="G243">
         <v>-0.0250304586649932</v>
@@ -6004,7 +6004,7 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.926551333478266</v>
+        <v>-2.93161577446255</v>
       </c>
       <c r="G244">
         <v>-0.04354852366881445</v>
@@ -6027,7 +6027,7 @@
         <v>276</v>
       </c>
       <c r="F245">
-        <v>-3.019056598279157</v>
+        <v>-3.024528566290706</v>
       </c>
       <c r="G245">
         <v>-0.05723271934982499</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.108888085337582</v>
+        <v>-3.113870517325203</v>
       </c>
       <c r="G246">
         <v>-0.06482813356561712</v>
@@ -6073,7 +6073,7 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.190298015122594</v>
+        <v>-3.19539815319411</v>
       </c>
       <c r="G247">
         <v>-0.06805097876230648</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.267086763155016</v>
+        <v>-3.271963796174929</v>
       </c>
       <c r="G248">
         <v>-0.06681828405940005</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.338769078987744</v>
+        <v>-3.341507789447114</v>
       </c>
       <c r="G249">
         <v>-0.05760174171475763</v>
@@ -6142,7 +6142,7 @@
         <v>738</v>
       </c>
       <c r="F250">
-        <v>-3.404252093427187</v>
+        <v>-3.40653486304329</v>
       </c>
       <c r="G250">
         <v>-0.04510061484400452</v>
@@ -6165,7 +6165,7 @@
         <v>830</v>
       </c>
       <c r="F251">
-        <v>-3.464318394231113</v>
+        <v>-3.465951205945215</v>
       </c>
       <c r="G251">
         <v>-0.02602466555336047</v>
@@ -6234,7 +6234,7 @@
         <v>141</v>
       </c>
       <c r="F254">
-        <v>-2.859022385229573</v>
+        <v>-2.86318891260805</v>
       </c>
       <c r="G254">
         <v>-0.0241816450302621</v>
@@ -6257,7 +6257,7 @@
         <v>283</v>
       </c>
       <c r="F255">
-        <v>-2.959473100997292</v>
+        <v>-2.963997755873526</v>
       </c>
       <c r="G255">
         <v>-0.04364111093397272</v>
@@ -6280,7 +6280,7 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.053031016123247</v>
+        <v>-3.057845849907247</v>
       </c>
       <c r="G256">
         <v>-0.05723884722613048</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.141855223936979</v>
+        <v>-3.147746915119647</v>
       </c>
       <c r="G257">
         <v>-0.06523516485980907</v>
@@ -6326,7 +6326,7 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.224855664051356</v>
+        <v>-3.230389976155747</v>
       </c>
       <c r="G258">
         <v>-0.06834797726552355</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.303548978242894</v>
+        <v>-3.308308840954089</v>
       </c>
       <c r="G259">
         <v>-0.06499168668186583</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.375349342777718</v>
+        <v>-3.379226113318104</v>
       </c>
       <c r="G260">
         <v>-0.05743932002365837</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.442034520148211</v>
+        <v>-3.44469009354968</v>
       </c>
       <c r="G261">
         <v>-0.04394327254395969</v>
@@ -6418,7 +6418,7 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.502643840541766</v>
+        <v>-3.5048853703882</v>
       </c>
       <c r="G262">
         <v>-0.0252635603647639</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.883195782478849</v>
+        <v>-2.88663317535716</v>
       </c>
       <c r="G265">
         <v>-0.0240632056775123</v>
@@ -6510,7 +6510,7 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.983340495676592</v>
+        <v>-2.988548881457617</v>
       </c>
       <c r="G266">
         <v>-0.04331321550334977</v>
@@ -6533,7 +6533,7 @@
         <v>617</v>
       </c>
       <c r="F267">
-        <v>-3.078373737307547</v>
+        <v>-3.083716140309118</v>
       </c>
       <c r="G267">
         <v>-0.05631636605077839</v>
@@ -6556,7 +6556,7 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.167873732495376</v>
+        <v>-3.173275406358634</v>
       </c>
       <c r="G268">
         <v>-0.06455489133007597</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.251608110444038</v>
+        <v>-3.257300388362103</v>
       </c>
       <c r="G269">
         <v>-0.06780675191923091</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.331177353307637</v>
+        <v>-3.335399839096191</v>
       </c>
       <c r="G270">
         <v>-0.06419752115149246</v>
@@ -6625,7 +6625,7 @@
         <v>1439</v>
       </c>
       <c r="F271">
-        <v>-3.402992630218043</v>
+        <v>-3.406438216347495</v>
       </c>
       <c r="G271">
         <v>-0.05688140820342391</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.470699926882973</v>
+        <v>-3.473139814193354</v>
       </c>
       <c r="G272">
         <v>-0.04387737884515908</v>
@@ -6671,7 +6671,7 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.531934137652331</v>
+        <v>-3.534145401539825</v>
       </c>
       <c r="G273">
         <v>-0.02466589200668384</v>
@@ -6740,7 +6740,7 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.901584800482094</v>
+        <v>-2.905070308770483</v>
       </c>
       <c r="G276">
         <v>-0.02406920687054059</v>
@@ -6763,7 +6763,7 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.002182589945451</v>
+        <v>-3.007753576465117</v>
       </c>
       <c r="G277">
         <v>-0.04227620044241398</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.0980740975509</v>
+        <v>-3.103019770104025</v>
       </c>
       <c r="G278">
         <v>-0.05607882283516297</v>
@@ -6809,7 +6809,7 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.187963133482202</v>
+        <v>-3.193322384894531</v>
       </c>
       <c r="G279">
         <v>-0.06318188816633419</v>
@@ -6832,7 +6832,7 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.273035933631117</v>
+        <v>-3.277787066803165</v>
       </c>
       <c r="G280">
         <v>-0.06621825962590311</v>
@@ -6855,7 +6855,7 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.352528063933899</v>
+        <v>-3.356539968013554</v>
       </c>
       <c r="G281">
         <v>-0.06398994315260564</v>
@@ -6878,7 +6878,7 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.425583392993906</v>
+        <v>-3.428907062509297</v>
       </c>
       <c r="G282">
         <v>-0.05612750293692592</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.492819830930784</v>
+        <v>-3.495227005974856</v>
       </c>
       <c r="G283">
         <v>-0.04295880299185728</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.55503584210588</v>
+        <v>-3.557246704782978</v>
       </c>
       <c r="G284">
         <v>-0.0244730013361007</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.917031869843392</v>
+        <v>-2.920345968088577</v>
       </c>
       <c r="G287">
         <v>-0.02367997741095973</v>
@@ -7016,7 +7016,7 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.017747137437067</v>
+        <v>-3.02364069377469</v>
       </c>
       <c r="G288">
         <v>-0.04251300891418719</v>
@@ -7039,7 +7039,7 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.113948027821744</v>
+        <v>-3.119066803580083</v>
       </c>
       <c r="G289">
         <v>-0.05551791606564294</v>
@@ -7062,7 +7062,7 @@
         <v>1548</v>
       </c>
       <c r="F290">
-        <v>-3.204795038623368</v>
+        <v>-3.210037286355824</v>
       </c>
       <c r="G290">
         <v>-0.06299904231392772</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.289882190957003</v>
+        <v>-3.295114779184526</v>
       </c>
       <c r="G291">
         <v>-0.0655803780886155</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.369779036285709</v>
+        <v>-3.373859581884342</v>
       </c>
       <c r="G292">
         <v>-0.06303955016071905</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.44317017159644</v>
+        <v>-3.446812906787265</v>
       </c>
       <c r="G293">
         <v>-0.05515012424061883</v>
@@ -7154,7 +7154,7 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.511174259827198</v>
+        <v>-3.513553177856656</v>
       </c>
       <c r="G294">
         <v>-0.04236717761340913</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.573426585177015</v>
+        <v>-3.575630697723033</v>
       </c>
       <c r="G295">
         <v>-0.02449152068444382</v>
@@ -7246,7 +7246,7 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.929349301208876</v>
+        <v>-2.932611854465612</v>
       </c>
       <c r="G298">
         <v>-0.02357381916767043</v>
@@ -7269,7 +7269,7 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.030879309779817</v>
+        <v>-3.036234937946506</v>
       </c>
       <c r="G299">
         <v>-0.04201270279780811</v>
@@ -7292,7 +7292,7 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.127251554473209</v>
+        <v>-3.132111741281946</v>
       </c>
       <c r="G300">
         <v>-0.0543073434687642</v>
@@ -7315,7 +7315,7 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.218315796108344</v>
+        <v>-3.223496936798708</v>
       </c>
       <c r="G301">
         <v>-0.06219144904681673</v>
@@ -7338,7 +7338,7 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.304054594288487</v>
+        <v>-3.308798118249894</v>
       </c>
       <c r="G302">
         <v>-0.06503915675330885</v>
@@ -7361,7 +7361,7 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.38364689440433</v>
+        <v>-3.387772340436344</v>
       </c>
       <c r="G303">
         <v>-0.06236990600344705</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.45834923233055</v>
+        <v>-3.461436997713451</v>
       </c>
       <c r="G304">
         <v>-0.05464736464488806</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.526402002354607</v>
+        <v>-3.528374929353729</v>
       </c>
       <c r="G305">
         <v>-0.04220518905553605</v>
@@ -7430,7 +7430,7 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.588716447193514</v>
+        <v>-3.590734543809615</v>
       </c>
       <c r="G306">
         <v>-0.02395110289660207</v>
@@ -7499,7 +7499,7 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.939759593641992</v>
+        <v>-2.94286615191264</v>
       </c>
       <c r="G309">
         <v>-0.02338508521976257</v>
@@ -7522,7 +7522,7 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.041639216086596</v>
+        <v>-3.046894837589852</v>
       </c>
       <c r="G310">
         <v>-0.04129000151007567</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.138552292021602</v>
+        <v>-3.143155263815385</v>
       </c>
       <c r="G311">
         <v>-0.05420531534682338</v>
@@ -7568,7 +7568,7 @@
         <v>2610</v>
       </c>
       <c r="F312">
-        <v>-3.229759206086767</v>
+        <v>-3.235100711166736</v>
       </c>
       <c r="G312">
         <v>-0.06159631211594552</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.315439718700854</v>
+        <v>-3.32027545916824</v>
       </c>
       <c r="G313">
         <v>-0.06397337201434161</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.396270155041174</v>
+        <v>-3.39982995008607</v>
       </c>
       <c r="G314">
         <v>-0.061438666420216</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.470299396594158</v>
+        <v>-3.473749804341944</v>
       </c>
       <c r="G315">
         <v>-0.05399105464408593</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.539051884288511</v>
+        <v>-3.540907758478565</v>
       </c>
       <c r="G316">
         <v>-0.0413182393111089</v>
@@ -7683,7 +7683,7 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.6014934184512</v>
+        <v>-3.603433053495804</v>
       </c>
       <c r="G317">
         <v>-0.02372300662380827</v>
@@ -7752,7 +7752,7 @@
         <v>821</v>
       </c>
       <c r="F320">
-        <v>-2.948417396449492</v>
+        <v>-2.951617714211739</v>
       </c>
       <c r="G320">
         <v>-0.0233819330146412</v>
@@ -7775,7 +7775,7 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.05057071886332</v>
+        <v>-3.055778697080845</v>
       </c>
       <c r="G321">
         <v>-0.0412592898511992</v>
@@ -7798,7 +7798,7 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.14809638274726</v>
+        <v>-3.152707778231721</v>
       </c>
       <c r="G322">
         <v>-0.05332638142041324</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.239435237463776</v>
+        <v>-3.244144779682376</v>
       </c>
       <c r="G323">
         <v>-0.06099802107311758</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.325694099330758</v>
+        <v>-3.329964285866212</v>
       </c>
       <c r="G324">
         <v>-0.06352861199624371</v>
@@ -7867,7 +7867,7 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.406258634139743</v>
+        <v>-3.409963085989417</v>
       </c>
       <c r="G325">
         <v>-0.06095986211832471</v>
@@ -7890,7 +7890,7 @@
         <v>5751</v>
       </c>
       <c r="F326">
-        <v>-3.481088537206477</v>
+        <v>-3.48381336327765</v>
       </c>
       <c r="G326">
         <v>-0.05364092179063251</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.549434679112862</v>
+        <v>-3.55158381673289</v>
       </c>
       <c r="G327">
         <v>-0.04087010370692101</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.612665606572998</v>
+        <v>-3.614286163429787</v>
       </c>
       <c r="G328">
         <v>-0.02339390262022029</v>
@@ -8005,7 +8005,7 @@
         <v>1017</v>
       </c>
       <c r="F331">
-        <v>-2.956253710334245</v>
+        <v>-2.95913471074413</v>
       </c>
       <c r="G331">
         <v>-0.02304604198804938</v>
@@ -8028,7 +8028,7 @@
         <v>2035</v>
       </c>
       <c r="F332">
-        <v>-3.058678315404536</v>
+        <v>-3.063446117951071</v>
       </c>
       <c r="G332">
         <v>-0.04084545509864856</v>
@@ -8051,7 +8051,7 @@
         <v>3053</v>
       </c>
       <c r="F333">
-        <v>-3.155908250782195</v>
+        <v>-3.160621630835472</v>
       </c>
       <c r="G333">
         <v>-0.05317217999790391</v>
@@ -8074,7 +8074,7 @@
         <v>4071</v>
       </c>
       <c r="F334">
-        <v>-3.247826832349809</v>
+        <v>-3.252518392231936</v>
       </c>
       <c r="G334">
         <v>-0.06057126192654172</v>
@@ -8097,7 +8097,7 @@
         <v>5089</v>
       </c>
       <c r="F335">
-        <v>-3.334563161944447</v>
+        <v>-3.338576013592679</v>
       </c>
       <c r="G335">
         <v>-0.06278717063128125</v>
@@ -8120,7 +8120,7 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.415132895232571</v>
+        <v>-3.418488784731534</v>
       </c>
       <c r="G336">
         <v>-0.06050505627801783</v>
@@ -8143,7 +8143,7 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.489858674897246</v>
+        <v>-3.492736207759783</v>
       </c>
       <c r="G337">
         <v>-0.05286449853341879</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.558842915543228</v>
+        <v>-3.560827885637969</v>
       </c>
       <c r="G338">
         <v>-0.04053172592297882</v>
@@ -8189,7 +8189,7 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.621847992123753</v>
+        <v>-3.623448259486291</v>
       </c>
       <c r="G339">
         <v>-0.02310751223477731</v>

</xml_diff>

<commit_message>
updated data with new 5000 generations GA sims (started 03.08.2019 - ended 03.10.2019)
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -1542,7 +1542,7 @@
         <v>34</v>
       </c>
       <c r="F50">
-        <v>-2.846633632435351</v>
+        <v>-2.847363329405048</v>
       </c>
       <c r="G50">
         <v>-0.06196268929837656</v>
@@ -4026,7 +4026,7 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.028777124162508</v>
+        <v>-3.029271039784648</v>
       </c>
       <c r="G158">
         <v>-0.06574624348211056</v>
@@ -4371,7 +4371,7 @@
         <v>101</v>
       </c>
       <c r="F173">
-        <v>-3.097159355244004</v>
+        <v>-3.097176751905331</v>
       </c>
       <c r="G173">
         <v>-0.05859013799830659</v>
@@ -5521,7 +5521,7 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.913247058229718</v>
+        <v>-2.913274284622731</v>
       </c>
       <c r="G223">
         <v>-0.05728340565328049</v>
@@ -5613,7 +5613,7 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.217850332889162</v>
+        <v>-3.217863772144251</v>
       </c>
       <c r="G227">
         <v>-0.05736411736875813</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.280542670767227</v>
+        <v>-3.280582468107533</v>
       </c>
       <c r="G228">
         <v>-0.04455329302800359</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.979650874432433</v>
+        <v>-2.979661250041501</v>
       </c>
       <c r="G234">
         <v>-0.05795588987540001</v>
@@ -5820,7 +5820,7 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.147255395055307</v>
+        <v>-3.147473383737164</v>
       </c>
       <c r="G236">
         <v>-0.06931697938274617</v>
@@ -5843,7 +5843,7 @@
         <v>336</v>
       </c>
       <c r="F237">
-        <v>-3.224023189232544</v>
+        <v>-3.224099959899654</v>
       </c>
       <c r="G237">
         <v>-0.06632166244271054</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.291330448086803</v>
+        <v>-3.29158834514734</v>
       </c>
       <c r="G238">
         <v>-0.05800286097577989</v>
@@ -5889,7 +5889,7 @@
         <v>448</v>
       </c>
       <c r="F239">
-        <v>-3.355501881764296</v>
+        <v>-3.355524892450933</v>
       </c>
       <c r="G239">
         <v>-0.04473968315851939</v>
@@ -6027,7 +6027,7 @@
         <v>276</v>
       </c>
       <c r="F245">
-        <v>-3.024528566290706</v>
+        <v>-3.024556656727945</v>
       </c>
       <c r="G245">
         <v>-0.05723271934982499</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.113870517325203</v>
+        <v>-3.113958547558499</v>
       </c>
       <c r="G246">
         <v>-0.06482813356561712</v>
@@ -6073,7 +6073,7 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.19539815319411</v>
+        <v>-3.195457824564384</v>
       </c>
       <c r="G247">
         <v>-0.06805097876230648</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.271963796174929</v>
+        <v>-3.272072816821676</v>
       </c>
       <c r="G248">
         <v>-0.06681828405940005</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.341507789447114</v>
+        <v>-3.341534022330322</v>
       </c>
       <c r="G249">
         <v>-0.05760174171475763</v>
@@ -6142,7 +6142,7 @@
         <v>738</v>
       </c>
       <c r="F250">
-        <v>-3.40653486304329</v>
+        <v>-3.406579662273886</v>
       </c>
       <c r="G250">
         <v>-0.04510061484400452</v>
@@ -6257,7 +6257,7 @@
         <v>283</v>
       </c>
       <c r="F255">
-        <v>-2.963997755873526</v>
+        <v>-2.964021928768352</v>
       </c>
       <c r="G255">
         <v>-0.04364111093397272</v>
@@ -6280,7 +6280,7 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.057845849907247</v>
+        <v>-3.057943108185491</v>
       </c>
       <c r="G256">
         <v>-0.05723884722613048</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.147746915119647</v>
+        <v>-3.147857987285641</v>
       </c>
       <c r="G257">
         <v>-0.06523516485980907</v>
@@ -6326,7 +6326,7 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.230389976155747</v>
+        <v>-3.230502321002861</v>
       </c>
       <c r="G258">
         <v>-0.06834797726552355</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.308308840954089</v>
+        <v>-3.308364894749349</v>
       </c>
       <c r="G259">
         <v>-0.06499168668186583</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.379226113318104</v>
+        <v>-3.379271940079538</v>
       </c>
       <c r="G260">
         <v>-0.05743932002365837</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.44469009354968</v>
+        <v>-3.444757276326715</v>
       </c>
       <c r="G261">
         <v>-0.04394327254395969</v>
@@ -6418,7 +6418,7 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.5048853703882</v>
+        <v>-3.504912815149955</v>
       </c>
       <c r="G262">
         <v>-0.0252635603647639</v>
@@ -6510,7 +6510,7 @@
         <v>411</v>
       </c>
       <c r="F266">
-        <v>-2.988548881457617</v>
+        <v>-2.988583457594388</v>
       </c>
       <c r="G266">
         <v>-0.04331321550334977</v>
@@ -6533,7 +6533,7 @@
         <v>617</v>
       </c>
       <c r="F267">
-        <v>-3.083716140309118</v>
+        <v>-3.083747118797938</v>
       </c>
       <c r="G267">
         <v>-0.05631636605077839</v>
@@ -6556,7 +6556,7 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.173275406358634</v>
+        <v>-3.17338101498985</v>
       </c>
       <c r="G268">
         <v>-0.06455489133007597</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.257300388362103</v>
+        <v>-3.257506832477579</v>
       </c>
       <c r="G269">
         <v>-0.06780675191923091</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.335399839096191</v>
+        <v>-3.335467732329208</v>
       </c>
       <c r="G270">
         <v>-0.06419752115149246</v>
@@ -6625,7 +6625,7 @@
         <v>1439</v>
       </c>
       <c r="F271">
-        <v>-3.406438216347495</v>
+        <v>-3.40650823760156</v>
       </c>
       <c r="G271">
         <v>-0.05688140820342391</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.473139814193354</v>
+        <v>-3.473242329533754</v>
       </c>
       <c r="G272">
         <v>-0.04387737884515908</v>
@@ -6671,7 +6671,7 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.534145401539825</v>
+        <v>-3.534178823147981</v>
       </c>
       <c r="G273">
         <v>-0.02466589200668384</v>
@@ -6740,7 +6740,7 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.905070308770483</v>
+        <v>-2.905081443542592</v>
       </c>
       <c r="G276">
         <v>-0.02406920687054059</v>
@@ -6763,7 +6763,7 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.007753576465117</v>
+        <v>-3.007809816131696</v>
       </c>
       <c r="G277">
         <v>-0.04227620044241398</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.103019770104025</v>
+        <v>-3.103068866715314</v>
       </c>
       <c r="G278">
         <v>-0.05607882283516297</v>
@@ -6809,7 +6809,7 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.193322384894531</v>
+        <v>-3.19345918119902</v>
       </c>
       <c r="G279">
         <v>-0.06318188816633419</v>
@@ -6832,7 +6832,7 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.277787066803165</v>
+        <v>-3.27791540919861</v>
       </c>
       <c r="G280">
         <v>-0.06621825962590311</v>
@@ -6855,7 +6855,7 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.356539968013554</v>
+        <v>-3.356682846191505</v>
       </c>
       <c r="G281">
         <v>-0.06398994315260564</v>
@@ -6878,7 +6878,7 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.428907062509297</v>
+        <v>-3.428988579794057</v>
       </c>
       <c r="G282">
         <v>-0.05612750293692592</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.495227005974856</v>
+        <v>-3.495291882214794</v>
       </c>
       <c r="G283">
         <v>-0.04295880299185728</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.557246704782978</v>
+        <v>-3.557303971857867</v>
       </c>
       <c r="G284">
         <v>-0.0244730013361007</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.920345968088577</v>
+        <v>-2.920372840900682</v>
       </c>
       <c r="G287">
         <v>-0.02367997741095973</v>
@@ -7016,7 +7016,7 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.02364069377469</v>
+        <v>-3.023708441915248</v>
       </c>
       <c r="G288">
         <v>-0.04251300891418719</v>
@@ -7039,7 +7039,7 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.119066803580083</v>
+        <v>-3.119148480561464</v>
       </c>
       <c r="G289">
         <v>-0.05551791606564294</v>
@@ -7062,7 +7062,7 @@
         <v>1548</v>
       </c>
       <c r="F290">
-        <v>-3.210037286355824</v>
+        <v>-3.210266918530571</v>
       </c>
       <c r="G290">
         <v>-0.06299904231392772</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.295114779184526</v>
+        <v>-3.295232931136971</v>
       </c>
       <c r="G291">
         <v>-0.0655803780886155</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.373859581884342</v>
+        <v>-3.374028071074377</v>
       </c>
       <c r="G292">
         <v>-0.06303955016071905</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.446812906787265</v>
+        <v>-3.446989022551367</v>
       </c>
       <c r="G293">
         <v>-0.05515012424061883</v>
@@ -7154,7 +7154,7 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.513553177856656</v>
+        <v>-3.513611906020523</v>
       </c>
       <c r="G294">
         <v>-0.04236717761340913</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.575630697723033</v>
+        <v>-3.575695261926112</v>
       </c>
       <c r="G295">
         <v>-0.02449152068444382</v>
@@ -7246,7 +7246,7 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.932611854465612</v>
+        <v>-2.932636993683525</v>
       </c>
       <c r="G298">
         <v>-0.02357381916767043</v>
@@ -7269,7 +7269,7 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.036234937946506</v>
+        <v>-3.036356251775248</v>
       </c>
       <c r="G299">
         <v>-0.04201270279780811</v>
@@ -7292,7 +7292,7 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.132111741281946</v>
+        <v>-3.132205758788848</v>
       </c>
       <c r="G300">
         <v>-0.0543073434687642</v>
@@ -7315,7 +7315,7 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.223496936798708</v>
+        <v>-3.223654417848852</v>
       </c>
       <c r="G301">
         <v>-0.06219144904681673</v>
@@ -7338,7 +7338,7 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.308798118249894</v>
+        <v>-3.308923757593324</v>
       </c>
       <c r="G302">
         <v>-0.06503915675330885</v>
@@ -7361,7 +7361,7 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.387772340436344</v>
+        <v>-3.3879805413396</v>
       </c>
       <c r="G303">
         <v>-0.06236990600344705</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.461436997713451</v>
+        <v>-3.461625250008425</v>
       </c>
       <c r="G304">
         <v>-0.05464736464488806</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.528374929353729</v>
+        <v>-3.528450113799827</v>
       </c>
       <c r="G305">
         <v>-0.04220518905553605</v>
@@ -7430,7 +7430,7 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.590734543809615</v>
+        <v>-3.590830647460414</v>
       </c>
       <c r="G306">
         <v>-0.02395110289660207</v>
@@ -7522,7 +7522,7 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.046894837589852</v>
+        <v>-3.047023753634885</v>
       </c>
       <c r="G310">
         <v>-0.04129000151007567</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.143155263815385</v>
+        <v>-3.143304376754101</v>
       </c>
       <c r="G311">
         <v>-0.05420531534682338</v>
@@ -7568,7 +7568,7 @@
         <v>2610</v>
       </c>
       <c r="F312">
-        <v>-3.235100711166736</v>
+        <v>-3.235320472243015</v>
       </c>
       <c r="G312">
         <v>-0.06159631211594552</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.32027545916824</v>
+        <v>-3.32051480760932</v>
       </c>
       <c r="G313">
         <v>-0.06397337201434161</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.39982995008607</v>
+        <v>-3.400014245160864</v>
       </c>
       <c r="G314">
         <v>-0.061438666420216</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.473749804341944</v>
+        <v>-3.473912623648221</v>
       </c>
       <c r="G315">
         <v>-0.05399105464408593</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.540907758478565</v>
+        <v>-3.541055091318504</v>
       </c>
       <c r="G316">
         <v>-0.0413182393111089</v>
@@ -7683,7 +7683,7 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.603433053495804</v>
+        <v>-3.603478373974208</v>
       </c>
       <c r="G317">
         <v>-0.02372300662380827</v>
@@ -7752,7 +7752,7 @@
         <v>821</v>
       </c>
       <c r="F320">
-        <v>-2.951617714211739</v>
+        <v>-2.951649812661532</v>
       </c>
       <c r="G320">
         <v>-0.0233819330146412</v>
@@ -7775,7 +7775,7 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.055778697080845</v>
+        <v>-3.055948907401567</v>
       </c>
       <c r="G321">
         <v>-0.0412592898511992</v>
@@ -7798,7 +7798,7 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.152707778231721</v>
+        <v>-3.152863255870566</v>
       </c>
       <c r="G322">
         <v>-0.05332638142041324</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.244144779682376</v>
+        <v>-3.244344609954935</v>
       </c>
       <c r="G323">
         <v>-0.06099802107311758</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.329964285866212</v>
+        <v>-3.330190749330464</v>
       </c>
       <c r="G324">
         <v>-0.06352861199624371</v>
@@ -7867,7 +7867,7 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.409963085989417</v>
+        <v>-3.41012628034601</v>
       </c>
       <c r="G325">
         <v>-0.06095986211832471</v>
@@ -7890,7 +7890,7 @@
         <v>5751</v>
       </c>
       <c r="F326">
-        <v>-3.48381336327765</v>
+        <v>-3.484001573272431</v>
       </c>
       <c r="G326">
         <v>-0.05364092179063251</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.55158381673289</v>
+        <v>-3.551679437867892</v>
       </c>
       <c r="G327">
         <v>-0.04087010370692101</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.614286163429787</v>
+        <v>-3.614400897872223</v>
       </c>
       <c r="G328">
         <v>-0.02339390262022029</v>
@@ -8005,7 +8005,7 @@
         <v>1017</v>
       </c>
       <c r="F331">
-        <v>-2.95913471074413</v>
+        <v>-2.959177922907605</v>
       </c>
       <c r="G331">
         <v>-0.02304604198804938</v>
@@ -8028,7 +8028,7 @@
         <v>2035</v>
       </c>
       <c r="F332">
-        <v>-3.063446117951071</v>
+        <v>-3.063644383045004</v>
       </c>
       <c r="G332">
         <v>-0.04084545509864856</v>
@@ -8051,7 +8051,7 @@
         <v>3053</v>
       </c>
       <c r="F333">
-        <v>-3.160621630835472</v>
+        <v>-3.160789252012596</v>
       </c>
       <c r="G333">
         <v>-0.05317217999790391</v>
@@ -8074,7 +8074,7 @@
         <v>4071</v>
       </c>
       <c r="F334">
-        <v>-3.252518392231936</v>
+        <v>-3.25276570079152</v>
       </c>
       <c r="G334">
         <v>-0.06057126192654172</v>
@@ -8097,7 +8097,7 @@
         <v>5089</v>
       </c>
       <c r="F335">
-        <v>-3.338576013592679</v>
+        <v>-3.338815710521684</v>
       </c>
       <c r="G335">
         <v>-0.06278717063128125</v>
@@ -8120,7 +8120,7 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.418488784731534</v>
+        <v>-3.418683347953833</v>
       </c>
       <c r="G336">
         <v>-0.06050505627801783</v>
@@ -8143,7 +8143,7 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.492736207759783</v>
+        <v>-3.492912858164739</v>
       </c>
       <c r="G337">
         <v>-0.05286449853341879</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.560827885637969</v>
+        <v>-3.560941762816751</v>
       </c>
       <c r="G338">
         <v>-0.04053172592297882</v>
@@ -8189,7 +8189,7 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.623448259486291</v>
+        <v>-3.623541557974249</v>
       </c>
       <c r="G339">
         <v>-0.02310751223477731</v>

</xml_diff>

<commit_message>
data updated rom 03.11.2019
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/cuboctahedron/cuboctahedron_AgAu_data.xlsx
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.540437986829659</v>
+        <v>-2.540474844570498</v>
       </c>
       <c r="G27">
         <v>-0.04326276145102503</v>
@@ -3037,7 +3037,7 @@
         <v>43</v>
       </c>
       <c r="F115">
-        <v>-2.80345334059629</v>
+        <v>-2.803613412253912</v>
       </c>
       <c r="G115">
         <v>-0.05583094422105916</v>
@@ -3382,7 +3382,7 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.88791067186791</v>
+        <v>-2.888047734825423</v>
       </c>
       <c r="G130">
         <v>-0.06315778161906183</v>
@@ -4026,7 +4026,7 @@
         <v>86</v>
       </c>
       <c r="F158">
-        <v>-3.029271039784648</v>
+        <v>-3.029317759171294</v>
       </c>
       <c r="G158">
         <v>-0.06574624348211056</v>
@@ -4325,7 +4325,7 @@
         <v>99</v>
       </c>
       <c r="F171">
-        <v>-3.088218023675337</v>
+        <v>-3.088235420336663</v>
       </c>
       <c r="G171">
         <v>-0.06144085835089474</v>
@@ -4509,7 +4509,7 @@
         <v>107</v>
       </c>
       <c r="F179">
-        <v>-3.123519849513359</v>
+        <v>-3.124174713224597</v>
       </c>
       <c r="G179">
         <v>-0.05517185268375624</v>
@@ -5521,7 +5521,7 @@
         <v>92</v>
       </c>
       <c r="F223">
-        <v>-2.913274284622731</v>
+        <v>-2.913309804869715</v>
       </c>
       <c r="G223">
         <v>-0.05728340565328049</v>
@@ -5567,7 +5567,7 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.076902673708512</v>
+        <v>-3.076917804555529</v>
       </c>
       <c r="G225">
         <v>-0.06851272909896111</v>
@@ -5590,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.150904134009064</v>
+        <v>-3.150938017413439</v>
       </c>
       <c r="G226">
         <v>-0.06749295502671293</v>
@@ -5613,7 +5613,7 @@
         <v>216</v>
       </c>
       <c r="F227">
-        <v>-3.217863772144251</v>
+        <v>-3.217891054079637</v>
       </c>
       <c r="G227">
         <v>-0.05736411736875813</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.280582468107533</v>
+        <v>-3.280639993961369</v>
       </c>
       <c r="G228">
         <v>-0.04455329302800359</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.790013498592089</v>
+        <v>-2.79002809337312</v>
       </c>
       <c r="G232">
         <v>-0.02527176346397342</v>
@@ -5797,7 +5797,7 @@
         <v>224</v>
       </c>
       <c r="F235">
-        <v>-3.066215640758489</v>
+        <v>-3.066263679871699</v>
       </c>
       <c r="G235">
         <v>-0.06540721728834087</v>
@@ -5820,7 +5820,7 @@
         <v>280</v>
       </c>
       <c r="F236">
-        <v>-3.147473383737164</v>
+        <v>-3.14757131180186</v>
       </c>
       <c r="G236">
         <v>-0.06931697938274617</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.29158834514734</v>
+        <v>-3.291765168377015</v>
       </c>
       <c r="G238">
         <v>-0.05800286097577989</v>
@@ -5981,7 +5981,7 @@
         <v>92</v>
       </c>
       <c r="F243">
-        <v>-2.832910615195931</v>
+        <v>-2.832945225879762</v>
       </c>
       <c r="G243">
         <v>-0.0250304586649932</v>
@@ -6004,7 +6004,7 @@
         <v>184</v>
       </c>
       <c r="F244">
-        <v>-2.93161577446255</v>
+        <v>-2.931685011046211</v>
       </c>
       <c r="G244">
         <v>-0.04354852366881445</v>
@@ -6050,7 +6050,7 @@
         <v>369</v>
       </c>
       <c r="F246">
-        <v>-3.113958547558499</v>
+        <v>-3.114104678461579</v>
       </c>
       <c r="G246">
         <v>-0.06482813356561712</v>
@@ -6073,7 +6073,7 @@
         <v>461</v>
       </c>
       <c r="F247">
-        <v>-3.195457824564384</v>
+        <v>-3.195536714578507</v>
       </c>
       <c r="G247">
         <v>-0.06805097876230648</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.272072816821676</v>
+        <v>-3.27212459219117</v>
       </c>
       <c r="G248">
         <v>-0.06681828405940005</v>
@@ -6119,7 +6119,7 @@
         <v>646</v>
       </c>
       <c r="F249">
-        <v>-3.341534022330322</v>
+        <v>-3.341675908617004</v>
       </c>
       <c r="G249">
         <v>-0.05760174171475763</v>
@@ -6142,7 +6142,7 @@
         <v>738</v>
       </c>
       <c r="F250">
-        <v>-3.406579662273886</v>
+        <v>-3.406622428841292</v>
       </c>
       <c r="G250">
         <v>-0.04510061484400452</v>
@@ -6234,7 +6234,7 @@
         <v>141</v>
       </c>
       <c r="F254">
-        <v>-2.86318891260805</v>
+        <v>-2.863245638167534</v>
       </c>
       <c r="G254">
         <v>-0.0241816450302621</v>
@@ -6280,7 +6280,7 @@
         <v>424</v>
       </c>
       <c r="F256">
-        <v>-3.057943108185491</v>
+        <v>-3.058033887324544</v>
       </c>
       <c r="G256">
         <v>-0.05723884722613048</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.147857987285641</v>
+        <v>-3.147902634235793</v>
       </c>
       <c r="G257">
         <v>-0.06523516485980907</v>
@@ -6326,7 +6326,7 @@
         <v>707</v>
       </c>
       <c r="F258">
-        <v>-3.230502321002861</v>
+        <v>-3.230768473754967</v>
       </c>
       <c r="G258">
         <v>-0.06834797726552355</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.308364894749349</v>
+        <v>-3.308466748511286</v>
       </c>
       <c r="G259">
         <v>-0.06499168668186583</v>
@@ -6372,7 +6372,7 @@
         <v>990</v>
       </c>
       <c r="F260">
-        <v>-3.379271940079538</v>
+        <v>-3.379356842202722</v>
       </c>
       <c r="G260">
         <v>-0.05743932002365837</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.444757276326715</v>
+        <v>-3.444922756180121</v>
       </c>
       <c r="G261">
         <v>-0.04394327254395969</v>
@@ -6418,7 +6418,7 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.504912815149955</v>
+        <v>-3.504948328638029</v>
       </c>
       <c r="G262">
         <v>-0.0252635603647639</v>
@@ -6487,7 +6487,7 @@
         <v>205</v>
       </c>
       <c r="F265">
-        <v>-2.88663317535716</v>
+        <v>-2.886648705576499</v>
       </c>
       <c r="G265">
         <v>-0.0240632056775123</v>
@@ -6533,7 +6533,7 @@
         <v>617</v>
       </c>
       <c r="F267">
-        <v>-3.083747118797938</v>
+        <v>-3.083786685881001</v>
       </c>
       <c r="G267">
         <v>-0.05631636605077839</v>
@@ -6556,7 +6556,7 @@
         <v>822</v>
       </c>
       <c r="F268">
-        <v>-3.17338101498985</v>
+        <v>-3.173468430173576</v>
       </c>
       <c r="G268">
         <v>-0.06455489133007597</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.257506832477579</v>
+        <v>-3.257669730213949</v>
       </c>
       <c r="G269">
         <v>-0.06780675191923091</v>
@@ -6602,7 +6602,7 @@
         <v>1234</v>
       </c>
       <c r="F270">
-        <v>-3.335467732329208</v>
+        <v>-3.335670191620075</v>
       </c>
       <c r="G270">
         <v>-0.06419752115149246</v>
@@ -6625,7 +6625,7 @@
         <v>1439</v>
       </c>
       <c r="F271">
-        <v>-3.40650823760156</v>
+        <v>-3.40660842473607</v>
       </c>
       <c r="G271">
         <v>-0.05688140820342391</v>
@@ -6648,7 +6648,7 @@
         <v>1645</v>
       </c>
       <c r="F272">
-        <v>-3.473242329533754</v>
+        <v>-3.473262160184327</v>
       </c>
       <c r="G272">
         <v>-0.04387737884515908</v>
@@ -6671,7 +6671,7 @@
         <v>1851</v>
       </c>
       <c r="F273">
-        <v>-3.534178823147981</v>
+        <v>-3.534221975637664</v>
       </c>
       <c r="G273">
         <v>-0.02466589200668384</v>
@@ -6740,7 +6740,7 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.905081443542592</v>
+        <v>-2.905106566928623</v>
       </c>
       <c r="G276">
         <v>-0.02406920687054059</v>
@@ -6763,7 +6763,7 @@
         <v>573</v>
       </c>
       <c r="F277">
-        <v>-3.007809816131696</v>
+        <v>-3.007820904161077</v>
       </c>
       <c r="G277">
         <v>-0.04227620044241398</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.103068866715314</v>
+        <v>-3.103132038571233</v>
       </c>
       <c r="G278">
         <v>-0.05607882283516297</v>
@@ -6809,7 +6809,7 @@
         <v>1147</v>
       </c>
       <c r="F279">
-        <v>-3.19345918119902</v>
+        <v>-3.193762605824891</v>
       </c>
       <c r="G279">
         <v>-0.06318188816633419</v>
@@ -6832,7 +6832,7 @@
         <v>1434</v>
       </c>
       <c r="F280">
-        <v>-3.27791540919861</v>
+        <v>-3.278058965241721</v>
       </c>
       <c r="G280">
         <v>-0.06621825962590311</v>
@@ -6855,7 +6855,7 @@
         <v>1721</v>
       </c>
       <c r="F281">
-        <v>-3.356682846191505</v>
+        <v>-3.356846270897324</v>
       </c>
       <c r="G281">
         <v>-0.06398994315260564</v>
@@ -6878,7 +6878,7 @@
         <v>2008</v>
       </c>
       <c r="F282">
-        <v>-3.428988579794057</v>
+        <v>-3.429274291602242</v>
       </c>
       <c r="G282">
         <v>-0.05612750293692592</v>
@@ -6901,7 +6901,7 @@
         <v>2295</v>
       </c>
       <c r="F283">
-        <v>-3.495291882214794</v>
+        <v>-3.495357739826885</v>
       </c>
       <c r="G283">
         <v>-0.04295880299185728</v>
@@ -6924,7 +6924,7 @@
         <v>2582</v>
       </c>
       <c r="F284">
-        <v>-3.557303971857867</v>
+        <v>-3.55732313451188</v>
       </c>
       <c r="G284">
         <v>-0.0244730013361007</v>
@@ -6993,7 +6993,7 @@
         <v>387</v>
       </c>
       <c r="F287">
-        <v>-2.920372840900682</v>
+        <v>-2.920438861383591</v>
       </c>
       <c r="G287">
         <v>-0.02367997741095973</v>
@@ -7016,7 +7016,7 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.023708441915248</v>
+        <v>-3.023811459835784</v>
       </c>
       <c r="G288">
         <v>-0.04251300891418719</v>
@@ -7039,7 +7039,7 @@
         <v>1161</v>
       </c>
       <c r="F289">
-        <v>-3.119148480561464</v>
+        <v>-3.119289594855693</v>
       </c>
       <c r="G289">
         <v>-0.05551791606564294</v>
@@ -7062,7 +7062,7 @@
         <v>1548</v>
       </c>
       <c r="F290">
-        <v>-3.210266918530571</v>
+        <v>-3.210469430083216</v>
       </c>
       <c r="G290">
         <v>-0.06299904231392772</v>
@@ -7085,7 +7085,7 @@
         <v>1935</v>
       </c>
       <c r="F291">
-        <v>-3.295232931136971</v>
+        <v>-3.295422915021144</v>
       </c>
       <c r="G291">
         <v>-0.0655803780886155</v>
@@ -7108,7 +7108,7 @@
         <v>2322</v>
       </c>
       <c r="F292">
-        <v>-3.374028071074377</v>
+        <v>-3.374246703705101</v>
       </c>
       <c r="G292">
         <v>-0.06303955016071905</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.446989022551367</v>
+        <v>-3.447102678076216</v>
       </c>
       <c r="G293">
         <v>-0.05515012424061883</v>
@@ -7154,7 +7154,7 @@
         <v>3096</v>
       </c>
       <c r="F294">
-        <v>-3.513611906020523</v>
+        <v>-3.513691383394569</v>
       </c>
       <c r="G294">
         <v>-0.04236717761340913</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.575695261926112</v>
+        <v>-3.575790549707246</v>
       </c>
       <c r="G295">
         <v>-0.02449152068444382</v>
@@ -7246,7 +7246,7 @@
         <v>508</v>
       </c>
       <c r="F298">
-        <v>-2.932636993683525</v>
+        <v>-2.932655848096963</v>
       </c>
       <c r="G298">
         <v>-0.02357381916767043</v>
@@ -7269,7 +7269,7 @@
         <v>1016</v>
       </c>
       <c r="F299">
-        <v>-3.036356251775248</v>
+        <v>-3.036501063241313</v>
       </c>
       <c r="G299">
         <v>-0.04201270279780811</v>
@@ -7292,7 +7292,7 @@
         <v>1524</v>
       </c>
       <c r="F300">
-        <v>-3.132205758788848</v>
+        <v>-3.13234083570705</v>
       </c>
       <c r="G300">
         <v>-0.0543073434687642</v>
@@ -7315,7 +7315,7 @@
         <v>2033</v>
       </c>
       <c r="F301">
-        <v>-3.223654417848852</v>
+        <v>-3.223928165975573</v>
       </c>
       <c r="G301">
         <v>-0.06219144904681673</v>
@@ -7338,7 +7338,7 @@
         <v>2541</v>
       </c>
       <c r="F302">
-        <v>-3.308923757593324</v>
+        <v>-3.309177904399856</v>
       </c>
       <c r="G302">
         <v>-0.06503915675330885</v>
@@ -7361,7 +7361,7 @@
         <v>3049</v>
       </c>
       <c r="F303">
-        <v>-3.3879805413396</v>
+        <v>-3.388179810705326</v>
       </c>
       <c r="G303">
         <v>-0.06236990600344705</v>
@@ -7384,7 +7384,7 @@
         <v>3558</v>
       </c>
       <c r="F304">
-        <v>-3.461625250008425</v>
+        <v>-3.461866498325764</v>
       </c>
       <c r="G304">
         <v>-0.05464736464488806</v>
@@ -7407,7 +7407,7 @@
         <v>4066</v>
       </c>
       <c r="F305">
-        <v>-3.528450113799827</v>
+        <v>-3.528573556442502</v>
       </c>
       <c r="G305">
         <v>-0.04220518905553605</v>
@@ -7430,7 +7430,7 @@
         <v>4574</v>
       </c>
       <c r="F306">
-        <v>-3.590830647460414</v>
+        <v>-3.590938492743553</v>
       </c>
       <c r="G306">
         <v>-0.02395110289660207</v>
@@ -7499,7 +7499,7 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.94286615191264</v>
+        <v>-2.942920006667157</v>
       </c>
       <c r="G309">
         <v>-0.02338508521976257</v>
@@ -7522,7 +7522,7 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.047023753634885</v>
+        <v>-3.047234594693424</v>
       </c>
       <c r="G310">
         <v>-0.04129000151007567</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.143304376754101</v>
+        <v>-3.143484222912882</v>
       </c>
       <c r="G311">
         <v>-0.05420531534682338</v>
@@ -7568,7 +7568,7 @@
         <v>2610</v>
       </c>
       <c r="F312">
-        <v>-3.235320472243015</v>
+        <v>-3.235571227764392</v>
       </c>
       <c r="G312">
         <v>-0.06159631211594552</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.32051480760932</v>
+        <v>-3.320786266926356</v>
       </c>
       <c r="G313">
         <v>-0.06397337201434161</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.400014245160864</v>
+        <v>-3.400258304735245</v>
       </c>
       <c r="G314">
         <v>-0.061438666420216</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.473912623648221</v>
+        <v>-3.474085115357173</v>
       </c>
       <c r="G315">
         <v>-0.05399105464408593</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.541055091318504</v>
+        <v>-3.541198542655984</v>
       </c>
       <c r="G316">
         <v>-0.0413182393111089</v>
@@ -7683,7 +7683,7 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.603478373974208</v>
+        <v>-3.603589511528047</v>
       </c>
       <c r="G317">
         <v>-0.02372300662380827</v>
@@ -7752,7 +7752,7 @@
         <v>821</v>
       </c>
       <c r="F320">
-        <v>-2.951649812661532</v>
+        <v>-2.951681911111284</v>
       </c>
       <c r="G320">
         <v>-0.0233819330146412</v>
@@ -7775,7 +7775,7 @@
         <v>1643</v>
       </c>
       <c r="F321">
-        <v>-3.055948907401567</v>
+        <v>-3.056192146779531</v>
       </c>
       <c r="G321">
         <v>-0.0412592898511992</v>
@@ -7798,7 +7798,7 @@
         <v>2465</v>
       </c>
       <c r="F322">
-        <v>-3.152863255870566</v>
+        <v>-3.153027162980202</v>
       </c>
       <c r="G322">
         <v>-0.05332638142041324</v>
@@ -7821,7 +7821,7 @@
         <v>3286</v>
       </c>
       <c r="F323">
-        <v>-3.244344609954935</v>
+        <v>-3.244634265669324</v>
       </c>
       <c r="G323">
         <v>-0.06099802107311758</v>
@@ -7844,7 +7844,7 @@
         <v>4108</v>
       </c>
       <c r="F324">
-        <v>-3.330190749330464</v>
+        <v>-3.330427147780999</v>
       </c>
       <c r="G324">
         <v>-0.06352861199624371</v>
@@ -7867,7 +7867,7 @@
         <v>4930</v>
       </c>
       <c r="F325">
-        <v>-3.41012628034601</v>
+        <v>-3.41031751669806</v>
       </c>
       <c r="G325">
         <v>-0.06095986211832471</v>
@@ -7890,7 +7890,7 @@
         <v>5751</v>
       </c>
       <c r="F326">
-        <v>-3.484001573272431</v>
+        <v>-3.484248451398082</v>
       </c>
       <c r="G326">
         <v>-0.05364092179063251</v>
@@ -7913,7 +7913,7 @@
         <v>6573</v>
       </c>
       <c r="F327">
-        <v>-3.551679437867892</v>
+        <v>-3.551860452015902</v>
       </c>
       <c r="G327">
         <v>-0.04087010370692101</v>
@@ -7936,7 +7936,7 @@
         <v>7395</v>
       </c>
       <c r="F328">
-        <v>-3.614400897872223</v>
+        <v>-3.614497557467764</v>
       </c>
       <c r="G328">
         <v>-0.02339390262022029</v>
@@ -8005,7 +8005,7 @@
         <v>1017</v>
       </c>
       <c r="F331">
-        <v>-2.959177922907605</v>
+        <v>-2.959209306797173</v>
       </c>
       <c r="G331">
         <v>-0.02304604198804938</v>
@@ -8028,7 +8028,7 @@
         <v>2035</v>
       </c>
       <c r="F332">
-        <v>-3.063644383045004</v>
+        <v>-3.063915140266591</v>
       </c>
       <c r="G332">
         <v>-0.04084545509864856</v>
@@ -8051,7 +8051,7 @@
         <v>3053</v>
       </c>
       <c r="F333">
-        <v>-3.160789252012596</v>
+        <v>-3.161016428670024</v>
       </c>
       <c r="G333">
         <v>-0.05317217999790391</v>
@@ -8074,7 +8074,7 @@
         <v>4071</v>
       </c>
       <c r="F334">
-        <v>-3.25276570079152</v>
+        <v>-3.25303491774717</v>
       </c>
       <c r="G334">
         <v>-0.06057126192654172</v>
@@ -8097,7 +8097,7 @@
         <v>5089</v>
       </c>
       <c r="F335">
-        <v>-3.338815710521684</v>
+        <v>-3.339164617685162</v>
       </c>
       <c r="G335">
         <v>-0.06278717063128125</v>
@@ -8120,7 +8120,7 @@
         <v>6107</v>
       </c>
       <c r="F336">
-        <v>-3.418683347953833</v>
+        <v>-3.418931257105607</v>
       </c>
       <c r="G336">
         <v>-0.06050505627801783</v>
@@ -8143,7 +8143,7 @@
         <v>7125</v>
       </c>
       <c r="F337">
-        <v>-3.492912858164739</v>
+        <v>-3.493213208677458</v>
       </c>
       <c r="G337">
         <v>-0.05286449853341879</v>
@@ -8166,7 +8166,7 @@
         <v>8143</v>
       </c>
       <c r="F338">
-        <v>-3.560941762816751</v>
+        <v>-3.561115709136236</v>
       </c>
       <c r="G338">
         <v>-0.04053172592297882</v>
@@ -8189,7 +8189,7 @@
         <v>9161</v>
       </c>
       <c r="F339">
-        <v>-3.623541557974249</v>
+        <v>-3.623635563646868</v>
       </c>
       <c r="G339">
         <v>-0.02310751223477731</v>

</xml_diff>